<commit_message>
Atualiza├º├úo manual da base Atendimento.xlsx
</commit_message>
<xml_diff>
--- a/Atendimento.xlsx
+++ b/Atendimento.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\glaudoberto.filho\Desktop\Projetos Python\app_fup\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\glaudoberto.filho\Desktop\Projetos Python\app_fup_frontend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48473E2C-8D25-4DE7-A86E-69A73E20C2CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{333E4148-E646-4175-AC91-C92FB240CEB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2021" uniqueCount="394">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2029" uniqueCount="395">
   <si>
     <t>SC</t>
   </si>
@@ -1226,6 +1226,9 @@
   </si>
   <si>
     <t>previsão de entrega</t>
+  </si>
+  <si>
+    <t>Glaudoberto</t>
   </si>
 </sst>
 </file>
@@ -1292,7 +1295,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1344,6 +1347,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1401,7 +1410,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1569,6 +1578,18 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="10" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1751,8 +1772,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0C573FEE-B8A0-4FE7-911C-81B026DE4530}" name="Tabela1" displayName="Tabela1" ref="A1:T194" totalsRowShown="0" headerRowDxfId="36" dataDxfId="35">
-  <autoFilter ref="A1:T194" xr:uid="{0C573FEE-B8A0-4FE7-911C-81B026DE4530}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0C573FEE-B8A0-4FE7-911C-81B026DE4530}" name="Tabela1" displayName="Tabela1" ref="A1:T195" totalsRowShown="0" headerRowDxfId="36" dataDxfId="35">
+  <autoFilter ref="A1:T195" xr:uid="{0C573FEE-B8A0-4FE7-911C-81B026DE4530}">
     <filterColumn colId="5">
       <filters>
         <filter val="68317"/>
@@ -2239,10 +2260,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T194"/>
+  <dimension ref="A1:T195"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P116" sqref="P116"/>
+    <sheetView tabSelected="1" topLeftCell="A139" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A195" sqref="A195:T195"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -14681,6 +14702,70 @@
         <v>0</v>
       </c>
       <c r="T194" s="51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="195" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A195" s="63">
+        <v>45864</v>
+      </c>
+      <c r="B195" s="63">
+        <v>45864</v>
+      </c>
+      <c r="C195" s="63" t="s">
+        <v>7</v>
+      </c>
+      <c r="D195" s="63" t="s">
+        <v>15</v>
+      </c>
+      <c r="E195" s="63" t="s">
+        <v>113</v>
+      </c>
+      <c r="F195" s="64">
+        <v>70000</v>
+      </c>
+      <c r="G195" s="64" t="s">
+        <v>394</v>
+      </c>
+      <c r="H195" s="64" t="s">
+        <v>300</v>
+      </c>
+      <c r="I195" s="65">
+        <f>NETWORKDAYS(B195, A195)</f>
+        <v>0</v>
+      </c>
+      <c r="J195" s="64">
+        <v>70001</v>
+      </c>
+      <c r="K195" s="64">
+        <v>2931</v>
+      </c>
+      <c r="L195" s="64" t="s">
+        <v>381</v>
+      </c>
+      <c r="M195" s="63">
+        <v>45868</v>
+      </c>
+      <c r="N195" s="66">
+        <v>3500</v>
+      </c>
+      <c r="O195" s="64" t="s">
+        <v>122</v>
+      </c>
+      <c r="P195" s="64">
+        <v>30</v>
+      </c>
+      <c r="Q195" s="64" t="s">
+        <v>24</v>
+      </c>
+      <c r="R195" s="64">
+        <f>DATEDIF(Tabela1[[#This Row],[Atendimento]],Tabela1[[#This Row],[previsão de entrega]],"D")</f>
+        <v>4</v>
+      </c>
+      <c r="S195" s="66">
+        <v>320</v>
+      </c>
+      <c r="T195" s="66">
         <v>0</v>
       </c>
     </row>
@@ -14959,7 +15044,7 @@
       </c>
       <c r="E2" s="24">
         <f t="shared" ref="E2:E6" ca="1" si="0">TODAY()</f>
-        <v>45852</v>
+        <v>45864</v>
       </c>
       <c r="F2" s="22" t="str">
         <f ca="1">IF(Tabela4[[#This Row],[Hoje]] &lt;= Tabela4[[#This Row],[Validade]],
@@ -14967,7 +15052,7 @@
       "Negociar",
       "Faltam " &amp; DATEDIF(Tabela4[[#This Row],[Hoje]],Tabela4[[#This Row],[Validade]],"D") &amp; " dias para vencer"),
    "Venceu há " &amp; DATEDIF(Tabela4[[#This Row],[Validade]],Tabela4[[#This Row],[Hoje]],"D") &amp; " dias")</f>
-        <v>Faltam 614 dias para vencer</v>
+        <v>Faltam 602 dias para vencer</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.35">
@@ -14985,7 +15070,7 @@
       </c>
       <c r="E3" s="26">
         <f t="shared" ca="1" si="0"/>
-        <v>45852</v>
+        <v>45864</v>
       </c>
       <c r="F3" s="21" t="str">
         <f ca="1">IF(Tabela4[[#This Row],[Hoje]] &lt;= Tabela4[[#This Row],[Validade]],
@@ -14993,7 +15078,7 @@
       "Negociar",
       "Faltam " &amp; DATEDIF(Tabela4[[#This Row],[Hoje]],Tabela4[[#This Row],[Validade]],"D") &amp; " dias para vencer"),
    "Venceu há " &amp; DATEDIF(Tabela4[[#This Row],[Validade]],Tabela4[[#This Row],[Hoje]],"D") &amp; " dias")</f>
-        <v>Venceu há 286 dias</v>
+        <v>Venceu há 298 dias</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.35">
@@ -15011,7 +15096,7 @@
       </c>
       <c r="E4" s="40">
         <f t="shared" ca="1" si="0"/>
-        <v>45852</v>
+        <v>45864</v>
       </c>
       <c r="F4" s="41" t="str">
         <f ca="1">IF(Tabela4[[#This Row],[Hoje]] &lt;= Tabela4[[#This Row],[Validade]],
@@ -15019,7 +15104,7 @@
       "Negociar",
       "Faltam " &amp; DATEDIF(Tabela4[[#This Row],[Hoje]],Tabela4[[#This Row],[Validade]],"D") &amp; " dias para vencer"),
    "Venceu há " &amp; DATEDIF(Tabela4[[#This Row],[Validade]],Tabela4[[#This Row],[Hoje]],"D") &amp; " dias")</f>
-        <v>Negociar</v>
+        <v>Venceu há 6 dias</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.35">
@@ -15037,7 +15122,7 @@
       </c>
       <c r="E5" s="17">
         <f t="shared" ca="1" si="0"/>
-        <v>45852</v>
+        <v>45864</v>
       </c>
       <c r="F5" s="3" t="str">
         <f ca="1">IF(Tabela4[[#This Row],[Hoje]] &lt;= Tabela4[[#This Row],[Validade]],
@@ -15063,7 +15148,7 @@
       </c>
       <c r="E6" s="17">
         <f t="shared" ca="1" si="0"/>
-        <v>45852</v>
+        <v>45864</v>
       </c>
       <c r="F6" s="3" t="str">
         <f ca="1">IF(Tabela4[[#This Row],[Hoje]] &lt;= Tabela4[[#This Row],[Validade]],
@@ -15089,7 +15174,7 @@
       </c>
       <c r="E7" s="26">
         <f t="shared" ref="E7:E9" ca="1" si="1">TODAY()</f>
-        <v>45852</v>
+        <v>45864</v>
       </c>
       <c r="F7" s="21" t="str">
         <f ca="1">IF(Tabela4[[#This Row],[Hoje]] &lt;= Tabela4[[#This Row],[Validade]],
@@ -15097,7 +15182,7 @@
       "Negociar",
       "Faltam " &amp; DATEDIF(Tabela4[[#This Row],[Hoje]],Tabela4[[#This Row],[Validade]],"D") &amp; " dias para vencer"),
    "Venceu há " &amp; DATEDIF(Tabela4[[#This Row],[Validade]],Tabela4[[#This Row],[Hoje]],"D") &amp; " dias")</f>
-        <v>Venceu há 118 dias</v>
+        <v>Venceu há 130 dias</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.35">
@@ -15115,7 +15200,7 @@
       </c>
       <c r="E8" s="26">
         <f t="shared" ca="1" si="1"/>
-        <v>45852</v>
+        <v>45864</v>
       </c>
       <c r="F8" s="21" t="str">
         <f ca="1">IF(Tabela4[[#This Row],[Hoje]] &lt;= Tabela4[[#This Row],[Validade]],
@@ -15123,7 +15208,7 @@
       "Negociar",
       "Faltam " &amp; DATEDIF(Tabela4[[#This Row],[Hoje]],Tabela4[[#This Row],[Validade]],"D") &amp; " dias para vencer"),
    "Venceu há " &amp; DATEDIF(Tabela4[[#This Row],[Validade]],Tabela4[[#This Row],[Hoje]],"D") &amp; " dias")</f>
-        <v>Venceu há 861 dias</v>
+        <v>Venceu há 873 dias</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.35">
@@ -15141,7 +15226,7 @@
       </c>
       <c r="E9" s="24">
         <f t="shared" ca="1" si="1"/>
-        <v>45852</v>
+        <v>45864</v>
       </c>
       <c r="F9" s="22" t="str">
         <f ca="1">IF(Tabela4[[#This Row],[Hoje]] &lt;= Tabela4[[#This Row],[Validade]],
@@ -15149,7 +15234,7 @@
       "Negociar",
       "Faltam " &amp; DATEDIF(Tabela4[[#This Row],[Hoje]],Tabela4[[#This Row],[Validade]],"D") &amp; " dias para vencer"),
    "Venceu há " &amp; DATEDIF(Tabela4[[#This Row],[Validade]],Tabela4[[#This Row],[Hoje]],"D") &amp; " dias")</f>
-        <v>Faltam 430 dias para vencer</v>
+        <v>Faltam 418 dias para vencer</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.35">
@@ -15167,7 +15252,7 @@
       </c>
       <c r="E10" s="24">
         <f ca="1">TODAY()</f>
-        <v>45852</v>
+        <v>45864</v>
       </c>
       <c r="F10" s="22" t="str">
         <f ca="1">IF(Tabela4[[#This Row],[Hoje]] &lt;= Tabela4[[#This Row],[Validade]],
@@ -15175,7 +15260,7 @@
       "Negociar",
       "Faltam " &amp; DATEDIF(Tabela4[[#This Row],[Hoje]],Tabela4[[#This Row],[Validade]],"D") &amp; " dias para vencer"),
    "Venceu há " &amp; DATEDIF(Tabela4[[#This Row],[Validade]],Tabela4[[#This Row],[Hoje]],"D") &amp; " dias")</f>
-        <v>Faltam 351 dias para vencer</v>
+        <v>Faltam 339 dias para vencer</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.35">
@@ -15193,7 +15278,7 @@
       </c>
       <c r="E11" s="24">
         <f ca="1">TODAY()</f>
-        <v>45852</v>
+        <v>45864</v>
       </c>
       <c r="F11" s="22" t="str">
         <f ca="1">IF(Tabela4[[#This Row],[Hoje]] &lt;= Tabela4[[#This Row],[Validade]],
@@ -15201,7 +15286,7 @@
       "Negociar",
       "Faltam " &amp; DATEDIF(Tabela4[[#This Row],[Hoje]],Tabela4[[#This Row],[Validade]],"D") &amp; " dias para vencer"),
    "Venceu há " &amp; DATEDIF(Tabela4[[#This Row],[Validade]],Tabela4[[#This Row],[Hoje]],"D") &amp; " dias")</f>
-        <v>Faltam 140 dias para vencer</v>
+        <v>Faltam 128 dias para vencer</v>
       </c>
     </row>
   </sheetData>
@@ -16652,9 +16737,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -16784,26 +16872,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{258E5A34-0198-4570-927D-9873053383F0}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F1DB20CA-6C9E-462A-9B1E-209C1B3156BD}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="b7545978-8353-4157-ab02-92f5c69a97d9"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -16827,9 +16904,17 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F1DB20CA-6C9E-462A-9B1E-209C1B3156BD}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{258E5A34-0198-4570-927D-9873053383F0}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="b7545978-8353-4157-ab02-92f5c69a97d9"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Atualização de base e código
</commit_message>
<xml_diff>
--- a/Atendimento.xlsx
+++ b/Atendimento.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\PUBLICO\Compras\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\glaudoberto.filho\Desktop\Projetos Python\app_fup_frontend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F2A02F8-5AF9-4AF1-A683-6A3F04F4A2E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{639662BA-467F-4F10-BA20-604BC6341315}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1653,6 +1653,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1742,16 +1743,7 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0C573FEE-B8A0-4FE7-911C-81B026DE4530}" name="Tabela1" displayName="Tabela1" ref="A1:T226" totalsRowShown="0" headerRowDxfId="36" dataDxfId="35">
-  <autoFilter ref="A1:T226" xr:uid="{0C573FEE-B8A0-4FE7-911C-81B026DE4530}">
-    <filterColumn colId="16">
-      <filters>
-        <filter val="AGUARDANDO APROVAÇÃO"/>
-        <filter val="AGUARDANDO ENTREGA"/>
-        <filter val="AGUARDANDO PAGAMENTO"/>
-        <filter val="AJUSTE"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:T226" xr:uid="{0C573FEE-B8A0-4FE7-911C-81B026DE4530}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:T146">
     <sortCondition ref="A1:A146"/>
   </sortState>
@@ -2120,8 +2112,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T226"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K224" sqref="K224"/>
+    <sheetView tabSelected="1" topLeftCell="I16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2211,7 +2203,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="2" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A2" s="6">
         <v>45782</v>
       </c>
@@ -2275,7 +2267,7 @@
         <v>285.3</v>
       </c>
     </row>
-    <row r="3" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A3" s="6">
         <v>45784</v>
       </c>
@@ -2339,7 +2331,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A4" s="6">
         <v>45784</v>
       </c>
@@ -2403,7 +2395,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A5" s="6">
         <v>45784</v>
       </c>
@@ -2467,7 +2459,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A6" s="6">
         <v>45784</v>
       </c>
@@ -2531,7 +2523,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A7" s="6">
         <v>45784</v>
       </c>
@@ -2595,7 +2587,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A8" s="6">
         <v>45785</v>
       </c>
@@ -2659,7 +2651,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A9" s="6">
         <v>45785</v>
       </c>
@@ -2723,7 +2715,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A10" s="6">
         <v>45785</v>
       </c>
@@ -2851,7 +2843,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A12" s="6">
         <v>45786</v>
       </c>
@@ -2915,7 +2907,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A13" s="6">
         <v>45786</v>
       </c>
@@ -2979,7 +2971,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A14" s="6">
         <v>45786</v>
       </c>
@@ -3043,7 +3035,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A15" s="6">
         <v>45786</v>
       </c>
@@ -3107,7 +3099,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A16" s="6">
         <v>45786</v>
       </c>
@@ -3171,7 +3163,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A17" s="6">
         <v>45786</v>
       </c>
@@ -3235,7 +3227,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A18" s="6">
         <v>45789</v>
       </c>
@@ -3299,7 +3291,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A19" s="6">
         <v>45789</v>
       </c>
@@ -3363,7 +3355,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A20" s="6">
         <v>45790</v>
       </c>
@@ -3427,7 +3419,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A21" s="6">
         <v>45790</v>
       </c>
@@ -3491,7 +3483,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A22" s="6">
         <v>45790</v>
       </c>
@@ -3555,7 +3547,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A23" s="28">
         <v>45790</v>
       </c>
@@ -3619,7 +3611,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A24" s="6">
         <v>45791</v>
       </c>
@@ -3683,7 +3675,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A25" s="6">
         <v>45791</v>
       </c>
@@ -3747,7 +3739,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A26" s="6">
         <v>45792</v>
       </c>
@@ -3811,7 +3803,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A27" s="6">
         <v>45792</v>
       </c>
@@ -3875,7 +3867,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A28" s="6">
         <v>45792</v>
       </c>
@@ -3939,7 +3931,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A29" s="6">
         <v>45792</v>
       </c>
@@ -4003,7 +3995,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A30" s="6">
         <v>45792</v>
       </c>
@@ -4067,7 +4059,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A31" s="6">
         <v>45793</v>
       </c>
@@ -4131,7 +4123,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A32" s="6">
         <v>45793</v>
       </c>
@@ -4195,7 +4187,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A33" s="6">
         <v>45793</v>
       </c>
@@ -4259,7 +4251,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A34" s="6">
         <v>45793</v>
       </c>
@@ -4323,7 +4315,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A35" s="6">
         <v>45796</v>
       </c>
@@ -4387,7 +4379,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A36" s="6">
         <v>45796</v>
       </c>
@@ -4451,7 +4443,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A37" s="6">
         <v>45796</v>
       </c>
@@ -4515,7 +4507,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A38" s="6">
         <v>45796</v>
       </c>
@@ -4579,7 +4571,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A39" s="6">
         <v>45797</v>
       </c>
@@ -4643,7 +4635,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A40" s="6">
         <v>45797</v>
       </c>
@@ -4707,7 +4699,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A41" s="6">
         <v>45797</v>
       </c>
@@ -4771,7 +4763,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A42" s="6">
         <v>45797</v>
       </c>
@@ -4835,7 +4827,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A43" s="6">
         <v>45797</v>
       </c>
@@ -4899,7 +4891,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A44" s="6">
         <v>45797</v>
       </c>
@@ -4963,7 +4955,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A45" s="6">
         <v>45797</v>
       </c>
@@ -5027,7 +5019,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A46" s="6">
         <v>45797</v>
       </c>
@@ -5091,7 +5083,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A47" s="6">
         <v>45797</v>
       </c>
@@ -5155,7 +5147,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A48" s="6">
         <v>45798</v>
       </c>
@@ -5219,7 +5211,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A49" s="6">
         <v>45798</v>
       </c>
@@ -5283,7 +5275,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A50" s="6">
         <v>45798</v>
       </c>
@@ -5347,7 +5339,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A51" s="6">
         <v>45798</v>
       </c>
@@ -5411,7 +5403,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A52" s="6">
         <v>45798</v>
       </c>
@@ -5475,7 +5467,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A53" s="6">
         <v>45798</v>
       </c>
@@ -5539,7 +5531,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A54" s="6">
         <v>45798</v>
       </c>
@@ -5667,7 +5659,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A56" s="6">
         <v>45799</v>
       </c>
@@ -5731,7 +5723,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A57" s="6">
         <v>45799</v>
       </c>
@@ -5795,7 +5787,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A58" s="6">
         <v>45800</v>
       </c>
@@ -5859,7 +5851,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A59" s="6">
         <v>45800</v>
       </c>
@@ -5923,7 +5915,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A60" s="6">
         <v>45800</v>
       </c>
@@ -5987,7 +5979,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A61" s="6">
         <v>45800</v>
       </c>
@@ -6051,7 +6043,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A62" s="6">
         <v>45800</v>
       </c>
@@ -6115,7 +6107,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A63" s="6">
         <v>45800</v>
       </c>
@@ -6179,7 +6171,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A64" s="6">
         <v>45800</v>
       </c>
@@ -6243,7 +6235,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A65" s="6">
         <v>45800</v>
       </c>
@@ -6307,7 +6299,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A66" s="6">
         <v>45800</v>
       </c>
@@ -6371,7 +6363,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A67" s="6">
         <v>45803</v>
       </c>
@@ -6435,7 +6427,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A68" s="6">
         <v>45804</v>
       </c>
@@ -6499,7 +6491,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A69" s="6">
         <v>45804</v>
       </c>
@@ -6563,7 +6555,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A70" s="6">
         <v>45805</v>
       </c>
@@ -6627,7 +6619,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A71" s="6">
         <v>45806</v>
       </c>
@@ -6691,7 +6683,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A72" s="6">
         <v>45806</v>
       </c>
@@ -6755,7 +6747,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A73" s="6">
         <v>45806</v>
       </c>
@@ -6819,7 +6811,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A74" s="6">
         <v>45806</v>
       </c>
@@ -6883,7 +6875,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A75" s="6">
         <v>45806</v>
       </c>
@@ -6947,7 +6939,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A76" s="6">
         <v>45806</v>
       </c>
@@ -7011,7 +7003,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A77" s="6">
         <v>45807</v>
       </c>
@@ -7075,7 +7067,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A78" s="6">
         <v>45810</v>
       </c>
@@ -7139,7 +7131,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A79" s="6">
         <v>45810</v>
       </c>
@@ -7203,7 +7195,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A80" s="6">
         <v>45810</v>
       </c>
@@ -7267,7 +7259,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A81" s="6">
         <v>45810</v>
       </c>
@@ -7331,7 +7323,7 @@
         <v>285.3</v>
       </c>
     </row>
-    <row r="82" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A82" s="6">
         <v>45810</v>
       </c>
@@ -7395,7 +7387,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A83" s="6">
         <v>45810</v>
       </c>
@@ -7459,7 +7451,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A84" s="6">
         <v>45810</v>
       </c>
@@ -7523,7 +7515,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A85" s="6">
         <v>45810</v>
       </c>
@@ -7587,7 +7579,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A86" s="28">
         <v>45810</v>
       </c>
@@ -7651,7 +7643,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A87" s="6">
         <v>45811</v>
       </c>
@@ -7715,7 +7707,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A88" s="6">
         <v>45811</v>
       </c>
@@ -7779,7 +7771,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A89" s="6">
         <v>45811</v>
       </c>
@@ -7843,7 +7835,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A90" s="6">
         <v>45812</v>
       </c>
@@ -7907,7 +7899,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A91" s="6">
         <v>45812</v>
       </c>
@@ -7971,7 +7963,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A92" s="6">
         <v>45812</v>
       </c>
@@ -8035,7 +8027,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A93" s="6">
         <v>45812</v>
       </c>
@@ -8099,7 +8091,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A94" s="6">
         <v>45812</v>
       </c>
@@ -8163,7 +8155,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A95" s="6">
         <v>45812</v>
       </c>
@@ -8227,7 +8219,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A96" s="6">
         <v>45812</v>
       </c>
@@ -8291,7 +8283,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A97" s="6">
         <v>45813</v>
       </c>
@@ -8355,7 +8347,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A98" s="6">
         <v>45813</v>
       </c>
@@ -8419,7 +8411,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A99" s="6">
         <v>45813</v>
       </c>
@@ -8483,7 +8475,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A100" s="6">
         <v>45813</v>
       </c>
@@ -8547,7 +8539,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A101" s="6">
         <v>45813</v>
       </c>
@@ -8611,7 +8603,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A102" s="6">
         <v>45813</v>
       </c>
@@ -8675,7 +8667,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A103" s="6">
         <v>45814</v>
       </c>
@@ -8739,7 +8731,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A104" s="6">
         <v>45817</v>
       </c>
@@ -8803,7 +8795,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A105" s="6">
         <v>45817</v>
       </c>
@@ -8867,7 +8859,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A106" s="6">
         <v>45818</v>
       </c>
@@ -8931,7 +8923,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A107" s="6">
         <v>45818</v>
       </c>
@@ -8995,7 +8987,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A108" s="6">
         <v>45818</v>
       </c>
@@ -9249,7 +9241,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A112" s="6">
         <v>45818</v>
       </c>
@@ -9377,7 +9369,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A114" s="6">
         <v>45819</v>
       </c>
@@ -9441,7 +9433,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A115" s="6">
         <v>45819</v>
       </c>
@@ -9505,7 +9497,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A116" s="6">
         <v>45819</v>
       </c>
@@ -9569,7 +9561,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A117" s="6">
         <v>45820</v>
       </c>
@@ -9633,7 +9625,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A118" s="6">
         <v>45820</v>
       </c>
@@ -9697,7 +9689,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A119" s="6">
         <v>45820</v>
       </c>
@@ -9761,7 +9753,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="120" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A120" s="6">
         <v>45820</v>
       </c>
@@ -9825,7 +9817,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A121" s="6">
         <v>45820</v>
       </c>
@@ -9889,7 +9881,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="122" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A122" s="6">
         <v>45821</v>
       </c>
@@ -9953,7 +9945,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="123" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A123" s="6">
         <v>45821</v>
       </c>
@@ -10017,7 +10009,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="124" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A124" s="6">
         <v>45821</v>
       </c>
@@ -10081,7 +10073,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A125" s="6">
         <v>45824</v>
       </c>
@@ -10145,7 +10137,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="126" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A126" s="6">
         <v>45824</v>
       </c>
@@ -10209,7 +10201,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A127" s="6">
         <v>45824</v>
       </c>
@@ -10273,7 +10265,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="128" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A128" s="6">
         <v>45824</v>
       </c>
@@ -10337,7 +10329,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="129" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A129" s="6">
         <v>45824</v>
       </c>
@@ -10401,7 +10393,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="130" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A130" s="6">
         <v>45825</v>
       </c>
@@ -10465,7 +10457,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="131" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A131" s="6">
         <v>45825</v>
       </c>
@@ -10657,7 +10649,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="134" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A134" s="6">
         <v>45826</v>
       </c>
@@ -10721,7 +10713,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="135" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A135" s="6">
         <v>45826</v>
       </c>
@@ -10785,7 +10777,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="136" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A136" s="6">
         <v>45826</v>
       </c>
@@ -10849,7 +10841,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="137" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A137" s="6">
         <v>45826</v>
       </c>
@@ -10977,7 +10969,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="139" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A139" s="6">
         <v>45826</v>
       </c>
@@ -11041,7 +11033,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="140" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A140" s="6">
         <v>45826</v>
       </c>
@@ -11105,7 +11097,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="141" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A141" s="6">
         <v>45826</v>
       </c>
@@ -11169,7 +11161,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="142" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A142" s="6">
         <v>45826</v>
       </c>
@@ -11233,7 +11225,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="143" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A143" s="6">
         <v>45826</v>
       </c>
@@ -11297,7 +11289,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="144" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A144" s="6">
         <v>45826</v>
       </c>
@@ -11361,7 +11353,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="145" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A145" s="6">
         <v>45826</v>
       </c>
@@ -11425,7 +11417,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="146" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A146" s="6">
         <v>45826</v>
       </c>
@@ -11489,7 +11481,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="147" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A147" s="6">
         <v>45831</v>
       </c>
@@ -11553,7 +11545,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="148" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A148" s="6">
         <v>45831</v>
       </c>
@@ -11617,7 +11609,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="149" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A149" s="6">
         <v>45831</v>
       </c>
@@ -11745,7 +11737,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="151" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A151" s="6">
         <v>45831</v>
       </c>
@@ -11809,7 +11801,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="152" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A152" s="6">
         <v>45831</v>
       </c>
@@ -11873,7 +11865,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="153" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A153" s="6">
         <v>45831</v>
       </c>
@@ -11937,7 +11929,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="154" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A154" s="6">
         <v>45831</v>
       </c>
@@ -12001,7 +11993,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="155" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A155" s="6">
         <v>45831</v>
       </c>
@@ -12065,7 +12057,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="156" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A156" s="6">
         <v>45833</v>
       </c>
@@ -12129,7 +12121,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="157" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A157" s="6">
         <v>45833</v>
       </c>
@@ -12193,7 +12185,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="158" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A158" s="6">
         <v>45833</v>
       </c>
@@ -12257,7 +12249,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="159" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A159" s="6">
         <v>45833</v>
       </c>
@@ -12321,7 +12313,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="160" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A160" s="6">
         <v>45833</v>
       </c>
@@ -12385,7 +12377,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="161" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A161" s="6">
         <v>45834</v>
       </c>
@@ -12449,7 +12441,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="162" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A162" s="6">
         <v>45834</v>
       </c>
@@ -12513,7 +12505,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="163" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A163" s="6">
         <v>45834</v>
       </c>
@@ -12577,7 +12569,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="164" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A164" s="6">
         <v>45834</v>
       </c>
@@ -12641,7 +12633,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="165" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A165" s="6">
         <v>45835</v>
       </c>
@@ -12705,7 +12697,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="166" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A166" s="6">
         <v>45835</v>
       </c>
@@ -12769,7 +12761,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="167" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A167" s="6">
         <v>45839</v>
       </c>
@@ -12833,7 +12825,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="168" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A168" s="6">
         <v>45839</v>
       </c>
@@ -12897,7 +12889,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="169" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A169" s="6">
         <v>45839</v>
       </c>
@@ -12961,7 +12953,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="170" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A170" s="6">
         <v>45839</v>
       </c>
@@ -13025,7 +13017,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="171" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A171" s="6">
         <v>45839</v>
       </c>
@@ -13089,7 +13081,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="172" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A172" s="6">
         <v>45839</v>
       </c>
@@ -13217,7 +13209,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="174" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A174" s="6">
         <v>45840</v>
       </c>
@@ -13345,7 +13337,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="176" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A176" s="6">
         <v>45841</v>
       </c>
@@ -13409,7 +13401,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="177" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A177" s="6">
         <v>45842</v>
       </c>
@@ -13473,7 +13465,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="178" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A178" s="6">
         <v>45842</v>
       </c>
@@ -13537,7 +13529,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="179" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A179" s="6">
         <v>45846</v>
       </c>
@@ -13601,7 +13593,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="180" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A180" s="6">
         <v>45846</v>
       </c>
@@ -13665,7 +13657,7 @@
         <v>285.3</v>
       </c>
     </row>
-    <row r="181" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A181" s="6">
         <v>45846</v>
       </c>
@@ -13857,7 +13849,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="184" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A184" s="6">
         <v>45846</v>
       </c>
@@ -13985,7 +13977,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="186" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A186" s="6">
         <v>45848</v>
       </c>
@@ -14113,7 +14105,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="188" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A188" s="6">
         <v>45848</v>
       </c>
@@ -14177,7 +14169,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="189" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A189" s="6">
         <v>45848</v>
       </c>
@@ -14241,7 +14233,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="190" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A190" s="6">
         <v>45848</v>
       </c>
@@ -14305,7 +14297,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="191" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A191" s="6">
         <v>45849</v>
       </c>
@@ -14433,7 +14425,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="193" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A193" s="6">
         <v>45849</v>
       </c>
@@ -14497,7 +14489,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="194" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A194" s="6">
         <v>45849</v>
       </c>
@@ -14561,7 +14553,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="195" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="195" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A195" s="6">
         <v>45853</v>
       </c>
@@ -14625,7 +14617,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="196" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="196" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A196" s="6">
         <v>45853</v>
       </c>
@@ -14689,7 +14681,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="197" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="197" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A197" s="6">
         <v>45853</v>
       </c>
@@ -14753,7 +14745,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="198" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="198" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A198" s="6">
         <v>45854</v>
       </c>
@@ -14817,7 +14809,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="199" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="199" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A199" s="6">
         <v>45854</v>
       </c>
@@ -14881,7 +14873,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="200" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="200" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A200" s="6">
         <v>45854</v>
       </c>
@@ -14945,7 +14937,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="201" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="201" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A201" s="6">
         <v>45854</v>
       </c>
@@ -15009,7 +15001,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="202" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="202" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A202" s="6">
         <v>45854</v>
       </c>
@@ -15073,7 +15065,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="203" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="203" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A203" s="6">
         <v>45855</v>
       </c>
@@ -15137,7 +15129,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="204" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="204" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A204" s="6">
         <v>45855</v>
       </c>
@@ -15201,7 +15193,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="205" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="205" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A205" s="6">
         <v>45855</v>
       </c>
@@ -15457,7 +15449,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="209" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="209" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A209" s="6">
         <v>45859</v>
       </c>
@@ -15521,7 +15513,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="210" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="210" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A210" s="6">
         <v>45859</v>
       </c>
@@ -15585,7 +15577,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="211" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="211" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A211" s="6">
         <v>45859</v>
       </c>
@@ -15649,7 +15641,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="212" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="212" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A212" s="6">
         <v>45859</v>
       </c>
@@ -15713,7 +15705,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="213" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="213" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A213" s="6">
         <v>45859</v>
       </c>
@@ -15777,7 +15769,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="214" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="214" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A214" s="6">
         <v>45859</v>
       </c>
@@ -15969,7 +15961,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="217" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="217" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A217" s="6">
         <v>45860</v>
       </c>
@@ -16033,7 +16025,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="218" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="218" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A218" s="6">
         <v>45860</v>
       </c>
@@ -16225,7 +16217,7 @@
         <v>141.4</v>
       </c>
     </row>
-    <row r="221" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="221" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A221" s="6">
         <v>45862</v>
       </c>
@@ -16289,7 +16281,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="222" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="222" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A222" s="6">
         <v>45862</v>
       </c>
@@ -16353,7 +16345,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="223" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="223" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A223" s="6">
         <v>45863</v>
       </c>
@@ -16481,7 +16473,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="225" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+    <row r="225" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A225" s="6">
         <v>45863</v>
       </c>

</xml_diff>

<commit_message>
Atualização Banco de dados
</commit_message>
<xml_diff>
--- a/Atendimento.xlsx
+++ b/Atendimento.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\PUBLICO\Compras\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFA06748-2258-433D-B4CF-3D2C8C8FC81B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E002E670-6C05-4DB9-AE8E-6436BFF6C3EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="base_dados" sheetId="1" r:id="rId1"/>
@@ -2120,8 +2120,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T226"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M182" sqref="M182"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L113" sqref="L113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -10952,7 +10952,7 @@
         <v>322</v>
       </c>
       <c r="M138" s="11">
-        <v>45860</v>
+        <v>45867</v>
       </c>
       <c r="N138" s="14">
         <v>2922.9</v>
@@ -10968,7 +10968,7 @@
       </c>
       <c r="R138" s="12">
         <f>DATEDIF(Tabela1[[#This Row],[Atendimento]],Tabela1[[#This Row],[Previsao de Entrega]],"D")</f>
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="S138" s="14">
         <v>0</v>
@@ -15841,67 +15841,67 @@
         <v>0</v>
       </c>
     </row>
-    <row r="215" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A215" s="11">
+    <row r="215" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A215" s="6">
         <v>45860</v>
       </c>
-      <c r="B215" s="11">
+      <c r="B215" s="6">
         <v>45860</v>
       </c>
-      <c r="C215" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="D215" s="11" t="s">
+      <c r="C215" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D215" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="E215" s="11" t="s">
+      <c r="E215" s="6" t="s">
         <v>113</v>
       </c>
-      <c r="F215" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="G215" s="12" t="s">
+      <c r="F215" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="G215" s="7" t="s">
         <v>387</v>
       </c>
-      <c r="H215" s="12" t="s">
+      <c r="H215" s="7" t="s">
         <v>138</v>
       </c>
-      <c r="I215" s="13">
+      <c r="I215" s="10">
         <f t="shared" ref="I215:I220" si="14">NETWORKDAYS(B215, A215)</f>
         <v>1</v>
       </c>
-      <c r="J215" s="12">
+      <c r="J215" s="7">
         <v>66374</v>
       </c>
-      <c r="K215" s="12" t="s">
+      <c r="K215" s="7" t="s">
         <v>139</v>
       </c>
-      <c r="L215" s="12" t="s">
+      <c r="L215" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="M215" s="11">
+      <c r="M215" s="6">
         <v>45867</v>
       </c>
-      <c r="N215" s="14">
+      <c r="N215" s="8">
         <v>528</v>
       </c>
-      <c r="O215" s="12" t="s">
+      <c r="O215" s="7" t="s">
         <v>122</v>
       </c>
-      <c r="P215" s="12">
+      <c r="P215" s="7">
         <v>28</v>
       </c>
-      <c r="Q215" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="R215" s="12">
-        <f>DATEDIF(Tabela1[[#This Row],[Atendimento]],Tabela1[[#This Row],[Previsao de Entrega]],"D")</f>
-        <v>7</v>
-      </c>
-      <c r="S215" s="14">
-        <v>0</v>
-      </c>
-      <c r="T215" s="14">
+      <c r="Q215" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="R215" s="7">
+        <f>DATEDIF(Tabela1[[#This Row],[Atendimento]],Tabela1[[#This Row],[Previsao de Entrega]],"D")</f>
+        <v>7</v>
+      </c>
+      <c r="S215" s="8">
+        <v>0</v>
+      </c>
+      <c r="T215" s="8">
         <v>0</v>
       </c>
     </row>
@@ -18553,12 +18553,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -18688,15 +18685,26 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F1DB20CA-6C9E-462A-9B1E-209C1B3156BD}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{258E5A34-0198-4570-927D-9873053383F0}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="b7545978-8353-4157-ab02-92f5c69a97d9"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -18720,17 +18728,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{258E5A34-0198-4570-927D-9873053383F0}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F1DB20CA-6C9E-462A-9B1E-209C1B3156BD}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="b7545978-8353-4157-ab02-92f5c69a97d9"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Atualização de Base 04-08
</commit_message>
<xml_diff>
--- a/Atendimento.xlsx
+++ b/Atendimento.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\PUBLICO\Compras\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6776E3D-3F94-4A34-B84A-4261D8499DEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A4553A7-8913-4AF3-B286-526CE3ADE6EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -47,7 +47,7 @@
     <author>Filho, Glaudoberto</author>
   </authors>
   <commentList>
-    <comment ref="T181" authorId="0" shapeId="0" xr:uid="{6F0B1F1F-8317-47FC-8965-8B65A4B64726}">
+    <comment ref="T218" authorId="0" shapeId="0" xr:uid="{6F0B1F1F-8317-47FC-8965-8B65A4B64726}">
       <text>
         <r>
           <rPr>
@@ -76,7 +76,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2367" uniqueCount="400">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2393" uniqueCount="402">
   <si>
     <t>SC</t>
   </si>
@@ -1276,6 +1276,12 @@
   </si>
   <si>
     <t>DALLANESE COM.E MANUF.DE PARAFUSOS LTDA</t>
+  </si>
+  <si>
+    <t>YESCODE AUTOMACAO LTDA - ME</t>
+  </si>
+  <si>
+    <t>CADSERVICE PRODUTOS ELETRONICOS LTDA</t>
   </si>
 </sst>
 </file>
@@ -1418,7 +1424,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1549,9 +1555,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1735,8 +1738,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0C573FEE-B8A0-4FE7-911C-81B026DE4530}" name="Tabela1" displayName="Tabela1" ref="A1:T235" totalsRowShown="0" headerRowDxfId="36" dataDxfId="35">
-  <autoFilter ref="A1:T235" xr:uid="{0C573FEE-B8A0-4FE7-911C-81B026DE4530}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0C573FEE-B8A0-4FE7-911C-81B026DE4530}" name="Tabela1" displayName="Tabela1" ref="A1:T238" totalsRowShown="0" headerRowDxfId="36" dataDxfId="35">
+  <autoFilter ref="A1:T238" xr:uid="{0C573FEE-B8A0-4FE7-911C-81B026DE4530}">
     <filterColumn colId="16">
       <filters>
         <filter val="AGUARDANDO APROVAÇÃO"/>
@@ -1744,8 +1747,8 @@
       </filters>
     </filterColumn>
   </autoFilter>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A11:T231">
-    <sortCondition ref="M1:M231"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A11:T238">
+    <sortCondition ref="A1:A238"/>
   </sortState>
   <tableColumns count="20">
     <tableColumn id="1" xr3:uid="{FD977268-8F92-4E92-82D7-959136F54294}" name="Atendimento" dataDxfId="34"/>
@@ -2110,10 +2113,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T235"/>
+  <dimension ref="A1:T238"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E181" sqref="E181"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L181" sqref="L181"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2781,63 +2784,63 @@
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A11" s="11">
-        <v>45848</v>
+        <v>45785</v>
       </c>
       <c r="B11" s="11">
-        <v>45848</v>
+        <v>45784</v>
       </c>
       <c r="C11" s="11" t="s">
         <v>7</v>
       </c>
       <c r="D11" s="11" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="E11" s="11" t="s">
         <v>113</v>
       </c>
       <c r="F11" s="12">
-        <v>68459</v>
+        <v>68369</v>
       </c>
       <c r="G11" s="12" t="s">
-        <v>364</v>
+        <v>39</v>
       </c>
       <c r="H11" s="12" t="s">
-        <v>365</v>
+        <v>98</v>
       </c>
       <c r="I11" s="13">
-        <f t="shared" ref="I11:I74" si="1">NETWORKDAYS(B11, A11)</f>
-        <v>1</v>
+        <f>NETWORKDAYS(B11, A11)</f>
+        <v>2</v>
       </c>
       <c r="J11" s="12">
-        <v>66162</v>
+        <v>65234</v>
       </c>
       <c r="K11" s="12">
-        <v>11781</v>
+        <v>11610</v>
       </c>
       <c r="L11" s="12" t="s">
-        <v>366</v>
+        <v>38</v>
       </c>
       <c r="M11" s="11">
-        <v>45855</v>
+        <v>45881</v>
       </c>
       <c r="N11" s="14">
-        <v>5396.77</v>
+        <v>9114.5499999999993</v>
       </c>
       <c r="O11" s="12" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="P11" s="12">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="Q11" s="12" t="s">
         <v>24</v>
       </c>
       <c r="R11" s="12">
         <f>DATEDIF(Tabela1[[#This Row],[Atendimento]],Tabela1[[#This Row],[Previsao de Entrega]],"D")</f>
-        <v>7</v>
+        <v>96</v>
       </c>
       <c r="S11" s="14">
-        <v>284.04000000000002</v>
+        <v>183.5</v>
       </c>
       <c r="T11" s="14">
         <v>0</v>
@@ -2869,7 +2872,7 @@
         <v>32</v>
       </c>
       <c r="I12" s="10">
-        <f t="shared" si="1"/>
+        <f>NETWORKDAYS(B12, A12)</f>
         <v>1</v>
       </c>
       <c r="J12" s="7">
@@ -2933,7 +2936,7 @@
         <v>138</v>
       </c>
       <c r="I13" s="10">
-        <f t="shared" si="1"/>
+        <f>NETWORKDAYS(B13, A13)</f>
         <v>1</v>
       </c>
       <c r="J13" s="7">
@@ -2997,7 +3000,7 @@
         <v>32</v>
       </c>
       <c r="I14" s="10">
-        <f t="shared" si="1"/>
+        <f>NETWORKDAYS(B14, A14)</f>
         <v>1</v>
       </c>
       <c r="J14" s="7">
@@ -3061,7 +3064,7 @@
         <v>91</v>
       </c>
       <c r="I15" s="10">
-        <f t="shared" si="1"/>
+        <f>NETWORKDAYS(B15, A15)</f>
         <v>2</v>
       </c>
       <c r="J15" s="7">
@@ -3125,7 +3128,7 @@
         <v>91</v>
       </c>
       <c r="I16" s="10">
-        <f t="shared" si="1"/>
+        <f>NETWORKDAYS(B16, A16)</f>
         <v>10</v>
       </c>
       <c r="J16" s="7">
@@ -3189,7 +3192,7 @@
         <v>34</v>
       </c>
       <c r="I17" s="10">
-        <f t="shared" si="1"/>
+        <f>NETWORKDAYS(B17, A17)</f>
         <v>2</v>
       </c>
       <c r="J17" s="7">
@@ -3253,7 +3256,7 @@
         <v>34</v>
       </c>
       <c r="I18" s="10">
-        <f t="shared" si="1"/>
+        <f>NETWORKDAYS(B18, A18)</f>
         <v>9</v>
       </c>
       <c r="J18" s="7">
@@ -3317,7 +3320,7 @@
         <v>91</v>
       </c>
       <c r="I19" s="10">
-        <f t="shared" si="1"/>
+        <f>NETWORKDAYS(B19, A19)</f>
         <v>1</v>
       </c>
       <c r="J19" s="7">
@@ -3381,7 +3384,7 @@
         <v>32</v>
       </c>
       <c r="I20" s="10">
-        <f t="shared" si="1"/>
+        <f>NETWORKDAYS(B20, A20)</f>
         <v>1</v>
       </c>
       <c r="J20" s="7">
@@ -3445,7 +3448,7 @@
         <v>98</v>
       </c>
       <c r="I21" s="10">
-        <f t="shared" si="1"/>
+        <f>NETWORKDAYS(B21, A21)</f>
         <v>20</v>
       </c>
       <c r="J21" s="7">
@@ -3509,7 +3512,7 @@
         <v>98</v>
       </c>
       <c r="I22" s="10">
-        <f t="shared" si="1"/>
+        <f>NETWORKDAYS(B22, A22)</f>
         <v>3</v>
       </c>
       <c r="J22" s="7">
@@ -3573,7 +3576,7 @@
         <v>96</v>
       </c>
       <c r="I23" s="34">
-        <f t="shared" si="1"/>
+        <f>NETWORKDAYS(B23, A23)</f>
         <v>2</v>
       </c>
       <c r="J23" s="29">
@@ -3637,7 +3640,7 @@
         <v>34</v>
       </c>
       <c r="I24" s="10">
-        <f t="shared" si="1"/>
+        <f>NETWORKDAYS(B24, A24)</f>
         <v>2</v>
       </c>
       <c r="J24" s="7">
@@ -3701,7 +3704,7 @@
         <v>126</v>
       </c>
       <c r="I25" s="10">
-        <f t="shared" si="1"/>
+        <f>NETWORKDAYS(B25, A25)</f>
         <v>1</v>
       </c>
       <c r="J25" s="7">
@@ -3765,7 +3768,7 @@
         <v>130</v>
       </c>
       <c r="I26" s="10">
-        <f t="shared" si="1"/>
+        <f>NETWORKDAYS(B26, A26)</f>
         <v>1</v>
       </c>
       <c r="J26" s="7">
@@ -3829,7 +3832,7 @@
         <v>32</v>
       </c>
       <c r="I27" s="10">
-        <f t="shared" si="1"/>
+        <f>NETWORKDAYS(B27, A27)</f>
         <v>1</v>
       </c>
       <c r="J27" s="7">
@@ -3893,7 +3896,7 @@
         <v>32</v>
       </c>
       <c r="I28" s="10">
-        <f t="shared" si="1"/>
+        <f>NETWORKDAYS(B28, A28)</f>
         <v>1</v>
       </c>
       <c r="J28" s="7">
@@ -3957,7 +3960,7 @@
         <v>32</v>
       </c>
       <c r="I29" s="10">
-        <f t="shared" si="1"/>
+        <f>NETWORKDAYS(B29, A29)</f>
         <v>1</v>
       </c>
       <c r="J29" s="7">
@@ -4021,7 +4024,7 @@
         <v>138</v>
       </c>
       <c r="I30" s="10">
-        <f t="shared" si="1"/>
+        <f>NETWORKDAYS(B30, A30)</f>
         <v>1</v>
       </c>
       <c r="J30" s="7">
@@ -4085,7 +4088,7 @@
         <v>32</v>
       </c>
       <c r="I31" s="10">
-        <f t="shared" si="1"/>
+        <f>NETWORKDAYS(B31, A31)</f>
         <v>1</v>
       </c>
       <c r="J31" s="7">
@@ -4149,7 +4152,7 @@
         <v>130</v>
       </c>
       <c r="I32" s="10">
-        <f t="shared" si="1"/>
+        <f>NETWORKDAYS(B32, A32)</f>
         <v>3</v>
       </c>
       <c r="J32" s="7">
@@ -4213,7 +4216,7 @@
         <v>130</v>
       </c>
       <c r="I33" s="10">
-        <f t="shared" si="1"/>
+        <f>NETWORKDAYS(B33, A33)</f>
         <v>36</v>
       </c>
       <c r="J33" s="7">
@@ -4277,7 +4280,7 @@
         <v>34</v>
       </c>
       <c r="I34" s="10">
-        <f t="shared" si="1"/>
+        <f>NETWORKDAYS(B34, A34)</f>
         <v>1</v>
       </c>
       <c r="J34" s="7">
@@ -4341,7 +4344,7 @@
         <v>130</v>
       </c>
       <c r="I35" s="10">
-        <f t="shared" si="1"/>
+        <f>NETWORKDAYS(B35, A35)</f>
         <v>37</v>
       </c>
       <c r="J35" s="7">
@@ -4405,7 +4408,7 @@
         <v>98</v>
       </c>
       <c r="I36" s="10">
-        <f t="shared" si="1"/>
+        <f>NETWORKDAYS(B36, A36)</f>
         <v>4</v>
       </c>
       <c r="J36" s="7">
@@ -4469,7 +4472,7 @@
         <v>91</v>
       </c>
       <c r="I37" s="10">
-        <f t="shared" si="1"/>
+        <f>NETWORKDAYS(B37, A37)</f>
         <v>3</v>
       </c>
       <c r="J37" s="7">
@@ -4533,7 +4536,7 @@
         <v>91</v>
       </c>
       <c r="I38" s="10">
-        <f t="shared" si="1"/>
+        <f>NETWORKDAYS(B38, A38)</f>
         <v>3</v>
       </c>
       <c r="J38" s="7">
@@ -4597,7 +4600,7 @@
         <v>130</v>
       </c>
       <c r="I39" s="10">
-        <f t="shared" si="1"/>
+        <f>NETWORKDAYS(B39, A39)</f>
         <v>1</v>
       </c>
       <c r="J39" s="7">
@@ -4661,7 +4664,7 @@
         <v>32</v>
       </c>
       <c r="I40" s="10">
-        <f t="shared" si="1"/>
+        <f>NETWORKDAYS(B40, A40)</f>
         <v>1</v>
       </c>
       <c r="J40" s="7">
@@ -4725,7 +4728,7 @@
         <v>98</v>
       </c>
       <c r="I41" s="10">
-        <f t="shared" si="1"/>
+        <f>NETWORKDAYS(B41, A41)</f>
         <v>1</v>
       </c>
       <c r="J41" s="7">
@@ -4789,7 +4792,7 @@
         <v>34</v>
       </c>
       <c r="I42" s="10">
-        <f t="shared" si="1"/>
+        <f>NETWORKDAYS(B42, A42)</f>
         <v>9</v>
       </c>
       <c r="J42" s="7">
@@ -4853,7 +4856,7 @@
         <v>130</v>
       </c>
       <c r="I43" s="10">
-        <f t="shared" si="1"/>
+        <f>NETWORKDAYS(B43, A43)</f>
         <v>1</v>
       </c>
       <c r="J43" s="7">
@@ -4917,7 +4920,7 @@
         <v>34</v>
       </c>
       <c r="I44" s="10">
-        <f t="shared" si="1"/>
+        <f>NETWORKDAYS(B44, A44)</f>
         <v>9</v>
       </c>
       <c r="J44" s="7">
@@ -4981,7 +4984,7 @@
         <v>34</v>
       </c>
       <c r="I45" s="10">
-        <f t="shared" si="1"/>
+        <f>NETWORKDAYS(B45, A45)</f>
         <v>9</v>
       </c>
       <c r="J45" s="7">
@@ -5045,7 +5048,7 @@
         <v>32</v>
       </c>
       <c r="I46" s="10">
-        <f t="shared" si="1"/>
+        <f>NETWORKDAYS(B46, A46)</f>
         <v>1</v>
       </c>
       <c r="J46" s="7">
@@ -5109,7 +5112,7 @@
         <v>32</v>
       </c>
       <c r="I47" s="10">
-        <f t="shared" si="1"/>
+        <f>NETWORKDAYS(B47, A47)</f>
         <v>2</v>
       </c>
       <c r="J47" s="7">
@@ -5173,7 +5176,7 @@
         <v>130</v>
       </c>
       <c r="I48" s="10">
-        <f t="shared" si="1"/>
+        <f>NETWORKDAYS(B48, A48)</f>
         <v>1</v>
       </c>
       <c r="J48" s="7">
@@ -5237,7 +5240,7 @@
         <v>130</v>
       </c>
       <c r="I49" s="10">
-        <f t="shared" si="1"/>
+        <f>NETWORKDAYS(B49, A49)</f>
         <v>1</v>
       </c>
       <c r="J49" s="7">
@@ -5301,7 +5304,7 @@
         <v>130</v>
       </c>
       <c r="I50" s="10">
-        <f t="shared" si="1"/>
+        <f>NETWORKDAYS(B50, A50)</f>
         <v>1</v>
       </c>
       <c r="J50" s="7">
@@ -5365,7 +5368,7 @@
         <v>130</v>
       </c>
       <c r="I51" s="10">
-        <f t="shared" si="1"/>
+        <f>NETWORKDAYS(B51, A51)</f>
         <v>1</v>
       </c>
       <c r="J51" s="7">
@@ -5429,7 +5432,7 @@
         <v>98</v>
       </c>
       <c r="I52" s="10">
-        <f t="shared" si="1"/>
+        <f>NETWORKDAYS(B52, A52)</f>
         <v>1</v>
       </c>
       <c r="J52" s="7">
@@ -5493,7 +5496,7 @@
         <v>98</v>
       </c>
       <c r="I53" s="10">
-        <f t="shared" si="1"/>
+        <f>NETWORKDAYS(B53, A53)</f>
         <v>9</v>
       </c>
       <c r="J53" s="7">
@@ -5557,7 +5560,7 @@
         <v>34</v>
       </c>
       <c r="I54" s="10">
-        <f t="shared" si="1"/>
+        <f>NETWORKDAYS(B54, A54)</f>
         <v>1</v>
       </c>
       <c r="J54" s="7">
@@ -5596,66 +5599,66 @@
       </c>
     </row>
     <row r="55" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A55" s="11">
-        <v>45831</v>
-      </c>
-      <c r="B55" s="11">
-        <v>45824</v>
-      </c>
-      <c r="C55" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="D55" s="11" t="s">
+      <c r="A55" s="31">
+        <v>45798</v>
+      </c>
+      <c r="B55" s="31">
+        <v>45786</v>
+      </c>
+      <c r="C55" s="31" t="s">
+        <v>7</v>
+      </c>
+      <c r="D55" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="E55" s="11" t="s">
+      <c r="E55" s="31" t="s">
         <v>124</v>
       </c>
-      <c r="F55" s="12">
-        <v>68439</v>
-      </c>
-      <c r="G55" s="12" t="s">
+      <c r="F55" s="32">
+        <v>68378</v>
+      </c>
+      <c r="G55" s="32" t="s">
         <v>125</v>
       </c>
-      <c r="H55" s="12" t="s">
+      <c r="H55" s="32" t="s">
         <v>126</v>
       </c>
-      <c r="I55" s="13">
-        <f t="shared" si="1"/>
-        <v>6</v>
-      </c>
-      <c r="J55" s="12">
-        <v>65915</v>
-      </c>
-      <c r="K55" s="12">
+      <c r="I55" s="27">
+        <f>NETWORKDAYS(B55, A55)</f>
+        <v>9</v>
+      </c>
+      <c r="J55" s="32">
+        <v>65472</v>
+      </c>
+      <c r="K55" s="32">
         <v>2201</v>
       </c>
-      <c r="L55" s="12" t="s">
+      <c r="L55" s="32" t="s">
         <v>203</v>
       </c>
-      <c r="M55" s="11">
-        <v>45861</v>
-      </c>
-      <c r="N55" s="14">
-        <v>1401.04</v>
-      </c>
-      <c r="O55" s="12" t="s">
+      <c r="M55" s="31">
+        <v>45869</v>
+      </c>
+      <c r="N55" s="33">
+        <v>26920</v>
+      </c>
+      <c r="O55" s="32" t="s">
         <v>122</v>
       </c>
-      <c r="P55" s="12">
-        <v>120</v>
-      </c>
-      <c r="Q55" s="12" t="s">
+      <c r="P55" s="32">
+        <v>28</v>
+      </c>
+      <c r="Q55" s="32" t="s">
         <v>24</v>
       </c>
-      <c r="R55" s="12">
-        <f>DATEDIF(Tabela1[[#This Row],[Atendimento]],Tabela1[[#This Row],[Previsao de Entrega]],"D")</f>
-        <v>30</v>
-      </c>
-      <c r="S55" s="14">
-        <v>0</v>
-      </c>
-      <c r="T55" s="14">
+      <c r="R55" s="32">
+        <f>DATEDIF(Tabela1[[#This Row],[Atendimento]],Tabela1[[#This Row],[Previsao de Entrega]],"D")</f>
+        <v>71</v>
+      </c>
+      <c r="S55" s="33">
+        <v>0</v>
+      </c>
+      <c r="T55" s="33">
         <v>0</v>
       </c>
     </row>
@@ -5685,7 +5688,7 @@
         <v>130</v>
       </c>
       <c r="I56" s="10">
-        <f t="shared" si="1"/>
+        <f>NETWORKDAYS(B56, A56)</f>
         <v>1</v>
       </c>
       <c r="J56" s="7">
@@ -5749,7 +5752,7 @@
         <v>96</v>
       </c>
       <c r="I57" s="10">
-        <f t="shared" si="1"/>
+        <f>NETWORKDAYS(B57, A57)</f>
         <v>2</v>
       </c>
       <c r="J57" s="7">
@@ -5813,7 +5816,7 @@
         <v>32</v>
       </c>
       <c r="I58" s="10">
-        <f t="shared" si="1"/>
+        <f>NETWORKDAYS(B58, A58)</f>
         <v>1</v>
       </c>
       <c r="J58" s="7">
@@ -5877,7 +5880,7 @@
         <v>32</v>
       </c>
       <c r="I59" s="10">
-        <f t="shared" si="1"/>
+        <f>NETWORKDAYS(B59, A59)</f>
         <v>1</v>
       </c>
       <c r="J59" s="7">
@@ -5941,7 +5944,7 @@
         <v>32</v>
       </c>
       <c r="I60" s="10">
-        <f t="shared" si="1"/>
+        <f>NETWORKDAYS(B60, A60)</f>
         <v>1</v>
       </c>
       <c r="J60" s="7">
@@ -6005,7 +6008,7 @@
         <v>34</v>
       </c>
       <c r="I61" s="10">
-        <f t="shared" si="1"/>
+        <f>NETWORKDAYS(B61, A61)</f>
         <v>10</v>
       </c>
       <c r="J61" s="7">
@@ -6069,7 +6072,7 @@
         <v>130</v>
       </c>
       <c r="I62" s="10">
-        <f t="shared" si="1"/>
+        <f>NETWORKDAYS(B62, A62)</f>
         <v>1</v>
       </c>
       <c r="J62" s="7">
@@ -6133,7 +6136,7 @@
         <v>34</v>
       </c>
       <c r="I63" s="10">
-        <f t="shared" si="1"/>
+        <f>NETWORKDAYS(B63, A63)</f>
         <v>18</v>
       </c>
       <c r="J63" s="7">
@@ -6197,7 +6200,7 @@
         <v>91</v>
       </c>
       <c r="I64" s="10">
-        <f t="shared" si="1"/>
+        <f>NETWORKDAYS(B64, A64)</f>
         <v>4</v>
       </c>
       <c r="J64" s="7">
@@ -6261,7 +6264,7 @@
         <v>98</v>
       </c>
       <c r="I65" s="10">
-        <f t="shared" si="1"/>
+        <f>NETWORKDAYS(B65, A65)</f>
         <v>1</v>
       </c>
       <c r="J65" s="7">
@@ -6325,7 +6328,7 @@
         <v>98</v>
       </c>
       <c r="I66" s="10">
-        <f t="shared" si="1"/>
+        <f>NETWORKDAYS(B66, A66)</f>
         <v>2</v>
       </c>
       <c r="J66" s="7">
@@ -6389,7 +6392,7 @@
         <v>91</v>
       </c>
       <c r="I67" s="10">
-        <f t="shared" si="1"/>
+        <f>NETWORKDAYS(B67, A67)</f>
         <v>3</v>
       </c>
       <c r="J67" s="7">
@@ -6453,7 +6456,7 @@
         <v>32</v>
       </c>
       <c r="I68" s="10">
-        <f t="shared" si="1"/>
+        <f>NETWORKDAYS(B68, A68)</f>
         <v>1</v>
       </c>
       <c r="J68" s="7">
@@ -6517,7 +6520,7 @@
         <v>34</v>
       </c>
       <c r="I69" s="10">
-        <f t="shared" si="1"/>
+        <f>NETWORKDAYS(B69, A69)</f>
         <v>1</v>
       </c>
       <c r="J69" s="7">
@@ -6581,7 +6584,7 @@
         <v>98</v>
       </c>
       <c r="I70" s="10">
-        <f t="shared" si="1"/>
+        <f>NETWORKDAYS(B70, A70)</f>
         <v>4</v>
       </c>
       <c r="J70" s="7">
@@ -6645,7 +6648,7 @@
         <v>98</v>
       </c>
       <c r="I71" s="10">
-        <f t="shared" si="1"/>
+        <f>NETWORKDAYS(B71, A71)</f>
         <v>3</v>
       </c>
       <c r="J71" s="7">
@@ -6709,7 +6712,7 @@
         <v>98</v>
       </c>
       <c r="I72" s="10">
-        <f t="shared" si="1"/>
+        <f>NETWORKDAYS(B72, A72)</f>
         <v>2</v>
       </c>
       <c r="J72" s="7">
@@ -6773,7 +6776,7 @@
         <v>98</v>
       </c>
       <c r="I73" s="10">
-        <f t="shared" si="1"/>
+        <f>NETWORKDAYS(B73, A73)</f>
         <v>8</v>
       </c>
       <c r="J73" s="7">
@@ -6837,7 +6840,7 @@
         <v>98</v>
       </c>
       <c r="I74" s="10">
-        <f t="shared" si="1"/>
+        <f>NETWORKDAYS(B74, A74)</f>
         <v>26</v>
       </c>
       <c r="J74" s="7">
@@ -6901,7 +6904,7 @@
         <v>98</v>
       </c>
       <c r="I75" s="10">
-        <f t="shared" ref="I75:I137" si="2">NETWORKDAYS(B75, A75)</f>
+        <f>NETWORKDAYS(B75, A75)</f>
         <v>6</v>
       </c>
       <c r="J75" s="7">
@@ -6965,7 +6968,7 @@
         <v>91</v>
       </c>
       <c r="I76" s="10">
-        <f t="shared" si="2"/>
+        <f>NETWORKDAYS(B76, A76)</f>
         <v>3</v>
       </c>
       <c r="J76" s="7">
@@ -7029,7 +7032,7 @@
         <v>98</v>
       </c>
       <c r="I77" s="10">
-        <f t="shared" si="2"/>
+        <f>NETWORKDAYS(B77, A77)</f>
         <v>2</v>
       </c>
       <c r="J77" s="7">
@@ -7093,7 +7096,7 @@
         <v>32</v>
       </c>
       <c r="I78" s="10">
-        <f t="shared" si="2"/>
+        <f>NETWORKDAYS(B78, A78)</f>
         <v>1</v>
       </c>
       <c r="J78" s="7">
@@ -7157,7 +7160,7 @@
         <v>32</v>
       </c>
       <c r="I79" s="10">
-        <f t="shared" si="2"/>
+        <f>NETWORKDAYS(B79, A79)</f>
         <v>1</v>
       </c>
       <c r="J79" s="7">
@@ -7221,7 +7224,7 @@
         <v>138</v>
       </c>
       <c r="I80" s="10">
-        <f t="shared" si="2"/>
+        <f>NETWORKDAYS(B80, A80)</f>
         <v>1</v>
       </c>
       <c r="J80" s="7">
@@ -7285,7 +7288,7 @@
         <v>130</v>
       </c>
       <c r="I81" s="10">
-        <f t="shared" si="2"/>
+        <f>NETWORKDAYS(B81, A81)</f>
         <v>1</v>
       </c>
       <c r="J81" s="7">
@@ -7349,7 +7352,7 @@
         <v>98</v>
       </c>
       <c r="I82" s="10">
-        <f t="shared" si="2"/>
+        <f>NETWORKDAYS(B82, A82)</f>
         <v>1</v>
       </c>
       <c r="J82" s="7">
@@ -7413,7 +7416,7 @@
         <v>130</v>
       </c>
       <c r="I83" s="10">
-        <f t="shared" si="2"/>
+        <f>NETWORKDAYS(B83, A83)</f>
         <v>1</v>
       </c>
       <c r="J83" s="7">
@@ -7477,7 +7480,7 @@
         <v>98</v>
       </c>
       <c r="I84" s="10">
-        <f t="shared" si="2"/>
+        <f>NETWORKDAYS(B84, A84)</f>
         <v>2</v>
       </c>
       <c r="J84" s="7">
@@ -7541,7 +7544,7 @@
         <v>98</v>
       </c>
       <c r="I85" s="10">
-        <f t="shared" si="2"/>
+        <f>NETWORKDAYS(B85, A85)</f>
         <v>2</v>
       </c>
       <c r="J85" s="7">
@@ -7605,7 +7608,7 @@
         <v>34</v>
       </c>
       <c r="I86" s="34">
-        <f t="shared" si="2"/>
+        <f>NETWORKDAYS(B86, A86)</f>
         <v>2</v>
       </c>
       <c r="J86" s="29">
@@ -7669,7 +7672,7 @@
         <v>34</v>
       </c>
       <c r="I87" s="10">
-        <f t="shared" si="2"/>
+        <f>NETWORKDAYS(B87, A87)</f>
         <v>1</v>
       </c>
       <c r="J87" s="7">
@@ -7733,7 +7736,7 @@
         <v>32</v>
       </c>
       <c r="I88" s="10">
-        <f t="shared" si="2"/>
+        <f>NETWORKDAYS(B88, A88)</f>
         <v>1</v>
       </c>
       <c r="J88" s="7">
@@ -7797,7 +7800,7 @@
         <v>126</v>
       </c>
       <c r="I89" s="10">
-        <f t="shared" si="2"/>
+        <f>NETWORKDAYS(B89, A89)</f>
         <v>1</v>
       </c>
       <c r="J89" s="7">
@@ -7861,7 +7864,7 @@
         <v>98</v>
       </c>
       <c r="I90" s="10">
-        <f t="shared" si="2"/>
+        <f>NETWORKDAYS(B90, A90)</f>
         <v>1</v>
       </c>
       <c r="J90" s="7">
@@ -7925,7 +7928,7 @@
         <v>32</v>
       </c>
       <c r="I91" s="10">
-        <f t="shared" si="2"/>
+        <f>NETWORKDAYS(B91, A91)</f>
         <v>1</v>
       </c>
       <c r="J91" s="7">
@@ -7989,7 +7992,7 @@
         <v>98</v>
       </c>
       <c r="I92" s="10">
-        <f t="shared" si="2"/>
+        <f>NETWORKDAYS(B92, A92)</f>
         <v>4</v>
       </c>
       <c r="J92" s="7">
@@ -8053,7 +8056,7 @@
         <v>126</v>
       </c>
       <c r="I93" s="10">
-        <f t="shared" si="2"/>
+        <f>NETWORKDAYS(B93, A93)</f>
         <v>3</v>
       </c>
       <c r="J93" s="7">
@@ -8117,7 +8120,7 @@
         <v>126</v>
       </c>
       <c r="I94" s="10">
-        <f t="shared" si="2"/>
+        <f>NETWORKDAYS(B94, A94)</f>
         <v>1</v>
       </c>
       <c r="J94" s="7">
@@ -8181,7 +8184,7 @@
         <v>34</v>
       </c>
       <c r="I95" s="10">
-        <f t="shared" si="2"/>
+        <f>NETWORKDAYS(B95, A95)</f>
         <v>2</v>
       </c>
       <c r="J95" s="7">
@@ -8245,7 +8248,7 @@
         <v>130</v>
       </c>
       <c r="I96" s="10">
-        <f t="shared" si="2"/>
+        <f>NETWORKDAYS(B96, A96)</f>
         <v>1</v>
       </c>
       <c r="J96" s="7">
@@ -8309,7 +8312,7 @@
         <v>138</v>
       </c>
       <c r="I97" s="10">
-        <f t="shared" si="2"/>
+        <f>NETWORKDAYS(B97, A97)</f>
         <v>1</v>
       </c>
       <c r="J97" s="7">
@@ -8373,7 +8376,7 @@
         <v>98</v>
       </c>
       <c r="I98" s="10">
-        <f t="shared" si="2"/>
+        <f>NETWORKDAYS(B98, A98)</f>
         <v>1</v>
       </c>
       <c r="J98" s="7">
@@ -8437,7 +8440,7 @@
         <v>130</v>
       </c>
       <c r="I99" s="10">
-        <f t="shared" si="2"/>
+        <f>NETWORKDAYS(B99, A99)</f>
         <v>1</v>
       </c>
       <c r="J99" s="7">
@@ -8501,7 +8504,7 @@
         <v>130</v>
       </c>
       <c r="I100" s="10">
-        <f t="shared" si="2"/>
+        <f>NETWORKDAYS(B100, A100)</f>
         <v>24</v>
       </c>
       <c r="J100" s="7">
@@ -8565,7 +8568,7 @@
         <v>126</v>
       </c>
       <c r="I101" s="10">
-        <f t="shared" si="2"/>
+        <f>NETWORKDAYS(B101, A101)</f>
         <v>25</v>
       </c>
       <c r="J101" s="7">
@@ -8629,7 +8632,7 @@
         <v>98</v>
       </c>
       <c r="I102" s="10">
-        <f t="shared" si="2"/>
+        <f>NETWORKDAYS(B102, A102)</f>
         <v>1</v>
       </c>
       <c r="J102" s="7">
@@ -8693,7 +8696,7 @@
         <v>91</v>
       </c>
       <c r="I103" s="10">
-        <f t="shared" si="2"/>
+        <f>NETWORKDAYS(B103, A103)</f>
         <v>3</v>
       </c>
       <c r="J103" s="7">
@@ -8757,7 +8760,7 @@
         <v>91</v>
       </c>
       <c r="I104" s="10">
-        <f t="shared" si="2"/>
+        <f>NETWORKDAYS(B104, A104)</f>
         <v>3</v>
       </c>
       <c r="J104" s="7">
@@ -8821,7 +8824,7 @@
         <v>32</v>
       </c>
       <c r="I105" s="10">
-        <f t="shared" si="2"/>
+        <f>NETWORKDAYS(B105, A105)</f>
         <v>1</v>
       </c>
       <c r="J105" s="7">
@@ -8885,7 +8888,7 @@
         <v>32</v>
       </c>
       <c r="I106" s="10">
-        <f t="shared" si="2"/>
+        <f>NETWORKDAYS(B106, A106)</f>
         <v>1</v>
       </c>
       <c r="J106" s="7">
@@ -8949,7 +8952,7 @@
         <v>98</v>
       </c>
       <c r="I107" s="10">
-        <f t="shared" si="2"/>
+        <f>NETWORKDAYS(B107, A107)</f>
         <v>1</v>
       </c>
       <c r="J107" s="7">
@@ -9013,7 +9016,7 @@
         <v>91</v>
       </c>
       <c r="I108" s="10">
-        <f t="shared" si="2"/>
+        <f>NETWORKDAYS(B108, A108)</f>
         <v>2</v>
       </c>
       <c r="J108" s="7">
@@ -9052,130 +9055,130 @@
       </c>
     </row>
     <row r="109" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A109" s="11">
-        <v>45866</v>
-      </c>
-      <c r="B109" s="11">
-        <v>45863</v>
-      </c>
-      <c r="C109" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="D109" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="E109" s="11" t="s">
+      <c r="A109" s="40">
+        <v>45818</v>
+      </c>
+      <c r="B109" s="40">
+        <v>45811</v>
+      </c>
+      <c r="C109" s="40" t="s">
+        <v>7</v>
+      </c>
+      <c r="D109" s="40" t="s">
+        <v>15</v>
+      </c>
+      <c r="E109" s="40" t="s">
         <v>113</v>
       </c>
-      <c r="F109" s="12">
-        <v>68481</v>
-      </c>
-      <c r="G109" s="12" t="s">
-        <v>372</v>
-      </c>
-      <c r="H109" s="12" t="s">
-        <v>373</v>
-      </c>
-      <c r="I109" s="13">
-        <f t="shared" si="2"/>
-        <v>2</v>
-      </c>
-      <c r="J109" s="12">
-        <v>66462</v>
-      </c>
-      <c r="K109" s="12">
-        <v>10535</v>
-      </c>
-      <c r="L109" s="12" t="s">
-        <v>391</v>
-      </c>
-      <c r="M109" s="11">
-        <v>45868</v>
-      </c>
-      <c r="N109" s="14">
-        <v>300</v>
-      </c>
-      <c r="O109" s="12" t="s">
+      <c r="F109" s="41">
+        <v>68329</v>
+      </c>
+      <c r="G109" s="41" t="s">
+        <v>95</v>
+      </c>
+      <c r="H109" s="41" t="s">
+        <v>96</v>
+      </c>
+      <c r="I109" s="42">
+        <f>NETWORKDAYS(B109, A109)</f>
+        <v>6</v>
+      </c>
+      <c r="J109" s="41">
+        <v>66494</v>
+      </c>
+      <c r="K109" s="41">
+        <v>224</v>
+      </c>
+      <c r="L109" s="41" t="s">
+        <v>295</v>
+      </c>
+      <c r="M109" s="40">
+        <v>45869</v>
+      </c>
+      <c r="N109" s="43">
+        <v>7774.51</v>
+      </c>
+      <c r="O109" s="41" t="s">
+        <v>121</v>
+      </c>
+      <c r="P109" s="41">
+        <v>0</v>
+      </c>
+      <c r="Q109" s="41" t="s">
+        <v>360</v>
+      </c>
+      <c r="R109" s="41">
+        <f>DATEDIF(Tabela1[[#This Row],[Atendimento]],Tabela1[[#This Row],[Previsao de Entrega]],"D")</f>
+        <v>51</v>
+      </c>
+      <c r="S109" s="43">
+        <v>0</v>
+      </c>
+      <c r="T109" s="43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A110" s="11">
+        <v>45818</v>
+      </c>
+      <c r="B110" s="11">
+        <v>45813</v>
+      </c>
+      <c r="C110" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D110" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="E110" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="F110" s="12">
+        <v>68422</v>
+      </c>
+      <c r="G110" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="H110" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="I110" s="13">
+        <f>NETWORKDAYS(B110, A110)</f>
+        <v>4</v>
+      </c>
+      <c r="J110" s="12">
+        <v>65725</v>
+      </c>
+      <c r="K110" s="12">
+        <v>1450</v>
+      </c>
+      <c r="L110" s="12" t="s">
+        <v>229</v>
+      </c>
+      <c r="M110" s="11">
+        <v>45877</v>
+      </c>
+      <c r="N110" s="14">
+        <v>239.63</v>
+      </c>
+      <c r="O110" s="12" t="s">
         <v>122</v>
       </c>
-      <c r="P109" s="12">
-        <v>14</v>
-      </c>
-      <c r="Q109" s="12" t="s">
+      <c r="P110" s="12">
+        <v>120</v>
+      </c>
+      <c r="Q110" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="R109" s="12">
-        <f>DATEDIF(Tabela1[[#This Row],[Atendimento]],Tabela1[[#This Row],[Previsao de Entrega]],"D")</f>
-        <v>2</v>
-      </c>
-      <c r="S109" s="14">
-        <v>0</v>
-      </c>
-      <c r="T109" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="110" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A110" s="31">
-        <v>45798</v>
-      </c>
-      <c r="B110" s="31">
-        <v>45786</v>
-      </c>
-      <c r="C110" s="31" t="s">
-        <v>7</v>
-      </c>
-      <c r="D110" s="31" t="s">
-        <v>15</v>
-      </c>
-      <c r="E110" s="31" t="s">
-        <v>124</v>
-      </c>
-      <c r="F110" s="32">
-        <v>68378</v>
-      </c>
-      <c r="G110" s="32" t="s">
-        <v>125</v>
-      </c>
-      <c r="H110" s="32" t="s">
-        <v>126</v>
-      </c>
-      <c r="I110" s="27">
-        <f t="shared" si="2"/>
-        <v>9</v>
-      </c>
-      <c r="J110" s="32">
-        <v>65472</v>
-      </c>
-      <c r="K110" s="32">
-        <v>2201</v>
-      </c>
-      <c r="L110" s="32" t="s">
-        <v>203</v>
-      </c>
-      <c r="M110" s="31">
-        <v>45869</v>
-      </c>
-      <c r="N110" s="33">
-        <v>26920</v>
-      </c>
-      <c r="O110" s="32" t="s">
-        <v>122</v>
-      </c>
-      <c r="P110" s="32">
-        <v>28</v>
-      </c>
-      <c r="Q110" s="32" t="s">
-        <v>24</v>
-      </c>
-      <c r="R110" s="32">
-        <f>DATEDIF(Tabela1[[#This Row],[Atendimento]],Tabela1[[#This Row],[Previsao de Entrega]],"D")</f>
-        <v>71</v>
-      </c>
-      <c r="S110" s="33">
-        <v>0</v>
-      </c>
-      <c r="T110" s="33">
+      <c r="R110" s="12">
+        <f>DATEDIF(Tabela1[[#This Row],[Atendimento]],Tabela1[[#This Row],[Previsao de Entrega]],"D")</f>
+        <v>59</v>
+      </c>
+      <c r="S110" s="14">
+        <v>0</v>
+      </c>
+      <c r="T110" s="14">
         <v>0</v>
       </c>
     </row>
@@ -9205,7 +9208,7 @@
         <v>91</v>
       </c>
       <c r="I111" s="10">
-        <f t="shared" si="2"/>
+        <f>NETWORKDAYS(B111, A111)</f>
         <v>4</v>
       </c>
       <c r="J111" s="7">
@@ -9244,66 +9247,66 @@
       </c>
     </row>
     <row r="112" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A112" s="40">
-        <v>45818</v>
-      </c>
-      <c r="B112" s="40">
-        <v>45811</v>
-      </c>
-      <c r="C112" s="40" t="s">
-        <v>7</v>
-      </c>
-      <c r="D112" s="40" t="s">
+      <c r="A112" s="11">
+        <v>45826</v>
+      </c>
+      <c r="B112" s="11">
+        <v>45789</v>
+      </c>
+      <c r="C112" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D112" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="E112" s="40" t="s">
-        <v>113</v>
-      </c>
-      <c r="F112" s="41">
-        <v>68329</v>
-      </c>
-      <c r="G112" s="41" t="s">
-        <v>95</v>
-      </c>
-      <c r="H112" s="41" t="s">
-        <v>96</v>
-      </c>
-      <c r="I112" s="42">
-        <f t="shared" si="2"/>
-        <v>6</v>
-      </c>
-      <c r="J112" s="41">
-        <v>66494</v>
-      </c>
-      <c r="K112" s="41">
-        <v>224</v>
-      </c>
-      <c r="L112" s="41" t="s">
-        <v>295</v>
-      </c>
-      <c r="M112" s="40">
-        <v>45869</v>
-      </c>
-      <c r="N112" s="43">
-        <v>7774.51</v>
-      </c>
-      <c r="O112" s="41" t="s">
-        <v>121</v>
-      </c>
-      <c r="P112" s="41">
-        <v>0</v>
-      </c>
-      <c r="Q112" s="41" t="s">
-        <v>360</v>
-      </c>
-      <c r="R112" s="41">
-        <f>DATEDIF(Tabela1[[#This Row],[Atendimento]],Tabela1[[#This Row],[Previsao de Entrega]],"D")</f>
-        <v>51</v>
-      </c>
-      <c r="S112" s="43">
-        <v>0</v>
-      </c>
-      <c r="T112" s="43">
+      <c r="E112" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="F112" s="12">
+        <v>68384</v>
+      </c>
+      <c r="G112" s="12" t="s">
+        <v>125</v>
+      </c>
+      <c r="H112" s="12" t="s">
+        <v>126</v>
+      </c>
+      <c r="I112" s="13">
+        <f>NETWORKDAYS(B112, A112)</f>
+        <v>28</v>
+      </c>
+      <c r="J112" s="12">
+        <v>65867</v>
+      </c>
+      <c r="K112" s="12">
+        <v>1463</v>
+      </c>
+      <c r="L112" s="12" t="s">
+        <v>317</v>
+      </c>
+      <c r="M112" s="11">
+        <v>45874</v>
+      </c>
+      <c r="N112" s="14">
+        <v>4215.5</v>
+      </c>
+      <c r="O112" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="P112" s="12">
+        <v>28</v>
+      </c>
+      <c r="Q112" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="R112" s="12">
+        <f>DATEDIF(Tabela1[[#This Row],[Atendimento]],Tabela1[[#This Row],[Previsao de Entrega]],"D")</f>
+        <v>48</v>
+      </c>
+      <c r="S112" s="14">
+        <v>0</v>
+      </c>
+      <c r="T112" s="14">
         <v>0</v>
       </c>
     </row>
@@ -9333,7 +9336,7 @@
         <v>32</v>
       </c>
       <c r="I113" s="10">
-        <f t="shared" si="2"/>
+        <f>NETWORKDAYS(B113, A113)</f>
         <v>1</v>
       </c>
       <c r="J113" s="7">
@@ -9397,7 +9400,7 @@
         <v>96</v>
       </c>
       <c r="I114" s="10">
-        <f t="shared" si="2"/>
+        <f>NETWORKDAYS(B114, A114)</f>
         <v>1</v>
       </c>
       <c r="J114" s="7">
@@ -9461,7 +9464,7 @@
         <v>91</v>
       </c>
       <c r="I115" s="10">
-        <f t="shared" si="2"/>
+        <f>NETWORKDAYS(B115, A115)</f>
         <v>2</v>
       </c>
       <c r="J115" s="7">
@@ -9525,7 +9528,7 @@
         <v>32</v>
       </c>
       <c r="I116" s="10">
-        <f t="shared" si="2"/>
+        <f>NETWORKDAYS(B116, A116)</f>
         <v>1</v>
       </c>
       <c r="J116" s="7">
@@ -9589,7 +9592,7 @@
         <v>98</v>
       </c>
       <c r="I117" s="10">
-        <f t="shared" si="2"/>
+        <f>NETWORKDAYS(B117, A117)</f>
         <v>1</v>
       </c>
       <c r="J117" s="7">
@@ -9653,7 +9656,7 @@
         <v>91</v>
       </c>
       <c r="I118" s="10">
-        <f t="shared" si="2"/>
+        <f>NETWORKDAYS(B118, A118)</f>
         <v>5</v>
       </c>
       <c r="J118" s="7">
@@ -9717,7 +9720,7 @@
         <v>91</v>
       </c>
       <c r="I119" s="10">
-        <f t="shared" si="2"/>
+        <f>NETWORKDAYS(B119, A119)</f>
         <v>1</v>
       </c>
       <c r="J119" s="7">
@@ -9781,7 +9784,7 @@
         <v>91</v>
       </c>
       <c r="I120" s="10">
-        <f t="shared" si="2"/>
+        <f>NETWORKDAYS(B120, A120)</f>
         <v>1</v>
       </c>
       <c r="J120" s="7">
@@ -9845,7 +9848,7 @@
         <v>98</v>
       </c>
       <c r="I121" s="10">
-        <f t="shared" si="2"/>
+        <f>NETWORKDAYS(B121, A121)</f>
         <v>1</v>
       </c>
       <c r="J121" s="7">
@@ -9909,7 +9912,7 @@
         <v>126</v>
       </c>
       <c r="I122" s="10">
-        <f t="shared" si="2"/>
+        <f>NETWORKDAYS(B122, A122)</f>
         <v>18</v>
       </c>
       <c r="J122" s="7">
@@ -9973,7 +9976,7 @@
         <v>91</v>
       </c>
       <c r="I123" s="10">
-        <f t="shared" si="2"/>
+        <f>NETWORKDAYS(B123, A123)</f>
         <v>1</v>
       </c>
       <c r="J123" s="7">
@@ -10037,7 +10040,7 @@
         <v>34</v>
       </c>
       <c r="I124" s="10">
-        <f t="shared" si="2"/>
+        <f>NETWORKDAYS(B124, A124)</f>
         <v>1</v>
       </c>
       <c r="J124" s="7">
@@ -10101,7 +10104,7 @@
         <v>130</v>
       </c>
       <c r="I125" s="10">
-        <f t="shared" si="2"/>
+        <f>NETWORKDAYS(B125, A125)</f>
         <v>1</v>
       </c>
       <c r="J125" s="7">
@@ -10165,7 +10168,7 @@
         <v>130</v>
       </c>
       <c r="I126" s="10">
-        <f t="shared" si="2"/>
+        <f>NETWORKDAYS(B126, A126)</f>
         <v>1</v>
       </c>
       <c r="J126" s="7">
@@ -10229,7 +10232,7 @@
         <v>98</v>
       </c>
       <c r="I127" s="10">
-        <f t="shared" si="2"/>
+        <f>NETWORKDAYS(B127, A127)</f>
         <v>1</v>
       </c>
       <c r="J127" s="7">
@@ -10293,7 +10296,7 @@
         <v>130</v>
       </c>
       <c r="I128" s="10">
-        <f t="shared" si="2"/>
+        <f>NETWORKDAYS(B128, A128)</f>
         <v>1</v>
       </c>
       <c r="J128" s="7">
@@ -10357,7 +10360,7 @@
         <v>32</v>
       </c>
       <c r="I129" s="10">
-        <f t="shared" si="2"/>
+        <f>NETWORKDAYS(B129, A129)</f>
         <v>1</v>
       </c>
       <c r="J129" s="7">
@@ -10421,7 +10424,7 @@
         <v>32</v>
       </c>
       <c r="I130" s="10">
-        <f t="shared" si="2"/>
+        <f>NETWORKDAYS(B130, A130)</f>
         <v>1</v>
       </c>
       <c r="J130" s="7">
@@ -10460,75 +10463,75 @@
       </c>
     </row>
     <row r="131" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A131" s="11">
-        <v>45839</v>
-      </c>
-      <c r="B131" s="11">
-        <v>45824</v>
-      </c>
-      <c r="C131" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="D131" s="11" t="s">
+      <c r="A131" s="49">
+        <v>45826</v>
+      </c>
+      <c r="B131" s="49">
+        <v>45826</v>
+      </c>
+      <c r="C131" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="D131" s="49" t="s">
         <v>15</v>
       </c>
-      <c r="E131" s="11" t="s">
+      <c r="E131" s="49" t="s">
         <v>124</v>
       </c>
-      <c r="F131" s="12">
-        <v>68438</v>
-      </c>
-      <c r="G131" s="12" t="s">
+      <c r="F131" s="50" t="s">
+        <v>3</v>
+      </c>
+      <c r="G131" s="50" t="s">
         <v>125</v>
       </c>
-      <c r="H131" s="12" t="s">
+      <c r="H131" s="50" t="s">
         <v>126</v>
       </c>
-      <c r="I131" s="13">
-        <f t="shared" si="2"/>
-        <v>12</v>
-      </c>
-      <c r="J131" s="12">
-        <v>66025</v>
-      </c>
-      <c r="K131" s="12">
-        <v>3034</v>
-      </c>
-      <c r="L131" s="12" t="s">
-        <v>349</v>
-      </c>
-      <c r="M131" s="11">
-        <v>45870</v>
-      </c>
-      <c r="N131" s="14">
-        <v>2087</v>
-      </c>
-      <c r="O131" s="12" t="s">
+      <c r="I131" s="51">
+        <f>NETWORKDAYS(B131, A131)</f>
+        <v>1</v>
+      </c>
+      <c r="J131" s="50">
+        <v>66341</v>
+      </c>
+      <c r="K131" s="50">
+        <v>11758</v>
+      </c>
+      <c r="L131" s="50" t="s">
+        <v>316</v>
+      </c>
+      <c r="M131" s="49">
+        <v>45880</v>
+      </c>
+      <c r="N131" s="52">
+        <v>924.61</v>
+      </c>
+      <c r="O131" s="50" t="s">
         <v>122</v>
       </c>
-      <c r="P131" s="12">
-        <v>90</v>
-      </c>
-      <c r="Q131" s="12" t="s">
+      <c r="P131" s="50">
+        <v>28</v>
+      </c>
+      <c r="Q131" s="50" t="s">
         <v>24</v>
       </c>
-      <c r="R131" s="12">
-        <f>DATEDIF(Tabela1[[#This Row],[Atendimento]],Tabela1[[#This Row],[Previsao de Entrega]],"D")</f>
-        <v>31</v>
-      </c>
-      <c r="S131" s="14">
-        <v>0</v>
-      </c>
-      <c r="T131" s="14">
+      <c r="R131" s="50">
+        <f>DATEDIF(Tabela1[[#This Row],[Atendimento]],Tabela1[[#This Row],[Previsao de Entrega]],"D")</f>
+        <v>54</v>
+      </c>
+      <c r="S131" s="52">
+        <v>0</v>
+      </c>
+      <c r="T131" s="52">
         <v>0</v>
       </c>
     </row>
     <row r="132" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A132" s="11">
-        <v>45826</v>
+        <v>45831</v>
       </c>
       <c r="B132" s="11">
-        <v>45789</v>
+        <v>45824</v>
       </c>
       <c r="C132" s="11" t="s">
         <v>7</v>
@@ -10540,7 +10543,7 @@
         <v>124</v>
       </c>
       <c r="F132" s="12">
-        <v>68384</v>
+        <v>68439</v>
       </c>
       <c r="G132" s="12" t="s">
         <v>125</v>
@@ -10549,36 +10552,36 @@
         <v>126</v>
       </c>
       <c r="I132" s="13">
-        <f t="shared" si="2"/>
-        <v>28</v>
+        <f>NETWORKDAYS(B132, A132)</f>
+        <v>6</v>
       </c>
       <c r="J132" s="12">
-        <v>65867</v>
+        <v>65915</v>
       </c>
       <c r="K132" s="12">
-        <v>1463</v>
+        <v>2201</v>
       </c>
       <c r="L132" s="12" t="s">
-        <v>317</v>
+        <v>203</v>
       </c>
       <c r="M132" s="11">
-        <v>45874</v>
+        <v>45861</v>
       </c>
       <c r="N132" s="14">
-        <v>4215.5</v>
+        <v>1401.04</v>
       </c>
       <c r="O132" s="12" t="s">
         <v>122</v>
       </c>
       <c r="P132" s="12">
-        <v>28</v>
+        <v>120</v>
       </c>
       <c r="Q132" s="12" t="s">
         <v>24</v>
       </c>
       <c r="R132" s="12">
         <f>DATEDIF(Tabela1[[#This Row],[Atendimento]],Tabela1[[#This Row],[Previsao de Entrega]],"D")</f>
-        <v>48</v>
+        <v>30</v>
       </c>
       <c r="S132" s="14">
         <v>0</v>
@@ -10613,7 +10616,7 @@
         <v>98</v>
       </c>
       <c r="I133" s="10">
-        <f t="shared" si="2"/>
+        <f>NETWORKDAYS(B133, A133)</f>
         <v>7</v>
       </c>
       <c r="J133" s="7">
@@ -10677,7 +10680,7 @@
         <v>126</v>
       </c>
       <c r="I134" s="10">
-        <f t="shared" si="2"/>
+        <f>NETWORKDAYS(B134, A134)</f>
         <v>6</v>
       </c>
       <c r="J134" s="7">
@@ -10741,7 +10744,7 @@
         <v>126</v>
       </c>
       <c r="I135" s="10">
-        <f t="shared" si="2"/>
+        <f>NETWORKDAYS(B135, A135)</f>
         <v>7</v>
       </c>
       <c r="J135" s="7">
@@ -10805,7 +10808,7 @@
         <v>32</v>
       </c>
       <c r="I136" s="10">
-        <f t="shared" si="2"/>
+        <f>NETWORKDAYS(B136, A136)</f>
         <v>1</v>
       </c>
       <c r="J136" s="7">
@@ -10845,22 +10848,22 @@
     </row>
     <row r="137" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A137" s="11">
-        <v>45855</v>
+        <v>45839</v>
       </c>
       <c r="B137" s="11">
-        <v>45855</v>
+        <v>45824</v>
       </c>
       <c r="C137" s="11" t="s">
         <v>7</v>
       </c>
       <c r="D137" s="11" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="E137" s="11" t="s">
-        <v>142</v>
-      </c>
-      <c r="F137" s="12" t="s">
-        <v>3</v>
+        <v>124</v>
+      </c>
+      <c r="F137" s="12">
+        <v>68438</v>
       </c>
       <c r="G137" s="12" t="s">
         <v>125</v>
@@ -10869,39 +10872,39 @@
         <v>126</v>
       </c>
       <c r="I137" s="13">
-        <f t="shared" si="2"/>
-        <v>1</v>
+        <f>NETWORKDAYS(B137, A137)</f>
+        <v>12</v>
       </c>
       <c r="J137" s="12">
-        <v>66308</v>
+        <v>66025</v>
       </c>
       <c r="K137" s="12">
-        <v>11757</v>
+        <v>3034</v>
       </c>
       <c r="L137" s="12" t="s">
-        <v>305</v>
+        <v>349</v>
       </c>
       <c r="M137" s="11">
-        <v>45873</v>
+        <v>45870</v>
       </c>
       <c r="N137" s="14">
-        <v>1428.29</v>
+        <v>2087</v>
       </c>
       <c r="O137" s="12" t="s">
         <v>122</v>
       </c>
       <c r="P137" s="12">
-        <v>28</v>
+        <v>90</v>
       </c>
       <c r="Q137" s="12" t="s">
         <v>24</v>
       </c>
       <c r="R137" s="12">
         <f>DATEDIF(Tabela1[[#This Row],[Atendimento]],Tabela1[[#This Row],[Previsao de Entrega]],"D")</f>
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="S137" s="14">
-        <v>320</v>
+        <v>0</v>
       </c>
       <c r="T137" s="14">
         <v>0</v>
@@ -10933,7 +10936,7 @@
         <v>98</v>
       </c>
       <c r="I138" s="10">
-        <f t="shared" ref="I138:I200" si="3">NETWORKDAYS(B138, A138)</f>
+        <f>NETWORKDAYS(B138, A138)</f>
         <v>2</v>
       </c>
       <c r="J138" s="7">
@@ -10997,7 +11000,7 @@
         <v>98</v>
       </c>
       <c r="I139" s="10">
-        <f t="shared" si="3"/>
+        <f>NETWORKDAYS(B139, A139)</f>
         <v>7</v>
       </c>
       <c r="J139" s="7">
@@ -11061,7 +11064,7 @@
         <v>98</v>
       </c>
       <c r="I140" s="10">
-        <f t="shared" si="3"/>
+        <f>NETWORKDAYS(B140, A140)</f>
         <v>18</v>
       </c>
       <c r="J140" s="7">
@@ -11125,7 +11128,7 @@
         <v>91</v>
       </c>
       <c r="I141" s="10">
-        <f t="shared" si="3"/>
+        <f>NETWORKDAYS(B141, A141)</f>
         <v>6</v>
       </c>
       <c r="J141" s="7">
@@ -11189,7 +11192,7 @@
         <v>130</v>
       </c>
       <c r="I142" s="10">
-        <f t="shared" si="3"/>
+        <f>NETWORKDAYS(B142, A142)</f>
         <v>1</v>
       </c>
       <c r="J142" s="7">
@@ -11253,7 +11256,7 @@
         <v>373</v>
       </c>
       <c r="I143" s="10">
-        <f t="shared" si="3"/>
+        <f>NETWORKDAYS(B143, A143)</f>
         <v>1</v>
       </c>
       <c r="J143" s="7">
@@ -11317,7 +11320,7 @@
         <v>98</v>
       </c>
       <c r="I144" s="10">
-        <f t="shared" si="3"/>
+        <f>NETWORKDAYS(B144, A144)</f>
         <v>1</v>
       </c>
       <c r="J144" s="7">
@@ -11381,7 +11384,7 @@
         <v>34</v>
       </c>
       <c r="I145" s="10">
-        <f t="shared" si="3"/>
+        <f>NETWORKDAYS(B145, A145)</f>
         <v>1</v>
       </c>
       <c r="J145" s="7">
@@ -11445,7 +11448,7 @@
         <v>98</v>
       </c>
       <c r="I146" s="10">
-        <f t="shared" si="3"/>
+        <f>NETWORKDAYS(B146, A146)</f>
         <v>1</v>
       </c>
       <c r="J146" s="7">
@@ -11509,7 +11512,7 @@
         <v>138</v>
       </c>
       <c r="I147" s="10">
-        <f t="shared" si="3"/>
+        <f>NETWORKDAYS(B147, A147)</f>
         <v>1</v>
       </c>
       <c r="J147" s="7">
@@ -11573,7 +11576,7 @@
         <v>91</v>
       </c>
       <c r="I148" s="10">
-        <f t="shared" si="3"/>
+        <f>NETWORKDAYS(B148, A148)</f>
         <v>9</v>
       </c>
       <c r="J148" s="7">
@@ -11637,7 +11640,7 @@
         <v>98</v>
       </c>
       <c r="I149" s="10">
-        <f t="shared" si="3"/>
+        <f>NETWORKDAYS(B149, A149)</f>
         <v>1</v>
       </c>
       <c r="J149" s="7">
@@ -11701,7 +11704,7 @@
         <v>130</v>
       </c>
       <c r="I150" s="10">
-        <f t="shared" si="3"/>
+        <f>NETWORKDAYS(B150, A150)</f>
         <v>1</v>
       </c>
       <c r="J150" s="7">
@@ -11765,7 +11768,7 @@
         <v>32</v>
       </c>
       <c r="I151" s="10">
-        <f t="shared" si="3"/>
+        <f>NETWORKDAYS(B151, A151)</f>
         <v>1</v>
       </c>
       <c r="J151" s="7">
@@ -11829,7 +11832,7 @@
         <v>91</v>
       </c>
       <c r="I152" s="10">
-        <f t="shared" si="3"/>
+        <f>NETWORKDAYS(B152, A152)</f>
         <v>1</v>
       </c>
       <c r="J152" s="7">
@@ -11893,7 +11896,7 @@
         <v>32</v>
       </c>
       <c r="I153" s="10">
-        <f t="shared" si="3"/>
+        <f>NETWORKDAYS(B153, A153)</f>
         <v>1</v>
       </c>
       <c r="J153" s="7">
@@ -11957,7 +11960,7 @@
         <v>34</v>
       </c>
       <c r="I154" s="10">
-        <f t="shared" si="3"/>
+        <f>NETWORKDAYS(B154, A154)</f>
         <v>1</v>
       </c>
       <c r="J154" s="7">
@@ -12021,7 +12024,7 @@
         <v>130</v>
       </c>
       <c r="I155" s="10">
-        <f t="shared" si="3"/>
+        <f>NETWORKDAYS(B155, A155)</f>
         <v>1</v>
       </c>
       <c r="J155" s="7">
@@ -12085,7 +12088,7 @@
         <v>98</v>
       </c>
       <c r="I156" s="10">
-        <f t="shared" si="3"/>
+        <f>NETWORKDAYS(B156, A156)</f>
         <v>1</v>
       </c>
       <c r="J156" s="7">
@@ -12149,7 +12152,7 @@
         <v>91</v>
       </c>
       <c r="I157" s="10">
-        <f t="shared" si="3"/>
+        <f>NETWORKDAYS(B157, A157)</f>
         <v>1</v>
       </c>
       <c r="J157" s="7">
@@ -12213,7 +12216,7 @@
         <v>91</v>
       </c>
       <c r="I158" s="10">
-        <f t="shared" si="3"/>
+        <f>NETWORKDAYS(B158, A158)</f>
         <v>1</v>
       </c>
       <c r="J158" s="7">
@@ -12277,7 +12280,7 @@
         <v>32</v>
       </c>
       <c r="I159" s="10">
-        <f t="shared" si="3"/>
+        <f>NETWORKDAYS(B159, A159)</f>
         <v>1</v>
       </c>
       <c r="J159" s="7">
@@ -12341,7 +12344,7 @@
         <v>32</v>
       </c>
       <c r="I160" s="10">
-        <f t="shared" si="3"/>
+        <f>NETWORKDAYS(B160, A160)</f>
         <v>1</v>
       </c>
       <c r="J160" s="7">
@@ -12405,7 +12408,7 @@
         <v>32</v>
       </c>
       <c r="I161" s="10">
-        <f t="shared" si="3"/>
+        <f>NETWORKDAYS(B161, A161)</f>
         <v>1</v>
       </c>
       <c r="J161" s="7">
@@ -12469,7 +12472,7 @@
         <v>32</v>
       </c>
       <c r="I162" s="10">
-        <f t="shared" si="3"/>
+        <f>NETWORKDAYS(B162, A162)</f>
         <v>1</v>
       </c>
       <c r="J162" s="7">
@@ -12533,7 +12536,7 @@
         <v>185</v>
       </c>
       <c r="I163" s="10">
-        <f t="shared" si="3"/>
+        <f>NETWORKDAYS(B163, A163)</f>
         <v>1</v>
       </c>
       <c r="J163" s="7">
@@ -12597,7 +12600,7 @@
         <v>91</v>
       </c>
       <c r="I164" s="10">
-        <f t="shared" si="3"/>
+        <f>NETWORKDAYS(B164, A164)</f>
         <v>17</v>
       </c>
       <c r="J164" s="7">
@@ -12661,7 +12664,7 @@
         <v>98</v>
       </c>
       <c r="I165" s="10">
-        <f t="shared" si="3"/>
+        <f>NETWORKDAYS(B165, A165)</f>
         <v>2</v>
       </c>
       <c r="J165" s="7">
@@ -12725,7 +12728,7 @@
         <v>91</v>
       </c>
       <c r="I166" s="10">
-        <f t="shared" si="3"/>
+        <f>NETWORKDAYS(B166, A166)</f>
         <v>4</v>
       </c>
       <c r="J166" s="7">
@@ -12789,7 +12792,7 @@
         <v>130</v>
       </c>
       <c r="I167" s="10">
-        <f t="shared" si="3"/>
+        <f>NETWORKDAYS(B167, A167)</f>
         <v>5</v>
       </c>
       <c r="J167" s="7">
@@ -12853,7 +12856,7 @@
         <v>32</v>
       </c>
       <c r="I168" s="10">
-        <f t="shared" si="3"/>
+        <f>NETWORKDAYS(B168, A168)</f>
         <v>1</v>
       </c>
       <c r="J168" s="7">
@@ -12917,7 +12920,7 @@
         <v>130</v>
       </c>
       <c r="I169" s="10">
-        <f t="shared" si="3"/>
+        <f>NETWORKDAYS(B169, A169)</f>
         <v>5</v>
       </c>
       <c r="J169" s="7">
@@ -12981,7 +12984,7 @@
         <v>130</v>
       </c>
       <c r="I170" s="10">
-        <f t="shared" si="3"/>
+        <f>NETWORKDAYS(B170, A170)</f>
         <v>1</v>
       </c>
       <c r="J170" s="7">
@@ -13045,7 +13048,7 @@
         <v>34</v>
       </c>
       <c r="I171" s="13">
-        <f t="shared" si="3"/>
+        <f>NETWORKDAYS(B171, A171)</f>
         <v>1</v>
       </c>
       <c r="J171" s="12">
@@ -13109,7 +13112,7 @@
         <v>130</v>
       </c>
       <c r="I172" s="10">
-        <f t="shared" si="3"/>
+        <f>NETWORKDAYS(B172, A172)</f>
         <v>1</v>
       </c>
       <c r="J172" s="7">
@@ -13173,7 +13176,7 @@
         <v>98</v>
       </c>
       <c r="I173" s="13">
-        <f t="shared" si="3"/>
+        <f>NETWORKDAYS(B173, A173)</f>
         <v>1</v>
       </c>
       <c r="J173" s="12">
@@ -13237,7 +13240,7 @@
         <v>32</v>
       </c>
       <c r="I174" s="10">
-        <f t="shared" si="3"/>
+        <f>NETWORKDAYS(B174, A174)</f>
         <v>1</v>
       </c>
       <c r="J174" s="7">
@@ -13301,7 +13304,7 @@
         <v>32</v>
       </c>
       <c r="I175" s="10">
-        <f t="shared" si="3"/>
+        <f>NETWORKDAYS(B175, A175)</f>
         <v>1</v>
       </c>
       <c r="J175" s="7">
@@ -13365,7 +13368,7 @@
         <v>138</v>
       </c>
       <c r="I176" s="10">
-        <f t="shared" si="3"/>
+        <f>NETWORKDAYS(B176, A176)</f>
         <v>1</v>
       </c>
       <c r="J176" s="7">
@@ -13429,7 +13432,7 @@
         <v>32</v>
       </c>
       <c r="I177" s="10">
-        <f t="shared" si="3"/>
+        <f>NETWORKDAYS(B177, A177)</f>
         <v>1</v>
       </c>
       <c r="J177" s="7">
@@ -13493,7 +13496,7 @@
         <v>130</v>
       </c>
       <c r="I178" s="10">
-        <f t="shared" si="3"/>
+        <f>NETWORKDAYS(B178, A178)</f>
         <v>1</v>
       </c>
       <c r="J178" s="7">
@@ -13557,7 +13560,7 @@
         <v>34</v>
       </c>
       <c r="I179" s="10">
-        <f t="shared" si="3"/>
+        <f>NETWORKDAYS(B179, A179)</f>
         <v>1</v>
       </c>
       <c r="J179" s="7">
@@ -13597,60 +13600,60 @@
     </row>
     <row r="180" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A180" s="11">
-        <v>45868</v>
+        <v>45846</v>
       </c>
       <c r="B180" s="11">
-        <v>45868</v>
+        <v>45846</v>
       </c>
       <c r="C180" s="11" t="s">
-        <v>128</v>
+        <v>7</v>
       </c>
       <c r="D180" s="11" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="E180" s="11" t="s">
-        <v>395</v>
+        <v>113</v>
       </c>
       <c r="F180" s="12">
-        <v>68487</v>
+        <v>68456</v>
       </c>
       <c r="G180" s="12" t="s">
-        <v>396</v>
+        <v>321</v>
       </c>
       <c r="H180" s="12" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="I180" s="13">
-        <f t="shared" si="3"/>
+        <f>NETWORKDAYS(B180, A180)</f>
         <v>1</v>
       </c>
       <c r="J180" s="12">
-        <v>66489</v>
+        <v>66118</v>
       </c>
       <c r="K180" s="12">
-        <v>11614</v>
+        <v>2289</v>
       </c>
       <c r="L180" s="12" t="s">
-        <v>397</v>
+        <v>361</v>
       </c>
       <c r="M180" s="11">
-        <v>45874</v>
+        <v>45877</v>
       </c>
       <c r="N180" s="14">
-        <v>6633</v>
+        <v>607.57000000000005</v>
       </c>
       <c r="O180" s="12" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="P180" s="12">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="Q180" s="12" t="s">
         <v>24</v>
       </c>
       <c r="R180" s="12">
         <f>DATEDIF(Tabela1[[#This Row],[Atendimento]],Tabela1[[#This Row],[Previsao de Entrega]],"D")</f>
-        <v>6</v>
+        <v>31</v>
       </c>
       <c r="S180" s="14">
         <v>0</v>
@@ -13661,10 +13664,10 @@
     </row>
     <row r="181" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A181" s="11">
-        <v>45861</v>
+        <v>45848</v>
       </c>
       <c r="B181" s="11">
-        <v>45861</v>
+        <v>45848</v>
       </c>
       <c r="C181" s="11" t="s">
         <v>7</v>
@@ -13673,54 +13676,54 @@
         <v>15</v>
       </c>
       <c r="E181" s="11" t="s">
-        <v>124</v>
-      </c>
-      <c r="F181" s="12" t="s">
-        <v>3</v>
+        <v>113</v>
+      </c>
+      <c r="F181" s="12">
+        <v>68459</v>
       </c>
       <c r="G181" s="12" t="s">
-        <v>125</v>
+        <v>364</v>
       </c>
       <c r="H181" s="12" t="s">
-        <v>126</v>
+        <v>365</v>
       </c>
       <c r="I181" s="13">
-        <f t="shared" si="3"/>
+        <f>NETWORKDAYS(B181, A181)</f>
         <v>1</v>
       </c>
       <c r="J181" s="12">
-        <v>66301</v>
+        <v>66162</v>
       </c>
       <c r="K181" s="12">
-        <v>1522</v>
+        <v>11781</v>
       </c>
       <c r="L181" s="12" t="s">
-        <v>388</v>
+        <v>366</v>
       </c>
       <c r="M181" s="11">
-        <v>45875</v>
+        <v>45855</v>
       </c>
       <c r="N181" s="14">
-        <v>1023.45</v>
+        <v>5396.77</v>
       </c>
       <c r="O181" s="12" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="P181" s="12">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="Q181" s="12" t="s">
         <v>24</v>
       </c>
       <c r="R181" s="12">
         <f>DATEDIF(Tabela1[[#This Row],[Atendimento]],Tabela1[[#This Row],[Previsao de Entrega]],"D")</f>
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="S181" s="14">
-        <v>0</v>
+        <v>284.04000000000002</v>
       </c>
       <c r="T181" s="14">
-        <v>141.4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="182" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
@@ -13749,7 +13752,7 @@
         <v>91</v>
       </c>
       <c r="I182" s="10">
-        <f t="shared" si="3"/>
+        <f>NETWORKDAYS(B182, A182)</f>
         <v>1</v>
       </c>
       <c r="J182" s="7">
@@ -13789,10 +13792,10 @@
     </row>
     <row r="183" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A183" s="11">
-        <v>45868</v>
+        <v>45848</v>
       </c>
       <c r="B183" s="11">
-        <v>45862</v>
+        <v>45848</v>
       </c>
       <c r="C183" s="11" t="s">
         <v>7</v>
@@ -13804,48 +13807,48 @@
         <v>113</v>
       </c>
       <c r="F183" s="12">
-        <v>68476</v>
+        <v>68457</v>
       </c>
       <c r="G183" s="12" t="s">
-        <v>227</v>
+        <v>33</v>
       </c>
       <c r="H183" s="12" t="s">
-        <v>98</v>
+        <v>34</v>
       </c>
       <c r="I183" s="13">
-        <f t="shared" si="3"/>
-        <v>5</v>
+        <f>NETWORKDAYS(B183, A183)</f>
+        <v>1</v>
       </c>
       <c r="J183" s="12">
-        <v>66491</v>
+        <v>66126</v>
       </c>
       <c r="K183" s="12">
-        <v>11522</v>
+        <v>2931</v>
       </c>
       <c r="L183" s="12" t="s">
-        <v>377</v>
+        <v>367</v>
       </c>
       <c r="M183" s="11">
-        <v>45875</v>
+        <v>45879</v>
       </c>
       <c r="N183" s="14">
-        <v>398.42</v>
+        <v>3500</v>
       </c>
       <c r="O183" s="12" t="s">
         <v>122</v>
       </c>
       <c r="P183" s="12">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="Q183" s="12" t="s">
         <v>24</v>
       </c>
       <c r="R183" s="12">
         <f>DATEDIF(Tabela1[[#This Row],[Atendimento]],Tabela1[[#This Row],[Previsao de Entrega]],"D")</f>
-        <v>7</v>
+        <v>31</v>
       </c>
       <c r="S183" s="14">
-        <v>0</v>
+        <v>320</v>
       </c>
       <c r="T183" s="14">
         <v>0</v>
@@ -13877,7 +13880,7 @@
         <v>98</v>
       </c>
       <c r="I184" s="10">
-        <f t="shared" si="3"/>
+        <f>NETWORKDAYS(B184, A184)</f>
         <v>1</v>
       </c>
       <c r="J184" s="7">
@@ -13941,7 +13944,7 @@
         <v>91</v>
       </c>
       <c r="I185" s="10">
-        <f t="shared" si="3"/>
+        <f>NETWORKDAYS(B185, A185)</f>
         <v>4</v>
       </c>
       <c r="J185" s="7">
@@ -14005,7 +14008,7 @@
         <v>34</v>
       </c>
       <c r="I186" s="10">
-        <f t="shared" si="3"/>
+        <f>NETWORKDAYS(B186, A186)</f>
         <v>1</v>
       </c>
       <c r="J186" s="7">
@@ -14069,7 +14072,7 @@
         <v>96</v>
       </c>
       <c r="I187" s="10">
-        <f t="shared" si="3"/>
+        <f>NETWORKDAYS(B187, A187)</f>
         <v>1</v>
       </c>
       <c r="J187" s="7">
@@ -14133,7 +14136,7 @@
         <v>32</v>
       </c>
       <c r="I188" s="10">
-        <f t="shared" si="3"/>
+        <f>NETWORKDAYS(B188, A188)</f>
         <v>1</v>
       </c>
       <c r="J188" s="7">
@@ -14197,7 +14200,7 @@
         <v>34</v>
       </c>
       <c r="I189" s="10">
-        <f t="shared" si="3"/>
+        <f>NETWORKDAYS(B189, A189)</f>
         <v>1</v>
       </c>
       <c r="J189" s="7">
@@ -14261,7 +14264,7 @@
         <v>91</v>
       </c>
       <c r="I190" s="10">
-        <f t="shared" si="3"/>
+        <f>NETWORKDAYS(B190, A190)</f>
         <v>4</v>
       </c>
       <c r="J190" s="7">
@@ -14325,7 +14328,7 @@
         <v>91</v>
       </c>
       <c r="I191" s="10">
-        <f t="shared" si="3"/>
+        <f>NETWORKDAYS(B191, A191)</f>
         <v>1</v>
       </c>
       <c r="J191" s="7">
@@ -14389,7 +14392,7 @@
         <v>34</v>
       </c>
       <c r="I192" s="10">
-        <f t="shared" si="3"/>
+        <f>NETWORKDAYS(B192, A192)</f>
         <v>1</v>
       </c>
       <c r="J192" s="7">
@@ -14453,7 +14456,7 @@
         <v>98</v>
       </c>
       <c r="I193" s="10">
-        <f t="shared" si="3"/>
+        <f>NETWORKDAYS(B193, A193)</f>
         <v>1</v>
       </c>
       <c r="J193" s="7">
@@ -14517,7 +14520,7 @@
         <v>373</v>
       </c>
       <c r="I194" s="10">
-        <f t="shared" si="3"/>
+        <f>NETWORKDAYS(B194, A194)</f>
         <v>1</v>
       </c>
       <c r="J194" s="7">
@@ -14581,7 +14584,7 @@
         <v>32</v>
       </c>
       <c r="I195" s="10">
-        <f t="shared" si="3"/>
+        <f>NETWORKDAYS(B195, A195)</f>
         <v>1</v>
       </c>
       <c r="J195" s="7">
@@ -14645,7 +14648,7 @@
         <v>373</v>
       </c>
       <c r="I196" s="10">
-        <f t="shared" si="3"/>
+        <f>NETWORKDAYS(B196, A196)</f>
         <v>1</v>
       </c>
       <c r="J196" s="7">
@@ -14709,7 +14712,7 @@
         <v>373</v>
       </c>
       <c r="I197" s="10">
-        <f t="shared" si="3"/>
+        <f>NETWORKDAYS(B197, A197)</f>
         <v>1</v>
       </c>
       <c r="J197" s="7">
@@ -14773,7 +14776,7 @@
         <v>373</v>
       </c>
       <c r="I198" s="10">
-        <f t="shared" si="3"/>
+        <f>NETWORKDAYS(B198, A198)</f>
         <v>1</v>
       </c>
       <c r="J198" s="7">
@@ -14837,7 +14840,7 @@
         <v>32</v>
       </c>
       <c r="I199" s="10">
-        <f t="shared" si="3"/>
+        <f>NETWORKDAYS(B199, A199)</f>
         <v>1</v>
       </c>
       <c r="J199" s="7">
@@ -14901,7 +14904,7 @@
         <v>32</v>
       </c>
       <c r="I200" s="10">
-        <f t="shared" si="3"/>
+        <f>NETWORKDAYS(B200, A200)</f>
         <v>1</v>
       </c>
       <c r="J200" s="7">
@@ -14965,7 +14968,7 @@
         <v>130</v>
       </c>
       <c r="I201" s="10">
-        <f t="shared" ref="I201:I232" si="4">NETWORKDAYS(B201, A201)</f>
+        <f>NETWORKDAYS(B201, A201)</f>
         <v>1</v>
       </c>
       <c r="J201" s="7">
@@ -15029,7 +15032,7 @@
         <v>32</v>
       </c>
       <c r="I202" s="10">
-        <f t="shared" si="4"/>
+        <f>NETWORKDAYS(B202, A202)</f>
         <v>1</v>
       </c>
       <c r="J202" s="7">
@@ -15093,7 +15096,7 @@
         <v>32</v>
       </c>
       <c r="I203" s="10">
-        <f t="shared" si="4"/>
+        <f>NETWORKDAYS(B203, A203)</f>
         <v>1</v>
       </c>
       <c r="J203" s="7">
@@ -15133,63 +15136,63 @@
     </row>
     <row r="204" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A204" s="11">
-        <v>45818</v>
+        <v>45849</v>
       </c>
       <c r="B204" s="11">
-        <v>45813</v>
+        <v>45849</v>
       </c>
       <c r="C204" s="11" t="s">
         <v>7</v>
       </c>
       <c r="D204" s="11" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="E204" s="11" t="s">
-        <v>124</v>
-      </c>
-      <c r="F204" s="12">
-        <v>68422</v>
+        <v>113</v>
+      </c>
+      <c r="F204" s="12" t="s">
+        <v>3</v>
       </c>
       <c r="G204" s="12" t="s">
-        <v>90</v>
+        <v>372</v>
       </c>
       <c r="H204" s="12" t="s">
-        <v>91</v>
+        <v>373</v>
       </c>
       <c r="I204" s="13">
-        <f t="shared" si="4"/>
-        <v>4</v>
+        <f>NETWORKDAYS(B204, A204)</f>
+        <v>1</v>
       </c>
       <c r="J204" s="12">
-        <v>65725</v>
+        <v>66166</v>
       </c>
       <c r="K204" s="12">
-        <v>1450</v>
+        <v>11782</v>
       </c>
       <c r="L204" s="12" t="s">
-        <v>229</v>
+        <v>371</v>
       </c>
       <c r="M204" s="11">
-        <v>45877</v>
+        <v>45880</v>
       </c>
       <c r="N204" s="14">
-        <v>239.63</v>
+        <v>2250</v>
       </c>
       <c r="O204" s="12" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="P204" s="12">
-        <v>120</v>
+        <v>30</v>
       </c>
       <c r="Q204" s="12" t="s">
         <v>24</v>
       </c>
       <c r="R204" s="12">
         <f>DATEDIF(Tabela1[[#This Row],[Atendimento]],Tabela1[[#This Row],[Previsao de Entrega]],"D")</f>
-        <v>59</v>
+        <v>31</v>
       </c>
       <c r="S204" s="14">
-        <v>0</v>
+        <v>250</v>
       </c>
       <c r="T204" s="14">
         <v>0</v>
@@ -15197,63 +15200,63 @@
     </row>
     <row r="205" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A205" s="11">
-        <v>45846</v>
+        <v>45855</v>
       </c>
       <c r="B205" s="11">
-        <v>45846</v>
+        <v>45855</v>
       </c>
       <c r="C205" s="11" t="s">
         <v>7</v>
       </c>
       <c r="D205" s="11" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="E205" s="11" t="s">
-        <v>113</v>
-      </c>
-      <c r="F205" s="12">
-        <v>68456</v>
+        <v>142</v>
+      </c>
+      <c r="F205" s="12" t="s">
+        <v>3</v>
       </c>
       <c r="G205" s="12" t="s">
-        <v>321</v>
+        <v>125</v>
       </c>
       <c r="H205" s="12" t="s">
-        <v>91</v>
+        <v>126</v>
       </c>
       <c r="I205" s="13">
-        <f t="shared" si="4"/>
+        <f>NETWORKDAYS(B205, A205)</f>
         <v>1</v>
       </c>
       <c r="J205" s="12">
-        <v>66118</v>
+        <v>66308</v>
       </c>
       <c r="K205" s="12">
-        <v>2289</v>
+        <v>11757</v>
       </c>
       <c r="L205" s="12" t="s">
-        <v>361</v>
+        <v>305</v>
       </c>
       <c r="M205" s="11">
-        <v>45877</v>
+        <v>45873</v>
       </c>
       <c r="N205" s="14">
-        <v>607.57000000000005</v>
+        <v>1428.29</v>
       </c>
       <c r="O205" s="12" t="s">
         <v>122</v>
       </c>
       <c r="P205" s="12">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="Q205" s="12" t="s">
         <v>24</v>
       </c>
       <c r="R205" s="12">
         <f>DATEDIF(Tabela1[[#This Row],[Atendimento]],Tabela1[[#This Row],[Previsao de Entrega]],"D")</f>
-        <v>31</v>
+        <v>18</v>
       </c>
       <c r="S205" s="14">
-        <v>0</v>
+        <v>320</v>
       </c>
       <c r="T205" s="14">
         <v>0</v>
@@ -15285,7 +15288,7 @@
         <v>373</v>
       </c>
       <c r="I206" s="10">
-        <f t="shared" si="4"/>
+        <f>NETWORKDAYS(B206, A206)</f>
         <v>1</v>
       </c>
       <c r="J206" s="7">
@@ -15349,7 +15352,7 @@
         <v>130</v>
       </c>
       <c r="I207" s="10">
-        <f t="shared" si="4"/>
+        <f>NETWORKDAYS(B207, A207)</f>
         <v>1</v>
       </c>
       <c r="J207" s="7">
@@ -15413,7 +15416,7 @@
         <v>130</v>
       </c>
       <c r="I208" s="10">
-        <f t="shared" si="4"/>
+        <f>NETWORKDAYS(B208, A208)</f>
         <v>1</v>
       </c>
       <c r="J208" s="7">
@@ -15477,7 +15480,7 @@
         <v>130</v>
       </c>
       <c r="I209" s="10">
-        <f t="shared" si="4"/>
+        <f>NETWORKDAYS(B209, A209)</f>
         <v>1</v>
       </c>
       <c r="J209" s="7">
@@ -15541,7 +15544,7 @@
         <v>130</v>
       </c>
       <c r="I210" s="10">
-        <f t="shared" si="4"/>
+        <f>NETWORKDAYS(B210, A210)</f>
         <v>1</v>
       </c>
       <c r="J210" s="7">
@@ -15605,7 +15608,7 @@
         <v>34</v>
       </c>
       <c r="I211" s="10">
-        <f t="shared" si="4"/>
+        <f>NETWORKDAYS(B211, A211)</f>
         <v>1</v>
       </c>
       <c r="J211" s="7">
@@ -15669,7 +15672,7 @@
         <v>32</v>
       </c>
       <c r="I212" s="10">
-        <f t="shared" si="4"/>
+        <f>NETWORKDAYS(B212, A212)</f>
         <v>1</v>
       </c>
       <c r="J212" s="7">
@@ -15733,7 +15736,7 @@
         <v>138</v>
       </c>
       <c r="I213" s="10">
-        <f t="shared" si="4"/>
+        <f>NETWORKDAYS(B213, A213)</f>
         <v>1</v>
       </c>
       <c r="J213" s="7">
@@ -15797,7 +15800,7 @@
         <v>91</v>
       </c>
       <c r="I214" s="10">
-        <f t="shared" si="4"/>
+        <f>NETWORKDAYS(B214, A214)</f>
         <v>1</v>
       </c>
       <c r="J214" s="7">
@@ -15861,7 +15864,7 @@
         <v>98</v>
       </c>
       <c r="I215" s="10">
-        <f t="shared" si="4"/>
+        <f>NETWORKDAYS(B215, A215)</f>
         <v>1</v>
       </c>
       <c r="J215" s="7">
@@ -15925,7 +15928,7 @@
         <v>138</v>
       </c>
       <c r="I216" s="10">
-        <f t="shared" si="4"/>
+        <f>NETWORKDAYS(B216, A216)</f>
         <v>1</v>
       </c>
       <c r="J216" s="7">
@@ -15965,130 +15968,130 @@
     </row>
     <row r="217" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A217" s="11">
-        <v>45848</v>
+        <v>45856</v>
       </c>
       <c r="B217" s="11">
-        <v>45848</v>
+        <v>45856</v>
       </c>
       <c r="C217" s="11" t="s">
         <v>7</v>
       </c>
       <c r="D217" s="11" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="E217" s="11" t="s">
-        <v>113</v>
+        <v>124</v>
       </c>
       <c r="F217" s="12">
-        <v>68457</v>
+        <v>68466</v>
       </c>
       <c r="G217" s="12" t="s">
-        <v>33</v>
+        <v>125</v>
       </c>
       <c r="H217" s="12" t="s">
-        <v>34</v>
+        <v>126</v>
       </c>
       <c r="I217" s="13">
-        <f t="shared" si="4"/>
+        <f>NETWORKDAYS(B217, A217)</f>
         <v>1</v>
       </c>
       <c r="J217" s="12">
-        <v>66126</v>
+        <v>66337</v>
       </c>
       <c r="K217" s="12">
-        <v>2931</v>
+        <v>11736</v>
       </c>
       <c r="L217" s="12" t="s">
-        <v>367</v>
+        <v>127</v>
       </c>
       <c r="M217" s="11">
-        <v>45879</v>
+        <v>45889</v>
       </c>
       <c r="N217" s="14">
-        <v>3500</v>
+        <v>16134.54</v>
       </c>
       <c r="O217" s="12" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="P217" s="12">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="Q217" s="12" t="s">
         <v>24</v>
       </c>
       <c r="R217" s="12">
         <f>DATEDIF(Tabela1[[#This Row],[Atendimento]],Tabela1[[#This Row],[Previsao de Entrega]],"D")</f>
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="S217" s="14">
-        <v>320</v>
+        <v>25720</v>
       </c>
       <c r="T217" s="14">
         <v>0</v>
       </c>
     </row>
     <row r="218" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A218" s="49">
-        <v>45826</v>
-      </c>
-      <c r="B218" s="49">
-        <v>45826</v>
-      </c>
-      <c r="C218" s="49" t="s">
-        <v>7</v>
-      </c>
-      <c r="D218" s="49" t="s">
+      <c r="A218" s="11">
+        <v>45861</v>
+      </c>
+      <c r="B218" s="11">
+        <v>45861</v>
+      </c>
+      <c r="C218" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D218" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="E218" s="49" t="s">
+      <c r="E218" s="11" t="s">
         <v>124</v>
       </c>
-      <c r="F218" s="50" t="s">
-        <v>3</v>
-      </c>
-      <c r="G218" s="50" t="s">
+      <c r="F218" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="G218" s="12" t="s">
         <v>125</v>
       </c>
-      <c r="H218" s="50" t="s">
+      <c r="H218" s="12" t="s">
         <v>126</v>
       </c>
-      <c r="I218" s="51">
-        <f t="shared" si="4"/>
+      <c r="I218" s="13">
+        <f>NETWORKDAYS(B218, A218)</f>
         <v>1</v>
       </c>
-      <c r="J218" s="50">
-        <v>66341</v>
-      </c>
-      <c r="K218" s="50">
-        <v>11758</v>
-      </c>
-      <c r="L218" s="50" t="s">
-        <v>316</v>
-      </c>
-      <c r="M218" s="49">
-        <v>45880</v>
-      </c>
-      <c r="N218" s="52">
-        <v>924.61</v>
-      </c>
-      <c r="O218" s="50" t="s">
+      <c r="J218" s="12">
+        <v>66301</v>
+      </c>
+      <c r="K218" s="12">
+        <v>1522</v>
+      </c>
+      <c r="L218" s="12" t="s">
+        <v>388</v>
+      </c>
+      <c r="M218" s="11">
+        <v>45875</v>
+      </c>
+      <c r="N218" s="14">
+        <v>1023.45</v>
+      </c>
+      <c r="O218" s="12" t="s">
         <v>122</v>
       </c>
-      <c r="P218" s="50">
+      <c r="P218" s="12">
         <v>28</v>
       </c>
-      <c r="Q218" s="50" t="s">
+      <c r="Q218" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="R218" s="50">
-        <f>DATEDIF(Tabela1[[#This Row],[Atendimento]],Tabela1[[#This Row],[Previsao de Entrega]],"D")</f>
-        <v>54</v>
-      </c>
-      <c r="S218" s="52">
-        <v>0</v>
-      </c>
-      <c r="T218" s="52">
-        <v>0</v>
+      <c r="R218" s="12">
+        <f>DATEDIF(Tabela1[[#This Row],[Atendimento]],Tabela1[[#This Row],[Previsao de Entrega]],"D")</f>
+        <v>14</v>
+      </c>
+      <c r="S218" s="14">
+        <v>0</v>
+      </c>
+      <c r="T218" s="14">
+        <v>141.4</v>
       </c>
     </row>
     <row r="219" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
@@ -16117,7 +16120,7 @@
         <v>130</v>
       </c>
       <c r="I219" s="10">
-        <f t="shared" si="4"/>
+        <f>NETWORKDAYS(B219, A219)</f>
         <v>1</v>
       </c>
       <c r="J219" s="7">
@@ -16181,7 +16184,7 @@
         <v>130</v>
       </c>
       <c r="I220" s="10">
-        <f t="shared" si="4"/>
+        <f>NETWORKDAYS(B220, A220)</f>
         <v>1</v>
       </c>
       <c r="J220" s="7">
@@ -16245,7 +16248,7 @@
         <v>98</v>
       </c>
       <c r="I221" s="10">
-        <f t="shared" si="4"/>
+        <f>NETWORKDAYS(B221, A221)</f>
         <v>1</v>
       </c>
       <c r="J221" s="7">
@@ -16285,10 +16288,10 @@
     </row>
     <row r="222" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A222" s="11">
-        <v>45849</v>
+        <v>45863</v>
       </c>
       <c r="B222" s="11">
-        <v>45849</v>
+        <v>45863</v>
       </c>
       <c r="C222" s="11" t="s">
         <v>7</v>
@@ -16299,36 +16302,36 @@
       <c r="E222" s="11" t="s">
         <v>113</v>
       </c>
-      <c r="F222" s="12" t="s">
-        <v>3</v>
+      <c r="F222" s="12">
+        <v>68479</v>
       </c>
       <c r="G222" s="12" t="s">
-        <v>372</v>
+        <v>389</v>
       </c>
       <c r="H222" s="12" t="s">
-        <v>373</v>
+        <v>91</v>
       </c>
       <c r="I222" s="13">
-        <f t="shared" si="4"/>
+        <f>NETWORKDAYS(B222, A222)</f>
         <v>1</v>
       </c>
       <c r="J222" s="12">
-        <v>66166</v>
+        <v>66454</v>
       </c>
       <c r="K222" s="12">
-        <v>11782</v>
+        <v>11788</v>
       </c>
       <c r="L222" s="12" t="s">
-        <v>371</v>
+        <v>390</v>
       </c>
       <c r="M222" s="11">
-        <v>45880</v>
+        <v>45889</v>
       </c>
       <c r="N222" s="14">
-        <v>2250</v>
+        <v>4122.3</v>
       </c>
       <c r="O222" s="12" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="P222" s="12">
         <v>30</v>
@@ -16338,10 +16341,10 @@
       </c>
       <c r="R222" s="12">
         <f>DATEDIF(Tabela1[[#This Row],[Atendimento]],Tabela1[[#This Row],[Previsao de Entrega]],"D")</f>
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="S222" s="14">
-        <v>250</v>
+        <v>0</v>
       </c>
       <c r="T222" s="14">
         <v>0</v>
@@ -16373,7 +16376,7 @@
         <v>32</v>
       </c>
       <c r="I223" s="10">
-        <f t="shared" si="4"/>
+        <f>NETWORKDAYS(B223, A223)</f>
         <v>1</v>
       </c>
       <c r="J223" s="7">
@@ -16413,63 +16416,63 @@
     </row>
     <row r="224" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A224" s="11">
-        <v>45867</v>
+        <v>45866</v>
       </c>
       <c r="B224" s="11">
-        <v>45867</v>
+        <v>45863</v>
       </c>
       <c r="C224" s="11" t="s">
         <v>7</v>
       </c>
       <c r="D224" s="11" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="E224" s="11" t="s">
-        <v>124</v>
-      </c>
-      <c r="F224" s="12" t="s">
-        <v>3</v>
+        <v>113</v>
+      </c>
+      <c r="F224" s="12">
+        <v>68481</v>
       </c>
       <c r="G224" s="12" t="s">
-        <v>125</v>
+        <v>372</v>
       </c>
       <c r="H224" s="12" t="s">
-        <v>126</v>
+        <v>373</v>
       </c>
       <c r="I224" s="13">
-        <f t="shared" si="4"/>
-        <v>1</v>
+        <f>NETWORKDAYS(B224, A224)</f>
+        <v>2</v>
       </c>
       <c r="J224" s="12">
-        <v>66471</v>
+        <v>66462</v>
       </c>
       <c r="K224" s="12">
-        <v>9</v>
+        <v>10535</v>
       </c>
       <c r="L224" s="12" t="s">
-        <v>398</v>
+        <v>391</v>
       </c>
       <c r="M224" s="11">
-        <v>45880</v>
+        <v>45868</v>
       </c>
       <c r="N224" s="14">
-        <v>6505.5</v>
+        <v>300</v>
       </c>
       <c r="O224" s="12" t="s">
         <v>122</v>
       </c>
       <c r="P224" s="12">
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="Q224" s="12" t="s">
         <v>24</v>
       </c>
       <c r="R224" s="12">
         <f>DATEDIF(Tabela1[[#This Row],[Atendimento]],Tabela1[[#This Row],[Previsao de Entrega]],"D")</f>
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="S224" s="14">
-        <v>135</v>
+        <v>0</v>
       </c>
       <c r="T224" s="14">
         <v>0</v>
@@ -16477,63 +16480,63 @@
     </row>
     <row r="225" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A225" s="11">
-        <v>45785</v>
+        <v>45867</v>
       </c>
       <c r="B225" s="11">
-        <v>45784</v>
+        <v>45867</v>
       </c>
       <c r="C225" s="11" t="s">
         <v>7</v>
       </c>
       <c r="D225" s="11" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="E225" s="11" t="s">
-        <v>113</v>
-      </c>
-      <c r="F225" s="12">
-        <v>68369</v>
+        <v>124</v>
+      </c>
+      <c r="F225" s="12" t="s">
+        <v>3</v>
       </c>
       <c r="G225" s="12" t="s">
-        <v>39</v>
+        <v>125</v>
       </c>
       <c r="H225" s="12" t="s">
-        <v>98</v>
+        <v>126</v>
       </c>
       <c r="I225" s="13">
-        <f t="shared" si="4"/>
-        <v>2</v>
+        <f>NETWORKDAYS(B225, A225)</f>
+        <v>1</v>
       </c>
       <c r="J225" s="12">
-        <v>65234</v>
+        <v>66471</v>
       </c>
       <c r="K225" s="12">
-        <v>11610</v>
+        <v>9</v>
       </c>
       <c r="L225" s="12" t="s">
-        <v>38</v>
+        <v>398</v>
       </c>
       <c r="M225" s="11">
-        <v>45881</v>
+        <v>45880</v>
       </c>
       <c r="N225" s="14">
-        <v>9114.5499999999993</v>
+        <v>6505.5</v>
       </c>
       <c r="O225" s="12" t="s">
         <v>122</v>
       </c>
       <c r="P225" s="12">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="Q225" s="12" t="s">
         <v>24</v>
       </c>
       <c r="R225" s="12">
         <f>DATEDIF(Tabela1[[#This Row],[Atendimento]],Tabela1[[#This Row],[Previsao de Entrega]],"D")</f>
-        <v>96</v>
+        <v>13</v>
       </c>
       <c r="S225" s="14">
-        <v>183.5</v>
+        <v>135</v>
       </c>
       <c r="T225" s="14">
         <v>0</v>
@@ -16565,7 +16568,7 @@
         <v>32</v>
       </c>
       <c r="I226" s="10">
-        <f t="shared" si="4"/>
+        <f>NETWORKDAYS(B226, A226)</f>
         <v>1</v>
       </c>
       <c r="J226" s="7">
@@ -16629,7 +16632,7 @@
         <v>96</v>
       </c>
       <c r="I227" s="13">
-        <f t="shared" si="4"/>
+        <f>NETWORKDAYS(B227, A227)</f>
         <v>1</v>
       </c>
       <c r="J227" s="12">
@@ -16669,63 +16672,63 @@
     </row>
     <row r="228" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A228" s="11">
-        <v>45863</v>
+        <v>45867</v>
       </c>
       <c r="B228" s="11">
-        <v>45863</v>
+        <v>45866</v>
       </c>
       <c r="C228" s="11" t="s">
         <v>7</v>
       </c>
       <c r="D228" s="11" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="E228" s="11" t="s">
-        <v>113</v>
+        <v>124</v>
       </c>
       <c r="F228" s="12">
-        <v>68479</v>
+        <v>68483</v>
       </c>
       <c r="G228" s="12" t="s">
-        <v>389</v>
+        <v>125</v>
       </c>
       <c r="H228" s="12" t="s">
-        <v>91</v>
+        <v>126</v>
       </c>
       <c r="I228" s="13">
-        <f t="shared" si="4"/>
-        <v>1</v>
+        <f>NETWORKDAYS(B228, A228)</f>
+        <v>2</v>
       </c>
       <c r="J228" s="12">
-        <v>66454</v>
+        <v>66467</v>
       </c>
       <c r="K228" s="12">
-        <v>11788</v>
+        <v>11164</v>
       </c>
       <c r="L228" s="12" t="s">
-        <v>390</v>
+        <v>298</v>
       </c>
       <c r="M228" s="11">
-        <v>45889</v>
+        <v>45908</v>
       </c>
       <c r="N228" s="14">
-        <v>4122.3</v>
+        <v>2623.03</v>
       </c>
       <c r="O228" s="12" t="s">
         <v>122</v>
       </c>
       <c r="P228" s="12">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="Q228" s="12" t="s">
         <v>24</v>
       </c>
       <c r="R228" s="12">
         <f>DATEDIF(Tabela1[[#This Row],[Atendimento]],Tabela1[[#This Row],[Previsao de Entrega]],"D")</f>
-        <v>26</v>
+        <v>41</v>
       </c>
       <c r="S228" s="14">
-        <v>0</v>
+        <v>52</v>
       </c>
       <c r="T228" s="14">
         <v>0</v>
@@ -16733,63 +16736,63 @@
     </row>
     <row r="229" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A229" s="11">
-        <v>45856</v>
+        <v>45868</v>
       </c>
       <c r="B229" s="11">
-        <v>45856</v>
+        <v>45868</v>
       </c>
       <c r="C229" s="11" t="s">
-        <v>7</v>
+        <v>128</v>
       </c>
       <c r="D229" s="11" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="E229" s="11" t="s">
-        <v>124</v>
+        <v>395</v>
       </c>
       <c r="F229" s="12">
-        <v>68466</v>
+        <v>68487</v>
       </c>
       <c r="G229" s="12" t="s">
-        <v>125</v>
+        <v>396</v>
       </c>
       <c r="H229" s="12" t="s">
-        <v>126</v>
+        <v>96</v>
       </c>
       <c r="I229" s="13">
-        <f t="shared" si="4"/>
+        <f>NETWORKDAYS(B229, A229)</f>
         <v>1</v>
       </c>
       <c r="J229" s="12">
-        <v>66337</v>
+        <v>66489</v>
       </c>
       <c r="K229" s="12">
-        <v>11736</v>
+        <v>11614</v>
       </c>
       <c r="L229" s="12" t="s">
-        <v>127</v>
+        <v>397</v>
       </c>
       <c r="M229" s="11">
-        <v>45889</v>
+        <v>45874</v>
       </c>
       <c r="N229" s="14">
-        <v>16134.54</v>
+        <v>6633</v>
       </c>
       <c r="O229" s="12" t="s">
         <v>121</v>
       </c>
       <c r="P229" s="12">
-        <v>28</v>
+        <v>1</v>
       </c>
       <c r="Q229" s="12" t="s">
         <v>24</v>
       </c>
       <c r="R229" s="12">
         <f>DATEDIF(Tabela1[[#This Row],[Atendimento]],Tabela1[[#This Row],[Previsao de Entrega]],"D")</f>
-        <v>33</v>
+        <v>6</v>
       </c>
       <c r="S229" s="14">
-        <v>25720</v>
+        <v>0</v>
       </c>
       <c r="T229" s="14">
         <v>0</v>
@@ -16821,7 +16824,7 @@
         <v>34</v>
       </c>
       <c r="I230" s="10">
-        <f t="shared" si="4"/>
+        <f>NETWORKDAYS(B230, A230)</f>
         <v>1</v>
       </c>
       <c r="J230" s="7">
@@ -16861,47 +16864,47 @@
     </row>
     <row r="231" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A231" s="11">
-        <v>45867</v>
+        <v>45868</v>
       </c>
       <c r="B231" s="11">
-        <v>45866</v>
+        <v>45862</v>
       </c>
       <c r="C231" s="11" t="s">
         <v>7</v>
       </c>
       <c r="D231" s="11" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="E231" s="11" t="s">
-        <v>124</v>
+        <v>113</v>
       </c>
       <c r="F231" s="12">
-        <v>68483</v>
+        <v>68476</v>
       </c>
       <c r="G231" s="12" t="s">
-        <v>125</v>
+        <v>227</v>
       </c>
       <c r="H231" s="12" t="s">
-        <v>126</v>
+        <v>98</v>
       </c>
       <c r="I231" s="13">
-        <f t="shared" si="4"/>
-        <v>2</v>
+        <f>NETWORKDAYS(B231, A231)</f>
+        <v>5</v>
       </c>
       <c r="J231" s="12">
-        <v>66467</v>
+        <v>66491</v>
       </c>
       <c r="K231" s="12">
-        <v>11164</v>
+        <v>11522</v>
       </c>
       <c r="L231" s="12" t="s">
-        <v>298</v>
+        <v>377</v>
       </c>
       <c r="M231" s="11">
-        <v>45908</v>
+        <v>45875</v>
       </c>
       <c r="N231" s="14">
-        <v>2623.03</v>
+        <v>398.42</v>
       </c>
       <c r="O231" s="12" t="s">
         <v>122</v>
@@ -16914,10 +16917,10 @@
       </c>
       <c r="R231" s="12">
         <f>DATEDIF(Tabela1[[#This Row],[Atendimento]],Tabela1[[#This Row],[Previsao de Entrega]],"D")</f>
-        <v>41</v>
+        <v>7</v>
       </c>
       <c r="S231" s="14">
-        <v>52</v>
+        <v>0</v>
       </c>
       <c r="T231" s="14">
         <v>0</v>
@@ -16949,7 +16952,7 @@
         <v>126</v>
       </c>
       <c r="I232" s="13">
-        <f t="shared" si="4"/>
+        <f>NETWORKDAYS(B232, A232)</f>
         <v>1</v>
       </c>
       <c r="J232" s="12">
@@ -17052,66 +17055,66 @@
       </c>
     </row>
     <row r="234" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A234" s="40">
+      <c r="A234" s="11">
         <v>45870</v>
       </c>
-      <c r="B234" s="40">
+      <c r="B234" s="11">
         <v>45869</v>
       </c>
-      <c r="C234" s="40" t="s">
-        <v>7</v>
-      </c>
-      <c r="D234" s="40" t="s">
-        <v>15</v>
-      </c>
-      <c r="E234" s="40" t="s">
+      <c r="C234" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D234" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="E234" s="11" t="s">
         <v>113</v>
       </c>
-      <c r="F234" s="41">
+      <c r="F234" s="12">
         <v>68491</v>
       </c>
-      <c r="G234" s="41" t="s">
+      <c r="G234" s="12" t="s">
         <v>372</v>
       </c>
-      <c r="H234" s="41" t="s">
+      <c r="H234" s="12" t="s">
         <v>373</v>
       </c>
-      <c r="I234" s="42">
+      <c r="I234" s="13">
         <f>NETWORKDAYS(B234, A234)</f>
         <v>2</v>
       </c>
-      <c r="J234" s="41">
+      <c r="J234" s="12">
         <v>66521</v>
       </c>
-      <c r="K234" s="54">
+      <c r="K234" s="12">
         <v>3061</v>
       </c>
-      <c r="L234" s="41" t="s">
+      <c r="L234" s="12" t="s">
         <v>192</v>
       </c>
-      <c r="M234" s="40">
+      <c r="M234" s="11">
         <v>45883</v>
       </c>
-      <c r="N234" s="43">
+      <c r="N234" s="14">
         <v>3000</v>
       </c>
-      <c r="O234" s="41" t="s">
+      <c r="O234" s="12" t="s">
         <v>122</v>
       </c>
-      <c r="P234" s="41">
+      <c r="P234" s="12">
         <v>15</v>
       </c>
-      <c r="Q234" s="41" t="s">
-        <v>360</v>
-      </c>
-      <c r="R234" s="54">
+      <c r="Q234" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="R234" s="12">
         <f>DATEDIF(Tabela1[[#This Row],[Atendimento]],Tabela1[[#This Row],[Previsao de Entrega]],"D")</f>
         <v>13</v>
       </c>
-      <c r="S234" s="43">
-        <v>0</v>
-      </c>
-      <c r="T234" s="43">
+      <c r="S234" s="14">
+        <v>50</v>
+      </c>
+      <c r="T234" s="14">
         <v>0</v>
       </c>
     </row>
@@ -17147,7 +17150,7 @@
       <c r="J235" s="41">
         <v>66522</v>
       </c>
-      <c r="K235" s="54">
+      <c r="K235" s="41">
         <v>679</v>
       </c>
       <c r="L235" s="41" t="s">
@@ -17168,7 +17171,7 @@
       <c r="Q235" s="41" t="s">
         <v>360</v>
       </c>
-      <c r="R235" s="54">
+      <c r="R235" s="41">
         <f>DATEDIF(Tabela1[[#This Row],[Atendimento]],Tabela1[[#This Row],[Previsao de Entrega]],"D")</f>
         <v>11</v>
       </c>
@@ -17176,6 +17179,198 @@
         <v>0</v>
       </c>
       <c r="T235" s="43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="236" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A236" s="40">
+        <v>45870</v>
+      </c>
+      <c r="B236" s="40">
+        <v>45867</v>
+      </c>
+      <c r="C236" s="40" t="s">
+        <v>7</v>
+      </c>
+      <c r="D236" s="40" t="s">
+        <v>5</v>
+      </c>
+      <c r="E236" s="40" t="s">
+        <v>113</v>
+      </c>
+      <c r="F236" s="41">
+        <v>68485</v>
+      </c>
+      <c r="G236" s="41" t="s">
+        <v>372</v>
+      </c>
+      <c r="H236" s="41" t="s">
+        <v>373</v>
+      </c>
+      <c r="I236" s="42">
+        <f>NETWORKDAYS(B236, A236)</f>
+        <v>4</v>
+      </c>
+      <c r="J236" s="41">
+        <v>66526</v>
+      </c>
+      <c r="K236" s="41">
+        <v>3061</v>
+      </c>
+      <c r="L236" s="41" t="s">
+        <v>192</v>
+      </c>
+      <c r="M236" s="40">
+        <v>45877</v>
+      </c>
+      <c r="N236" s="43">
+        <v>1150</v>
+      </c>
+      <c r="O236" s="41" t="s">
+        <v>122</v>
+      </c>
+      <c r="P236" s="41">
+        <v>15</v>
+      </c>
+      <c r="Q236" s="41" t="s">
+        <v>360</v>
+      </c>
+      <c r="R236" s="41">
+        <f>DATEDIF(Tabela1[[#This Row],[Atendimento]],Tabela1[[#This Row],[Previsao de Entrega]],"D")</f>
+        <v>7</v>
+      </c>
+      <c r="S236" s="43">
+        <v>0</v>
+      </c>
+      <c r="T236" s="43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="237" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A237" s="11">
+        <v>45870</v>
+      </c>
+      <c r="B237" s="11">
+        <v>45870</v>
+      </c>
+      <c r="C237" s="11" t="s">
+        <v>128</v>
+      </c>
+      <c r="D237" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="E237" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="F237" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="G237" s="12" t="s">
+        <v>125</v>
+      </c>
+      <c r="H237" s="12" t="s">
+        <v>126</v>
+      </c>
+      <c r="I237" s="13">
+        <f>NETWORKDAYS(B237, A237)</f>
+        <v>1</v>
+      </c>
+      <c r="J237" s="12">
+        <v>66430</v>
+      </c>
+      <c r="K237" s="12">
+        <v>333</v>
+      </c>
+      <c r="L237" s="12" t="s">
+        <v>401</v>
+      </c>
+      <c r="M237" s="11">
+        <v>46113</v>
+      </c>
+      <c r="N237" s="14">
+        <v>281569.34000000003</v>
+      </c>
+      <c r="O237" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="P237" s="12">
+        <v>120</v>
+      </c>
+      <c r="Q237" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="R237" s="12">
+        <f>DATEDIF(Tabela1[[#This Row],[Atendimento]],Tabela1[[#This Row],[Previsao de Entrega]],"D")</f>
+        <v>243</v>
+      </c>
+      <c r="S237" s="14">
+        <v>0</v>
+      </c>
+      <c r="T237" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="238" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A238" s="40">
+        <v>45873</v>
+      </c>
+      <c r="B238" s="40">
+        <v>45873</v>
+      </c>
+      <c r="C238" s="40" t="s">
+        <v>7</v>
+      </c>
+      <c r="D238" s="40" t="s">
+        <v>5</v>
+      </c>
+      <c r="E238" s="40" t="s">
+        <v>113</v>
+      </c>
+      <c r="F238" s="41" t="s">
+        <v>3</v>
+      </c>
+      <c r="G238" s="41" t="s">
+        <v>129</v>
+      </c>
+      <c r="H238" s="41" t="s">
+        <v>130</v>
+      </c>
+      <c r="I238" s="42">
+        <f>NETWORKDAYS(B238, A238)</f>
+        <v>1</v>
+      </c>
+      <c r="J238" s="41">
+        <v>66529</v>
+      </c>
+      <c r="K238" s="41">
+        <v>2856</v>
+      </c>
+      <c r="L238" s="41" t="s">
+        <v>400</v>
+      </c>
+      <c r="M238" s="40">
+        <v>45875</v>
+      </c>
+      <c r="N238" s="43">
+        <v>5600</v>
+      </c>
+      <c r="O238" s="41" t="s">
+        <v>122</v>
+      </c>
+      <c r="P238" s="41">
+        <v>30</v>
+      </c>
+      <c r="Q238" s="41" t="s">
+        <v>360</v>
+      </c>
+      <c r="R238" s="41">
+        <f>DATEDIF(Tabela1[[#This Row],[Atendimento]],Tabela1[[#This Row],[Previsao de Entrega]],"D")</f>
+        <v>2</v>
+      </c>
+      <c r="S238" s="43">
+        <v>0</v>
+      </c>
+      <c r="T238" s="43">
         <v>0</v>
       </c>
     </row>
@@ -17452,7 +17647,7 @@
       </c>
       <c r="E2" s="24">
         <f t="shared" ref="E2:E6" ca="1" si="0">TODAY()</f>
-        <v>45870</v>
+        <v>45873</v>
       </c>
       <c r="F2" s="22" t="str">
         <f ca="1">IF(Tabela4[[#This Row],[Hoje]] &lt;= Tabela4[[#This Row],[Validade]],
@@ -17460,7 +17655,7 @@
       "Negociar",
       "Faltam " &amp; DATEDIF(Tabela4[[#This Row],[Hoje]],Tabela4[[#This Row],[Validade]],"D") &amp; " dias para vencer"),
    "Venceu há " &amp; DATEDIF(Tabela4[[#This Row],[Validade]],Tabela4[[#This Row],[Hoje]],"D") &amp; " dias")</f>
-        <v>Faltam 596 dias para vencer</v>
+        <v>Faltam 593 dias para vencer</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.35">
@@ -17478,7 +17673,7 @@
       </c>
       <c r="E3" s="26">
         <f t="shared" ca="1" si="0"/>
-        <v>45870</v>
+        <v>45873</v>
       </c>
       <c r="F3" s="21" t="str">
         <f ca="1">IF(Tabela4[[#This Row],[Hoje]] &lt;= Tabela4[[#This Row],[Validade]],
@@ -17486,7 +17681,7 @@
       "Negociar",
       "Faltam " &amp; DATEDIF(Tabela4[[#This Row],[Hoje]],Tabela4[[#This Row],[Validade]],"D") &amp; " dias para vencer"),
    "Venceu há " &amp; DATEDIF(Tabela4[[#This Row],[Validade]],Tabela4[[#This Row],[Hoje]],"D") &amp; " dias")</f>
-        <v>Venceu há 304 dias</v>
+        <v>Venceu há 307 dias</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.35">
@@ -17504,7 +17699,7 @@
       </c>
       <c r="E4" s="36">
         <f t="shared" ca="1" si="0"/>
-        <v>45870</v>
+        <v>45873</v>
       </c>
       <c r="F4" s="37" t="str">
         <f ca="1">IF(Tabela4[[#This Row],[Hoje]] &lt;= Tabela4[[#This Row],[Validade]],
@@ -17512,7 +17707,7 @@
       "Negociar",
       "Faltam " &amp; DATEDIF(Tabela4[[#This Row],[Hoje]],Tabela4[[#This Row],[Validade]],"D") &amp; " dias para vencer"),
    "Venceu há " &amp; DATEDIF(Tabela4[[#This Row],[Validade]],Tabela4[[#This Row],[Hoje]],"D") &amp; " dias")</f>
-        <v>Venceu há 12 dias</v>
+        <v>Venceu há 15 dias</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.35">
@@ -17530,7 +17725,7 @@
       </c>
       <c r="E5" s="17">
         <f t="shared" ca="1" si="0"/>
-        <v>45870</v>
+        <v>45873</v>
       </c>
       <c r="F5" s="3" t="str">
         <f ca="1">IF(Tabela4[[#This Row],[Hoje]] &lt;= Tabela4[[#This Row],[Validade]],
@@ -17556,7 +17751,7 @@
       </c>
       <c r="E6" s="17">
         <f t="shared" ca="1" si="0"/>
-        <v>45870</v>
+        <v>45873</v>
       </c>
       <c r="F6" s="3" t="str">
         <f ca="1">IF(Tabela4[[#This Row],[Hoje]] &lt;= Tabela4[[#This Row],[Validade]],
@@ -17582,7 +17777,7 @@
       </c>
       <c r="E7" s="26">
         <f t="shared" ref="E7:E9" ca="1" si="1">TODAY()</f>
-        <v>45870</v>
+        <v>45873</v>
       </c>
       <c r="F7" s="21" t="str">
         <f ca="1">IF(Tabela4[[#This Row],[Hoje]] &lt;= Tabela4[[#This Row],[Validade]],
@@ -17590,7 +17785,7 @@
       "Negociar",
       "Faltam " &amp; DATEDIF(Tabela4[[#This Row],[Hoje]],Tabela4[[#This Row],[Validade]],"D") &amp; " dias para vencer"),
    "Venceu há " &amp; DATEDIF(Tabela4[[#This Row],[Validade]],Tabela4[[#This Row],[Hoje]],"D") &amp; " dias")</f>
-        <v>Venceu há 136 dias</v>
+        <v>Venceu há 139 dias</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.35">
@@ -17608,7 +17803,7 @@
       </c>
       <c r="E8" s="26">
         <f t="shared" ca="1" si="1"/>
-        <v>45870</v>
+        <v>45873</v>
       </c>
       <c r="F8" s="21" t="str">
         <f ca="1">IF(Tabela4[[#This Row],[Hoje]] &lt;= Tabela4[[#This Row],[Validade]],
@@ -17616,7 +17811,7 @@
       "Negociar",
       "Faltam " &amp; DATEDIF(Tabela4[[#This Row],[Hoje]],Tabela4[[#This Row],[Validade]],"D") &amp; " dias para vencer"),
    "Venceu há " &amp; DATEDIF(Tabela4[[#This Row],[Validade]],Tabela4[[#This Row],[Hoje]],"D") &amp; " dias")</f>
-        <v>Venceu há 879 dias</v>
+        <v>Venceu há 882 dias</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.35">
@@ -17634,7 +17829,7 @@
       </c>
       <c r="E9" s="24">
         <f t="shared" ca="1" si="1"/>
-        <v>45870</v>
+        <v>45873</v>
       </c>
       <c r="F9" s="22" t="str">
         <f ca="1">IF(Tabela4[[#This Row],[Hoje]] &lt;= Tabela4[[#This Row],[Validade]],
@@ -17642,7 +17837,7 @@
       "Negociar",
       "Faltam " &amp; DATEDIF(Tabela4[[#This Row],[Hoje]],Tabela4[[#This Row],[Validade]],"D") &amp; " dias para vencer"),
    "Venceu há " &amp; DATEDIF(Tabela4[[#This Row],[Validade]],Tabela4[[#This Row],[Hoje]],"D") &amp; " dias")</f>
-        <v>Faltam 412 dias para vencer</v>
+        <v>Faltam 409 dias para vencer</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.35">
@@ -17660,7 +17855,7 @@
       </c>
       <c r="E10" s="24">
         <f ca="1">TODAY()</f>
-        <v>45870</v>
+        <v>45873</v>
       </c>
       <c r="F10" s="22" t="str">
         <f ca="1">IF(Tabela4[[#This Row],[Hoje]] &lt;= Tabela4[[#This Row],[Validade]],
@@ -17668,7 +17863,7 @@
       "Negociar",
       "Faltam " &amp; DATEDIF(Tabela4[[#This Row],[Hoje]],Tabela4[[#This Row],[Validade]],"D") &amp; " dias para vencer"),
    "Venceu há " &amp; DATEDIF(Tabela4[[#This Row],[Validade]],Tabela4[[#This Row],[Hoje]],"D") &amp; " dias")</f>
-        <v>Faltam 333 dias para vencer</v>
+        <v>Faltam 330 dias para vencer</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.35">
@@ -17686,7 +17881,7 @@
       </c>
       <c r="E11" s="24">
         <f ca="1">TODAY()</f>
-        <v>45870</v>
+        <v>45873</v>
       </c>
       <c r="F11" s="22" t="str">
         <f ca="1">IF(Tabela4[[#This Row],[Hoje]] &lt;= Tabela4[[#This Row],[Validade]],
@@ -17694,7 +17889,7 @@
       "Negociar",
       "Faltam " &amp; DATEDIF(Tabela4[[#This Row],[Hoje]],Tabela4[[#This Row],[Validade]],"D") &amp; " dias para vencer"),
    "Venceu há " &amp; DATEDIF(Tabela4[[#This Row],[Validade]],Tabela4[[#This Row],[Hoje]],"D") &amp; " dias")</f>
-        <v>Faltam 122 dias para vencer</v>
+        <v>Faltam 119 dias para vencer</v>
       </c>
     </row>
   </sheetData>
@@ -19119,15 +19314,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010068C9492B0923CC418696A025D9B79530" ma:contentTypeVersion="1" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="12b5152450087b045156d8e5bdb7ac17">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="b7545978-8353-4157-ab02-92f5c69a97d9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="74a8823586b7fc5940aaf3e9d5b706e7" ns3:_="">
     <xsd:import namespace="b7545978-8353-4157-ab02-92f5c69a97d9"/>
@@ -19253,6 +19439,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -19260,14 +19455,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F1DB20CA-6C9E-462A-9B1E-209C1B3156BD}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AED76536-08DB-4BCA-BAA6-597FC860B20C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -19281,6 +19468,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F1DB20CA-6C9E-462A-9B1E-209C1B3156BD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Atualização de Base 05-08
</commit_message>
<xml_diff>
--- a/Atendimento.xlsx
+++ b/Atendimento.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\PUBLICO\Compras\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A4553A7-8913-4AF3-B286-526CE3ADE6EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75669927-1480-4851-BC31-81B9B26C398C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -47,7 +47,7 @@
     <author>Filho, Glaudoberto</author>
   </authors>
   <commentList>
-    <comment ref="T218" authorId="0" shapeId="0" xr:uid="{6F0B1F1F-8317-47FC-8965-8B65A4B64726}">
+    <comment ref="T181" authorId="0" shapeId="0" xr:uid="{6F0B1F1F-8317-47FC-8965-8B65A4B64726}">
       <text>
         <r>
           <rPr>
@@ -76,7 +76,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2393" uniqueCount="402">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2469" uniqueCount="405">
   <si>
     <t>SC</t>
   </si>
@@ -1282,6 +1282,15 @@
   </si>
   <si>
     <t>CADSERVICE PRODUTOS ELETRONICOS LTDA</t>
+  </si>
+  <si>
+    <t>CARBOROIL COMERCIO DE DERIVADOS DE PETROLEO LTDA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">INDUSTRIA E COMERCIO DE MOLAS CASA VERDE LTDA </t>
+  </si>
+  <si>
+    <t>INDUSTRIA E COMERCIO DE MOLAS CASA VERDE LTDA</t>
   </si>
 </sst>
 </file>
@@ -1738,8 +1747,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0C573FEE-B8A0-4FE7-911C-81B026DE4530}" name="Tabela1" displayName="Tabela1" ref="A1:T238" totalsRowShown="0" headerRowDxfId="36" dataDxfId="35">
-  <autoFilter ref="A1:T238" xr:uid="{0C573FEE-B8A0-4FE7-911C-81B026DE4530}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0C573FEE-B8A0-4FE7-911C-81B026DE4530}" name="Tabela1" displayName="Tabela1" ref="A1:T246" totalsRowShown="0" headerRowDxfId="36" dataDxfId="35">
+  <autoFilter ref="A1:T246" xr:uid="{0C573FEE-B8A0-4FE7-911C-81B026DE4530}">
     <filterColumn colId="16">
       <filters>
         <filter val="AGUARDANDO APROVAÇÃO"/>
@@ -1747,8 +1756,8 @@
       </filters>
     </filterColumn>
   </autoFilter>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A11:T238">
-    <sortCondition ref="A1:A238"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A11:T246">
+    <sortCondition ref="M1:M246"/>
   </sortState>
   <tableColumns count="20">
     <tableColumn id="1" xr3:uid="{FD977268-8F92-4E92-82D7-959136F54294}" name="Atendimento" dataDxfId="34"/>
@@ -1837,8 +1846,8 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{BB230BD9-36EF-4D37-BEB8-0438680DF5A9}" name="Tabela6" displayName="Tabela6" ref="A1:E36" totalsRowShown="0">
-  <autoFilter ref="A1:E36" xr:uid="{BB230BD9-36EF-4D37-BEB8-0438680DF5A9}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{BB230BD9-36EF-4D37-BEB8-0438680DF5A9}" name="Tabela6" displayName="Tabela6" ref="A1:E38" totalsRowShown="0">
+  <autoFilter ref="A1:E38" xr:uid="{BB230BD9-36EF-4D37-BEB8-0438680DF5A9}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{40ADAE7E-AD00-4188-9DB3-F04A606A9D2B}" name="data"/>
     <tableColumn id="2" xr3:uid="{D9B738D8-98DD-4AD6-8BCF-D51CBE71FF94}" name="solicitante"/>
@@ -2113,10 +2122,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T238"/>
+  <dimension ref="A1:T246"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L181" sqref="L181"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L204" sqref="L204"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2784,63 +2793,63 @@
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A11" s="11">
-        <v>45785</v>
+        <v>45848</v>
       </c>
       <c r="B11" s="11">
-        <v>45784</v>
+        <v>45848</v>
       </c>
       <c r="C11" s="11" t="s">
         <v>7</v>
       </c>
       <c r="D11" s="11" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="E11" s="11" t="s">
         <v>113</v>
       </c>
       <c r="F11" s="12">
-        <v>68369</v>
+        <v>68459</v>
       </c>
       <c r="G11" s="12" t="s">
-        <v>39</v>
+        <v>364</v>
       </c>
       <c r="H11" s="12" t="s">
-        <v>98</v>
+        <v>365</v>
       </c>
       <c r="I11" s="13">
         <f>NETWORKDAYS(B11, A11)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J11" s="12">
-        <v>65234</v>
+        <v>66162</v>
       </c>
       <c r="K11" s="12">
-        <v>11610</v>
+        <v>11781</v>
       </c>
       <c r="L11" s="12" t="s">
-        <v>38</v>
+        <v>366</v>
       </c>
       <c r="M11" s="11">
-        <v>45881</v>
+        <v>45855</v>
       </c>
       <c r="N11" s="14">
-        <v>9114.5499999999993</v>
+        <v>5396.77</v>
       </c>
       <c r="O11" s="12" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="P11" s="12">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="Q11" s="12" t="s">
         <v>24</v>
       </c>
       <c r="R11" s="12">
         <f>DATEDIF(Tabela1[[#This Row],[Atendimento]],Tabela1[[#This Row],[Previsao de Entrega]],"D")</f>
-        <v>96</v>
+        <v>7</v>
       </c>
       <c r="S11" s="14">
-        <v>183.5</v>
+        <v>284.04000000000002</v>
       </c>
       <c r="T11" s="14">
         <v>0</v>
@@ -5599,66 +5608,66 @@
       </c>
     </row>
     <row r="55" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A55" s="31">
-        <v>45798</v>
-      </c>
-      <c r="B55" s="31">
-        <v>45786</v>
-      </c>
-      <c r="C55" s="31" t="s">
-        <v>7</v>
-      </c>
-      <c r="D55" s="31" t="s">
+      <c r="A55" s="11">
+        <v>45831</v>
+      </c>
+      <c r="B55" s="11">
+        <v>45824</v>
+      </c>
+      <c r="C55" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D55" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="E55" s="31" t="s">
+      <c r="E55" s="11" t="s">
         <v>124</v>
       </c>
-      <c r="F55" s="32">
-        <v>68378</v>
-      </c>
-      <c r="G55" s="32" t="s">
+      <c r="F55" s="12">
+        <v>68439</v>
+      </c>
+      <c r="G55" s="12" t="s">
         <v>125</v>
       </c>
-      <c r="H55" s="32" t="s">
+      <c r="H55" s="12" t="s">
         <v>126</v>
       </c>
-      <c r="I55" s="27">
+      <c r="I55" s="13">
         <f>NETWORKDAYS(B55, A55)</f>
-        <v>9</v>
-      </c>
-      <c r="J55" s="32">
-        <v>65472</v>
-      </c>
-      <c r="K55" s="32">
+        <v>6</v>
+      </c>
+      <c r="J55" s="12">
+        <v>65915</v>
+      </c>
+      <c r="K55" s="12">
         <v>2201</v>
       </c>
-      <c r="L55" s="32" t="s">
+      <c r="L55" s="12" t="s">
         <v>203</v>
       </c>
-      <c r="M55" s="31">
-        <v>45869</v>
-      </c>
-      <c r="N55" s="33">
-        <v>26920</v>
-      </c>
-      <c r="O55" s="32" t="s">
+      <c r="M55" s="11">
+        <v>45861</v>
+      </c>
+      <c r="N55" s="14">
+        <v>1401.04</v>
+      </c>
+      <c r="O55" s="12" t="s">
         <v>122</v>
       </c>
-      <c r="P55" s="32">
-        <v>28</v>
-      </c>
-      <c r="Q55" s="32" t="s">
+      <c r="P55" s="12">
+        <v>120</v>
+      </c>
+      <c r="Q55" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="R55" s="32">
-        <f>DATEDIF(Tabela1[[#This Row],[Atendimento]],Tabela1[[#This Row],[Previsao de Entrega]],"D")</f>
-        <v>71</v>
-      </c>
-      <c r="S55" s="33">
-        <v>0</v>
-      </c>
-      <c r="T55" s="33">
+      <c r="R55" s="12">
+        <f>DATEDIF(Tabela1[[#This Row],[Atendimento]],Tabela1[[#This Row],[Previsao de Entrega]],"D")</f>
+        <v>30</v>
+      </c>
+      <c r="S55" s="14">
+        <v>0</v>
+      </c>
+      <c r="T55" s="14">
         <v>0</v>
       </c>
     </row>
@@ -9054,131 +9063,131 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A109" s="40">
+    <row r="109" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A109" s="6">
         <v>45818</v>
       </c>
-      <c r="B109" s="40">
+      <c r="B109" s="6">
         <v>45811</v>
       </c>
-      <c r="C109" s="40" t="s">
-        <v>7</v>
-      </c>
-      <c r="D109" s="40" t="s">
+      <c r="C109" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D109" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="E109" s="40" t="s">
+      <c r="E109" s="6" t="s">
         <v>113</v>
       </c>
-      <c r="F109" s="41">
+      <c r="F109" s="7">
         <v>68329</v>
       </c>
-      <c r="G109" s="41" t="s">
+      <c r="G109" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="H109" s="41" t="s">
+      <c r="H109" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="I109" s="42">
+      <c r="I109" s="10">
         <f>NETWORKDAYS(B109, A109)</f>
         <v>6</v>
       </c>
-      <c r="J109" s="41">
+      <c r="J109" s="7">
         <v>66494</v>
       </c>
-      <c r="K109" s="41">
+      <c r="K109" s="7">
         <v>224</v>
       </c>
-      <c r="L109" s="41" t="s">
+      <c r="L109" s="7" t="s">
         <v>295</v>
       </c>
-      <c r="M109" s="40">
+      <c r="M109" s="6">
         <v>45869</v>
       </c>
-      <c r="N109" s="43">
-        <v>7774.51</v>
-      </c>
-      <c r="O109" s="41" t="s">
+      <c r="N109" s="8">
+        <v>6586.89</v>
+      </c>
+      <c r="O109" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="P109" s="41">
-        <v>0</v>
-      </c>
-      <c r="Q109" s="41" t="s">
-        <v>360</v>
-      </c>
-      <c r="R109" s="41">
+      <c r="P109" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q109" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="R109" s="7">
         <f>DATEDIF(Tabela1[[#This Row],[Atendimento]],Tabela1[[#This Row],[Previsao de Entrega]],"D")</f>
         <v>51</v>
       </c>
-      <c r="S109" s="43">
-        <v>0</v>
-      </c>
-      <c r="T109" s="43">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="110" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A110" s="11">
-        <v>45818</v>
-      </c>
-      <c r="B110" s="11">
-        <v>45813</v>
-      </c>
-      <c r="C110" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="D110" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="E110" s="11" t="s">
-        <v>124</v>
-      </c>
-      <c r="F110" s="12">
-        <v>68422</v>
-      </c>
-      <c r="G110" s="12" t="s">
-        <v>90</v>
-      </c>
-      <c r="H110" s="12" t="s">
-        <v>91</v>
-      </c>
-      <c r="I110" s="13">
+      <c r="S109" s="8">
+        <v>0</v>
+      </c>
+      <c r="T109" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A110" s="6">
+        <v>45866</v>
+      </c>
+      <c r="B110" s="6">
+        <v>45863</v>
+      </c>
+      <c r="C110" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D110" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E110" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="F110" s="7">
+        <v>68481</v>
+      </c>
+      <c r="G110" s="7" t="s">
+        <v>372</v>
+      </c>
+      <c r="H110" s="7" t="s">
+        <v>373</v>
+      </c>
+      <c r="I110" s="10">
         <f>NETWORKDAYS(B110, A110)</f>
-        <v>4</v>
-      </c>
-      <c r="J110" s="12">
-        <v>65725</v>
-      </c>
-      <c r="K110" s="12">
-        <v>1450</v>
-      </c>
-      <c r="L110" s="12" t="s">
-        <v>229</v>
-      </c>
-      <c r="M110" s="11">
-        <v>45877</v>
-      </c>
-      <c r="N110" s="14">
-        <v>239.63</v>
-      </c>
-      <c r="O110" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="J110" s="7">
+        <v>66462</v>
+      </c>
+      <c r="K110" s="7">
+        <v>10535</v>
+      </c>
+      <c r="L110" s="7" t="s">
+        <v>391</v>
+      </c>
+      <c r="M110" s="6">
+        <v>45868</v>
+      </c>
+      <c r="N110" s="8">
+        <v>300</v>
+      </c>
+      <c r="O110" s="7" t="s">
         <v>122</v>
       </c>
-      <c r="P110" s="12">
-        <v>120</v>
-      </c>
-      <c r="Q110" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="R110" s="12">
-        <f>DATEDIF(Tabela1[[#This Row],[Atendimento]],Tabela1[[#This Row],[Previsao de Entrega]],"D")</f>
-        <v>59</v>
-      </c>
-      <c r="S110" s="14">
-        <v>0</v>
-      </c>
-      <c r="T110" s="14">
+      <c r="P110" s="7">
+        <v>14</v>
+      </c>
+      <c r="Q110" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="R110" s="7">
+        <f>DATEDIF(Tabela1[[#This Row],[Atendimento]],Tabela1[[#This Row],[Previsao de Entrega]],"D")</f>
+        <v>2</v>
+      </c>
+      <c r="S110" s="8">
+        <v>0</v>
+      </c>
+      <c r="T110" s="8">
         <v>0</v>
       </c>
     </row>
@@ -9246,67 +9255,67 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A112" s="11">
+    <row r="112" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A112" s="6">
         <v>45826</v>
       </c>
-      <c r="B112" s="11">
+      <c r="B112" s="6">
         <v>45789</v>
       </c>
-      <c r="C112" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="D112" s="11" t="s">
+      <c r="C112" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D112" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="E112" s="11" t="s">
+      <c r="E112" s="6" t="s">
         <v>124</v>
       </c>
-      <c r="F112" s="12">
+      <c r="F112" s="7">
         <v>68384</v>
       </c>
-      <c r="G112" s="12" t="s">
+      <c r="G112" s="7" t="s">
         <v>125</v>
       </c>
-      <c r="H112" s="12" t="s">
+      <c r="H112" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="I112" s="13">
+      <c r="I112" s="10">
         <f>NETWORKDAYS(B112, A112)</f>
         <v>28</v>
       </c>
-      <c r="J112" s="12">
+      <c r="J112" s="7">
         <v>65867</v>
       </c>
-      <c r="K112" s="12">
+      <c r="K112" s="7">
         <v>1463</v>
       </c>
-      <c r="L112" s="12" t="s">
+      <c r="L112" s="7" t="s">
         <v>317</v>
       </c>
-      <c r="M112" s="11">
+      <c r="M112" s="6">
         <v>45874</v>
       </c>
-      <c r="N112" s="14">
+      <c r="N112" s="8">
         <v>4215.5</v>
       </c>
-      <c r="O112" s="12" t="s">
+      <c r="O112" s="7" t="s">
         <v>122</v>
       </c>
-      <c r="P112" s="12">
+      <c r="P112" s="7">
         <v>28</v>
       </c>
-      <c r="Q112" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="R112" s="12">
+      <c r="Q112" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="R112" s="7">
         <f>DATEDIF(Tabela1[[#This Row],[Atendimento]],Tabela1[[#This Row],[Previsao de Entrega]],"D")</f>
         <v>48</v>
       </c>
-      <c r="S112" s="14">
-        <v>0</v>
-      </c>
-      <c r="T112" s="14">
+      <c r="S112" s="8">
+        <v>0</v>
+      </c>
+      <c r="T112" s="8">
         <v>0</v>
       </c>
     </row>
@@ -10463,87 +10472,87 @@
       </c>
     </row>
     <row r="131" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A131" s="49">
-        <v>45826</v>
-      </c>
-      <c r="B131" s="49">
-        <v>45826</v>
-      </c>
-      <c r="C131" s="49" t="s">
-        <v>7</v>
-      </c>
-      <c r="D131" s="49" t="s">
+      <c r="A131" s="31">
+        <v>45798</v>
+      </c>
+      <c r="B131" s="31">
+        <v>45786</v>
+      </c>
+      <c r="C131" s="31" t="s">
+        <v>7</v>
+      </c>
+      <c r="D131" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="E131" s="49" t="s">
+      <c r="E131" s="31" t="s">
         <v>124</v>
       </c>
-      <c r="F131" s="50" t="s">
-        <v>3</v>
-      </c>
-      <c r="G131" s="50" t="s">
+      <c r="F131" s="32">
+        <v>68378</v>
+      </c>
+      <c r="G131" s="32" t="s">
         <v>125</v>
       </c>
-      <c r="H131" s="50" t="s">
+      <c r="H131" s="32" t="s">
         <v>126</v>
       </c>
-      <c r="I131" s="51">
+      <c r="I131" s="27">
         <f>NETWORKDAYS(B131, A131)</f>
-        <v>1</v>
-      </c>
-      <c r="J131" s="50">
-        <v>66341</v>
-      </c>
-      <c r="K131" s="50">
-        <v>11758</v>
-      </c>
-      <c r="L131" s="50" t="s">
-        <v>316</v>
-      </c>
-      <c r="M131" s="49">
-        <v>45880</v>
-      </c>
-      <c r="N131" s="52">
-        <v>924.61</v>
-      </c>
-      <c r="O131" s="50" t="s">
+        <v>9</v>
+      </c>
+      <c r="J131" s="32">
+        <v>65472</v>
+      </c>
+      <c r="K131" s="32">
+        <v>2201</v>
+      </c>
+      <c r="L131" s="32" t="s">
+        <v>203</v>
+      </c>
+      <c r="M131" s="31">
+        <v>45869</v>
+      </c>
+      <c r="N131" s="33">
+        <v>26920</v>
+      </c>
+      <c r="O131" s="32" t="s">
         <v>122</v>
       </c>
-      <c r="P131" s="50">
+      <c r="P131" s="32">
         <v>28</v>
       </c>
-      <c r="Q131" s="50" t="s">
+      <c r="Q131" s="32" t="s">
         <v>24</v>
       </c>
-      <c r="R131" s="50">
-        <f>DATEDIF(Tabela1[[#This Row],[Atendimento]],Tabela1[[#This Row],[Previsao de Entrega]],"D")</f>
-        <v>54</v>
-      </c>
-      <c r="S131" s="52">
-        <v>0</v>
-      </c>
-      <c r="T131" s="52">
+      <c r="R131" s="32">
+        <f>DATEDIF(Tabela1[[#This Row],[Atendimento]],Tabela1[[#This Row],[Previsao de Entrega]],"D")</f>
+        <v>71</v>
+      </c>
+      <c r="S131" s="33">
+        <v>0</v>
+      </c>
+      <c r="T131" s="33">
         <v>0</v>
       </c>
     </row>
     <row r="132" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A132" s="11">
-        <v>45831</v>
+        <v>45855</v>
       </c>
       <c r="B132" s="11">
-        <v>45824</v>
+        <v>45855</v>
       </c>
       <c r="C132" s="11" t="s">
         <v>7</v>
       </c>
       <c r="D132" s="11" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="E132" s="11" t="s">
-        <v>124</v>
-      </c>
-      <c r="F132" s="12">
-        <v>68439</v>
+        <v>142</v>
+      </c>
+      <c r="F132" s="12" t="s">
+        <v>3</v>
       </c>
       <c r="G132" s="12" t="s">
         <v>125</v>
@@ -10553,38 +10562,38 @@
       </c>
       <c r="I132" s="13">
         <f>NETWORKDAYS(B132, A132)</f>
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="J132" s="12">
-        <v>65915</v>
+        <v>66308</v>
       </c>
       <c r="K132" s="12">
-        <v>2201</v>
+        <v>11757</v>
       </c>
       <c r="L132" s="12" t="s">
-        <v>203</v>
+        <v>305</v>
       </c>
       <c r="M132" s="11">
-        <v>45861</v>
+        <v>45873</v>
       </c>
       <c r="N132" s="14">
-        <v>1401.04</v>
+        <v>1428.29</v>
       </c>
       <c r="O132" s="12" t="s">
         <v>122</v>
       </c>
       <c r="P132" s="12">
-        <v>120</v>
+        <v>28</v>
       </c>
       <c r="Q132" s="12" t="s">
         <v>24</v>
       </c>
       <c r="R132" s="12">
         <f>DATEDIF(Tabela1[[#This Row],[Atendimento]],Tabela1[[#This Row],[Previsao de Entrega]],"D")</f>
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="S132" s="14">
-        <v>0</v>
+        <v>320</v>
       </c>
       <c r="T132" s="14">
         <v>0</v>
@@ -10846,67 +10855,67 @@
         <v>0</v>
       </c>
     </row>
-    <row r="137" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A137" s="11">
-        <v>45839</v>
-      </c>
-      <c r="B137" s="11">
-        <v>45824</v>
-      </c>
-      <c r="C137" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="D137" s="11" t="s">
+    <row r="137" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A137" s="6">
+        <v>45873</v>
+      </c>
+      <c r="B137" s="6">
+        <v>45873</v>
+      </c>
+      <c r="C137" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D137" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="E137" s="11" t="s">
-        <v>124</v>
-      </c>
-      <c r="F137" s="12">
-        <v>68438</v>
-      </c>
-      <c r="G137" s="12" t="s">
-        <v>125</v>
-      </c>
-      <c r="H137" s="12" t="s">
-        <v>126</v>
-      </c>
-      <c r="I137" s="13">
+      <c r="E137" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="F137" s="7">
+        <v>68494</v>
+      </c>
+      <c r="G137" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="H137" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="I137" s="10">
         <f>NETWORKDAYS(B137, A137)</f>
-        <v>12</v>
-      </c>
-      <c r="J137" s="12">
-        <v>66025</v>
-      </c>
-      <c r="K137" s="12">
-        <v>3034</v>
-      </c>
-      <c r="L137" s="12" t="s">
-        <v>349</v>
-      </c>
-      <c r="M137" s="11">
-        <v>45870</v>
-      </c>
-      <c r="N137" s="14">
-        <v>2087</v>
-      </c>
-      <c r="O137" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="J137" s="7">
+        <v>66534</v>
+      </c>
+      <c r="K137" s="7">
+        <v>11790</v>
+      </c>
+      <c r="L137" s="7" t="s">
+        <v>402</v>
+      </c>
+      <c r="M137" s="6">
+        <v>45873</v>
+      </c>
+      <c r="N137" s="8">
+        <v>1475</v>
+      </c>
+      <c r="O137" s="7" t="s">
         <v>122</v>
       </c>
-      <c r="P137" s="12">
-        <v>90</v>
-      </c>
-      <c r="Q137" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="R137" s="12">
-        <f>DATEDIF(Tabela1[[#This Row],[Atendimento]],Tabela1[[#This Row],[Previsao de Entrega]],"D")</f>
-        <v>31</v>
-      </c>
-      <c r="S137" s="14">
-        <v>0</v>
-      </c>
-      <c r="T137" s="14">
+      <c r="P137" s="7">
+        <v>15</v>
+      </c>
+      <c r="Q137" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="R137" s="7">
+        <f>DATEDIF(Tabela1[[#This Row],[Atendimento]],Tabela1[[#This Row],[Previsao de Entrega]],"D")</f>
+        <v>0</v>
+      </c>
+      <c r="S137" s="8">
+        <v>204</v>
+      </c>
+      <c r="T137" s="8">
         <v>0</v>
       </c>
     </row>
@@ -13024,60 +13033,60 @@
     </row>
     <row r="171" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A171" s="11">
-        <v>45840</v>
+        <v>45839</v>
       </c>
       <c r="B171" s="11">
-        <v>45840</v>
+        <v>45824</v>
       </c>
       <c r="C171" s="11" t="s">
         <v>7</v>
       </c>
       <c r="D171" s="11" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="E171" s="11" t="s">
-        <v>113</v>
+        <v>124</v>
       </c>
       <c r="F171" s="12">
-        <v>68452</v>
+        <v>68438</v>
       </c>
       <c r="G171" s="12" t="s">
-        <v>33</v>
+        <v>125</v>
       </c>
       <c r="H171" s="12" t="s">
-        <v>34</v>
+        <v>126</v>
       </c>
       <c r="I171" s="13">
         <f>NETWORKDAYS(B171, A171)</f>
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="J171" s="12">
-        <v>66037</v>
+        <v>66025</v>
       </c>
       <c r="K171" s="12">
-        <v>11775</v>
+        <v>3034</v>
       </c>
       <c r="L171" s="12" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="M171" s="11">
         <v>45874</v>
       </c>
       <c r="N171" s="14">
-        <v>1750</v>
+        <v>2087</v>
       </c>
       <c r="O171" s="12" t="s">
         <v>122</v>
       </c>
       <c r="P171" s="12">
-        <v>30</v>
+        <v>90</v>
       </c>
       <c r="Q171" s="12" t="s">
         <v>24</v>
       </c>
       <c r="R171" s="12">
         <f>DATEDIF(Tabela1[[#This Row],[Atendimento]],Tabela1[[#This Row],[Previsao de Entrega]],"D")</f>
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="S171" s="14">
         <v>0</v>
@@ -13152,60 +13161,60 @@
     </row>
     <row r="173" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A173" s="11">
-        <v>45846</v>
+        <v>45868</v>
       </c>
       <c r="B173" s="11">
-        <v>45846</v>
+        <v>45868</v>
       </c>
       <c r="C173" s="11" t="s">
-        <v>7</v>
+        <v>128</v>
       </c>
       <c r="D173" s="11" t="s">
         <v>5</v>
       </c>
       <c r="E173" s="11" t="s">
-        <v>113</v>
+        <v>395</v>
       </c>
       <c r="F173" s="12">
-        <v>68461</v>
+        <v>68487</v>
       </c>
       <c r="G173" s="12" t="s">
-        <v>227</v>
+        <v>396</v>
       </c>
       <c r="H173" s="12" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="I173" s="13">
         <f>NETWORKDAYS(B173, A173)</f>
         <v>1</v>
       </c>
       <c r="J173" s="12">
-        <v>66119</v>
+        <v>66489</v>
       </c>
       <c r="K173" s="12">
-        <v>10677</v>
+        <v>11614</v>
       </c>
       <c r="L173" s="12" t="s">
-        <v>362</v>
+        <v>397</v>
       </c>
       <c r="M173" s="11">
         <v>45874</v>
       </c>
       <c r="N173" s="14">
-        <v>2800</v>
+        <v>6633</v>
       </c>
       <c r="O173" s="12" t="s">
         <v>121</v>
       </c>
       <c r="P173" s="12">
-        <v>30</v>
+        <v>1</v>
       </c>
       <c r="Q173" s="12" t="s">
         <v>24</v>
       </c>
       <c r="R173" s="12">
         <f>DATEDIF(Tabela1[[#This Row],[Atendimento]],Tabela1[[#This Row],[Previsao de Entrega]],"D")</f>
-        <v>28</v>
+        <v>6</v>
       </c>
       <c r="S173" s="14">
         <v>0</v>
@@ -13637,7 +13646,7 @@
         <v>361</v>
       </c>
       <c r="M180" s="11">
-        <v>45877</v>
+        <v>45875</v>
       </c>
       <c r="N180" s="14">
         <v>607.57000000000005</v>
@@ -13653,7 +13662,7 @@
       </c>
       <c r="R180" s="12">
         <f>DATEDIF(Tabela1[[#This Row],[Atendimento]],Tabela1[[#This Row],[Previsao de Entrega]],"D")</f>
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="S180" s="14">
         <v>0</v>
@@ -13664,10 +13673,10 @@
     </row>
     <row r="181" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A181" s="11">
-        <v>45848</v>
+        <v>45861</v>
       </c>
       <c r="B181" s="11">
-        <v>45848</v>
+        <v>45861</v>
       </c>
       <c r="C181" s="11" t="s">
         <v>7</v>
@@ -13676,54 +13685,54 @@
         <v>15</v>
       </c>
       <c r="E181" s="11" t="s">
-        <v>113</v>
-      </c>
-      <c r="F181" s="12">
-        <v>68459</v>
+        <v>124</v>
+      </c>
+      <c r="F181" s="12" t="s">
+        <v>3</v>
       </c>
       <c r="G181" s="12" t="s">
-        <v>364</v>
+        <v>125</v>
       </c>
       <c r="H181" s="12" t="s">
-        <v>365</v>
+        <v>126</v>
       </c>
       <c r="I181" s="13">
         <f>NETWORKDAYS(B181, A181)</f>
         <v>1</v>
       </c>
       <c r="J181" s="12">
-        <v>66162</v>
+        <v>66301</v>
       </c>
       <c r="K181" s="12">
-        <v>11781</v>
+        <v>1522</v>
       </c>
       <c r="L181" s="12" t="s">
-        <v>366</v>
+        <v>388</v>
       </c>
       <c r="M181" s="11">
-        <v>45855</v>
+        <v>45875</v>
       </c>
       <c r="N181" s="14">
-        <v>5396.77</v>
+        <v>1023.45</v>
       </c>
       <c r="O181" s="12" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="P181" s="12">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="Q181" s="12" t="s">
         <v>24</v>
       </c>
       <c r="R181" s="12">
         <f>DATEDIF(Tabela1[[#This Row],[Atendimento]],Tabela1[[#This Row],[Previsao de Entrega]],"D")</f>
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="S181" s="14">
-        <v>284.04000000000002</v>
+        <v>0</v>
       </c>
       <c r="T181" s="14">
-        <v>0</v>
+        <v>141.4</v>
       </c>
     </row>
     <row r="182" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
@@ -13792,10 +13801,10 @@
     </row>
     <row r="183" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A183" s="11">
-        <v>45848</v>
+        <v>45868</v>
       </c>
       <c r="B183" s="11">
-        <v>45848</v>
+        <v>45862</v>
       </c>
       <c r="C183" s="11" t="s">
         <v>7</v>
@@ -13807,48 +13816,48 @@
         <v>113</v>
       </c>
       <c r="F183" s="12">
-        <v>68457</v>
+        <v>68476</v>
       </c>
       <c r="G183" s="12" t="s">
-        <v>33</v>
+        <v>227</v>
       </c>
       <c r="H183" s="12" t="s">
-        <v>34</v>
+        <v>98</v>
       </c>
       <c r="I183" s="13">
         <f>NETWORKDAYS(B183, A183)</f>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="J183" s="12">
-        <v>66126</v>
+        <v>66491</v>
       </c>
       <c r="K183" s="12">
-        <v>2931</v>
+        <v>11522</v>
       </c>
       <c r="L183" s="12" t="s">
-        <v>367</v>
+        <v>377</v>
       </c>
       <c r="M183" s="11">
-        <v>45879</v>
+        <v>45875</v>
       </c>
       <c r="N183" s="14">
-        <v>3500</v>
+        <v>398.42</v>
       </c>
       <c r="O183" s="12" t="s">
         <v>122</v>
       </c>
       <c r="P183" s="12">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="Q183" s="12" t="s">
         <v>24</v>
       </c>
       <c r="R183" s="12">
         <f>DATEDIF(Tabela1[[#This Row],[Atendimento]],Tabela1[[#This Row],[Previsao de Entrega]],"D")</f>
-        <v>31</v>
+        <v>7</v>
       </c>
       <c r="S183" s="14">
-        <v>320</v>
+        <v>0</v>
       </c>
       <c r="T183" s="14">
         <v>0</v>
@@ -15135,130 +15144,130 @@
       </c>
     </row>
     <row r="204" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A204" s="11">
-        <v>45849</v>
-      </c>
-      <c r="B204" s="11">
-        <v>45849</v>
-      </c>
-      <c r="C204" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="D204" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="E204" s="11" t="s">
+      <c r="A204" s="40">
+        <v>45874</v>
+      </c>
+      <c r="B204" s="40">
+        <v>45874</v>
+      </c>
+      <c r="C204" s="40" t="s">
+        <v>7</v>
+      </c>
+      <c r="D204" s="40" t="s">
+        <v>15</v>
+      </c>
+      <c r="E204" s="40" t="s">
         <v>113</v>
       </c>
-      <c r="F204" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="G204" s="12" t="s">
-        <v>372</v>
-      </c>
-      <c r="H204" s="12" t="s">
-        <v>373</v>
-      </c>
-      <c r="I204" s="13">
+      <c r="F204" s="41" t="s">
+        <v>3</v>
+      </c>
+      <c r="G204" s="41" t="s">
+        <v>136</v>
+      </c>
+      <c r="H204" s="41" t="s">
+        <v>126</v>
+      </c>
+      <c r="I204" s="42">
         <f>NETWORKDAYS(B204, A204)</f>
         <v>1</v>
       </c>
-      <c r="J204" s="12">
-        <v>66166</v>
-      </c>
-      <c r="K204" s="12">
-        <v>11782</v>
-      </c>
-      <c r="L204" s="12" t="s">
-        <v>371</v>
-      </c>
-      <c r="M204" s="11">
-        <v>45880</v>
-      </c>
-      <c r="N204" s="14">
-        <v>2250</v>
-      </c>
-      <c r="O204" s="12" t="s">
-        <v>121</v>
-      </c>
-      <c r="P204" s="12">
-        <v>30</v>
-      </c>
-      <c r="Q204" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="R204" s="12">
-        <f>DATEDIF(Tabela1[[#This Row],[Atendimento]],Tabela1[[#This Row],[Previsao de Entrega]],"D")</f>
-        <v>31</v>
-      </c>
-      <c r="S204" s="14">
-        <v>250</v>
-      </c>
-      <c r="T204" s="14">
+      <c r="J204" s="41">
+        <v>66561</v>
+      </c>
+      <c r="K204" s="41">
+        <v>2785</v>
+      </c>
+      <c r="L204" s="41" t="s">
+        <v>208</v>
+      </c>
+      <c r="M204" s="40">
+        <v>45875</v>
+      </c>
+      <c r="N204" s="43">
+        <v>475</v>
+      </c>
+      <c r="O204" s="41" t="s">
+        <v>122</v>
+      </c>
+      <c r="P204" s="41">
+        <v>15</v>
+      </c>
+      <c r="Q204" s="41" t="s">
+        <v>360</v>
+      </c>
+      <c r="R204" s="41">
+        <f>DATEDIF(Tabela1[[#This Row],[Atendimento]],Tabela1[[#This Row],[Previsao de Entrega]],"D")</f>
+        <v>1</v>
+      </c>
+      <c r="S204" s="43">
+        <v>0</v>
+      </c>
+      <c r="T204" s="43">
         <v>0</v>
       </c>
     </row>
     <row r="205" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A205" s="11">
-        <v>45855</v>
-      </c>
-      <c r="B205" s="11">
-        <v>45855</v>
-      </c>
-      <c r="C205" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="D205" s="11" t="s">
+      <c r="A205" s="40">
+        <v>45874</v>
+      </c>
+      <c r="B205" s="40">
+        <v>45874</v>
+      </c>
+      <c r="C205" s="40" t="s">
+        <v>7</v>
+      </c>
+      <c r="D205" s="40" t="s">
         <v>5</v>
       </c>
-      <c r="E205" s="11" t="s">
+      <c r="E205" s="40" t="s">
         <v>142</v>
       </c>
-      <c r="F205" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="G205" s="12" t="s">
-        <v>125</v>
-      </c>
-      <c r="H205" s="12" t="s">
-        <v>126</v>
-      </c>
-      <c r="I205" s="13">
+      <c r="F205" s="41" t="s">
+        <v>3</v>
+      </c>
+      <c r="G205" s="41" t="s">
+        <v>3</v>
+      </c>
+      <c r="H205" s="41" t="s">
+        <v>138</v>
+      </c>
+      <c r="I205" s="42">
         <f>NETWORKDAYS(B205, A205)</f>
         <v>1</v>
       </c>
-      <c r="J205" s="12">
-        <v>66308</v>
-      </c>
-      <c r="K205" s="12">
-        <v>11757</v>
-      </c>
-      <c r="L205" s="12" t="s">
-        <v>305</v>
-      </c>
-      <c r="M205" s="11">
-        <v>45873</v>
-      </c>
-      <c r="N205" s="14">
-        <v>1428.29</v>
-      </c>
-      <c r="O205" s="12" t="s">
+      <c r="J205" s="41">
+        <v>66560</v>
+      </c>
+      <c r="K205" s="41">
+        <v>10692</v>
+      </c>
+      <c r="L205" s="41" t="s">
+        <v>71</v>
+      </c>
+      <c r="M205" s="40">
+        <v>45876</v>
+      </c>
+      <c r="N205" s="43">
+        <v>5026.62</v>
+      </c>
+      <c r="O205" s="41" t="s">
         <v>122</v>
       </c>
-      <c r="P205" s="12">
-        <v>28</v>
-      </c>
-      <c r="Q205" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="R205" s="12">
-        <f>DATEDIF(Tabela1[[#This Row],[Atendimento]],Tabela1[[#This Row],[Previsao de Entrega]],"D")</f>
-        <v>18</v>
-      </c>
-      <c r="S205" s="14">
-        <v>320</v>
-      </c>
-      <c r="T205" s="14">
+      <c r="P205" s="41">
+        <v>14</v>
+      </c>
+      <c r="Q205" s="41" t="s">
+        <v>360</v>
+      </c>
+      <c r="R205" s="41">
+        <f>DATEDIF(Tabela1[[#This Row],[Atendimento]],Tabela1[[#This Row],[Previsao de Entrega]],"D")</f>
+        <v>2</v>
+      </c>
+      <c r="S205" s="43">
+        <v>0</v>
+      </c>
+      <c r="T205" s="43">
         <v>0</v>
       </c>
     </row>
@@ -15968,10 +15977,10 @@
     </row>
     <row r="217" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A217" s="11">
-        <v>45856</v>
+        <v>45818</v>
       </c>
       <c r="B217" s="11">
-        <v>45856</v>
+        <v>45813</v>
       </c>
       <c r="C217" s="11" t="s">
         <v>7</v>
@@ -15983,115 +15992,115 @@
         <v>124</v>
       </c>
       <c r="F217" s="12">
-        <v>68466</v>
+        <v>68422</v>
       </c>
       <c r="G217" s="12" t="s">
-        <v>125</v>
+        <v>90</v>
       </c>
       <c r="H217" s="12" t="s">
-        <v>126</v>
+        <v>91</v>
       </c>
       <c r="I217" s="13">
         <f>NETWORKDAYS(B217, A217)</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="J217" s="12">
-        <v>66337</v>
+        <v>65725</v>
       </c>
       <c r="K217" s="12">
-        <v>11736</v>
+        <v>1450</v>
       </c>
       <c r="L217" s="12" t="s">
-        <v>127</v>
+        <v>229</v>
       </c>
       <c r="M217" s="11">
-        <v>45889</v>
+        <v>45877</v>
       </c>
       <c r="N217" s="14">
-        <v>16134.54</v>
+        <v>239.63</v>
       </c>
       <c r="O217" s="12" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="P217" s="12">
-        <v>28</v>
+        <v>120</v>
       </c>
       <c r="Q217" s="12" t="s">
         <v>24</v>
       </c>
       <c r="R217" s="12">
         <f>DATEDIF(Tabela1[[#This Row],[Atendimento]],Tabela1[[#This Row],[Previsao de Entrega]],"D")</f>
-        <v>33</v>
+        <v>59</v>
       </c>
       <c r="S217" s="14">
-        <v>25720</v>
+        <v>0</v>
       </c>
       <c r="T217" s="14">
         <v>0</v>
       </c>
     </row>
     <row r="218" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A218" s="11">
-        <v>45861</v>
-      </c>
-      <c r="B218" s="11">
-        <v>45861</v>
-      </c>
-      <c r="C218" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="D218" s="11" t="s">
+      <c r="A218" s="40">
+        <v>45870</v>
+      </c>
+      <c r="B218" s="40">
+        <v>45867</v>
+      </c>
+      <c r="C218" s="40" t="s">
+        <v>7</v>
+      </c>
+      <c r="D218" s="40" t="s">
+        <v>5</v>
+      </c>
+      <c r="E218" s="40" t="s">
+        <v>113</v>
+      </c>
+      <c r="F218" s="41">
+        <v>68485</v>
+      </c>
+      <c r="G218" s="41" t="s">
+        <v>372</v>
+      </c>
+      <c r="H218" s="41" t="s">
+        <v>373</v>
+      </c>
+      <c r="I218" s="42">
+        <f>NETWORKDAYS(B218, A218)</f>
+        <v>4</v>
+      </c>
+      <c r="J218" s="41">
+        <v>66526</v>
+      </c>
+      <c r="K218" s="41">
+        <v>3061</v>
+      </c>
+      <c r="L218" s="41" t="s">
+        <v>192</v>
+      </c>
+      <c r="M218" s="40">
+        <v>45877</v>
+      </c>
+      <c r="N218" s="43">
+        <v>1150</v>
+      </c>
+      <c r="O218" s="41" t="s">
+        <v>122</v>
+      </c>
+      <c r="P218" s="41">
         <v>15</v>
       </c>
-      <c r="E218" s="11" t="s">
-        <v>124</v>
-      </c>
-      <c r="F218" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="G218" s="12" t="s">
-        <v>125</v>
-      </c>
-      <c r="H218" s="12" t="s">
-        <v>126</v>
-      </c>
-      <c r="I218" s="13">
-        <f>NETWORKDAYS(B218, A218)</f>
-        <v>1</v>
-      </c>
-      <c r="J218" s="12">
-        <v>66301</v>
-      </c>
-      <c r="K218" s="12">
-        <v>1522</v>
-      </c>
-      <c r="L218" s="12" t="s">
-        <v>388</v>
-      </c>
-      <c r="M218" s="11">
-        <v>45875</v>
-      </c>
-      <c r="N218" s="14">
-        <v>1023.45</v>
-      </c>
-      <c r="O218" s="12" t="s">
-        <v>122</v>
-      </c>
-      <c r="P218" s="12">
-        <v>28</v>
-      </c>
-      <c r="Q218" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="R218" s="12">
-        <f>DATEDIF(Tabela1[[#This Row],[Atendimento]],Tabela1[[#This Row],[Previsao de Entrega]],"D")</f>
-        <v>14</v>
-      </c>
-      <c r="S218" s="14">
-        <v>0</v>
-      </c>
-      <c r="T218" s="14">
-        <v>141.4</v>
+      <c r="Q218" s="41" t="s">
+        <v>360</v>
+      </c>
+      <c r="R218" s="41">
+        <f>DATEDIF(Tabela1[[#This Row],[Atendimento]],Tabela1[[#This Row],[Previsao de Entrega]],"D")</f>
+        <v>7</v>
+      </c>
+      <c r="S218" s="43">
+        <v>0</v>
+      </c>
+      <c r="T218" s="43">
+        <v>0</v>
       </c>
     </row>
     <row r="219" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
@@ -16286,67 +16295,67 @@
         <v>0</v>
       </c>
     </row>
-    <row r="222" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A222" s="11">
+    <row r="222" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A222" s="6">
         <v>45863</v>
       </c>
-      <c r="B222" s="11">
+      <c r="B222" s="6">
         <v>45863</v>
       </c>
-      <c r="C222" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="D222" s="11" t="s">
+      <c r="C222" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D222" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E222" s="11" t="s">
+      <c r="E222" s="6" t="s">
         <v>113</v>
       </c>
-      <c r="F222" s="12">
+      <c r="F222" s="7">
         <v>68479</v>
       </c>
-      <c r="G222" s="12" t="s">
+      <c r="G222" s="7" t="s">
         <v>389</v>
       </c>
-      <c r="H222" s="12" t="s">
+      <c r="H222" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="I222" s="13">
+      <c r="I222" s="10">
         <f>NETWORKDAYS(B222, A222)</f>
         <v>1</v>
       </c>
-      <c r="J222" s="12">
+      <c r="J222" s="7">
         <v>66454</v>
       </c>
-      <c r="K222" s="12">
+      <c r="K222" s="7">
         <v>11788</v>
       </c>
-      <c r="L222" s="12" t="s">
+      <c r="L222" s="7" t="s">
         <v>390</v>
       </c>
-      <c r="M222" s="11">
+      <c r="M222" s="6">
         <v>45889</v>
       </c>
-      <c r="N222" s="14">
-        <v>4122.3</v>
-      </c>
-      <c r="O222" s="12" t="s">
+      <c r="N222" s="8">
+        <v>3867.5</v>
+      </c>
+      <c r="O222" s="7" t="s">
         <v>122</v>
       </c>
-      <c r="P222" s="12">
+      <c r="P222" s="7">
         <v>30</v>
       </c>
-      <c r="Q222" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="R222" s="12">
+      <c r="Q222" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="R222" s="7">
         <f>DATEDIF(Tabela1[[#This Row],[Atendimento]],Tabela1[[#This Row],[Previsao de Entrega]],"D")</f>
         <v>26</v>
       </c>
-      <c r="S222" s="14">
-        <v>0</v>
-      </c>
-      <c r="T222" s="14">
+      <c r="S222" s="8">
+        <v>0</v>
+      </c>
+      <c r="T222" s="8">
         <v>0</v>
       </c>
     </row>
@@ -16415,115 +16424,115 @@
       </c>
     </row>
     <row r="224" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A224" s="11">
-        <v>45866</v>
-      </c>
-      <c r="B224" s="11">
-        <v>45863</v>
-      </c>
-      <c r="C224" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="D224" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="E224" s="11" t="s">
-        <v>113</v>
-      </c>
-      <c r="F224" s="12">
-        <v>68481</v>
-      </c>
-      <c r="G224" s="12" t="s">
-        <v>372</v>
-      </c>
-      <c r="H224" s="12" t="s">
-        <v>373</v>
-      </c>
-      <c r="I224" s="13">
+      <c r="A224" s="49">
+        <v>45826</v>
+      </c>
+      <c r="B224" s="49">
+        <v>45826</v>
+      </c>
+      <c r="C224" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="D224" s="49" t="s">
+        <v>15</v>
+      </c>
+      <c r="E224" s="49" t="s">
+        <v>124</v>
+      </c>
+      <c r="F224" s="50" t="s">
+        <v>3</v>
+      </c>
+      <c r="G224" s="50" t="s">
+        <v>125</v>
+      </c>
+      <c r="H224" s="50" t="s">
+        <v>126</v>
+      </c>
+      <c r="I224" s="51">
         <f>NETWORKDAYS(B224, A224)</f>
-        <v>2</v>
-      </c>
-      <c r="J224" s="12">
-        <v>66462</v>
-      </c>
-      <c r="K224" s="12">
-        <v>10535</v>
-      </c>
-      <c r="L224" s="12" t="s">
-        <v>391</v>
-      </c>
-      <c r="M224" s="11">
-        <v>45868</v>
-      </c>
-      <c r="N224" s="14">
-        <v>300</v>
-      </c>
-      <c r="O224" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="J224" s="50">
+        <v>66341</v>
+      </c>
+      <c r="K224" s="50">
+        <v>11758</v>
+      </c>
+      <c r="L224" s="50" t="s">
+        <v>316</v>
+      </c>
+      <c r="M224" s="49">
+        <v>45880</v>
+      </c>
+      <c r="N224" s="52">
+        <v>924.61</v>
+      </c>
+      <c r="O224" s="50" t="s">
         <v>122</v>
       </c>
-      <c r="P224" s="12">
-        <v>14</v>
-      </c>
-      <c r="Q224" s="12" t="s">
+      <c r="P224" s="50">
+        <v>28</v>
+      </c>
+      <c r="Q224" s="50" t="s">
         <v>24</v>
       </c>
-      <c r="R224" s="12">
-        <f>DATEDIF(Tabela1[[#This Row],[Atendimento]],Tabela1[[#This Row],[Previsao de Entrega]],"D")</f>
-        <v>2</v>
-      </c>
-      <c r="S224" s="14">
-        <v>0</v>
-      </c>
-      <c r="T224" s="14">
+      <c r="R224" s="50">
+        <f>DATEDIF(Tabela1[[#This Row],[Atendimento]],Tabela1[[#This Row],[Previsao de Entrega]],"D")</f>
+        <v>54</v>
+      </c>
+      <c r="S224" s="52">
+        <v>0</v>
+      </c>
+      <c r="T224" s="52">
         <v>0</v>
       </c>
     </row>
     <row r="225" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A225" s="11">
-        <v>45867</v>
+        <v>45849</v>
       </c>
       <c r="B225" s="11">
-        <v>45867</v>
+        <v>45849</v>
       </c>
       <c r="C225" s="11" t="s">
         <v>7</v>
       </c>
       <c r="D225" s="11" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="E225" s="11" t="s">
-        <v>124</v>
+        <v>113</v>
       </c>
       <c r="F225" s="12" t="s">
         <v>3</v>
       </c>
       <c r="G225" s="12" t="s">
-        <v>125</v>
+        <v>372</v>
       </c>
       <c r="H225" s="12" t="s">
-        <v>126</v>
+        <v>373</v>
       </c>
       <c r="I225" s="13">
         <f>NETWORKDAYS(B225, A225)</f>
         <v>1</v>
       </c>
       <c r="J225" s="12">
-        <v>66471</v>
+        <v>66166</v>
       </c>
       <c r="K225" s="12">
-        <v>9</v>
+        <v>11782</v>
       </c>
       <c r="L225" s="12" t="s">
-        <v>398</v>
+        <v>371</v>
       </c>
       <c r="M225" s="11">
         <v>45880</v>
       </c>
       <c r="N225" s="14">
-        <v>6505.5</v>
+        <v>2250</v>
       </c>
       <c r="O225" s="12" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="P225" s="12">
         <v>30</v>
@@ -16533,10 +16542,10 @@
       </c>
       <c r="R225" s="12">
         <f>DATEDIF(Tabela1[[#This Row],[Atendimento]],Tabela1[[#This Row],[Previsao de Entrega]],"D")</f>
-        <v>13</v>
+        <v>31</v>
       </c>
       <c r="S225" s="14">
-        <v>135</v>
+        <v>250</v>
       </c>
       <c r="T225" s="14">
         <v>0</v>
@@ -16614,57 +16623,57 @@
         <v>45867</v>
       </c>
       <c r="C227" s="11" t="s">
-        <v>128</v>
+        <v>7</v>
       </c>
       <c r="D227" s="11" t="s">
         <v>15</v>
       </c>
       <c r="E227" s="11" t="s">
-        <v>113</v>
-      </c>
-      <c r="F227" s="12">
-        <v>68486</v>
+        <v>124</v>
+      </c>
+      <c r="F227" s="12" t="s">
+        <v>3</v>
       </c>
       <c r="G227" s="12" t="s">
-        <v>296</v>
+        <v>125</v>
       </c>
       <c r="H227" s="12" t="s">
-        <v>96</v>
+        <v>126</v>
       </c>
       <c r="I227" s="13">
         <f>NETWORKDAYS(B227, A227)</f>
         <v>1</v>
       </c>
       <c r="J227" s="12">
-        <v>66478</v>
+        <v>66471</v>
       </c>
       <c r="K227" s="12">
-        <v>10460</v>
+        <v>9</v>
       </c>
       <c r="L227" s="12" t="s">
-        <v>394</v>
+        <v>398</v>
       </c>
       <c r="M227" s="11">
-        <v>45883</v>
+        <v>45880</v>
       </c>
       <c r="N227" s="14">
-        <v>4789.6099999999997</v>
+        <v>6505.5</v>
       </c>
       <c r="O227" s="12" t="s">
         <v>122</v>
       </c>
       <c r="P227" s="12">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="Q227" s="12" t="s">
         <v>24</v>
       </c>
       <c r="R227" s="12">
         <f>DATEDIF(Tabela1[[#This Row],[Atendimento]],Tabela1[[#This Row],[Previsao de Entrega]],"D")</f>
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="S227" s="14">
-        <v>1509.38</v>
+        <v>135</v>
       </c>
       <c r="T227" s="14">
         <v>0</v>
@@ -16672,47 +16681,47 @@
     </row>
     <row r="228" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A228" s="11">
-        <v>45867</v>
+        <v>45785</v>
       </c>
       <c r="B228" s="11">
-        <v>45866</v>
+        <v>45784</v>
       </c>
       <c r="C228" s="11" t="s">
         <v>7</v>
       </c>
       <c r="D228" s="11" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="E228" s="11" t="s">
-        <v>124</v>
+        <v>113</v>
       </c>
       <c r="F228" s="12">
-        <v>68483</v>
+        <v>68369</v>
       </c>
       <c r="G228" s="12" t="s">
-        <v>125</v>
+        <v>39</v>
       </c>
       <c r="H228" s="12" t="s">
-        <v>126</v>
+        <v>98</v>
       </c>
       <c r="I228" s="13">
         <f>NETWORKDAYS(B228, A228)</f>
         <v>2</v>
       </c>
       <c r="J228" s="12">
-        <v>66467</v>
+        <v>65234</v>
       </c>
       <c r="K228" s="12">
-        <v>11164</v>
+        <v>11610</v>
       </c>
       <c r="L228" s="12" t="s">
-        <v>298</v>
+        <v>38</v>
       </c>
       <c r="M228" s="11">
-        <v>45908</v>
+        <v>45881</v>
       </c>
       <c r="N228" s="14">
-        <v>2623.03</v>
+        <v>9114.5499999999993</v>
       </c>
       <c r="O228" s="12" t="s">
         <v>122</v>
@@ -16725,10 +16734,10 @@
       </c>
       <c r="R228" s="12">
         <f>DATEDIF(Tabela1[[#This Row],[Atendimento]],Tabela1[[#This Row],[Previsao de Entrega]],"D")</f>
-        <v>41</v>
+        <v>96</v>
       </c>
       <c r="S228" s="14">
-        <v>52</v>
+        <v>183.5</v>
       </c>
       <c r="T228" s="14">
         <v>0</v>
@@ -16736,60 +16745,60 @@
     </row>
     <row r="229" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A229" s="11">
-        <v>45868</v>
+        <v>45870</v>
       </c>
       <c r="B229" s="11">
-        <v>45868</v>
+        <v>45863</v>
       </c>
       <c r="C229" s="11" t="s">
-        <v>128</v>
+        <v>7</v>
       </c>
       <c r="D229" s="11" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="E229" s="11" t="s">
-        <v>395</v>
+        <v>113</v>
       </c>
       <c r="F229" s="12">
-        <v>68487</v>
+        <v>68482</v>
       </c>
       <c r="G229" s="12" t="s">
-        <v>396</v>
+        <v>129</v>
       </c>
       <c r="H229" s="12" t="s">
-        <v>96</v>
+        <v>130</v>
       </c>
       <c r="I229" s="13">
         <f>NETWORKDAYS(B229, A229)</f>
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="J229" s="12">
-        <v>66489</v>
+        <v>66522</v>
       </c>
       <c r="K229" s="12">
-        <v>11614</v>
+        <v>679</v>
       </c>
       <c r="L229" s="12" t="s">
-        <v>397</v>
+        <v>346</v>
       </c>
       <c r="M229" s="11">
-        <v>45874</v>
+        <v>45881</v>
       </c>
       <c r="N229" s="14">
-        <v>6633</v>
+        <v>5173.3</v>
       </c>
       <c r="O229" s="12" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="P229" s="12">
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="Q229" s="12" t="s">
         <v>24</v>
       </c>
       <c r="R229" s="12">
         <f>DATEDIF(Tabela1[[#This Row],[Atendimento]],Tabela1[[#This Row],[Previsao de Entrega]],"D")</f>
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="S229" s="14">
         <v>0</v>
@@ -16864,47 +16873,47 @@
     </row>
     <row r="231" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A231" s="11">
-        <v>45868</v>
+        <v>45867</v>
       </c>
       <c r="B231" s="11">
-        <v>45862</v>
+        <v>45867</v>
       </c>
       <c r="C231" s="11" t="s">
-        <v>7</v>
+        <v>128</v>
       </c>
       <c r="D231" s="11" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="E231" s="11" t="s">
         <v>113</v>
       </c>
       <c r="F231" s="12">
-        <v>68476</v>
+        <v>68486</v>
       </c>
       <c r="G231" s="12" t="s">
-        <v>227</v>
+        <v>296</v>
       </c>
       <c r="H231" s="12" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="I231" s="13">
         <f>NETWORKDAYS(B231, A231)</f>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="J231" s="12">
-        <v>66491</v>
+        <v>66478</v>
       </c>
       <c r="K231" s="12">
-        <v>11522</v>
+        <v>10460</v>
       </c>
       <c r="L231" s="12" t="s">
-        <v>377</v>
+        <v>394</v>
       </c>
       <c r="M231" s="11">
-        <v>45875</v>
+        <v>45883</v>
       </c>
       <c r="N231" s="14">
-        <v>398.42</v>
+        <v>4789.6099999999997</v>
       </c>
       <c r="O231" s="12" t="s">
         <v>122</v>
@@ -16917,10 +16926,10 @@
       </c>
       <c r="R231" s="12">
         <f>DATEDIF(Tabela1[[#This Row],[Atendimento]],Tabela1[[#This Row],[Previsao de Entrega]],"D")</f>
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="S231" s="14">
-        <v>0</v>
+        <v>1509.38</v>
       </c>
       <c r="T231" s="14">
         <v>0</v>
@@ -16928,63 +16937,63 @@
     </row>
     <row r="232" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A232" s="11">
-        <v>45868</v>
+        <v>45870</v>
       </c>
       <c r="B232" s="11">
-        <v>45868</v>
+        <v>45869</v>
       </c>
       <c r="C232" s="11" t="s">
         <v>7</v>
       </c>
       <c r="D232" s="11" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="E232" s="11" t="s">
-        <v>124</v>
-      </c>
-      <c r="F232" s="12" t="s">
-        <v>3</v>
+        <v>113</v>
+      </c>
+      <c r="F232" s="12">
+        <v>68491</v>
       </c>
       <c r="G232" s="12" t="s">
-        <v>125</v>
+        <v>372</v>
       </c>
       <c r="H232" s="12" t="s">
-        <v>126</v>
+        <v>373</v>
       </c>
       <c r="I232" s="13">
         <f>NETWORKDAYS(B232, A232)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J232" s="12">
-        <v>66504</v>
+        <v>66521</v>
       </c>
       <c r="K232" s="12">
-        <v>3034</v>
+        <v>3061</v>
       </c>
       <c r="L232" s="12" t="s">
-        <v>349</v>
+        <v>192</v>
       </c>
       <c r="M232" s="11">
-        <v>45897</v>
+        <v>45883</v>
       </c>
       <c r="N232" s="14">
-        <v>2364.3000000000002</v>
+        <v>3000</v>
       </c>
       <c r="O232" s="12" t="s">
         <v>122</v>
       </c>
       <c r="P232" s="12">
-        <v>90</v>
+        <v>15</v>
       </c>
       <c r="Q232" s="12" t="s">
         <v>24</v>
       </c>
       <c r="R232" s="12">
         <f>DATEDIF(Tabela1[[#This Row],[Atendimento]],Tabela1[[#This Row],[Previsao de Entrega]],"D")</f>
-        <v>29</v>
+        <v>13</v>
       </c>
       <c r="S232" s="14">
-        <v>80</v>
+        <v>50</v>
       </c>
       <c r="T232" s="14">
         <v>0</v>
@@ -16992,10 +17001,10 @@
     </row>
     <row r="233" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A233" s="11">
-        <v>45869</v>
+        <v>45856</v>
       </c>
       <c r="B233" s="11">
-        <v>45869</v>
+        <v>45856</v>
       </c>
       <c r="C233" s="11" t="s">
         <v>7</v>
@@ -17006,8 +17015,8 @@
       <c r="E233" s="11" t="s">
         <v>124</v>
       </c>
-      <c r="F233" s="12" t="s">
-        <v>3</v>
+      <c r="F233" s="12">
+        <v>68466</v>
       </c>
       <c r="G233" s="12" t="s">
         <v>125</v>
@@ -17020,35 +17029,35 @@
         <v>1</v>
       </c>
       <c r="J233" s="12">
-        <v>66427</v>
+        <v>66337</v>
       </c>
       <c r="K233" s="12">
-        <v>1277</v>
+        <v>11736</v>
       </c>
       <c r="L233" s="12" t="s">
-        <v>399</v>
+        <v>127</v>
       </c>
       <c r="M233" s="11">
-        <v>45897</v>
+        <v>45889</v>
       </c>
       <c r="N233" s="14">
-        <v>2715.75</v>
+        <v>16134.54</v>
       </c>
       <c r="O233" s="12" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="P233" s="12">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="Q233" s="12" t="s">
         <v>24</v>
       </c>
       <c r="R233" s="12">
         <f>DATEDIF(Tabela1[[#This Row],[Atendimento]],Tabela1[[#This Row],[Previsao de Entrega]],"D")</f>
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="S233" s="14">
-        <v>950</v>
+        <v>25720</v>
       </c>
       <c r="T233" s="14">
         <v>0</v>
@@ -17056,252 +17065,252 @@
     </row>
     <row r="234" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A234" s="11">
-        <v>45870</v>
+        <v>45868</v>
       </c>
       <c r="B234" s="11">
-        <v>45869</v>
+        <v>45868</v>
       </c>
       <c r="C234" s="11" t="s">
         <v>7</v>
       </c>
       <c r="D234" s="11" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="E234" s="11" t="s">
-        <v>113</v>
-      </c>
-      <c r="F234" s="12">
-        <v>68491</v>
+        <v>124</v>
+      </c>
+      <c r="F234" s="12" t="s">
+        <v>3</v>
       </c>
       <c r="G234" s="12" t="s">
-        <v>372</v>
+        <v>125</v>
       </c>
       <c r="H234" s="12" t="s">
-        <v>373</v>
+        <v>126</v>
       </c>
       <c r="I234" s="13">
         <f>NETWORKDAYS(B234, A234)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J234" s="12">
-        <v>66521</v>
+        <v>66504</v>
       </c>
       <c r="K234" s="12">
-        <v>3061</v>
+        <v>3034</v>
       </c>
       <c r="L234" s="12" t="s">
-        <v>192</v>
+        <v>349</v>
       </c>
       <c r="M234" s="11">
-        <v>45883</v>
+        <v>45897</v>
       </c>
       <c r="N234" s="14">
-        <v>3000</v>
+        <v>66522</v>
       </c>
       <c r="O234" s="12" t="s">
         <v>122</v>
       </c>
       <c r="P234" s="12">
-        <v>15</v>
+        <v>90</v>
       </c>
       <c r="Q234" s="12" t="s">
         <v>24</v>
       </c>
       <c r="R234" s="12">
         <f>DATEDIF(Tabela1[[#This Row],[Atendimento]],Tabela1[[#This Row],[Previsao de Entrega]],"D")</f>
-        <v>13</v>
+        <v>29</v>
       </c>
       <c r="S234" s="14">
-        <v>50</v>
+        <v>80</v>
       </c>
       <c r="T234" s="14">
         <v>0</v>
       </c>
     </row>
     <row r="235" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A235" s="40">
-        <v>45870</v>
-      </c>
-      <c r="B235" s="40">
-        <v>45863</v>
-      </c>
-      <c r="C235" s="40" t="s">
-        <v>7</v>
-      </c>
-      <c r="D235" s="40" t="s">
+      <c r="A235" s="11">
+        <v>45869</v>
+      </c>
+      <c r="B235" s="11">
+        <v>45869</v>
+      </c>
+      <c r="C235" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D235" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="E235" s="40" t="s">
+      <c r="E235" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="F235" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="G235" s="12" t="s">
+        <v>125</v>
+      </c>
+      <c r="H235" s="12" t="s">
+        <v>126</v>
+      </c>
+      <c r="I235" s="13">
+        <f>NETWORKDAYS(B235, A235)</f>
+        <v>1</v>
+      </c>
+      <c r="J235" s="12">
+        <v>66427</v>
+      </c>
+      <c r="K235" s="12">
+        <v>1277</v>
+      </c>
+      <c r="L235" s="12" t="s">
+        <v>399</v>
+      </c>
+      <c r="M235" s="11">
+        <v>45897</v>
+      </c>
+      <c r="N235" s="14">
+        <v>2715.75</v>
+      </c>
+      <c r="O235" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="P235" s="12">
+        <v>30</v>
+      </c>
+      <c r="Q235" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="R235" s="12">
+        <f>DATEDIF(Tabela1[[#This Row],[Atendimento]],Tabela1[[#This Row],[Previsao de Entrega]],"D")</f>
+        <v>28</v>
+      </c>
+      <c r="S235" s="14">
+        <v>950</v>
+      </c>
+      <c r="T235" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="236" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A236" s="11">
+        <v>45840</v>
+      </c>
+      <c r="B236" s="11">
+        <v>45840</v>
+      </c>
+      <c r="C236" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D236" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="E236" s="11" t="s">
         <v>113</v>
       </c>
-      <c r="F235" s="41">
-        <v>68482</v>
-      </c>
-      <c r="G235" s="41" t="s">
-        <v>129</v>
-      </c>
-      <c r="H235" s="41" t="s">
-        <v>130</v>
-      </c>
-      <c r="I235" s="42">
-        <f>NETWORKDAYS(B235, A235)</f>
-        <v>6</v>
-      </c>
-      <c r="J235" s="41">
-        <v>66522</v>
-      </c>
-      <c r="K235" s="41">
-        <v>679</v>
-      </c>
-      <c r="L235" s="41" t="s">
-        <v>346</v>
-      </c>
-      <c r="M235" s="40">
-        <v>45881</v>
-      </c>
-      <c r="N235" s="43">
-        <v>5173.3</v>
-      </c>
-      <c r="O235" s="41" t="s">
+      <c r="F236" s="12">
+        <v>68452</v>
+      </c>
+      <c r="G236" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="H236" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="I236" s="13">
+        <f>NETWORKDAYS(B236, A236)</f>
+        <v>1</v>
+      </c>
+      <c r="J236" s="12">
+        <v>66037</v>
+      </c>
+      <c r="K236" s="12">
+        <v>11775</v>
+      </c>
+      <c r="L236" s="12" t="s">
+        <v>353</v>
+      </c>
+      <c r="M236" s="11">
+        <v>45905</v>
+      </c>
+      <c r="N236" s="14">
+        <v>1750</v>
+      </c>
+      <c r="O236" s="12" t="s">
         <v>122</v>
       </c>
-      <c r="P235" s="41">
+      <c r="P236" s="12">
         <v>30</v>
       </c>
-      <c r="Q235" s="41" t="s">
-        <v>360</v>
-      </c>
-      <c r="R235" s="41">
-        <f>DATEDIF(Tabela1[[#This Row],[Atendimento]],Tabela1[[#This Row],[Previsao de Entrega]],"D")</f>
-        <v>11</v>
-      </c>
-      <c r="S235" s="43">
-        <v>0</v>
-      </c>
-      <c r="T235" s="43">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="236" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A236" s="40">
-        <v>45870</v>
-      </c>
-      <c r="B236" s="40">
-        <v>45867</v>
-      </c>
-      <c r="C236" s="40" t="s">
-        <v>7</v>
-      </c>
-      <c r="D236" s="40" t="s">
-        <v>5</v>
-      </c>
-      <c r="E236" s="40" t="s">
-        <v>113</v>
-      </c>
-      <c r="F236" s="41">
-        <v>68485</v>
-      </c>
-      <c r="G236" s="41" t="s">
-        <v>372</v>
-      </c>
-      <c r="H236" s="41" t="s">
-        <v>373</v>
-      </c>
-      <c r="I236" s="42">
-        <f>NETWORKDAYS(B236, A236)</f>
-        <v>4</v>
-      </c>
-      <c r="J236" s="41">
-        <v>66526</v>
-      </c>
-      <c r="K236" s="41">
-        <v>3061</v>
-      </c>
-      <c r="L236" s="41" t="s">
-        <v>192</v>
-      </c>
-      <c r="M236" s="40">
-        <v>45877</v>
-      </c>
-      <c r="N236" s="43">
-        <v>1150</v>
-      </c>
-      <c r="O236" s="41" t="s">
-        <v>122</v>
-      </c>
-      <c r="P236" s="41">
-        <v>15</v>
-      </c>
-      <c r="Q236" s="41" t="s">
-        <v>360</v>
-      </c>
-      <c r="R236" s="41">
-        <f>DATEDIF(Tabela1[[#This Row],[Atendimento]],Tabela1[[#This Row],[Previsao de Entrega]],"D")</f>
-        <v>7</v>
-      </c>
-      <c r="S236" s="43">
-        <v>0</v>
-      </c>
-      <c r="T236" s="43">
+      <c r="Q236" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="R236" s="12">
+        <f>DATEDIF(Tabela1[[#This Row],[Atendimento]],Tabela1[[#This Row],[Previsao de Entrega]],"D")</f>
+        <v>65</v>
+      </c>
+      <c r="S236" s="14">
+        <v>0</v>
+      </c>
+      <c r="T236" s="14">
         <v>0</v>
       </c>
     </row>
     <row r="237" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A237" s="11">
-        <v>45870</v>
+        <v>45846</v>
       </c>
       <c r="B237" s="11">
-        <v>45870</v>
+        <v>45846</v>
       </c>
       <c r="C237" s="11" t="s">
-        <v>128</v>
+        <v>7</v>
       </c>
       <c r="D237" s="11" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="E237" s="11" t="s">
-        <v>124</v>
-      </c>
-      <c r="F237" s="12" t="s">
-        <v>3</v>
+        <v>113</v>
+      </c>
+      <c r="F237" s="12">
+        <v>68461</v>
       </c>
       <c r="G237" s="12" t="s">
-        <v>125</v>
+        <v>227</v>
       </c>
       <c r="H237" s="12" t="s">
-        <v>126</v>
+        <v>98</v>
       </c>
       <c r="I237" s="13">
         <f>NETWORKDAYS(B237, A237)</f>
         <v>1</v>
       </c>
       <c r="J237" s="12">
-        <v>66430</v>
+        <v>66119</v>
       </c>
       <c r="K237" s="12">
-        <v>333</v>
+        <v>10677</v>
       </c>
       <c r="L237" s="12" t="s">
-        <v>401</v>
+        <v>362</v>
       </c>
       <c r="M237" s="11">
-        <v>46113</v>
+        <v>45905</v>
       </c>
       <c r="N237" s="14">
-        <v>281569.34000000003</v>
+        <v>2800</v>
       </c>
       <c r="O237" s="12" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="P237" s="12">
-        <v>120</v>
+        <v>30</v>
       </c>
       <c r="Q237" s="12" t="s">
         <v>24</v>
       </c>
       <c r="R237" s="12">
         <f>DATEDIF(Tabela1[[#This Row],[Atendimento]],Tabela1[[#This Row],[Previsao de Entrega]],"D")</f>
-        <v>243</v>
+        <v>59</v>
       </c>
       <c r="S237" s="14">
         <v>0</v>
@@ -17310,67 +17319,579 @@
         <v>0</v>
       </c>
     </row>
-    <row r="238" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A238" s="40">
+    <row r="238" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A238" s="6">
         <v>45873</v>
       </c>
-      <c r="B238" s="40">
+      <c r="B238" s="6">
         <v>45873</v>
       </c>
-      <c r="C238" s="40" t="s">
-        <v>7</v>
-      </c>
-      <c r="D238" s="40" t="s">
+      <c r="C238" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D238" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E238" s="40" t="s">
+      <c r="E238" s="6" t="s">
         <v>113</v>
       </c>
-      <c r="F238" s="41" t="s">
-        <v>3</v>
-      </c>
-      <c r="G238" s="41" t="s">
+      <c r="F238" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="G238" s="7" t="s">
         <v>129</v>
       </c>
-      <c r="H238" s="41" t="s">
+      <c r="H238" s="7" t="s">
         <v>130</v>
       </c>
-      <c r="I238" s="42">
+      <c r="I238" s="10">
         <f>NETWORKDAYS(B238, A238)</f>
         <v>1</v>
       </c>
-      <c r="J238" s="41">
+      <c r="J238" s="7">
         <v>66529</v>
       </c>
-      <c r="K238" s="41">
+      <c r="K238" s="7">
         <v>2856</v>
       </c>
-      <c r="L238" s="41" t="s">
+      <c r="L238" s="7" t="s">
         <v>400</v>
       </c>
-      <c r="M238" s="40">
+      <c r="M238" s="6">
         <v>45875</v>
       </c>
-      <c r="N238" s="43">
+      <c r="N238" s="8">
         <v>5600</v>
       </c>
-      <c r="O238" s="41" t="s">
+      <c r="O238" s="7" t="s">
         <v>122</v>
       </c>
-      <c r="P238" s="41">
+      <c r="P238" s="7">
         <v>30</v>
       </c>
-      <c r="Q238" s="41" t="s">
+      <c r="Q238" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="R238" s="7">
+        <f>DATEDIF(Tabela1[[#This Row],[Atendimento]],Tabela1[[#This Row],[Previsao de Entrega]],"D")</f>
+        <v>2</v>
+      </c>
+      <c r="S238" s="8">
+        <v>0</v>
+      </c>
+      <c r="T238" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="239" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A239" s="6">
+        <v>45873</v>
+      </c>
+      <c r="B239" s="6">
+        <v>45873</v>
+      </c>
+      <c r="C239" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D239" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E239" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="F239" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="G239" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="H239" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="I239" s="10">
+        <f>NETWORKDAYS(B239, A239)</f>
+        <v>1</v>
+      </c>
+      <c r="J239" s="7">
+        <v>66530</v>
+      </c>
+      <c r="K239" s="7">
+        <v>280</v>
+      </c>
+      <c r="L239" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="M239" s="6">
+        <v>45875</v>
+      </c>
+      <c r="N239" s="8">
+        <v>15507.16</v>
+      </c>
+      <c r="O239" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="P239" s="7">
+        <v>28</v>
+      </c>
+      <c r="Q239" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="R239" s="7">
+        <f>DATEDIF(Tabela1[[#This Row],[Atendimento]],Tabela1[[#This Row],[Previsao de Entrega]],"D")</f>
+        <v>2</v>
+      </c>
+      <c r="S239" s="8">
+        <v>0</v>
+      </c>
+      <c r="T239" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="240" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A240" s="6">
+        <v>45873</v>
+      </c>
+      <c r="B240" s="6">
+        <v>45873</v>
+      </c>
+      <c r="C240" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D240" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E240" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="F240" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="G240" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="H240" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="I240" s="10">
+        <f>NETWORKDAYS(B240, A240)</f>
+        <v>1</v>
+      </c>
+      <c r="J240" s="7">
+        <v>66532</v>
+      </c>
+      <c r="K240" s="7">
+        <v>11263</v>
+      </c>
+      <c r="L240" s="7" t="s">
+        <v>190</v>
+      </c>
+      <c r="M240" s="6">
+        <v>45875</v>
+      </c>
+      <c r="N240" s="8">
+        <v>11841</v>
+      </c>
+      <c r="O240" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="P240" s="7">
+        <v>15</v>
+      </c>
+      <c r="Q240" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="R240" s="7">
+        <f>DATEDIF(Tabela1[[#This Row],[Atendimento]],Tabela1[[#This Row],[Previsao de Entrega]],"D")</f>
+        <v>2</v>
+      </c>
+      <c r="S240" s="8">
+        <v>0</v>
+      </c>
+      <c r="T240" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="241" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A241" s="6">
+        <v>45873</v>
+      </c>
+      <c r="B241" s="6">
+        <v>45873</v>
+      </c>
+      <c r="C241" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D241" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E241" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="F241" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="G241" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="H241" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="I241" s="10">
+        <f>NETWORKDAYS(B241, A241)</f>
+        <v>1</v>
+      </c>
+      <c r="J241" s="7">
+        <v>66533</v>
+      </c>
+      <c r="K241" s="7">
+        <v>495</v>
+      </c>
+      <c r="L241" s="7" t="s">
+        <v>189</v>
+      </c>
+      <c r="M241" s="6">
+        <v>45875</v>
+      </c>
+      <c r="N241" s="8">
+        <v>257</v>
+      </c>
+      <c r="O241" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="P241" s="7">
+        <v>14</v>
+      </c>
+      <c r="Q241" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="R241" s="7">
+        <f>DATEDIF(Tabela1[[#This Row],[Atendimento]],Tabela1[[#This Row],[Previsao de Entrega]],"D")</f>
+        <v>2</v>
+      </c>
+      <c r="S241" s="8">
+        <v>0</v>
+      </c>
+      <c r="T241" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="242" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A242" s="11">
+        <v>45848</v>
+      </c>
+      <c r="B242" s="11">
+        <v>45848</v>
+      </c>
+      <c r="C242" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D242" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="E242" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="F242" s="12">
+        <v>68457</v>
+      </c>
+      <c r="G242" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="H242" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="I242" s="13">
+        <f>NETWORKDAYS(B242, A242)</f>
+        <v>1</v>
+      </c>
+      <c r="J242" s="12">
+        <v>66126</v>
+      </c>
+      <c r="K242" s="12">
+        <v>2931</v>
+      </c>
+      <c r="L242" s="12" t="s">
+        <v>367</v>
+      </c>
+      <c r="M242" s="11">
+        <v>45905</v>
+      </c>
+      <c r="N242" s="14">
+        <v>3500</v>
+      </c>
+      <c r="O242" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="P242" s="12">
+        <v>30</v>
+      </c>
+      <c r="Q242" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="R242" s="12">
+        <f>DATEDIF(Tabela1[[#This Row],[Atendimento]],Tabela1[[#This Row],[Previsao de Entrega]],"D")</f>
+        <v>57</v>
+      </c>
+      <c r="S242" s="14">
+        <v>320</v>
+      </c>
+      <c r="T242" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="243" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A243" s="40">
+        <v>45874</v>
+      </c>
+      <c r="B243" s="40">
+        <v>45853</v>
+      </c>
+      <c r="C243" s="40" t="s">
+        <v>7</v>
+      </c>
+      <c r="D243" s="40" t="s">
+        <v>15</v>
+      </c>
+      <c r="E243" s="40" t="s">
+        <v>124</v>
+      </c>
+      <c r="F243" s="41">
+        <v>68465</v>
+      </c>
+      <c r="G243" s="41" t="s">
+        <v>125</v>
+      </c>
+      <c r="H243" s="41" t="s">
+        <v>126</v>
+      </c>
+      <c r="I243" s="42">
+        <f>NETWORKDAYS(B243, A243)</f>
+        <v>16</v>
+      </c>
+      <c r="J243" s="41">
+        <v>66555</v>
+      </c>
+      <c r="K243" s="41">
+        <v>11791</v>
+      </c>
+      <c r="L243" s="41" t="s">
+        <v>404</v>
+      </c>
+      <c r="M243" s="40">
+        <v>45906</v>
+      </c>
+      <c r="N243" s="43">
+        <v>1075.55</v>
+      </c>
+      <c r="O243" s="41" t="s">
+        <v>122</v>
+      </c>
+      <c r="P243" s="41">
+        <v>20</v>
+      </c>
+      <c r="Q243" s="41" t="s">
         <v>360</v>
       </c>
-      <c r="R238" s="41">
-        <f>DATEDIF(Tabela1[[#This Row],[Atendimento]],Tabela1[[#This Row],[Previsao de Entrega]],"D")</f>
+      <c r="R243" s="41">
+        <f>DATEDIF(Tabela1[[#This Row],[Atendimento]],Tabela1[[#This Row],[Previsao de Entrega]],"D")</f>
+        <v>32</v>
+      </c>
+      <c r="S243" s="43">
+        <v>0</v>
+      </c>
+      <c r="T243" s="43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="244" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A244" s="11">
+        <v>45867</v>
+      </c>
+      <c r="B244" s="11">
+        <v>45866</v>
+      </c>
+      <c r="C244" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D244" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="E244" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="F244" s="12">
+        <v>68483</v>
+      </c>
+      <c r="G244" s="12" t="s">
+        <v>125</v>
+      </c>
+      <c r="H244" s="12" t="s">
+        <v>126</v>
+      </c>
+      <c r="I244" s="13">
+        <f>NETWORKDAYS(B244, A244)</f>
         <v>2</v>
       </c>
-      <c r="S238" s="43">
-        <v>0</v>
-      </c>
-      <c r="T238" s="43">
+      <c r="J244" s="12">
+        <v>66467</v>
+      </c>
+      <c r="K244" s="12">
+        <v>11164</v>
+      </c>
+      <c r="L244" s="12" t="s">
+        <v>298</v>
+      </c>
+      <c r="M244" s="11">
+        <v>45908</v>
+      </c>
+      <c r="N244" s="14">
+        <v>2623.03</v>
+      </c>
+      <c r="O244" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="P244" s="12">
+        <v>28</v>
+      </c>
+      <c r="Q244" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="R244" s="12">
+        <f>DATEDIF(Tabela1[[#This Row],[Atendimento]],Tabela1[[#This Row],[Previsao de Entrega]],"D")</f>
+        <v>41</v>
+      </c>
+      <c r="S244" s="14">
+        <v>52</v>
+      </c>
+      <c r="T244" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="245" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A245" s="6">
+        <v>45874</v>
+      </c>
+      <c r="B245" s="6">
+        <v>45874</v>
+      </c>
+      <c r="C245" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D245" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E245" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="F245" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="G245" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="H245" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="I245" s="10">
+        <f>NETWORKDAYS(B245, A245)</f>
+        <v>1</v>
+      </c>
+      <c r="J245" s="7">
+        <v>64425</v>
+      </c>
+      <c r="K245" s="7">
+        <v>2954</v>
+      </c>
+      <c r="L245" s="7" t="s">
+        <v>292</v>
+      </c>
+      <c r="M245" s="6">
+        <v>45876</v>
+      </c>
+      <c r="N245" s="8">
+        <v>255.15</v>
+      </c>
+      <c r="O245" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="P245" s="7">
+        <v>30</v>
+      </c>
+      <c r="Q245" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="R245" s="7">
+        <f>DATEDIF(Tabela1[[#This Row],[Atendimento]],Tabela1[[#This Row],[Previsao de Entrega]],"D")</f>
+        <v>2</v>
+      </c>
+      <c r="S245" s="8">
+        <v>0</v>
+      </c>
+      <c r="T245" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="246" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A246" s="11">
+        <v>45870</v>
+      </c>
+      <c r="B246" s="11">
+        <v>45870</v>
+      </c>
+      <c r="C246" s="11" t="s">
+        <v>128</v>
+      </c>
+      <c r="D246" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="E246" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="F246" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="G246" s="12" t="s">
+        <v>125</v>
+      </c>
+      <c r="H246" s="12" t="s">
+        <v>126</v>
+      </c>
+      <c r="I246" s="13">
+        <f>NETWORKDAYS(B246, A246)</f>
+        <v>1</v>
+      </c>
+      <c r="J246" s="12">
+        <v>66430</v>
+      </c>
+      <c r="K246" s="12">
+        <v>333</v>
+      </c>
+      <c r="L246" s="12" t="s">
+        <v>401</v>
+      </c>
+      <c r="M246" s="11">
+        <v>46113</v>
+      </c>
+      <c r="N246" s="14">
+        <v>281569.34000000003</v>
+      </c>
+      <c r="O246" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="P246" s="12">
+        <v>120</v>
+      </c>
+      <c r="Q246" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="R246" s="12">
+        <f>DATEDIF(Tabela1[[#This Row],[Atendimento]],Tabela1[[#This Row],[Previsao de Entrega]],"D")</f>
+        <v>243</v>
+      </c>
+      <c r="S246" s="14">
+        <v>0</v>
+      </c>
+      <c r="T246" s="14">
         <v>0</v>
       </c>
     </row>
@@ -17647,7 +18168,7 @@
       </c>
       <c r="E2" s="24">
         <f t="shared" ref="E2:E6" ca="1" si="0">TODAY()</f>
-        <v>45873</v>
+        <v>45874</v>
       </c>
       <c r="F2" s="22" t="str">
         <f ca="1">IF(Tabela4[[#This Row],[Hoje]] &lt;= Tabela4[[#This Row],[Validade]],
@@ -17655,7 +18176,7 @@
       "Negociar",
       "Faltam " &amp; DATEDIF(Tabela4[[#This Row],[Hoje]],Tabela4[[#This Row],[Validade]],"D") &amp; " dias para vencer"),
    "Venceu há " &amp; DATEDIF(Tabela4[[#This Row],[Validade]],Tabela4[[#This Row],[Hoje]],"D") &amp; " dias")</f>
-        <v>Faltam 593 dias para vencer</v>
+        <v>Faltam 592 dias para vencer</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.35">
@@ -17673,7 +18194,7 @@
       </c>
       <c r="E3" s="26">
         <f t="shared" ca="1" si="0"/>
-        <v>45873</v>
+        <v>45874</v>
       </c>
       <c r="F3" s="21" t="str">
         <f ca="1">IF(Tabela4[[#This Row],[Hoje]] &lt;= Tabela4[[#This Row],[Validade]],
@@ -17681,7 +18202,7 @@
       "Negociar",
       "Faltam " &amp; DATEDIF(Tabela4[[#This Row],[Hoje]],Tabela4[[#This Row],[Validade]],"D") &amp; " dias para vencer"),
    "Venceu há " &amp; DATEDIF(Tabela4[[#This Row],[Validade]],Tabela4[[#This Row],[Hoje]],"D") &amp; " dias")</f>
-        <v>Venceu há 307 dias</v>
+        <v>Venceu há 308 dias</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.35">
@@ -17699,7 +18220,7 @@
       </c>
       <c r="E4" s="36">
         <f t="shared" ca="1" si="0"/>
-        <v>45873</v>
+        <v>45874</v>
       </c>
       <c r="F4" s="37" t="str">
         <f ca="1">IF(Tabela4[[#This Row],[Hoje]] &lt;= Tabela4[[#This Row],[Validade]],
@@ -17707,7 +18228,7 @@
       "Negociar",
       "Faltam " &amp; DATEDIF(Tabela4[[#This Row],[Hoje]],Tabela4[[#This Row],[Validade]],"D") &amp; " dias para vencer"),
    "Venceu há " &amp; DATEDIF(Tabela4[[#This Row],[Validade]],Tabela4[[#This Row],[Hoje]],"D") &amp; " dias")</f>
-        <v>Venceu há 15 dias</v>
+        <v>Venceu há 16 dias</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.35">
@@ -17725,7 +18246,7 @@
       </c>
       <c r="E5" s="17">
         <f t="shared" ca="1" si="0"/>
-        <v>45873</v>
+        <v>45874</v>
       </c>
       <c r="F5" s="3" t="str">
         <f ca="1">IF(Tabela4[[#This Row],[Hoje]] &lt;= Tabela4[[#This Row],[Validade]],
@@ -17751,7 +18272,7 @@
       </c>
       <c r="E6" s="17">
         <f t="shared" ca="1" si="0"/>
-        <v>45873</v>
+        <v>45874</v>
       </c>
       <c r="F6" s="3" t="str">
         <f ca="1">IF(Tabela4[[#This Row],[Hoje]] &lt;= Tabela4[[#This Row],[Validade]],
@@ -17777,7 +18298,7 @@
       </c>
       <c r="E7" s="26">
         <f t="shared" ref="E7:E9" ca="1" si="1">TODAY()</f>
-        <v>45873</v>
+        <v>45874</v>
       </c>
       <c r="F7" s="21" t="str">
         <f ca="1">IF(Tabela4[[#This Row],[Hoje]] &lt;= Tabela4[[#This Row],[Validade]],
@@ -17785,7 +18306,7 @@
       "Negociar",
       "Faltam " &amp; DATEDIF(Tabela4[[#This Row],[Hoje]],Tabela4[[#This Row],[Validade]],"D") &amp; " dias para vencer"),
    "Venceu há " &amp; DATEDIF(Tabela4[[#This Row],[Validade]],Tabela4[[#This Row],[Hoje]],"D") &amp; " dias")</f>
-        <v>Venceu há 139 dias</v>
+        <v>Venceu há 140 dias</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.35">
@@ -17803,7 +18324,7 @@
       </c>
       <c r="E8" s="26">
         <f t="shared" ca="1" si="1"/>
-        <v>45873</v>
+        <v>45874</v>
       </c>
       <c r="F8" s="21" t="str">
         <f ca="1">IF(Tabela4[[#This Row],[Hoje]] &lt;= Tabela4[[#This Row],[Validade]],
@@ -17811,7 +18332,7 @@
       "Negociar",
       "Faltam " &amp; DATEDIF(Tabela4[[#This Row],[Hoje]],Tabela4[[#This Row],[Validade]],"D") &amp; " dias para vencer"),
    "Venceu há " &amp; DATEDIF(Tabela4[[#This Row],[Validade]],Tabela4[[#This Row],[Hoje]],"D") &amp; " dias")</f>
-        <v>Venceu há 882 dias</v>
+        <v>Venceu há 883 dias</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.35">
@@ -17829,7 +18350,7 @@
       </c>
       <c r="E9" s="24">
         <f t="shared" ca="1" si="1"/>
-        <v>45873</v>
+        <v>45874</v>
       </c>
       <c r="F9" s="22" t="str">
         <f ca="1">IF(Tabela4[[#This Row],[Hoje]] &lt;= Tabela4[[#This Row],[Validade]],
@@ -17837,7 +18358,7 @@
       "Negociar",
       "Faltam " &amp; DATEDIF(Tabela4[[#This Row],[Hoje]],Tabela4[[#This Row],[Validade]],"D") &amp; " dias para vencer"),
    "Venceu há " &amp; DATEDIF(Tabela4[[#This Row],[Validade]],Tabela4[[#This Row],[Hoje]],"D") &amp; " dias")</f>
-        <v>Faltam 409 dias para vencer</v>
+        <v>Faltam 408 dias para vencer</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.35">
@@ -17855,7 +18376,7 @@
       </c>
       <c r="E10" s="24">
         <f ca="1">TODAY()</f>
-        <v>45873</v>
+        <v>45874</v>
       </c>
       <c r="F10" s="22" t="str">
         <f ca="1">IF(Tabela4[[#This Row],[Hoje]] &lt;= Tabela4[[#This Row],[Validade]],
@@ -17863,7 +18384,7 @@
       "Negociar",
       "Faltam " &amp; DATEDIF(Tabela4[[#This Row],[Hoje]],Tabela4[[#This Row],[Validade]],"D") &amp; " dias para vencer"),
    "Venceu há " &amp; DATEDIF(Tabela4[[#This Row],[Validade]],Tabela4[[#This Row],[Hoje]],"D") &amp; " dias")</f>
-        <v>Faltam 330 dias para vencer</v>
+        <v>Faltam 329 dias para vencer</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.35">
@@ -17881,7 +18402,7 @@
       </c>
       <c r="E11" s="24">
         <f ca="1">TODAY()</f>
-        <v>45873</v>
+        <v>45874</v>
       </c>
       <c r="F11" s="22" t="str">
         <f ca="1">IF(Tabela4[[#This Row],[Hoje]] &lt;= Tabela4[[#This Row],[Validade]],
@@ -17889,7 +18410,7 @@
       "Negociar",
       "Faltam " &amp; DATEDIF(Tabela4[[#This Row],[Hoje]],Tabela4[[#This Row],[Validade]],"D") &amp; " dias para vencer"),
    "Venceu há " &amp; DATEDIF(Tabela4[[#This Row],[Validade]],Tabela4[[#This Row],[Hoje]],"D") &amp; " dias")</f>
-        <v>Faltam 119 dias para vencer</v>
+        <v>Faltam 118 dias para vencer</v>
       </c>
     </row>
   </sheetData>
@@ -17911,7 +18432,7 @@
   <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B48" sqref="B48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -18629,10 +19150,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CC6577E-1BBE-47C5-96B8-0E0691F59A60}">
-  <dimension ref="A1:E36"/>
+  <dimension ref="A1:E38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -19254,6 +19775,40 @@
       </c>
       <c r="E36" t="s">
         <v>390</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A37" s="17">
+        <v>45873</v>
+      </c>
+      <c r="B37" t="s">
+        <v>286</v>
+      </c>
+      <c r="C37" t="s">
+        <v>287</v>
+      </c>
+      <c r="D37">
+        <v>11790</v>
+      </c>
+      <c r="E37" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A38" s="17">
+        <v>45874</v>
+      </c>
+      <c r="B38" t="s">
+        <v>286</v>
+      </c>
+      <c r="C38" t="s">
+        <v>287</v>
+      </c>
+      <c r="D38">
+        <v>11791</v>
+      </c>
+      <c r="E38" t="s">
+        <v>403</v>
       </c>
     </row>
   </sheetData>
@@ -19314,6 +19869,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010068C9492B0923CC418696A025D9B79530" ma:contentTypeVersion="1" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="12b5152450087b045156d8e5bdb7ac17">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="b7545978-8353-4157-ab02-92f5c69a97d9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="74a8823586b7fc5940aaf3e9d5b706e7" ns3:_="">
     <xsd:import namespace="b7545978-8353-4157-ab02-92f5c69a97d9"/>
@@ -19439,22 +20009,31 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{258E5A34-0198-4570-927D-9873053383F0}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="b7545978-8353-4157-ab02-92f5c69a97d9"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F1DB20CA-6C9E-462A-9B1E-209C1B3156BD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AED76536-08DB-4BCA-BAA6-597FC860B20C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -19470,28 +20049,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F1DB20CA-6C9E-462A-9B1E-209C1B3156BD}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{258E5A34-0198-4570-927D-9873053383F0}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="b7545978-8353-4157-ab02-92f5c69a97d9"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Atualização de Base = 12/08
</commit_message>
<xml_diff>
--- a/Atendimento.xlsx
+++ b/Atendimento.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\splfps01\data$\GROUP\PUBLICO\Compras\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\PUBLICO\Compras\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9348A454-B154-4B28-BAF7-6870D59D9686}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD5D64EC-004E-4BD4-9486-EA96EC0B9A6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="base_dados" sheetId="1" r:id="rId1"/>
@@ -76,7 +76,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2545" uniqueCount="409">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2574" uniqueCount="411">
   <si>
     <t>SC</t>
   </si>
@@ -1303,6 +1303,12 @@
   </si>
   <si>
     <t>METALEX FERRAMENTARIA INDUSTRIA E COMERCIO LTDA</t>
+  </si>
+  <si>
+    <t>Gabriela</t>
+  </si>
+  <si>
+    <t>C T MOL PINTURAS LTDA – ME</t>
   </si>
 </sst>
 </file>
@@ -1446,7 +1452,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1565,9 +1571,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1751,8 +1754,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0C573FEE-B8A0-4FE7-911C-81B026DE4530}" name="Tabela1" displayName="Tabela1" ref="A1:T254" totalsRowShown="0" headerRowDxfId="36" dataDxfId="35">
-  <autoFilter ref="A1:T254" xr:uid="{0C573FEE-B8A0-4FE7-911C-81B026DE4530}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0C573FEE-B8A0-4FE7-911C-81B026DE4530}" name="Tabela1" displayName="Tabela1" ref="A1:T257" totalsRowShown="0" headerRowDxfId="36" dataDxfId="35">
+  <autoFilter ref="A1:T257" xr:uid="{0C573FEE-B8A0-4FE7-911C-81B026DE4530}">
     <filterColumn colId="16">
       <filters>
         <filter val="AGUARDANDO APROVAÇÃO"/>
@@ -1760,8 +1763,8 @@
       </filters>
     </filterColumn>
   </autoFilter>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A11:T252">
-    <sortCondition ref="M1:M254"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A11:T257">
+    <sortCondition ref="M1:M257"/>
   </sortState>
   <tableColumns count="20">
     <tableColumn id="1" xr3:uid="{FD977268-8F92-4E92-82D7-959136F54294}" name="Atendimento" dataDxfId="34"/>
@@ -1850,8 +1853,8 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{BB230BD9-36EF-4D37-BEB8-0438680DF5A9}" name="Tabela6" displayName="Tabela6" ref="A1:E40" totalsRowShown="0">
-  <autoFilter ref="A1:E40" xr:uid="{BB230BD9-36EF-4D37-BEB8-0438680DF5A9}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{BB230BD9-36EF-4D37-BEB8-0438680DF5A9}" name="Tabela6" displayName="Tabela6" ref="A1:E41" totalsRowShown="0">
+  <autoFilter ref="A1:E41" xr:uid="{BB230BD9-36EF-4D37-BEB8-0438680DF5A9}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{40ADAE7E-AD00-4188-9DB3-F04A606A9D2B}" name="data"/>
     <tableColumn id="2" xr3:uid="{D9B738D8-98DD-4AD6-8BCF-D51CBE71FF94}" name="solicitante"/>
@@ -2126,35 +2129,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T254"/>
+  <dimension ref="A1:T257"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L188" sqref="L188"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H233" sqref="H233"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="18" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="16.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="16.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.81640625" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17.81640625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.7265625" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="7.453125" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="19.7265625" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="20.1796875" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="27.81640625" style="9" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.6328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="19.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="76.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="22.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="76.7265625" style="1" customWidth="1"/>
+    <col min="13" max="13" width="22.453125" style="1" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="15.26953125" style="2" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="15.81640625" style="1" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="26.1796875" style="1" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="25.1796875" style="1" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="26.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="12.6328125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12.54296875" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="19.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="16384" width="18" style="1"/>
+    <col min="21" max="16384" width="16.81640625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.35">
@@ -2821,7 +2824,7 @@
         <v>364</v>
       </c>
       <c r="I11" s="13">
-        <f>NETWORKDAYS(B11, A11)</f>
+        <f t="shared" ref="I11:I74" si="1">NETWORKDAYS(B11, A11)</f>
         <v>1</v>
       </c>
       <c r="J11" s="12">
@@ -2885,7 +2888,7 @@
         <v>32</v>
       </c>
       <c r="I12" s="10">
-        <f>NETWORKDAYS(B12, A12)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="J12" s="7">
@@ -2949,7 +2952,7 @@
         <v>138</v>
       </c>
       <c r="I13" s="10">
-        <f>NETWORKDAYS(B13, A13)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="J13" s="7">
@@ -3013,7 +3016,7 @@
         <v>32</v>
       </c>
       <c r="I14" s="10">
-        <f>NETWORKDAYS(B14, A14)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="J14" s="7">
@@ -3077,7 +3080,7 @@
         <v>91</v>
       </c>
       <c r="I15" s="10">
-        <f>NETWORKDAYS(B15, A15)</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="J15" s="7">
@@ -3141,7 +3144,7 @@
         <v>91</v>
       </c>
       <c r="I16" s="10">
-        <f>NETWORKDAYS(B16, A16)</f>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="J16" s="7">
@@ -3205,7 +3208,7 @@
         <v>34</v>
       </c>
       <c r="I17" s="10">
-        <f>NETWORKDAYS(B17, A17)</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="J17" s="7">
@@ -3269,7 +3272,7 @@
         <v>34</v>
       </c>
       <c r="I18" s="10">
-        <f>NETWORKDAYS(B18, A18)</f>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="J18" s="7">
@@ -3333,7 +3336,7 @@
         <v>91</v>
       </c>
       <c r="I19" s="10">
-        <f>NETWORKDAYS(B19, A19)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="J19" s="7">
@@ -3397,7 +3400,7 @@
         <v>32</v>
       </c>
       <c r="I20" s="10">
-        <f>NETWORKDAYS(B20, A20)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="J20" s="7">
@@ -3461,7 +3464,7 @@
         <v>98</v>
       </c>
       <c r="I21" s="10">
-        <f>NETWORKDAYS(B21, A21)</f>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="J21" s="7">
@@ -3525,7 +3528,7 @@
         <v>98</v>
       </c>
       <c r="I22" s="10">
-        <f>NETWORKDAYS(B22, A22)</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="J22" s="7">
@@ -3589,7 +3592,7 @@
         <v>96</v>
       </c>
       <c r="I23" s="30">
-        <f>NETWORKDAYS(B23, A23)</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="J23" s="28">
@@ -3653,7 +3656,7 @@
         <v>34</v>
       </c>
       <c r="I24" s="10">
-        <f>NETWORKDAYS(B24, A24)</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="J24" s="7">
@@ -3717,7 +3720,7 @@
         <v>126</v>
       </c>
       <c r="I25" s="10">
-        <f>NETWORKDAYS(B25, A25)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="J25" s="7">
@@ -3781,7 +3784,7 @@
         <v>130</v>
       </c>
       <c r="I26" s="10">
-        <f>NETWORKDAYS(B26, A26)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="J26" s="7">
@@ -3845,7 +3848,7 @@
         <v>32</v>
       </c>
       <c r="I27" s="10">
-        <f>NETWORKDAYS(B27, A27)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="J27" s="7">
@@ -3909,7 +3912,7 @@
         <v>32</v>
       </c>
       <c r="I28" s="10">
-        <f>NETWORKDAYS(B28, A28)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="J28" s="7">
@@ -3973,7 +3976,7 @@
         <v>32</v>
       </c>
       <c r="I29" s="10">
-        <f>NETWORKDAYS(B29, A29)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="J29" s="7">
@@ -4037,7 +4040,7 @@
         <v>138</v>
       </c>
       <c r="I30" s="10">
-        <f>NETWORKDAYS(B30, A30)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="J30" s="7">
@@ -4101,7 +4104,7 @@
         <v>32</v>
       </c>
       <c r="I31" s="10">
-        <f>NETWORKDAYS(B31, A31)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="J31" s="7">
@@ -4165,7 +4168,7 @@
         <v>130</v>
       </c>
       <c r="I32" s="10">
-        <f>NETWORKDAYS(B32, A32)</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="J32" s="7">
@@ -4229,7 +4232,7 @@
         <v>130</v>
       </c>
       <c r="I33" s="10">
-        <f>NETWORKDAYS(B33, A33)</f>
+        <f t="shared" si="1"/>
         <v>36</v>
       </c>
       <c r="J33" s="7">
@@ -4293,7 +4296,7 @@
         <v>34</v>
       </c>
       <c r="I34" s="10">
-        <f>NETWORKDAYS(B34, A34)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="J34" s="7">
@@ -4357,7 +4360,7 @@
         <v>130</v>
       </c>
       <c r="I35" s="10">
-        <f>NETWORKDAYS(B35, A35)</f>
+        <f t="shared" si="1"/>
         <v>37</v>
       </c>
       <c r="J35" s="7">
@@ -4421,7 +4424,7 @@
         <v>98</v>
       </c>
       <c r="I36" s="10">
-        <f>NETWORKDAYS(B36, A36)</f>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="J36" s="7">
@@ -4485,7 +4488,7 @@
         <v>91</v>
       </c>
       <c r="I37" s="10">
-        <f>NETWORKDAYS(B37, A37)</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="J37" s="7">
@@ -4549,7 +4552,7 @@
         <v>91</v>
       </c>
       <c r="I38" s="10">
-        <f>NETWORKDAYS(B38, A38)</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="J38" s="7">
@@ -4613,7 +4616,7 @@
         <v>130</v>
       </c>
       <c r="I39" s="10">
-        <f>NETWORKDAYS(B39, A39)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="J39" s="7">
@@ -4677,7 +4680,7 @@
         <v>32</v>
       </c>
       <c r="I40" s="10">
-        <f>NETWORKDAYS(B40, A40)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="J40" s="7">
@@ -4741,7 +4744,7 @@
         <v>98</v>
       </c>
       <c r="I41" s="10">
-        <f>NETWORKDAYS(B41, A41)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="J41" s="7">
@@ -4805,7 +4808,7 @@
         <v>34</v>
       </c>
       <c r="I42" s="10">
-        <f>NETWORKDAYS(B42, A42)</f>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="J42" s="7">
@@ -4869,7 +4872,7 @@
         <v>130</v>
       </c>
       <c r="I43" s="10">
-        <f>NETWORKDAYS(B43, A43)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="J43" s="7">
@@ -4933,7 +4936,7 @@
         <v>34</v>
       </c>
       <c r="I44" s="10">
-        <f>NETWORKDAYS(B44, A44)</f>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="J44" s="7">
@@ -4997,7 +5000,7 @@
         <v>34</v>
       </c>
       <c r="I45" s="10">
-        <f>NETWORKDAYS(B45, A45)</f>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="J45" s="7">
@@ -5061,7 +5064,7 @@
         <v>32</v>
       </c>
       <c r="I46" s="10">
-        <f>NETWORKDAYS(B46, A46)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="J46" s="7">
@@ -5125,7 +5128,7 @@
         <v>32</v>
       </c>
       <c r="I47" s="10">
-        <f>NETWORKDAYS(B47, A47)</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="J47" s="7">
@@ -5189,7 +5192,7 @@
         <v>130</v>
       </c>
       <c r="I48" s="10">
-        <f>NETWORKDAYS(B48, A48)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="J48" s="7">
@@ -5253,7 +5256,7 @@
         <v>130</v>
       </c>
       <c r="I49" s="10">
-        <f>NETWORKDAYS(B49, A49)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="J49" s="7">
@@ -5317,7 +5320,7 @@
         <v>130</v>
       </c>
       <c r="I50" s="10">
-        <f>NETWORKDAYS(B50, A50)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="J50" s="7">
@@ -5381,7 +5384,7 @@
         <v>130</v>
       </c>
       <c r="I51" s="10">
-        <f>NETWORKDAYS(B51, A51)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="J51" s="7">
@@ -5445,7 +5448,7 @@
         <v>98</v>
       </c>
       <c r="I52" s="10">
-        <f>NETWORKDAYS(B52, A52)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="J52" s="7">
@@ -5509,7 +5512,7 @@
         <v>98</v>
       </c>
       <c r="I53" s="10">
-        <f>NETWORKDAYS(B53, A53)</f>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="J53" s="7">
@@ -5573,7 +5576,7 @@
         <v>34</v>
       </c>
       <c r="I54" s="10">
-        <f>NETWORKDAYS(B54, A54)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="J54" s="7">
@@ -5637,7 +5640,7 @@
         <v>126</v>
       </c>
       <c r="I55" s="10">
-        <f>NETWORKDAYS(B55, A55)</f>
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="J55" s="7">
@@ -5701,7 +5704,7 @@
         <v>130</v>
       </c>
       <c r="I56" s="10">
-        <f>NETWORKDAYS(B56, A56)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="J56" s="7">
@@ -5765,7 +5768,7 @@
         <v>96</v>
       </c>
       <c r="I57" s="10">
-        <f>NETWORKDAYS(B57, A57)</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="J57" s="7">
@@ -5829,7 +5832,7 @@
         <v>32</v>
       </c>
       <c r="I58" s="10">
-        <f>NETWORKDAYS(B58, A58)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="J58" s="7">
@@ -5893,7 +5896,7 @@
         <v>32</v>
       </c>
       <c r="I59" s="10">
-        <f>NETWORKDAYS(B59, A59)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="J59" s="7">
@@ -5957,7 +5960,7 @@
         <v>32</v>
       </c>
       <c r="I60" s="10">
-        <f>NETWORKDAYS(B60, A60)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="J60" s="7">
@@ -6021,7 +6024,7 @@
         <v>34</v>
       </c>
       <c r="I61" s="10">
-        <f>NETWORKDAYS(B61, A61)</f>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="J61" s="7">
@@ -6085,7 +6088,7 @@
         <v>130</v>
       </c>
       <c r="I62" s="10">
-        <f>NETWORKDAYS(B62, A62)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="J62" s="7">
@@ -6149,7 +6152,7 @@
         <v>34</v>
       </c>
       <c r="I63" s="10">
-        <f>NETWORKDAYS(B63, A63)</f>
+        <f t="shared" si="1"/>
         <v>18</v>
       </c>
       <c r="J63" s="7">
@@ -6213,7 +6216,7 @@
         <v>91</v>
       </c>
       <c r="I64" s="10">
-        <f>NETWORKDAYS(B64, A64)</f>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="J64" s="7">
@@ -6277,7 +6280,7 @@
         <v>98</v>
       </c>
       <c r="I65" s="10">
-        <f>NETWORKDAYS(B65, A65)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="J65" s="7">
@@ -6341,7 +6344,7 @@
         <v>98</v>
       </c>
       <c r="I66" s="10">
-        <f>NETWORKDAYS(B66, A66)</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="J66" s="7">
@@ -6405,7 +6408,7 @@
         <v>91</v>
       </c>
       <c r="I67" s="10">
-        <f>NETWORKDAYS(B67, A67)</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="J67" s="7">
@@ -6469,7 +6472,7 @@
         <v>32</v>
       </c>
       <c r="I68" s="10">
-        <f>NETWORKDAYS(B68, A68)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="J68" s="7">
@@ -6533,7 +6536,7 @@
         <v>34</v>
       </c>
       <c r="I69" s="10">
-        <f>NETWORKDAYS(B69, A69)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="J69" s="7">
@@ -6597,7 +6600,7 @@
         <v>98</v>
       </c>
       <c r="I70" s="10">
-        <f>NETWORKDAYS(B70, A70)</f>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="J70" s="7">
@@ -6661,7 +6664,7 @@
         <v>98</v>
       </c>
       <c r="I71" s="10">
-        <f>NETWORKDAYS(B71, A71)</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="J71" s="7">
@@ -6725,7 +6728,7 @@
         <v>98</v>
       </c>
       <c r="I72" s="10">
-        <f>NETWORKDAYS(B72, A72)</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="J72" s="7">
@@ -6789,7 +6792,7 @@
         <v>98</v>
       </c>
       <c r="I73" s="10">
-        <f>NETWORKDAYS(B73, A73)</f>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="J73" s="7">
@@ -6853,7 +6856,7 @@
         <v>98</v>
       </c>
       <c r="I74" s="10">
-        <f>NETWORKDAYS(B74, A74)</f>
+        <f t="shared" si="1"/>
         <v>26</v>
       </c>
       <c r="J74" s="7">
@@ -6917,7 +6920,7 @@
         <v>98</v>
       </c>
       <c r="I75" s="10">
-        <f>NETWORKDAYS(B75, A75)</f>
+        <f t="shared" ref="I75:I138" si="2">NETWORKDAYS(B75, A75)</f>
         <v>6</v>
       </c>
       <c r="J75" s="7">
@@ -6981,7 +6984,7 @@
         <v>91</v>
       </c>
       <c r="I76" s="10">
-        <f>NETWORKDAYS(B76, A76)</f>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="J76" s="7">
@@ -7045,7 +7048,7 @@
         <v>98</v>
       </c>
       <c r="I77" s="10">
-        <f>NETWORKDAYS(B77, A77)</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="J77" s="7">
@@ -7109,7 +7112,7 @@
         <v>32</v>
       </c>
       <c r="I78" s="10">
-        <f>NETWORKDAYS(B78, A78)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="J78" s="7">
@@ -7173,7 +7176,7 @@
         <v>32</v>
       </c>
       <c r="I79" s="10">
-        <f>NETWORKDAYS(B79, A79)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="J79" s="7">
@@ -7237,7 +7240,7 @@
         <v>138</v>
       </c>
       <c r="I80" s="10">
-        <f>NETWORKDAYS(B80, A80)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="J80" s="7">
@@ -7301,7 +7304,7 @@
         <v>130</v>
       </c>
       <c r="I81" s="10">
-        <f>NETWORKDAYS(B81, A81)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="J81" s="7">
@@ -7365,7 +7368,7 @@
         <v>98</v>
       </c>
       <c r="I82" s="10">
-        <f>NETWORKDAYS(B82, A82)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="J82" s="7">
@@ -7429,7 +7432,7 @@
         <v>130</v>
       </c>
       <c r="I83" s="10">
-        <f>NETWORKDAYS(B83, A83)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="J83" s="7">
@@ -7493,7 +7496,7 @@
         <v>98</v>
       </c>
       <c r="I84" s="10">
-        <f>NETWORKDAYS(B84, A84)</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="J84" s="7">
@@ -7557,7 +7560,7 @@
         <v>98</v>
       </c>
       <c r="I85" s="10">
-        <f>NETWORKDAYS(B85, A85)</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="J85" s="7">
@@ -7621,7 +7624,7 @@
         <v>34</v>
       </c>
       <c r="I86" s="30">
-        <f>NETWORKDAYS(B86, A86)</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="J86" s="28">
@@ -7682,10 +7685,10 @@
         <v>3</v>
       </c>
       <c r="H87" s="7" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="I87" s="10">
-        <f>NETWORKDAYS(B87, A87)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="J87" s="7">
@@ -7749,7 +7752,7 @@
         <v>32</v>
       </c>
       <c r="I88" s="10">
-        <f>NETWORKDAYS(B88, A88)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="J88" s="7">
@@ -7813,7 +7816,7 @@
         <v>126</v>
       </c>
       <c r="I89" s="10">
-        <f>NETWORKDAYS(B89, A89)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="J89" s="7">
@@ -7877,7 +7880,7 @@
         <v>98</v>
       </c>
       <c r="I90" s="10">
-        <f>NETWORKDAYS(B90, A90)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="J90" s="7">
@@ -7941,7 +7944,7 @@
         <v>32</v>
       </c>
       <c r="I91" s="10">
-        <f>NETWORKDAYS(B91, A91)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="J91" s="7">
@@ -8005,7 +8008,7 @@
         <v>98</v>
       </c>
       <c r="I92" s="10">
-        <f>NETWORKDAYS(B92, A92)</f>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="J92" s="7">
@@ -8069,7 +8072,7 @@
         <v>126</v>
       </c>
       <c r="I93" s="10">
-        <f>NETWORKDAYS(B93, A93)</f>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="J93" s="7">
@@ -8133,7 +8136,7 @@
         <v>126</v>
       </c>
       <c r="I94" s="10">
-        <f>NETWORKDAYS(B94, A94)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="J94" s="7">
@@ -8197,7 +8200,7 @@
         <v>34</v>
       </c>
       <c r="I95" s="10">
-        <f>NETWORKDAYS(B95, A95)</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="J95" s="7">
@@ -8261,7 +8264,7 @@
         <v>130</v>
       </c>
       <c r="I96" s="10">
-        <f>NETWORKDAYS(B96, A96)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="J96" s="7">
@@ -8325,7 +8328,7 @@
         <v>138</v>
       </c>
       <c r="I97" s="10">
-        <f>NETWORKDAYS(B97, A97)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="J97" s="7">
@@ -8389,7 +8392,7 @@
         <v>98</v>
       </c>
       <c r="I98" s="10">
-        <f>NETWORKDAYS(B98, A98)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="J98" s="7">
@@ -8453,7 +8456,7 @@
         <v>130</v>
       </c>
       <c r="I99" s="10">
-        <f>NETWORKDAYS(B99, A99)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="J99" s="7">
@@ -8517,7 +8520,7 @@
         <v>130</v>
       </c>
       <c r="I100" s="10">
-        <f>NETWORKDAYS(B100, A100)</f>
+        <f t="shared" si="2"/>
         <v>24</v>
       </c>
       <c r="J100" s="7">
@@ -8581,7 +8584,7 @@
         <v>126</v>
       </c>
       <c r="I101" s="10">
-        <f>NETWORKDAYS(B101, A101)</f>
+        <f t="shared" si="2"/>
         <v>25</v>
       </c>
       <c r="J101" s="7">
@@ -8645,7 +8648,7 @@
         <v>98</v>
       </c>
       <c r="I102" s="10">
-        <f>NETWORKDAYS(B102, A102)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="J102" s="7">
@@ -8709,7 +8712,7 @@
         <v>91</v>
       </c>
       <c r="I103" s="10">
-        <f>NETWORKDAYS(B103, A103)</f>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="J103" s="7">
@@ -8773,7 +8776,7 @@
         <v>91</v>
       </c>
       <c r="I104" s="10">
-        <f>NETWORKDAYS(B104, A104)</f>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="J104" s="7">
@@ -8837,7 +8840,7 @@
         <v>32</v>
       </c>
       <c r="I105" s="10">
-        <f>NETWORKDAYS(B105, A105)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="J105" s="7">
@@ -8901,7 +8904,7 @@
         <v>32</v>
       </c>
       <c r="I106" s="10">
-        <f>NETWORKDAYS(B106, A106)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="J106" s="7">
@@ -8965,7 +8968,7 @@
         <v>98</v>
       </c>
       <c r="I107" s="10">
-        <f>NETWORKDAYS(B107, A107)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="J107" s="7">
@@ -9029,7 +9032,7 @@
         <v>96</v>
       </c>
       <c r="I108" s="10">
-        <f>NETWORKDAYS(B108, A108)</f>
+        <f t="shared" si="2"/>
         <v>6</v>
       </c>
       <c r="J108" s="7">
@@ -9093,7 +9096,7 @@
         <v>91</v>
       </c>
       <c r="I109" s="10">
-        <f>NETWORKDAYS(B109, A109)</f>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="J109" s="7">
@@ -9157,7 +9160,7 @@
         <v>91</v>
       </c>
       <c r="I110" s="10">
-        <f>NETWORKDAYS(B110, A110)</f>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="J110" s="7">
@@ -9221,7 +9224,7 @@
         <v>91</v>
       </c>
       <c r="I111" s="10">
-        <f>NETWORKDAYS(B111, A111)</f>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="J111" s="7">
@@ -9285,7 +9288,7 @@
         <v>126</v>
       </c>
       <c r="I112" s="10">
-        <f>NETWORKDAYS(B112, A112)</f>
+        <f t="shared" si="2"/>
         <v>9</v>
       </c>
       <c r="J112" s="7">
@@ -9349,7 +9352,7 @@
         <v>32</v>
       </c>
       <c r="I113" s="10">
-        <f>NETWORKDAYS(B113, A113)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="J113" s="7">
@@ -9413,7 +9416,7 @@
         <v>96</v>
       </c>
       <c r="I114" s="10">
-        <f>NETWORKDAYS(B114, A114)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="J114" s="7">
@@ -9477,7 +9480,7 @@
         <v>91</v>
       </c>
       <c r="I115" s="10">
-        <f>NETWORKDAYS(B115, A115)</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="J115" s="7">
@@ -9541,7 +9544,7 @@
         <v>32</v>
       </c>
       <c r="I116" s="10">
-        <f>NETWORKDAYS(B116, A116)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="J116" s="7">
@@ -9605,7 +9608,7 @@
         <v>98</v>
       </c>
       <c r="I117" s="10">
-        <f>NETWORKDAYS(B117, A117)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="J117" s="7">
@@ -9669,7 +9672,7 @@
         <v>91</v>
       </c>
       <c r="I118" s="10">
-        <f>NETWORKDAYS(B118, A118)</f>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="J118" s="7">
@@ -9733,7 +9736,7 @@
         <v>91</v>
       </c>
       <c r="I119" s="10">
-        <f>NETWORKDAYS(B119, A119)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="J119" s="7">
@@ -9797,7 +9800,7 @@
         <v>91</v>
       </c>
       <c r="I120" s="10">
-        <f>NETWORKDAYS(B120, A120)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="J120" s="7">
@@ -9861,7 +9864,7 @@
         <v>98</v>
       </c>
       <c r="I121" s="10">
-        <f>NETWORKDAYS(B121, A121)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="J121" s="7">
@@ -9925,7 +9928,7 @@
         <v>126</v>
       </c>
       <c r="I122" s="10">
-        <f>NETWORKDAYS(B122, A122)</f>
+        <f t="shared" si="2"/>
         <v>18</v>
       </c>
       <c r="J122" s="7">
@@ -9989,7 +9992,7 @@
         <v>91</v>
       </c>
       <c r="I123" s="10">
-        <f>NETWORKDAYS(B123, A123)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="J123" s="7">
@@ -10050,10 +10053,10 @@
         <v>3</v>
       </c>
       <c r="H124" s="7" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="I124" s="10">
-        <f>NETWORKDAYS(B124, A124)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="J124" s="7">
@@ -10117,7 +10120,7 @@
         <v>130</v>
       </c>
       <c r="I125" s="10">
-        <f>NETWORKDAYS(B125, A125)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="J125" s="7">
@@ -10181,7 +10184,7 @@
         <v>130</v>
       </c>
       <c r="I126" s="10">
-        <f>NETWORKDAYS(B126, A126)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="J126" s="7">
@@ -10245,7 +10248,7 @@
         <v>98</v>
       </c>
       <c r="I127" s="10">
-        <f>NETWORKDAYS(B127, A127)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="J127" s="7">
@@ -10309,7 +10312,7 @@
         <v>130</v>
       </c>
       <c r="I128" s="10">
-        <f>NETWORKDAYS(B128, A128)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="J128" s="7">
@@ -10373,7 +10376,7 @@
         <v>32</v>
       </c>
       <c r="I129" s="10">
-        <f>NETWORKDAYS(B129, A129)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="J129" s="7">
@@ -10437,7 +10440,7 @@
         <v>32</v>
       </c>
       <c r="I130" s="10">
-        <f>NETWORKDAYS(B130, A130)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="J130" s="7">
@@ -10501,7 +10504,7 @@
         <v>91</v>
       </c>
       <c r="I131" s="10">
-        <f>NETWORKDAYS(B131, A131)</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="J131" s="7">
@@ -10565,7 +10568,7 @@
         <v>126</v>
       </c>
       <c r="I132" s="10">
-        <f>NETWORKDAYS(B132, A132)</f>
+        <f t="shared" si="2"/>
         <v>28</v>
       </c>
       <c r="J132" s="7">
@@ -10629,7 +10632,7 @@
         <v>98</v>
       </c>
       <c r="I133" s="10">
-        <f>NETWORKDAYS(B133, A133)</f>
+        <f t="shared" si="2"/>
         <v>7</v>
       </c>
       <c r="J133" s="7">
@@ -10693,7 +10696,7 @@
         <v>126</v>
       </c>
       <c r="I134" s="10">
-        <f>NETWORKDAYS(B134, A134)</f>
+        <f t="shared" si="2"/>
         <v>6</v>
       </c>
       <c r="J134" s="7">
@@ -10757,7 +10760,7 @@
         <v>126</v>
       </c>
       <c r="I135" s="10">
-        <f>NETWORKDAYS(B135, A135)</f>
+        <f t="shared" si="2"/>
         <v>7</v>
       </c>
       <c r="J135" s="7">
@@ -10821,7 +10824,7 @@
         <v>32</v>
       </c>
       <c r="I136" s="10">
-        <f>NETWORKDAYS(B136, A136)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="J136" s="7">
@@ -10885,7 +10888,7 @@
         <v>98</v>
       </c>
       <c r="I137" s="10">
-        <f>NETWORKDAYS(B137, A137)</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="J137" s="7">
@@ -10949,7 +10952,7 @@
         <v>98</v>
       </c>
       <c r="I138" s="10">
-        <f>NETWORKDAYS(B138, A138)</f>
+        <f t="shared" si="2"/>
         <v>7</v>
       </c>
       <c r="J138" s="7">
@@ -11013,7 +11016,7 @@
         <v>98</v>
       </c>
       <c r="I139" s="10">
-        <f>NETWORKDAYS(B139, A139)</f>
+        <f t="shared" ref="I139:I202" si="3">NETWORKDAYS(B139, A139)</f>
         <v>18</v>
       </c>
       <c r="J139" s="7">
@@ -11077,7 +11080,7 @@
         <v>91</v>
       </c>
       <c r="I140" s="10">
-        <f>NETWORKDAYS(B140, A140)</f>
+        <f t="shared" si="3"/>
         <v>6</v>
       </c>
       <c r="J140" s="7">
@@ -11141,7 +11144,7 @@
         <v>130</v>
       </c>
       <c r="I141" s="10">
-        <f>NETWORKDAYS(B141, A141)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="J141" s="7">
@@ -11205,7 +11208,7 @@
         <v>372</v>
       </c>
       <c r="I142" s="10">
-        <f>NETWORKDAYS(B142, A142)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="J142" s="7">
@@ -11269,7 +11272,7 @@
         <v>98</v>
       </c>
       <c r="I143" s="10">
-        <f>NETWORKDAYS(B143, A143)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="J143" s="7">
@@ -11333,7 +11336,7 @@
         <v>34</v>
       </c>
       <c r="I144" s="10">
-        <f>NETWORKDAYS(B144, A144)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="J144" s="7">
@@ -11397,7 +11400,7 @@
         <v>126</v>
       </c>
       <c r="I145" s="10">
-        <f>NETWORKDAYS(B145, A145)</f>
+        <f t="shared" si="3"/>
         <v>12</v>
       </c>
       <c r="J145" s="7">
@@ -11435,67 +11438,67 @@
         <v>0</v>
       </c>
     </row>
-    <row r="146" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A146" s="11">
+    <row r="146" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A146" s="6">
         <v>45818</v>
       </c>
-      <c r="B146" s="11">
+      <c r="B146" s="6">
         <v>45813</v>
       </c>
-      <c r="C146" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="D146" s="11" t="s">
+      <c r="C146" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D146" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="E146" s="11" t="s">
+      <c r="E146" s="6" t="s">
         <v>124</v>
       </c>
-      <c r="F146" s="12">
+      <c r="F146" s="7">
         <v>68422</v>
       </c>
-      <c r="G146" s="12" t="s">
+      <c r="G146" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="H146" s="12" t="s">
+      <c r="H146" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="I146" s="13">
-        <f>NETWORKDAYS(B146, A146)</f>
+      <c r="I146" s="10">
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
-      <c r="J146" s="12">
+      <c r="J146" s="7">
         <v>65725</v>
       </c>
-      <c r="K146" s="12">
+      <c r="K146" s="7">
         <v>1450</v>
       </c>
-      <c r="L146" s="12" t="s">
+      <c r="L146" s="7" t="s">
         <v>229</v>
       </c>
-      <c r="M146" s="11">
+      <c r="M146" s="6">
         <v>45877</v>
       </c>
-      <c r="N146" s="14">
+      <c r="N146" s="8">
         <v>239.63</v>
       </c>
-      <c r="O146" s="12" t="s">
+      <c r="O146" s="7" t="s">
         <v>122</v>
       </c>
-      <c r="P146" s="12">
+      <c r="P146" s="7">
         <v>120</v>
       </c>
-      <c r="Q146" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="R146" s="12">
+      <c r="Q146" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="R146" s="7">
         <f>DATEDIF(Tabela1[[#This Row],[Atendimento]],Tabela1[[#This Row],[Previsao de Entrega]],"D")</f>
         <v>59</v>
       </c>
-      <c r="S146" s="14">
-        <v>0</v>
-      </c>
-      <c r="T146" s="14">
+      <c r="S146" s="8">
+        <v>0</v>
+      </c>
+      <c r="T146" s="8">
         <v>0</v>
       </c>
     </row>
@@ -11525,7 +11528,7 @@
         <v>98</v>
       </c>
       <c r="I147" s="10">
-        <f>NETWORKDAYS(B147, A147)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="J147" s="7">
@@ -11589,7 +11592,7 @@
         <v>138</v>
       </c>
       <c r="I148" s="10">
-        <f>NETWORKDAYS(B148, A148)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="J148" s="7">
@@ -11653,7 +11656,7 @@
         <v>91</v>
       </c>
       <c r="I149" s="10">
-        <f>NETWORKDAYS(B149, A149)</f>
+        <f t="shared" si="3"/>
         <v>9</v>
       </c>
       <c r="J149" s="7">
@@ -11717,7 +11720,7 @@
         <v>130</v>
       </c>
       <c r="I150" s="10">
-        <f>NETWORKDAYS(B150, A150)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="J150" s="7">
@@ -11781,7 +11784,7 @@
         <v>32</v>
       </c>
       <c r="I151" s="10">
-        <f>NETWORKDAYS(B151, A151)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="J151" s="7">
@@ -11845,7 +11848,7 @@
         <v>91</v>
       </c>
       <c r="I152" s="10">
-        <f>NETWORKDAYS(B152, A152)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="J152" s="7">
@@ -11909,7 +11912,7 @@
         <v>32</v>
       </c>
       <c r="I153" s="10">
-        <f>NETWORKDAYS(B153, A153)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="J153" s="7">
@@ -11973,7 +11976,7 @@
         <v>34</v>
       </c>
       <c r="I154" s="10">
-        <f>NETWORKDAYS(B154, A154)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="J154" s="7">
@@ -12037,7 +12040,7 @@
         <v>130</v>
       </c>
       <c r="I155" s="10">
-        <f>NETWORKDAYS(B155, A155)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="J155" s="7">
@@ -12101,7 +12104,7 @@
         <v>98</v>
       </c>
       <c r="I156" s="10">
-        <f>NETWORKDAYS(B156, A156)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="J156" s="7">
@@ -12165,7 +12168,7 @@
         <v>91</v>
       </c>
       <c r="I157" s="10">
-        <f>NETWORKDAYS(B157, A157)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="J157" s="7">
@@ -12229,7 +12232,7 @@
         <v>91</v>
       </c>
       <c r="I158" s="10">
-        <f>NETWORKDAYS(B158, A158)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="J158" s="7">
@@ -12293,7 +12296,7 @@
         <v>32</v>
       </c>
       <c r="I159" s="10">
-        <f>NETWORKDAYS(B159, A159)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="J159" s="7">
@@ -12357,7 +12360,7 @@
         <v>32</v>
       </c>
       <c r="I160" s="10">
-        <f>NETWORKDAYS(B160, A160)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="J160" s="7">
@@ -12421,7 +12424,7 @@
         <v>32</v>
       </c>
       <c r="I161" s="10">
-        <f>NETWORKDAYS(B161, A161)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="J161" s="7">
@@ -12485,7 +12488,7 @@
         <v>32</v>
       </c>
       <c r="I162" s="10">
-        <f>NETWORKDAYS(B162, A162)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="J162" s="7">
@@ -12549,7 +12552,7 @@
         <v>185</v>
       </c>
       <c r="I163" s="10">
-        <f>NETWORKDAYS(B163, A163)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="J163" s="7">
@@ -12613,7 +12616,7 @@
         <v>91</v>
       </c>
       <c r="I164" s="10">
-        <f>NETWORKDAYS(B164, A164)</f>
+        <f t="shared" si="3"/>
         <v>17</v>
       </c>
       <c r="J164" s="7">
@@ -12677,7 +12680,7 @@
         <v>98</v>
       </c>
       <c r="I165" s="10">
-        <f>NETWORKDAYS(B165, A165)</f>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="J165" s="7">
@@ -12741,7 +12744,7 @@
         <v>91</v>
       </c>
       <c r="I166" s="10">
-        <f>NETWORKDAYS(B166, A166)</f>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="J166" s="7">
@@ -12805,7 +12808,7 @@
         <v>130</v>
       </c>
       <c r="I167" s="10">
-        <f>NETWORKDAYS(B167, A167)</f>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
       <c r="J167" s="7">
@@ -12869,7 +12872,7 @@
         <v>32</v>
       </c>
       <c r="I168" s="10">
-        <f>NETWORKDAYS(B168, A168)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="J168" s="7">
@@ -12933,7 +12936,7 @@
         <v>130</v>
       </c>
       <c r="I169" s="10">
-        <f>NETWORKDAYS(B169, A169)</f>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
       <c r="J169" s="7">
@@ -12997,7 +13000,7 @@
         <v>130</v>
       </c>
       <c r="I170" s="10">
-        <f>NETWORKDAYS(B170, A170)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="J170" s="7">
@@ -13061,7 +13064,7 @@
         <v>126</v>
       </c>
       <c r="I171" s="10">
-        <f>NETWORKDAYS(B171, A171)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="J171" s="7">
@@ -13125,7 +13128,7 @@
         <v>130</v>
       </c>
       <c r="I172" s="10">
-        <f>NETWORKDAYS(B172, A172)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="J172" s="7">
@@ -13189,7 +13192,7 @@
         <v>372</v>
       </c>
       <c r="I173" s="13">
-        <f>NETWORKDAYS(B173, A173)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="J173" s="12">
@@ -13253,7 +13256,7 @@
         <v>32</v>
       </c>
       <c r="I174" s="10">
-        <f>NETWORKDAYS(B174, A174)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="J174" s="7">
@@ -13317,7 +13320,7 @@
         <v>32</v>
       </c>
       <c r="I175" s="10">
-        <f>NETWORKDAYS(B175, A175)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="J175" s="7">
@@ -13381,7 +13384,7 @@
         <v>138</v>
       </c>
       <c r="I176" s="10">
-        <f>NETWORKDAYS(B176, A176)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="J176" s="7">
@@ -13445,7 +13448,7 @@
         <v>32</v>
       </c>
       <c r="I177" s="10">
-        <f>NETWORKDAYS(B177, A177)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="J177" s="7">
@@ -13509,7 +13512,7 @@
         <v>130</v>
       </c>
       <c r="I178" s="10">
-        <f>NETWORKDAYS(B178, A178)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="J178" s="7">
@@ -13570,10 +13573,10 @@
         <v>3</v>
       </c>
       <c r="H179" s="7" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="I179" s="10">
-        <f>NETWORKDAYS(B179, A179)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="J179" s="7">
@@ -13612,66 +13615,66 @@
       </c>
     </row>
     <row r="180" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A180" s="41">
-        <v>45826</v>
-      </c>
-      <c r="B180" s="41">
-        <v>45826</v>
-      </c>
-      <c r="C180" s="41" t="s">
-        <v>7</v>
-      </c>
-      <c r="D180" s="41" t="s">
-        <v>15</v>
-      </c>
-      <c r="E180" s="41" t="s">
-        <v>124</v>
-      </c>
-      <c r="F180" s="42" t="s">
-        <v>3</v>
-      </c>
-      <c r="G180" s="42" t="s">
-        <v>125</v>
-      </c>
-      <c r="H180" s="42" t="s">
-        <v>126</v>
+      <c r="A180" s="11">
+        <v>45785</v>
+      </c>
+      <c r="B180" s="11">
+        <v>45784</v>
+      </c>
+      <c r="C180" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D180" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="E180" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="F180" s="12">
+        <v>68369</v>
+      </c>
+      <c r="G180" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="H180" s="12" t="s">
+        <v>98</v>
       </c>
       <c r="I180" s="13">
-        <f>NETWORKDAYS(B180, A180)</f>
-        <v>1</v>
-      </c>
-      <c r="J180" s="42">
-        <v>66341</v>
-      </c>
-      <c r="K180" s="42">
-        <v>11758</v>
-      </c>
-      <c r="L180" s="42" t="s">
-        <v>316</v>
-      </c>
-      <c r="M180" s="41">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="J180" s="12">
+        <v>65234</v>
+      </c>
+      <c r="K180" s="12">
+        <v>11610</v>
+      </c>
+      <c r="L180" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="M180" s="11">
         <v>45881</v>
       </c>
-      <c r="N180" s="43">
-        <v>924.61</v>
-      </c>
-      <c r="O180" s="42" t="s">
+      <c r="N180" s="14">
+        <v>9114.5499999999993</v>
+      </c>
+      <c r="O180" s="12" t="s">
         <v>122</v>
       </c>
-      <c r="P180" s="42">
+      <c r="P180" s="12">
         <v>28</v>
       </c>
-      <c r="Q180" s="42" t="s">
+      <c r="Q180" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="R180" s="42">
-        <f>DATEDIF(Tabela1[[#This Row],[Atendimento]],Tabela1[[#This Row],[Previsao de Entrega]],"D")</f>
-        <v>55</v>
-      </c>
-      <c r="S180" s="43">
-        <v>0</v>
-      </c>
-      <c r="T180" s="43">
+      <c r="R180" s="12">
+        <f>DATEDIF(Tabela1[[#This Row],[Atendimento]],Tabela1[[#This Row],[Previsao de Entrega]],"D")</f>
+        <v>96</v>
+      </c>
+      <c r="S180" s="14">
+        <v>183.5</v>
+      </c>
+      <c r="T180" s="14">
         <v>0</v>
       </c>
     </row>
@@ -13701,7 +13704,7 @@
         <v>91</v>
       </c>
       <c r="I181" s="10">
-        <f>NETWORKDAYS(B181, A181)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="J181" s="7">
@@ -13765,7 +13768,7 @@
         <v>91</v>
       </c>
       <c r="I182" s="13">
-        <f>NETWORKDAYS(B182, A182)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="J182" s="12">
@@ -13803,67 +13806,67 @@
         <v>0</v>
       </c>
     </row>
-    <row r="183" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A183" s="11">
-        <v>45785</v>
-      </c>
-      <c r="B183" s="11">
-        <v>45784</v>
-      </c>
-      <c r="C183" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="D183" s="11" t="s">
+    <row r="183" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A183" s="6">
+        <v>45846</v>
+      </c>
+      <c r="B183" s="6">
+        <v>45846</v>
+      </c>
+      <c r="C183" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D183" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E183" s="11" t="s">
+      <c r="E183" s="6" t="s">
         <v>113</v>
       </c>
-      <c r="F183" s="12">
-        <v>68369</v>
-      </c>
-      <c r="G183" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="H183" s="12" t="s">
+      <c r="F183" s="7">
+        <v>68461</v>
+      </c>
+      <c r="G183" s="7" t="s">
+        <v>227</v>
+      </c>
+      <c r="H183" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="I183" s="13">
-        <f>NETWORKDAYS(B183, A183)</f>
-        <v>2</v>
-      </c>
-      <c r="J183" s="12">
-        <v>65234</v>
-      </c>
-      <c r="K183" s="12">
-        <v>11610</v>
-      </c>
-      <c r="L183" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="M183" s="11">
-        <v>45881</v>
-      </c>
-      <c r="N183" s="14">
-        <v>9114.5499999999993</v>
-      </c>
-      <c r="O183" s="12" t="s">
-        <v>122</v>
-      </c>
-      <c r="P183" s="12">
-        <v>28</v>
-      </c>
-      <c r="Q183" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="R183" s="12">
-        <f>DATEDIF(Tabela1[[#This Row],[Atendimento]],Tabela1[[#This Row],[Previsao de Entrega]],"D")</f>
-        <v>96</v>
-      </c>
-      <c r="S183" s="14">
-        <v>183.5</v>
-      </c>
-      <c r="T183" s="14">
+      <c r="I183" s="10">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="J183" s="7">
+        <v>66119</v>
+      </c>
+      <c r="K183" s="7">
+        <v>10677</v>
+      </c>
+      <c r="L183" s="7" t="s">
+        <v>361</v>
+      </c>
+      <c r="M183" s="6">
+        <v>45905</v>
+      </c>
+      <c r="N183" s="8">
+        <v>2800</v>
+      </c>
+      <c r="O183" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="P183" s="7">
+        <v>30</v>
+      </c>
+      <c r="Q183" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="R183" s="7">
+        <f>DATEDIF(Tabela1[[#This Row],[Atendimento]],Tabela1[[#This Row],[Previsao de Entrega]],"D")</f>
+        <v>59</v>
+      </c>
+      <c r="S183" s="8">
+        <v>0</v>
+      </c>
+      <c r="T183" s="8">
         <v>0</v>
       </c>
     </row>
@@ -13893,7 +13896,7 @@
         <v>98</v>
       </c>
       <c r="I184" s="10">
-        <f>NETWORKDAYS(B184, A184)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="J184" s="7">
@@ -13957,7 +13960,7 @@
         <v>34</v>
       </c>
       <c r="I185" s="10">
-        <f>NETWORKDAYS(B185, A185)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="J185" s="7">
@@ -14021,7 +14024,7 @@
         <v>96</v>
       </c>
       <c r="I186" s="10">
-        <f>NETWORKDAYS(B186, A186)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="J186" s="7">
@@ -14085,7 +14088,7 @@
         <v>32</v>
       </c>
       <c r="I187" s="10">
-        <f>NETWORKDAYS(B187, A187)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="J187" s="7">
@@ -14124,66 +14127,66 @@
       </c>
     </row>
     <row r="188" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A188" s="11">
-        <v>45868</v>
-      </c>
-      <c r="B188" s="11">
-        <v>45868</v>
-      </c>
-      <c r="C188" s="11" t="s">
-        <v>128</v>
-      </c>
-      <c r="D188" s="11" t="s">
+      <c r="A188" s="46">
+        <v>45877</v>
+      </c>
+      <c r="B188" s="46">
+        <v>45877</v>
+      </c>
+      <c r="C188" s="46" t="s">
+        <v>7</v>
+      </c>
+      <c r="D188" s="46" t="s">
         <v>5</v>
       </c>
-      <c r="E188" s="11" t="s">
-        <v>394</v>
-      </c>
-      <c r="F188" s="12">
-        <v>68487</v>
-      </c>
-      <c r="G188" s="12" t="s">
-        <v>395</v>
-      </c>
-      <c r="H188" s="12" t="s">
-        <v>96</v>
-      </c>
-      <c r="I188" s="13">
-        <f>NETWORKDAYS(B188, A188)</f>
+      <c r="E188" s="46" t="s">
+        <v>142</v>
+      </c>
+      <c r="F188" s="47" t="s">
+        <v>3</v>
+      </c>
+      <c r="G188" s="47" t="s">
+        <v>3</v>
+      </c>
+      <c r="H188" s="47" t="s">
+        <v>32</v>
+      </c>
+      <c r="I188" s="48">
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="J188" s="12">
-        <v>66489</v>
-      </c>
-      <c r="K188" s="12">
-        <v>11614</v>
-      </c>
-      <c r="L188" s="12" t="s">
-        <v>396</v>
-      </c>
-      <c r="M188" s="11">
-        <v>45882</v>
-      </c>
-      <c r="N188" s="14">
-        <v>6633</v>
-      </c>
-      <c r="O188" s="12" t="s">
-        <v>121</v>
-      </c>
-      <c r="P188" s="12">
-        <v>1</v>
-      </c>
-      <c r="Q188" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="R188" s="12">
-        <f>DATEDIF(Tabela1[[#This Row],[Atendimento]],Tabela1[[#This Row],[Previsao de Entrega]],"D")</f>
-        <v>14</v>
-      </c>
-      <c r="S188" s="14">
-        <v>0</v>
-      </c>
-      <c r="T188" s="14">
+      <c r="J188" s="47">
+        <v>66627</v>
+      </c>
+      <c r="K188" s="47">
+        <v>11127</v>
+      </c>
+      <c r="L188" s="47" t="s">
+        <v>221</v>
+      </c>
+      <c r="M188" s="46">
+        <v>45881</v>
+      </c>
+      <c r="N188" s="49">
+        <v>547.91999999999996</v>
+      </c>
+      <c r="O188" s="47" t="s">
+        <v>122</v>
+      </c>
+      <c r="P188" s="47">
+        <v>35</v>
+      </c>
+      <c r="Q188" s="47" t="s">
+        <v>407</v>
+      </c>
+      <c r="R188" s="47">
+        <f>DATEDIF(Tabela1[[#This Row],[Atendimento]],Tabela1[[#This Row],[Previsao de Entrega]],"D")</f>
+        <v>4</v>
+      </c>
+      <c r="S188" s="49">
+        <v>0</v>
+      </c>
+      <c r="T188" s="49">
         <v>0</v>
       </c>
     </row>
@@ -14213,7 +14216,7 @@
         <v>34</v>
       </c>
       <c r="I189" s="10">
-        <f>NETWORKDAYS(B189, A189)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="J189" s="7">
@@ -14277,7 +14280,7 @@
         <v>91</v>
       </c>
       <c r="I190" s="10">
-        <f>NETWORKDAYS(B190, A190)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="J190" s="7">
@@ -14341,7 +14344,7 @@
         <v>34</v>
       </c>
       <c r="I191" s="10">
-        <f>NETWORKDAYS(B191, A191)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="J191" s="7">
@@ -14384,50 +14387,50 @@
         <v>45868</v>
       </c>
       <c r="B192" s="11">
-        <v>45862</v>
+        <v>45868</v>
       </c>
       <c r="C192" s="11" t="s">
-        <v>7</v>
+        <v>128</v>
       </c>
       <c r="D192" s="11" t="s">
         <v>5</v>
       </c>
       <c r="E192" s="11" t="s">
-        <v>113</v>
+        <v>394</v>
       </c>
       <c r="F192" s="12">
-        <v>68476</v>
+        <v>68487</v>
       </c>
       <c r="G192" s="12" t="s">
-        <v>227</v>
+        <v>395</v>
       </c>
       <c r="H192" s="12" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="I192" s="13">
-        <f>NETWORKDAYS(B192, A192)</f>
-        <v>5</v>
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
       <c r="J192" s="12">
-        <v>66491</v>
+        <v>66489</v>
       </c>
       <c r="K192" s="12">
-        <v>11522</v>
+        <v>11614</v>
       </c>
       <c r="L192" s="12" t="s">
-        <v>376</v>
+        <v>396</v>
       </c>
       <c r="M192" s="11">
         <v>45882</v>
       </c>
       <c r="N192" s="14">
-        <v>398.42</v>
+        <v>6633</v>
       </c>
       <c r="O192" s="12" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="P192" s="12">
-        <v>28</v>
+        <v>1</v>
       </c>
       <c r="Q192" s="12" t="s">
         <v>24</v>
@@ -14469,7 +14472,7 @@
         <v>98</v>
       </c>
       <c r="I193" s="10">
-        <f>NETWORKDAYS(B193, A193)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="J193" s="7">
@@ -14533,7 +14536,7 @@
         <v>372</v>
       </c>
       <c r="I194" s="10">
-        <f>NETWORKDAYS(B194, A194)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="J194" s="7">
@@ -14597,7 +14600,7 @@
         <v>32</v>
       </c>
       <c r="I195" s="10">
-        <f>NETWORKDAYS(B195, A195)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="J195" s="7">
@@ -14661,7 +14664,7 @@
         <v>372</v>
       </c>
       <c r="I196" s="10">
-        <f>NETWORKDAYS(B196, A196)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="J196" s="7">
@@ -14725,7 +14728,7 @@
         <v>372</v>
       </c>
       <c r="I197" s="10">
-        <f>NETWORKDAYS(B197, A197)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="J197" s="7">
@@ -14789,7 +14792,7 @@
         <v>372</v>
       </c>
       <c r="I198" s="10">
-        <f>NETWORKDAYS(B198, A198)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="J198" s="7">
@@ -14853,7 +14856,7 @@
         <v>32</v>
       </c>
       <c r="I199" s="10">
-        <f>NETWORKDAYS(B199, A199)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="J199" s="7">
@@ -14917,7 +14920,7 @@
         <v>32</v>
       </c>
       <c r="I200" s="10">
-        <f>NETWORKDAYS(B200, A200)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="J200" s="7">
@@ -14981,7 +14984,7 @@
         <v>126</v>
       </c>
       <c r="I201" s="10">
-        <f>NETWORKDAYS(B201, A201)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="J201" s="7">
@@ -15045,7 +15048,7 @@
         <v>130</v>
       </c>
       <c r="I202" s="10">
-        <f>NETWORKDAYS(B202, A202)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="J202" s="7">
@@ -15109,7 +15112,7 @@
         <v>32</v>
       </c>
       <c r="I203" s="10">
-        <f>NETWORKDAYS(B203, A203)</f>
+        <f t="shared" ref="I203:I257" si="4">NETWORKDAYS(B203, A203)</f>
         <v>1</v>
       </c>
       <c r="J203" s="7">
@@ -15173,7 +15176,7 @@
         <v>32</v>
       </c>
       <c r="I204" s="10">
-        <f>NETWORKDAYS(B204, A204)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="J204" s="7">
@@ -15237,7 +15240,7 @@
         <v>34</v>
       </c>
       <c r="I205" s="10">
-        <f>NETWORKDAYS(B205, A205)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="J205" s="7">
@@ -15301,7 +15304,7 @@
         <v>126</v>
       </c>
       <c r="I206" s="10">
-        <f>NETWORKDAYS(B206, A206)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="J206" s="7">
@@ -15365,7 +15368,7 @@
         <v>130</v>
       </c>
       <c r="I207" s="10">
-        <f>NETWORKDAYS(B207, A207)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="J207" s="7">
@@ -15429,7 +15432,7 @@
         <v>130</v>
       </c>
       <c r="I208" s="10">
-        <f>NETWORKDAYS(B208, A208)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="J208" s="7">
@@ -15493,7 +15496,7 @@
         <v>130</v>
       </c>
       <c r="I209" s="10">
-        <f>NETWORKDAYS(B209, A209)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="J209" s="7">
@@ -15557,7 +15560,7 @@
         <v>130</v>
       </c>
       <c r="I210" s="10">
-        <f>NETWORKDAYS(B210, A210)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="J210" s="7">
@@ -15621,7 +15624,7 @@
         <v>34</v>
       </c>
       <c r="I211" s="10">
-        <f>NETWORKDAYS(B211, A211)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="J211" s="7">
@@ -15685,7 +15688,7 @@
         <v>32</v>
       </c>
       <c r="I212" s="10">
-        <f>NETWORKDAYS(B212, A212)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="J212" s="7">
@@ -15749,7 +15752,7 @@
         <v>138</v>
       </c>
       <c r="I213" s="10">
-        <f>NETWORKDAYS(B213, A213)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="J213" s="7">
@@ -15813,7 +15816,7 @@
         <v>91</v>
       </c>
       <c r="I214" s="10">
-        <f>NETWORKDAYS(B214, A214)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="J214" s="7">
@@ -15877,7 +15880,7 @@
         <v>98</v>
       </c>
       <c r="I215" s="10">
-        <f>NETWORKDAYS(B215, A215)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="J215" s="7">
@@ -15941,7 +15944,7 @@
         <v>138</v>
       </c>
       <c r="I216" s="10">
-        <f>NETWORKDAYS(B216, A216)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="J216" s="7">
@@ -16005,7 +16008,7 @@
         <v>98</v>
       </c>
       <c r="I217" s="10">
-        <f>NETWORKDAYS(B217, A217)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="J217" s="7">
@@ -16044,66 +16047,66 @@
       </c>
     </row>
     <row r="218" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A218" s="11">
-        <v>45867</v>
-      </c>
-      <c r="B218" s="11">
-        <v>45867</v>
-      </c>
-      <c r="C218" s="11" t="s">
-        <v>128</v>
-      </c>
-      <c r="D218" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="E218" s="11" t="s">
+      <c r="A218" s="46">
+        <v>45868</v>
+      </c>
+      <c r="B218" s="46">
+        <v>45862</v>
+      </c>
+      <c r="C218" s="46" t="s">
+        <v>7</v>
+      </c>
+      <c r="D218" s="46" t="s">
+        <v>5</v>
+      </c>
+      <c r="E218" s="46" t="s">
         <v>113</v>
       </c>
-      <c r="F218" s="12">
-        <v>68486</v>
-      </c>
-      <c r="G218" s="12" t="s">
-        <v>296</v>
-      </c>
-      <c r="H218" s="12" t="s">
-        <v>96</v>
-      </c>
-      <c r="I218" s="13">
-        <f>NETWORKDAYS(B218, A218)</f>
-        <v>1</v>
-      </c>
-      <c r="J218" s="12">
-        <v>66478</v>
-      </c>
-      <c r="K218" s="12">
-        <v>10460</v>
-      </c>
-      <c r="L218" s="12" t="s">
-        <v>393</v>
-      </c>
-      <c r="M218" s="11">
-        <v>45883</v>
-      </c>
-      <c r="N218" s="14">
-        <v>4789.6099999999997</v>
-      </c>
-      <c r="O218" s="12" t="s">
+      <c r="F218" s="47">
+        <v>68476</v>
+      </c>
+      <c r="G218" s="47" t="s">
+        <v>227</v>
+      </c>
+      <c r="H218" s="47" t="s">
+        <v>98</v>
+      </c>
+      <c r="I218" s="48">
+        <f t="shared" si="4"/>
+        <v>5</v>
+      </c>
+      <c r="J218" s="47">
+        <v>66491</v>
+      </c>
+      <c r="K218" s="47">
+        <v>11522</v>
+      </c>
+      <c r="L218" s="47" t="s">
+        <v>376</v>
+      </c>
+      <c r="M218" s="46">
+        <v>45888</v>
+      </c>
+      <c r="N218" s="49">
+        <v>1680.4</v>
+      </c>
+      <c r="O218" s="47" t="s">
         <v>122</v>
       </c>
-      <c r="P218" s="12">
+      <c r="P218" s="47">
         <v>28</v>
       </c>
-      <c r="Q218" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="R218" s="12">
-        <f>DATEDIF(Tabela1[[#This Row],[Atendimento]],Tabela1[[#This Row],[Previsao de Entrega]],"D")</f>
-        <v>16</v>
-      </c>
-      <c r="S218" s="14">
-        <v>1509.38</v>
-      </c>
-      <c r="T218" s="14">
+      <c r="Q218" s="47" t="s">
+        <v>407</v>
+      </c>
+      <c r="R218" s="47">
+        <f>DATEDIF(Tabela1[[#This Row],[Atendimento]],Tabela1[[#This Row],[Previsao de Entrega]],"D")</f>
+        <v>20</v>
+      </c>
+      <c r="S218" s="49">
+        <v>0</v>
+      </c>
+      <c r="T218" s="49">
         <v>0</v>
       </c>
     </row>
@@ -16133,7 +16136,7 @@
         <v>130</v>
       </c>
       <c r="I219" s="10">
-        <f>NETWORKDAYS(B219, A219)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="J219" s="7">
@@ -16197,7 +16200,7 @@
         <v>130</v>
       </c>
       <c r="I220" s="10">
-        <f>NETWORKDAYS(B220, A220)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="J220" s="7">
@@ -16261,7 +16264,7 @@
         <v>98</v>
       </c>
       <c r="I221" s="10">
-        <f>NETWORKDAYS(B221, A221)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="J221" s="7">
@@ -16325,7 +16328,7 @@
         <v>91</v>
       </c>
       <c r="I222" s="10">
-        <f>NETWORKDAYS(B222, A222)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="J222" s="7">
@@ -16389,7 +16392,7 @@
         <v>32</v>
       </c>
       <c r="I223" s="10">
-        <f>NETWORKDAYS(B223, A223)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="J223" s="7">
@@ -16453,7 +16456,7 @@
         <v>372</v>
       </c>
       <c r="I224" s="10">
-        <f>NETWORKDAYS(B224, A224)</f>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="J224" s="7">
@@ -16517,7 +16520,7 @@
         <v>32</v>
       </c>
       <c r="I225" s="10">
-        <f>NETWORKDAYS(B225, A225)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="J225" s="7">
@@ -16556,128 +16559,128 @@
       </c>
     </row>
     <row r="226" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A226" s="11">
-        <v>45870</v>
-      </c>
-      <c r="B226" s="11">
-        <v>45869</v>
-      </c>
-      <c r="C226" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="D226" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="E226" s="11" t="s">
-        <v>113</v>
-      </c>
-      <c r="F226" s="12">
-        <v>68491</v>
-      </c>
-      <c r="G226" s="12" t="s">
-        <v>371</v>
-      </c>
-      <c r="H226" s="12" t="s">
-        <v>372</v>
+      <c r="A226" s="41">
+        <v>45826</v>
+      </c>
+      <c r="B226" s="41">
+        <v>45826</v>
+      </c>
+      <c r="C226" s="41" t="s">
+        <v>7</v>
+      </c>
+      <c r="D226" s="41" t="s">
+        <v>15</v>
+      </c>
+      <c r="E226" s="41" t="s">
+        <v>124</v>
+      </c>
+      <c r="F226" s="42" t="s">
+        <v>3</v>
+      </c>
+      <c r="G226" s="42" t="s">
+        <v>125</v>
+      </c>
+      <c r="H226" s="42" t="s">
+        <v>126</v>
       </c>
       <c r="I226" s="13">
-        <f>NETWORKDAYS(B226, A226)</f>
-        <v>2</v>
-      </c>
-      <c r="J226" s="12">
-        <v>66521</v>
-      </c>
-      <c r="K226" s="12">
-        <v>3061</v>
-      </c>
-      <c r="L226" s="12" t="s">
-        <v>192</v>
-      </c>
-      <c r="M226" s="11">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="J226" s="42">
+        <v>66341</v>
+      </c>
+      <c r="K226" s="42">
+        <v>11758</v>
+      </c>
+      <c r="L226" s="42" t="s">
+        <v>316</v>
+      </c>
+      <c r="M226" s="41">
         <v>45883</v>
       </c>
-      <c r="N226" s="14">
-        <v>3000</v>
-      </c>
-      <c r="O226" s="12" t="s">
+      <c r="N226" s="43">
+        <v>924.61</v>
+      </c>
+      <c r="O226" s="42" t="s">
         <v>122</v>
       </c>
-      <c r="P226" s="12">
-        <v>15</v>
-      </c>
-      <c r="Q226" s="12" t="s">
+      <c r="P226" s="42">
+        <v>28</v>
+      </c>
+      <c r="Q226" s="42" t="s">
         <v>24</v>
       </c>
-      <c r="R226" s="12">
-        <f>DATEDIF(Tabela1[[#This Row],[Atendimento]],Tabela1[[#This Row],[Previsao de Entrega]],"D")</f>
-        <v>13</v>
-      </c>
-      <c r="S226" s="14">
-        <v>50</v>
-      </c>
-      <c r="T226" s="14">
+      <c r="R226" s="42">
+        <f>DATEDIF(Tabela1[[#This Row],[Atendimento]],Tabela1[[#This Row],[Previsao de Entrega]],"D")</f>
+        <v>57</v>
+      </c>
+      <c r="S226" s="43">
+        <v>0</v>
+      </c>
+      <c r="T226" s="43">
         <v>0</v>
       </c>
     </row>
     <row r="227" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A227" s="11">
-        <v>45870</v>
+        <v>45867</v>
       </c>
       <c r="B227" s="11">
         <v>45867</v>
       </c>
       <c r="C227" s="11" t="s">
-        <v>7</v>
+        <v>128</v>
       </c>
       <c r="D227" s="11" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="E227" s="11" t="s">
         <v>113</v>
       </c>
       <c r="F227" s="12">
-        <v>68485</v>
+        <v>68486</v>
       </c>
       <c r="G227" s="12" t="s">
-        <v>371</v>
+        <v>296</v>
       </c>
       <c r="H227" s="12" t="s">
-        <v>372</v>
+        <v>96</v>
       </c>
       <c r="I227" s="13">
-        <f>NETWORKDAYS(B227, A227)</f>
-        <v>4</v>
+        <f t="shared" si="4"/>
+        <v>1</v>
       </c>
       <c r="J227" s="12">
-        <v>66526</v>
+        <v>66478</v>
       </c>
       <c r="K227" s="12">
-        <v>3061</v>
+        <v>10460</v>
       </c>
       <c r="L227" s="12" t="s">
-        <v>192</v>
+        <v>393</v>
       </c>
       <c r="M227" s="11">
-        <v>45884</v>
+        <v>45883</v>
       </c>
       <c r="N227" s="14">
-        <v>1150</v>
+        <v>4789.6099999999997</v>
       </c>
       <c r="O227" s="12" t="s">
         <v>122</v>
       </c>
       <c r="P227" s="12">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="Q227" s="12" t="s">
         <v>24</v>
       </c>
       <c r="R227" s="12">
         <f>DATEDIF(Tabela1[[#This Row],[Atendimento]],Tabela1[[#This Row],[Previsao de Entrega]],"D")</f>
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="S227" s="14">
-        <v>0</v>
+        <v>1080.08</v>
       </c>
       <c r="T227" s="14">
         <v>0</v>
@@ -16688,188 +16691,188 @@
         <v>45870</v>
       </c>
       <c r="B228" s="11">
-        <v>45863</v>
+        <v>45869</v>
       </c>
       <c r="C228" s="11" t="s">
         <v>7</v>
       </c>
       <c r="D228" s="11" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="E228" s="11" t="s">
         <v>113</v>
       </c>
       <c r="F228" s="12">
-        <v>68482</v>
+        <v>68491</v>
       </c>
       <c r="G228" s="12" t="s">
-        <v>129</v>
+        <v>371</v>
       </c>
       <c r="H228" s="12" t="s">
-        <v>130</v>
+        <v>372</v>
       </c>
       <c r="I228" s="13">
-        <f>NETWORKDAYS(B228, A228)</f>
-        <v>6</v>
+        <f t="shared" si="4"/>
+        <v>2</v>
       </c>
       <c r="J228" s="12">
-        <v>66522</v>
+        <v>66521</v>
       </c>
       <c r="K228" s="12">
-        <v>679</v>
+        <v>3061</v>
       </c>
       <c r="L228" s="12" t="s">
-        <v>346</v>
+        <v>192</v>
       </c>
       <c r="M228" s="11">
-        <v>45889</v>
+        <v>45883</v>
       </c>
       <c r="N228" s="14">
-        <v>6048.2</v>
+        <v>3000</v>
       </c>
       <c r="O228" s="12" t="s">
         <v>122</v>
       </c>
       <c r="P228" s="12">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="Q228" s="12" t="s">
         <v>24</v>
       </c>
       <c r="R228" s="12">
         <f>DATEDIF(Tabela1[[#This Row],[Atendimento]],Tabela1[[#This Row],[Previsao de Entrega]],"D")</f>
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="S228" s="14">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="T228" s="14">
         <v>0</v>
       </c>
     </row>
     <row r="229" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A229" s="46">
-        <v>45877</v>
-      </c>
-      <c r="B229" s="46">
-        <v>45877</v>
-      </c>
-      <c r="C229" s="46" t="s">
-        <v>7</v>
-      </c>
-      <c r="D229" s="46" t="s">
+      <c r="A229" s="11">
+        <v>45870</v>
+      </c>
+      <c r="B229" s="11">
+        <v>45867</v>
+      </c>
+      <c r="C229" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D229" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="E229" s="46" t="s">
+      <c r="E229" s="11" t="s">
         <v>113</v>
       </c>
-      <c r="F229" s="47">
-        <v>68458</v>
-      </c>
-      <c r="G229" s="47" t="s">
-        <v>227</v>
-      </c>
-      <c r="H229" s="47" t="s">
-        <v>98</v>
-      </c>
-      <c r="I229" s="48">
-        <f>NETWORKDAYS(B229, A229)</f>
-        <v>1</v>
-      </c>
-      <c r="J229" s="47">
-        <v>66605</v>
-      </c>
-      <c r="K229" s="47">
-        <v>561</v>
-      </c>
-      <c r="L229" s="47" t="s">
-        <v>324</v>
-      </c>
-      <c r="M229" s="46">
-        <v>45891</v>
-      </c>
-      <c r="N229" s="49">
-        <v>758.53</v>
-      </c>
-      <c r="O229" s="47" t="s">
+      <c r="F229" s="12">
+        <v>68485</v>
+      </c>
+      <c r="G229" s="12" t="s">
+        <v>371</v>
+      </c>
+      <c r="H229" s="12" t="s">
+        <v>372</v>
+      </c>
+      <c r="I229" s="13">
+        <f t="shared" si="4"/>
+        <v>4</v>
+      </c>
+      <c r="J229" s="12">
+        <v>66526</v>
+      </c>
+      <c r="K229" s="12">
+        <v>3061</v>
+      </c>
+      <c r="L229" s="12" t="s">
+        <v>192</v>
+      </c>
+      <c r="M229" s="11">
+        <v>45884</v>
+      </c>
+      <c r="N229" s="14">
+        <v>1150</v>
+      </c>
+      <c r="O229" s="12" t="s">
         <v>122</v>
       </c>
-      <c r="P229" s="47">
-        <v>28</v>
-      </c>
-      <c r="Q229" s="47" t="s">
-        <v>407</v>
-      </c>
-      <c r="R229" s="47">
+      <c r="P229" s="12">
+        <v>15</v>
+      </c>
+      <c r="Q229" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="R229" s="12">
         <f>DATEDIF(Tabela1[[#This Row],[Atendimento]],Tabela1[[#This Row],[Previsao de Entrega]],"D")</f>
         <v>14</v>
       </c>
-      <c r="S229" s="49">
-        <v>0</v>
-      </c>
-      <c r="T229" s="49">
+      <c r="S229" s="14">
+        <v>0</v>
+      </c>
+      <c r="T229" s="14">
         <v>0</v>
       </c>
     </row>
     <row r="230" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A230" s="11">
-        <v>45868</v>
+        <v>45880</v>
       </c>
       <c r="B230" s="11">
-        <v>45868</v>
+        <v>45869</v>
       </c>
       <c r="C230" s="11" t="s">
         <v>7</v>
       </c>
       <c r="D230" s="11" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="E230" s="11" t="s">
-        <v>124</v>
-      </c>
-      <c r="F230" s="12" t="s">
-        <v>3</v>
+        <v>113</v>
+      </c>
+      <c r="F230" s="12">
+        <v>68490</v>
       </c>
       <c r="G230" s="12" t="s">
-        <v>125</v>
+        <v>227</v>
       </c>
       <c r="H230" s="12" t="s">
-        <v>126</v>
+        <v>98</v>
       </c>
       <c r="I230" s="13">
-        <f>NETWORKDAYS(B230, A230)</f>
-        <v>1</v>
+        <f t="shared" si="4"/>
+        <v>8</v>
       </c>
       <c r="J230" s="12">
-        <v>66504</v>
+        <v>66638</v>
       </c>
       <c r="K230" s="12">
-        <v>3034</v>
+        <v>8992</v>
       </c>
       <c r="L230" s="12" t="s">
-        <v>349</v>
+        <v>180</v>
       </c>
       <c r="M230" s="11">
-        <v>45897</v>
+        <v>45884</v>
       </c>
       <c r="N230" s="14">
-        <v>66522</v>
+        <v>10750</v>
       </c>
       <c r="O230" s="12" t="s">
         <v>122</v>
       </c>
       <c r="P230" s="12">
-        <v>90</v>
+        <v>30</v>
       </c>
       <c r="Q230" s="12" t="s">
         <v>24</v>
       </c>
       <c r="R230" s="12">
         <f>DATEDIF(Tabela1[[#This Row],[Atendimento]],Tabela1[[#This Row],[Previsao de Entrega]],"D")</f>
-        <v>29</v>
+        <v>4</v>
       </c>
       <c r="S230" s="14">
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="T230" s="14">
         <v>0</v>
@@ -16901,7 +16904,7 @@
         <v>372</v>
       </c>
       <c r="I231" s="10">
-        <f>NETWORKDAYS(B231, A231)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="J231" s="7">
@@ -16941,10 +16944,10 @@
     </row>
     <row r="232" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A232" s="11">
-        <v>45869</v>
+        <v>45870</v>
       </c>
       <c r="B232" s="11">
-        <v>45869</v>
+        <v>45863</v>
       </c>
       <c r="C232" s="11" t="s">
         <v>7</v>
@@ -16953,35 +16956,35 @@
         <v>15</v>
       </c>
       <c r="E232" s="11" t="s">
-        <v>124</v>
-      </c>
-      <c r="F232" s="12" t="s">
-        <v>3</v>
+        <v>113</v>
+      </c>
+      <c r="F232" s="12">
+        <v>68482</v>
       </c>
       <c r="G232" s="12" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="H232" s="12" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="I232" s="13">
-        <f>NETWORKDAYS(B232, A232)</f>
-        <v>1</v>
+        <f t="shared" si="4"/>
+        <v>6</v>
       </c>
       <c r="J232" s="12">
-        <v>66427</v>
+        <v>66522</v>
       </c>
       <c r="K232" s="12">
-        <v>1277</v>
+        <v>679</v>
       </c>
       <c r="L232" s="12" t="s">
-        <v>398</v>
+        <v>346</v>
       </c>
       <c r="M232" s="11">
-        <v>45897</v>
+        <v>45889</v>
       </c>
       <c r="N232" s="14">
-        <v>2715.75</v>
+        <v>6048.2</v>
       </c>
       <c r="O232" s="12" t="s">
         <v>122</v>
@@ -16994,10 +16997,10 @@
       </c>
       <c r="R232" s="12">
         <f>DATEDIF(Tabela1[[#This Row],[Atendimento]],Tabela1[[#This Row],[Previsao de Entrega]],"D")</f>
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="S232" s="14">
-        <v>950</v>
+        <v>0</v>
       </c>
       <c r="T232" s="14">
         <v>0</v>
@@ -17005,127 +17008,127 @@
     </row>
     <row r="233" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A233" s="11">
-        <v>45875</v>
+        <v>45877</v>
       </c>
       <c r="B233" s="11">
-        <v>45873</v>
+        <v>45877</v>
       </c>
       <c r="C233" s="11" t="s">
-        <v>128</v>
+        <v>7</v>
       </c>
       <c r="D233" s="11" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="E233" s="11" t="s">
-        <v>124</v>
-      </c>
-      <c r="F233" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="G233" s="11" t="s">
-        <v>125</v>
-      </c>
-      <c r="H233" s="11" t="s">
-        <v>126</v>
+        <v>113</v>
+      </c>
+      <c r="F233" s="12">
+        <v>68458</v>
+      </c>
+      <c r="G233" s="12" t="s">
+        <v>227</v>
+      </c>
+      <c r="H233" s="12" t="s">
+        <v>98</v>
       </c>
       <c r="I233" s="13">
-        <f>NETWORKDAYS(B233, A233)</f>
-        <v>3</v>
+        <f t="shared" si="4"/>
+        <v>1</v>
       </c>
       <c r="J233" s="12">
-        <v>66430</v>
+        <v>66605</v>
       </c>
       <c r="K233" s="12">
-        <v>333</v>
+        <v>561</v>
       </c>
       <c r="L233" s="12" t="s">
-        <v>400</v>
+        <v>324</v>
       </c>
       <c r="M233" s="11">
-        <v>45901</v>
-      </c>
-      <c r="N233" s="45">
-        <v>1483685.03</v>
-      </c>
-      <c r="O233" s="11" t="s">
+        <v>45891</v>
+      </c>
+      <c r="N233" s="14">
+        <v>758.53</v>
+      </c>
+      <c r="O233" s="12" t="s">
         <v>122</v>
       </c>
       <c r="P233" s="12">
-        <v>90</v>
+        <v>28</v>
       </c>
       <c r="Q233" s="12" t="s">
         <v>24</v>
       </c>
       <c r="R233" s="12">
         <f>DATEDIF(Tabela1[[#This Row],[Atendimento]],Tabela1[[#This Row],[Previsao de Entrega]],"D")</f>
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="S233" s="14">
         <v>0</v>
       </c>
       <c r="T233" s="14">
-        <v>59008.35</v>
+        <v>0</v>
       </c>
     </row>
     <row r="234" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A234" s="11">
-        <v>45856</v>
+        <v>45880</v>
       </c>
       <c r="B234" s="11">
-        <v>45856</v>
+        <v>45868</v>
       </c>
       <c r="C234" s="11" t="s">
         <v>7</v>
       </c>
       <c r="D234" s="11" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="E234" s="11" t="s">
-        <v>124</v>
-      </c>
-      <c r="F234" s="12">
-        <v>68466</v>
+        <v>113</v>
+      </c>
+      <c r="F234" s="12" t="s">
+        <v>3</v>
       </c>
       <c r="G234" s="12" t="s">
-        <v>125</v>
+        <v>3</v>
       </c>
       <c r="H234" s="12" t="s">
-        <v>126</v>
+        <v>32</v>
       </c>
       <c r="I234" s="13">
-        <f>NETWORKDAYS(B234, A234)</f>
-        <v>1</v>
+        <f t="shared" si="4"/>
+        <v>9</v>
       </c>
       <c r="J234" s="12">
-        <v>66337</v>
+        <v>66629</v>
       </c>
       <c r="K234" s="12">
-        <v>11736</v>
+        <v>11121</v>
       </c>
       <c r="L234" s="12" t="s">
-        <v>127</v>
+        <v>143</v>
       </c>
       <c r="M234" s="11">
-        <v>45902</v>
+        <v>45894</v>
       </c>
       <c r="N234" s="14">
-        <v>16134.54</v>
+        <v>1242.04</v>
       </c>
       <c r="O234" s="12" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="P234" s="12">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="Q234" s="12" t="s">
         <v>24</v>
       </c>
       <c r="R234" s="12">
         <f>DATEDIF(Tabela1[[#This Row],[Atendimento]],Tabela1[[#This Row],[Previsao de Entrega]],"D")</f>
-        <v>46</v>
+        <v>14</v>
       </c>
       <c r="S234" s="14">
-        <v>25720</v>
+        <v>108</v>
       </c>
       <c r="T234" s="14">
         <v>0</v>
@@ -17133,63 +17136,63 @@
     </row>
     <row r="235" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A235" s="11">
-        <v>45840</v>
+        <v>45868</v>
       </c>
       <c r="B235" s="11">
-        <v>45840</v>
+        <v>45868</v>
       </c>
       <c r="C235" s="11" t="s">
         <v>7</v>
       </c>
       <c r="D235" s="11" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="E235" s="11" t="s">
-        <v>113</v>
-      </c>
-      <c r="F235" s="12">
-        <v>68452</v>
+        <v>124</v>
+      </c>
+      <c r="F235" s="12" t="s">
+        <v>3</v>
       </c>
       <c r="G235" s="12" t="s">
-        <v>33</v>
+        <v>125</v>
       </c>
       <c r="H235" s="12" t="s">
-        <v>34</v>
+        <v>126</v>
       </c>
       <c r="I235" s="13">
-        <f>NETWORKDAYS(B235, A235)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="J235" s="12">
-        <v>66037</v>
+        <v>66504</v>
       </c>
       <c r="K235" s="12">
-        <v>11775</v>
+        <v>3034</v>
       </c>
       <c r="L235" s="12" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="M235" s="11">
-        <v>45905</v>
+        <v>45897</v>
       </c>
       <c r="N235" s="14">
-        <v>1750</v>
+        <v>2220</v>
       </c>
       <c r="O235" s="12" t="s">
         <v>122</v>
       </c>
       <c r="P235" s="12">
-        <v>30</v>
+        <v>90</v>
       </c>
       <c r="Q235" s="12" t="s">
         <v>24</v>
       </c>
       <c r="R235" s="12">
         <f>DATEDIF(Tabela1[[#This Row],[Atendimento]],Tabela1[[#This Row],[Previsao de Entrega]],"D")</f>
-        <v>65</v>
+        <v>29</v>
       </c>
       <c r="S235" s="14">
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="T235" s="14">
         <v>0</v>
@@ -17197,50 +17200,50 @@
     </row>
     <row r="236" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A236" s="11">
-        <v>45846</v>
+        <v>45869</v>
       </c>
       <c r="B236" s="11">
-        <v>45846</v>
+        <v>45869</v>
       </c>
       <c r="C236" s="11" t="s">
         <v>7</v>
       </c>
       <c r="D236" s="11" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="E236" s="11" t="s">
-        <v>113</v>
-      </c>
-      <c r="F236" s="12">
-        <v>68461</v>
+        <v>124</v>
+      </c>
+      <c r="F236" s="12" t="s">
+        <v>3</v>
       </c>
       <c r="G236" s="12" t="s">
-        <v>227</v>
+        <v>125</v>
       </c>
       <c r="H236" s="12" t="s">
-        <v>98</v>
+        <v>126</v>
       </c>
       <c r="I236" s="13">
-        <f>NETWORKDAYS(B236, A236)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="J236" s="12">
-        <v>66119</v>
+        <v>66427</v>
       </c>
       <c r="K236" s="12">
-        <v>10677</v>
+        <v>1277</v>
       </c>
       <c r="L236" s="12" t="s">
-        <v>361</v>
+        <v>398</v>
       </c>
       <c r="M236" s="11">
-        <v>45905</v>
+        <v>45897</v>
       </c>
       <c r="N236" s="14">
-        <v>2800</v>
+        <v>2715.75</v>
       </c>
       <c r="O236" s="12" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="P236" s="12">
         <v>30</v>
@@ -17250,10 +17253,10 @@
       </c>
       <c r="R236" s="12">
         <f>DATEDIF(Tabela1[[#This Row],[Atendimento]],Tabela1[[#This Row],[Previsao de Entrega]],"D")</f>
-        <v>59</v>
+        <v>28</v>
       </c>
       <c r="S236" s="14">
-        <v>0</v>
+        <v>950</v>
       </c>
       <c r="T236" s="14">
         <v>0</v>
@@ -17285,7 +17288,7 @@
         <v>34</v>
       </c>
       <c r="I237" s="10">
-        <f>NETWORKDAYS(B237, A237)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="J237" s="7">
@@ -17349,7 +17352,7 @@
         <v>130</v>
       </c>
       <c r="I238" s="10">
-        <f>NETWORKDAYS(B238, A238)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="J238" s="7">
@@ -17413,7 +17416,7 @@
         <v>130</v>
       </c>
       <c r="I239" s="10">
-        <f>NETWORKDAYS(B239, A239)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="J239" s="7">
@@ -17477,7 +17480,7 @@
         <v>130</v>
       </c>
       <c r="I240" s="10">
-        <f>NETWORKDAYS(B240, A240)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="J240" s="7">
@@ -17541,7 +17544,7 @@
         <v>32</v>
       </c>
       <c r="I241" s="10">
-        <f>NETWORKDAYS(B241, A241)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="J241" s="7">
@@ -17605,7 +17608,7 @@
         <v>126</v>
       </c>
       <c r="I242" s="10">
-        <f>NETWORKDAYS(B242, A242)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="J242" s="7">
@@ -17669,7 +17672,7 @@
         <v>138</v>
       </c>
       <c r="I243" s="10">
-        <f>NETWORKDAYS(B243, A243)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="J243" s="7">
@@ -17709,66 +17712,66 @@
     </row>
     <row r="244" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A244" s="11">
-        <v>45848</v>
+        <v>45875</v>
       </c>
       <c r="B244" s="11">
-        <v>45848</v>
+        <v>45873</v>
       </c>
       <c r="C244" s="11" t="s">
-        <v>7</v>
+        <v>128</v>
       </c>
       <c r="D244" s="11" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="E244" s="11" t="s">
-        <v>113</v>
-      </c>
-      <c r="F244" s="12">
-        <v>68457</v>
-      </c>
-      <c r="G244" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="H244" s="12" t="s">
-        <v>34</v>
+        <v>124</v>
+      </c>
+      <c r="F244" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="G244" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="H244" s="11" t="s">
+        <v>126</v>
       </c>
       <c r="I244" s="13">
-        <f>NETWORKDAYS(B244, A244)</f>
-        <v>1</v>
+        <f t="shared" si="4"/>
+        <v>3</v>
       </c>
       <c r="J244" s="12">
-        <v>66126</v>
+        <v>66430</v>
       </c>
       <c r="K244" s="12">
-        <v>2931</v>
+        <v>333</v>
       </c>
       <c r="L244" s="12" t="s">
-        <v>366</v>
+        <v>400</v>
       </c>
       <c r="M244" s="11">
-        <v>45905</v>
-      </c>
-      <c r="N244" s="14">
-        <v>3500</v>
-      </c>
-      <c r="O244" s="12" t="s">
+        <v>45901</v>
+      </c>
+      <c r="N244" s="45">
+        <v>1483685.03</v>
+      </c>
+      <c r="O244" s="11" t="s">
         <v>122</v>
       </c>
       <c r="P244" s="12">
-        <v>30</v>
+        <v>90</v>
       </c>
       <c r="Q244" s="12" t="s">
         <v>24</v>
       </c>
       <c r="R244" s="12">
         <f>DATEDIF(Tabela1[[#This Row],[Atendimento]],Tabela1[[#This Row],[Previsao de Entrega]],"D")</f>
-        <v>57</v>
+        <v>26</v>
       </c>
       <c r="S244" s="14">
-        <v>320</v>
+        <v>0</v>
       </c>
       <c r="T244" s="14">
-        <v>0</v>
+        <v>59008.35</v>
       </c>
     </row>
     <row r="245" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
@@ -17797,7 +17800,7 @@
         <v>32</v>
       </c>
       <c r="I245" s="10">
-        <f>NETWORKDAYS(B245, A245)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="J245" s="7">
@@ -17837,10 +17840,10 @@
     </row>
     <row r="246" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A246" s="11">
-        <v>45874</v>
+        <v>45856</v>
       </c>
       <c r="B246" s="11">
-        <v>45853</v>
+        <v>45856</v>
       </c>
       <c r="C246" s="11" t="s">
         <v>7</v>
@@ -17852,7 +17855,7 @@
         <v>124</v>
       </c>
       <c r="F246" s="12">
-        <v>68465</v>
+        <v>68466</v>
       </c>
       <c r="G246" s="12" t="s">
         <v>125</v>
@@ -17861,39 +17864,39 @@
         <v>126</v>
       </c>
       <c r="I246" s="13">
-        <f>NETWORKDAYS(B246, A246)</f>
-        <v>16</v>
+        <f t="shared" si="4"/>
+        <v>1</v>
       </c>
       <c r="J246" s="12">
-        <v>66555</v>
+        <v>66337</v>
       </c>
       <c r="K246" s="12">
-        <v>11791</v>
+        <v>11736</v>
       </c>
       <c r="L246" s="12" t="s">
-        <v>403</v>
+        <v>127</v>
       </c>
       <c r="M246" s="11">
-        <v>45906</v>
+        <v>45902</v>
       </c>
       <c r="N246" s="14">
-        <v>1075.55</v>
+        <v>16134.54</v>
       </c>
       <c r="O246" s="12" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="P246" s="12">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="Q246" s="12" t="s">
         <v>24</v>
       </c>
       <c r="R246" s="12">
         <f>DATEDIF(Tabela1[[#This Row],[Atendimento]],Tabela1[[#This Row],[Previsao de Entrega]],"D")</f>
-        <v>32</v>
+        <v>46</v>
       </c>
       <c r="S246" s="14">
-        <v>1215.25</v>
+        <v>25720</v>
       </c>
       <c r="T246" s="14">
         <v>0</v>
@@ -17925,7 +17928,7 @@
         <v>32</v>
       </c>
       <c r="I247" s="10">
-        <f>NETWORKDAYS(B247, A247)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="J247" s="7">
@@ -17989,7 +17992,7 @@
         <v>98</v>
       </c>
       <c r="I248" s="10">
-        <f>NETWORKDAYS(B248, A248)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="J248" s="7">
@@ -18053,7 +18056,7 @@
         <v>98</v>
       </c>
       <c r="I249" s="10">
-        <f>NETWORKDAYS(B249, A249)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="J249" s="7">
@@ -18092,128 +18095,128 @@
       </c>
     </row>
     <row r="250" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A250" s="46">
-        <v>45877</v>
-      </c>
-      <c r="B250" s="46">
-        <v>45873</v>
-      </c>
-      <c r="C250" s="46" t="s">
-        <v>7</v>
-      </c>
-      <c r="D250" s="46" t="s">
+      <c r="A250" s="11">
+        <v>45840</v>
+      </c>
+      <c r="B250" s="11">
+        <v>45840</v>
+      </c>
+      <c r="C250" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D250" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="E250" s="46" t="s">
+      <c r="E250" s="11" t="s">
         <v>113</v>
       </c>
-      <c r="F250" s="47">
-        <v>68493</v>
-      </c>
-      <c r="G250" s="47" t="s">
-        <v>321</v>
-      </c>
-      <c r="H250" s="47" t="s">
-        <v>91</v>
-      </c>
-      <c r="I250" s="48">
-        <f>NETWORKDAYS(B250, A250)</f>
-        <v>5</v>
-      </c>
-      <c r="J250" s="47">
-        <v>66607</v>
-      </c>
-      <c r="K250" s="47">
-        <v>1586</v>
-      </c>
-      <c r="L250" s="47" t="s">
-        <v>408</v>
-      </c>
-      <c r="M250" s="46">
-        <v>45907</v>
-      </c>
-      <c r="N250" s="49">
-        <v>680</v>
-      </c>
-      <c r="O250" s="47" t="s">
+      <c r="F250" s="12">
+        <v>68452</v>
+      </c>
+      <c r="G250" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="H250" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="I250" s="13">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="J250" s="12">
+        <v>66037</v>
+      </c>
+      <c r="K250" s="12">
+        <v>11775</v>
+      </c>
+      <c r="L250" s="12" t="s">
+        <v>353</v>
+      </c>
+      <c r="M250" s="11">
+        <v>45905</v>
+      </c>
+      <c r="N250" s="14">
+        <v>1750</v>
+      </c>
+      <c r="O250" s="12" t="s">
         <v>122</v>
       </c>
-      <c r="P250" s="47">
+      <c r="P250" s="12">
         <v>30</v>
       </c>
-      <c r="Q250" s="47" t="s">
-        <v>407</v>
-      </c>
-      <c r="R250" s="47">
-        <f>DATEDIF(Tabela1[[#This Row],[Atendimento]],Tabela1[[#This Row],[Previsao de Entrega]],"D")</f>
-        <v>30</v>
-      </c>
-      <c r="S250" s="49">
-        <v>0</v>
-      </c>
-      <c r="T250" s="49">
+      <c r="Q250" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="R250" s="12">
+        <f>DATEDIF(Tabela1[[#This Row],[Atendimento]],Tabela1[[#This Row],[Previsao de Entrega]],"D")</f>
+        <v>65</v>
+      </c>
+      <c r="S250" s="14">
+        <v>0</v>
+      </c>
+      <c r="T250" s="14">
         <v>0</v>
       </c>
     </row>
     <row r="251" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A251" s="11">
-        <v>45867</v>
+        <v>45848</v>
       </c>
       <c r="B251" s="11">
-        <v>45866</v>
+        <v>45848</v>
       </c>
       <c r="C251" s="11" t="s">
         <v>7</v>
       </c>
       <c r="D251" s="11" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="E251" s="11" t="s">
-        <v>124</v>
+        <v>113</v>
       </c>
       <c r="F251" s="12">
-        <v>68483</v>
+        <v>68457</v>
       </c>
       <c r="G251" s="12" t="s">
-        <v>125</v>
+        <v>33</v>
       </c>
       <c r="H251" s="12" t="s">
-        <v>126</v>
+        <v>34</v>
       </c>
       <c r="I251" s="13">
-        <f>NETWORKDAYS(B251, A251)</f>
-        <v>2</v>
+        <f t="shared" si="4"/>
+        <v>1</v>
       </c>
       <c r="J251" s="12">
-        <v>66467</v>
+        <v>66126</v>
       </c>
       <c r="K251" s="12">
-        <v>11164</v>
+        <v>2931</v>
       </c>
       <c r="L251" s="12" t="s">
-        <v>298</v>
+        <v>366</v>
       </c>
       <c r="M251" s="11">
-        <v>45908</v>
+        <v>45905</v>
       </c>
       <c r="N251" s="14">
-        <v>2623.03</v>
+        <v>3500</v>
       </c>
       <c r="O251" s="12" t="s">
         <v>122</v>
       </c>
       <c r="P251" s="12">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="Q251" s="12" t="s">
         <v>24</v>
       </c>
       <c r="R251" s="12">
         <f>DATEDIF(Tabela1[[#This Row],[Atendimento]],Tabela1[[#This Row],[Previsao de Entrega]],"D")</f>
-        <v>41</v>
+        <v>57</v>
       </c>
       <c r="S251" s="14">
-        <v>52</v>
+        <v>320</v>
       </c>
       <c r="T251" s="14">
         <v>0</v>
@@ -18221,13 +18224,13 @@
     </row>
     <row r="252" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A252" s="11">
-        <v>45870</v>
+        <v>45874</v>
       </c>
       <c r="B252" s="11">
-        <v>45870</v>
+        <v>45853</v>
       </c>
       <c r="C252" s="11" t="s">
-        <v>128</v>
+        <v>7</v>
       </c>
       <c r="D252" s="11" t="s">
         <v>15</v>
@@ -18235,8 +18238,8 @@
       <c r="E252" s="11" t="s">
         <v>124</v>
       </c>
-      <c r="F252" s="12" t="s">
-        <v>3</v>
+      <c r="F252" s="12">
+        <v>68465</v>
       </c>
       <c r="G252" s="12" t="s">
         <v>125</v>
@@ -18245,39 +18248,39 @@
         <v>126</v>
       </c>
       <c r="I252" s="13">
-        <f>NETWORKDAYS(B252, A252)</f>
-        <v>1</v>
+        <f t="shared" si="4"/>
+        <v>16</v>
       </c>
       <c r="J252" s="12">
-        <v>66430</v>
+        <v>66555</v>
       </c>
       <c r="K252" s="12">
-        <v>333</v>
+        <v>11791</v>
       </c>
       <c r="L252" s="12" t="s">
-        <v>400</v>
+        <v>403</v>
       </c>
       <c r="M252" s="11">
-        <v>46113</v>
+        <v>45906</v>
       </c>
       <c r="N252" s="14">
-        <v>281569.34000000003</v>
+        <v>1075.55</v>
       </c>
       <c r="O252" s="12" t="s">
         <v>122</v>
       </c>
       <c r="P252" s="12">
-        <v>120</v>
+        <v>20</v>
       </c>
       <c r="Q252" s="12" t="s">
         <v>24</v>
       </c>
       <c r="R252" s="12">
         <f>DATEDIF(Tabela1[[#This Row],[Atendimento]],Tabela1[[#This Row],[Previsao de Entrega]],"D")</f>
-        <v>243</v>
+        <v>32</v>
       </c>
       <c r="S252" s="14">
-        <v>0</v>
+        <v>1215.25</v>
       </c>
       <c r="T252" s="14">
         <v>0</v>
@@ -18309,7 +18312,7 @@
         <v>32</v>
       </c>
       <c r="I253" s="10">
-        <f>NETWORKDAYS(B253, A253)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="J253" s="7">
@@ -18336,7 +18339,7 @@
       <c r="Q253" s="7" t="s">
         <v>116</v>
       </c>
-      <c r="R253" s="50">
+      <c r="R253" s="7">
         <f>DATEDIF(Tabela1[[#This Row],[Atendimento]],Tabela1[[#This Row],[Previsao de Entrega]],"D")</f>
         <v>0</v>
       </c>
@@ -18373,7 +18376,7 @@
         <v>32</v>
       </c>
       <c r="I254" s="10">
-        <f>NETWORKDAYS(B254, A254)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="J254" s="7">
@@ -18400,7 +18403,7 @@
       <c r="Q254" s="7" t="s">
         <v>116</v>
       </c>
-      <c r="R254" s="50">
+      <c r="R254" s="7">
         <f>DATEDIF(Tabela1[[#This Row],[Atendimento]],Tabela1[[#This Row],[Previsao de Entrega]],"D")</f>
         <v>0</v>
       </c>
@@ -18408,6 +18411,198 @@
         <v>0</v>
       </c>
       <c r="T254" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="255" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A255" s="11">
+        <v>45877</v>
+      </c>
+      <c r="B255" s="11">
+        <v>45873</v>
+      </c>
+      <c r="C255" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D255" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="E255" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="F255" s="12">
+        <v>68493</v>
+      </c>
+      <c r="G255" s="12" t="s">
+        <v>321</v>
+      </c>
+      <c r="H255" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="I255" s="13">
+        <f t="shared" si="4"/>
+        <v>5</v>
+      </c>
+      <c r="J255" s="12">
+        <v>66607</v>
+      </c>
+      <c r="K255" s="12">
+        <v>1586</v>
+      </c>
+      <c r="L255" s="12" t="s">
+        <v>408</v>
+      </c>
+      <c r="M255" s="11">
+        <v>45907</v>
+      </c>
+      <c r="N255" s="14">
+        <v>680</v>
+      </c>
+      <c r="O255" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="P255" s="12">
+        <v>30</v>
+      </c>
+      <c r="Q255" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="R255" s="12">
+        <f>DATEDIF(Tabela1[[#This Row],[Atendimento]],Tabela1[[#This Row],[Previsao de Entrega]],"D")</f>
+        <v>30</v>
+      </c>
+      <c r="S255" s="14">
+        <v>0</v>
+      </c>
+      <c r="T255" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="256" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A256" s="11">
+        <v>45867</v>
+      </c>
+      <c r="B256" s="11">
+        <v>45866</v>
+      </c>
+      <c r="C256" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D256" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="E256" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="F256" s="12">
+        <v>68483</v>
+      </c>
+      <c r="G256" s="12" t="s">
+        <v>125</v>
+      </c>
+      <c r="H256" s="12" t="s">
+        <v>126</v>
+      </c>
+      <c r="I256" s="13">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="J256" s="12">
+        <v>66467</v>
+      </c>
+      <c r="K256" s="12">
+        <v>11164</v>
+      </c>
+      <c r="L256" s="12" t="s">
+        <v>298</v>
+      </c>
+      <c r="M256" s="11">
+        <v>45908</v>
+      </c>
+      <c r="N256" s="14">
+        <v>2623.03</v>
+      </c>
+      <c r="O256" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="P256" s="12">
+        <v>28</v>
+      </c>
+      <c r="Q256" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="R256" s="12">
+        <f>DATEDIF(Tabela1[[#This Row],[Atendimento]],Tabela1[[#This Row],[Previsao de Entrega]],"D")</f>
+        <v>41</v>
+      </c>
+      <c r="S256" s="14">
+        <v>52</v>
+      </c>
+      <c r="T256" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="257" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A257" s="11">
+        <v>45870</v>
+      </c>
+      <c r="B257" s="11">
+        <v>45870</v>
+      </c>
+      <c r="C257" s="11" t="s">
+        <v>128</v>
+      </c>
+      <c r="D257" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="E257" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="F257" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="G257" s="12" t="s">
+        <v>125</v>
+      </c>
+      <c r="H257" s="12" t="s">
+        <v>126</v>
+      </c>
+      <c r="I257" s="13">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="J257" s="12">
+        <v>66430</v>
+      </c>
+      <c r="K257" s="12">
+        <v>333</v>
+      </c>
+      <c r="L257" s="12" t="s">
+        <v>400</v>
+      </c>
+      <c r="M257" s="11">
+        <v>46113</v>
+      </c>
+      <c r="N257" s="14">
+        <v>281569.34000000003</v>
+      </c>
+      <c r="O257" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="P257" s="12">
+        <v>120</v>
+      </c>
+      <c r="Q257" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="R257" s="12">
+        <f>DATEDIF(Tabela1[[#This Row],[Atendimento]],Tabela1[[#This Row],[Previsao de Entrega]],"D")</f>
+        <v>243</v>
+      </c>
+      <c r="S257" s="14">
+        <v>0</v>
+      </c>
+      <c r="T257" s="14">
         <v>0</v>
       </c>
     </row>
@@ -18684,7 +18879,7 @@
       </c>
       <c r="E2" s="24">
         <f t="shared" ref="E2:E6" ca="1" si="0">TODAY()</f>
-        <v>45877</v>
+        <v>45881</v>
       </c>
       <c r="F2" s="22" t="str">
         <f ca="1">IF(Tabela4[[#This Row],[Hoje]] &lt;= Tabela4[[#This Row],[Validade]],
@@ -18692,7 +18887,7 @@
       "Negociar",
       "Faltam " &amp; DATEDIF(Tabela4[[#This Row],[Hoje]],Tabela4[[#This Row],[Validade]],"D") &amp; " dias para vencer"),
    "Venceu há " &amp; DATEDIF(Tabela4[[#This Row],[Validade]],Tabela4[[#This Row],[Hoje]],"D") &amp; " dias")</f>
-        <v>Faltam 589 dias para vencer</v>
+        <v>Faltam 585 dias para vencer</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.35">
@@ -18710,7 +18905,7 @@
       </c>
       <c r="E3" s="26">
         <f t="shared" ca="1" si="0"/>
-        <v>45877</v>
+        <v>45881</v>
       </c>
       <c r="F3" s="21" t="str">
         <f ca="1">IF(Tabela4[[#This Row],[Hoje]] &lt;= Tabela4[[#This Row],[Validade]],
@@ -18718,7 +18913,7 @@
       "Negociar",
       "Faltam " &amp; DATEDIF(Tabela4[[#This Row],[Hoje]],Tabela4[[#This Row],[Validade]],"D") &amp; " dias para vencer"),
    "Venceu há " &amp; DATEDIF(Tabela4[[#This Row],[Validade]],Tabela4[[#This Row],[Hoje]],"D") &amp; " dias")</f>
-        <v>Venceu há 311 dias</v>
+        <v>Venceu há 315 dias</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.35">
@@ -18736,7 +18931,7 @@
       </c>
       <c r="E4" s="32">
         <f t="shared" ca="1" si="0"/>
-        <v>45877</v>
+        <v>45881</v>
       </c>
       <c r="F4" s="33" t="str">
         <f ca="1">IF(Tabela4[[#This Row],[Hoje]] &lt;= Tabela4[[#This Row],[Validade]],
@@ -18744,7 +18939,7 @@
       "Negociar",
       "Faltam " &amp; DATEDIF(Tabela4[[#This Row],[Hoje]],Tabela4[[#This Row],[Validade]],"D") &amp; " dias para vencer"),
    "Venceu há " &amp; DATEDIF(Tabela4[[#This Row],[Validade]],Tabela4[[#This Row],[Hoje]],"D") &amp; " dias")</f>
-        <v>Venceu há 19 dias</v>
+        <v>Venceu há 23 dias</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.35">
@@ -18762,7 +18957,7 @@
       </c>
       <c r="E5" s="17">
         <f t="shared" ca="1" si="0"/>
-        <v>45877</v>
+        <v>45881</v>
       </c>
       <c r="F5" s="3" t="str">
         <f ca="1">IF(Tabela4[[#This Row],[Hoje]] &lt;= Tabela4[[#This Row],[Validade]],
@@ -18788,7 +18983,7 @@
       </c>
       <c r="E6" s="17">
         <f t="shared" ca="1" si="0"/>
-        <v>45877</v>
+        <v>45881</v>
       </c>
       <c r="F6" s="3" t="str">
         <f ca="1">IF(Tabela4[[#This Row],[Hoje]] &lt;= Tabela4[[#This Row],[Validade]],
@@ -18814,7 +19009,7 @@
       </c>
       <c r="E7" s="26">
         <f t="shared" ref="E7:E9" ca="1" si="1">TODAY()</f>
-        <v>45877</v>
+        <v>45881</v>
       </c>
       <c r="F7" s="21" t="str">
         <f ca="1">IF(Tabela4[[#This Row],[Hoje]] &lt;= Tabela4[[#This Row],[Validade]],
@@ -18822,7 +19017,7 @@
       "Negociar",
       "Faltam " &amp; DATEDIF(Tabela4[[#This Row],[Hoje]],Tabela4[[#This Row],[Validade]],"D") &amp; " dias para vencer"),
    "Venceu há " &amp; DATEDIF(Tabela4[[#This Row],[Validade]],Tabela4[[#This Row],[Hoje]],"D") &amp; " dias")</f>
-        <v>Venceu há 143 dias</v>
+        <v>Venceu há 147 dias</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.35">
@@ -18840,7 +19035,7 @@
       </c>
       <c r="E8" s="26">
         <f t="shared" ca="1" si="1"/>
-        <v>45877</v>
+        <v>45881</v>
       </c>
       <c r="F8" s="21" t="str">
         <f ca="1">IF(Tabela4[[#This Row],[Hoje]] &lt;= Tabela4[[#This Row],[Validade]],
@@ -18848,7 +19043,7 @@
       "Negociar",
       "Faltam " &amp; DATEDIF(Tabela4[[#This Row],[Hoje]],Tabela4[[#This Row],[Validade]],"D") &amp; " dias para vencer"),
    "Venceu há " &amp; DATEDIF(Tabela4[[#This Row],[Validade]],Tabela4[[#This Row],[Hoje]],"D") &amp; " dias")</f>
-        <v>Venceu há 886 dias</v>
+        <v>Venceu há 890 dias</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.35">
@@ -18866,7 +19061,7 @@
       </c>
       <c r="E9" s="24">
         <f t="shared" ca="1" si="1"/>
-        <v>45877</v>
+        <v>45881</v>
       </c>
       <c r="F9" s="22" t="str">
         <f ca="1">IF(Tabela4[[#This Row],[Hoje]] &lt;= Tabela4[[#This Row],[Validade]],
@@ -18874,7 +19069,7 @@
       "Negociar",
       "Faltam " &amp; DATEDIF(Tabela4[[#This Row],[Hoje]],Tabela4[[#This Row],[Validade]],"D") &amp; " dias para vencer"),
    "Venceu há " &amp; DATEDIF(Tabela4[[#This Row],[Validade]],Tabela4[[#This Row],[Hoje]],"D") &amp; " dias")</f>
-        <v>Faltam 405 dias para vencer</v>
+        <v>Faltam 401 dias para vencer</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.35">
@@ -18892,7 +19087,7 @@
       </c>
       <c r="E10" s="24">
         <f ca="1">TODAY()</f>
-        <v>45877</v>
+        <v>45881</v>
       </c>
       <c r="F10" s="22" t="str">
         <f ca="1">IF(Tabela4[[#This Row],[Hoje]] &lt;= Tabela4[[#This Row],[Validade]],
@@ -18900,7 +19095,7 @@
       "Negociar",
       "Faltam " &amp; DATEDIF(Tabela4[[#This Row],[Hoje]],Tabela4[[#This Row],[Validade]],"D") &amp; " dias para vencer"),
    "Venceu há " &amp; DATEDIF(Tabela4[[#This Row],[Validade]],Tabela4[[#This Row],[Hoje]],"D") &amp; " dias")</f>
-        <v>Faltam 326 dias para vencer</v>
+        <v>Faltam 322 dias para vencer</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.35">
@@ -18918,7 +19113,7 @@
       </c>
       <c r="E11" s="24">
         <f ca="1">TODAY()</f>
-        <v>45877</v>
+        <v>45881</v>
       </c>
       <c r="F11" s="22" t="str">
         <f ca="1">IF(Tabela4[[#This Row],[Hoje]] &lt;= Tabela4[[#This Row],[Validade]],
@@ -18926,7 +19121,7 @@
       "Negociar",
       "Faltam " &amp; DATEDIF(Tabela4[[#This Row],[Hoje]],Tabela4[[#This Row],[Validade]],"D") &amp; " dias para vencer"),
    "Venceu há " &amp; DATEDIF(Tabela4[[#This Row],[Validade]],Tabela4[[#This Row],[Hoje]],"D") &amp; " dias")</f>
-        <v>Faltam 115 dias para vencer</v>
+        <v>Faltam 111 dias para vencer</v>
       </c>
     </row>
   </sheetData>
@@ -19666,10 +19861,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CC6577E-1BBE-47C5-96B8-0E0691F59A60}">
-  <dimension ref="A1:E40"/>
+  <dimension ref="A1:E41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -20359,6 +20554,23 @@
       </c>
       <c r="E40" t="s">
         <v>406</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A41" s="17">
+        <v>45880</v>
+      </c>
+      <c r="B41" t="s">
+        <v>409</v>
+      </c>
+      <c r="C41" t="s">
+        <v>287</v>
+      </c>
+      <c r="D41">
+        <v>11795</v>
+      </c>
+      <c r="E41" t="s">
+        <v>410</v>
       </c>
     </row>
   </sheetData>
@@ -20419,9 +20631,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -20551,26 +20766,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{258E5A34-0198-4570-927D-9873053383F0}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F1DB20CA-6C9E-462A-9B1E-209C1B3156BD}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="b7545978-8353-4157-ab02-92f5c69a97d9"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -20594,9 +20798,17 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F1DB20CA-6C9E-462A-9B1E-209C1B3156BD}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{258E5A34-0198-4570-927D-9873053383F0}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="b7545978-8353-4157-ab02-92f5c69a97d9"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Atualização Base = 12/08
</commit_message>
<xml_diff>
--- a/Atendimento.xlsx
+++ b/Atendimento.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\PUBLICO\Compras\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD5D64EC-004E-4BD4-9486-EA96EC0B9A6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24F456F7-9CE7-4B18-B33F-8262E1E652F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -76,7 +76,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2574" uniqueCount="411">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2590" uniqueCount="411">
   <si>
     <t>SC</t>
   </si>
@@ -1452,7 +1452,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1571,6 +1571,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1754,8 +1760,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0C573FEE-B8A0-4FE7-911C-81B026DE4530}" name="Tabela1" displayName="Tabela1" ref="A1:T257" totalsRowShown="0" headerRowDxfId="36" dataDxfId="35">
-  <autoFilter ref="A1:T257" xr:uid="{0C573FEE-B8A0-4FE7-911C-81B026DE4530}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0C573FEE-B8A0-4FE7-911C-81B026DE4530}" name="Tabela1" displayName="Tabela1" ref="A1:T259" totalsRowShown="0" headerRowDxfId="36" dataDxfId="35">
+  <autoFilter ref="A1:T259" xr:uid="{0C573FEE-B8A0-4FE7-911C-81B026DE4530}">
     <filterColumn colId="16">
       <filters>
         <filter val="AGUARDANDO APROVAÇÃO"/>
@@ -1763,8 +1769,8 @@
       </filters>
     </filterColumn>
   </autoFilter>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A11:T257">
-    <sortCondition ref="M1:M257"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A11:T259">
+    <sortCondition ref="M1:M259"/>
   </sortState>
   <tableColumns count="20">
     <tableColumn id="1" xr3:uid="{FD977268-8F92-4E92-82D7-959136F54294}" name="Atendimento" dataDxfId="34"/>
@@ -2129,10 +2135,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T257"/>
+  <dimension ref="A1:T259"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H233" sqref="H233"/>
+    <sheetView tabSelected="1" topLeftCell="A180" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K262" sqref="K262"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2153,7 +2159,7 @@
     <col min="14" max="14" width="15.26953125" style="2" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="15.81640625" style="1" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="26.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="25.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="25.1796875" style="1" customWidth="1"/>
     <col min="18" max="18" width="26.1796875" style="1" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="12.54296875" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="19.453125" style="1" bestFit="1" customWidth="1"/>
@@ -2824,7 +2830,7 @@
         <v>364</v>
       </c>
       <c r="I11" s="13">
-        <f t="shared" ref="I11:I74" si="1">NETWORKDAYS(B11, A11)</f>
+        <f>NETWORKDAYS(B11, A11)</f>
         <v>1</v>
       </c>
       <c r="J11" s="12">
@@ -2888,7 +2894,7 @@
         <v>32</v>
       </c>
       <c r="I12" s="10">
-        <f t="shared" si="1"/>
+        <f>NETWORKDAYS(B12, A12)</f>
         <v>1</v>
       </c>
       <c r="J12" s="7">
@@ -2952,7 +2958,7 @@
         <v>138</v>
       </c>
       <c r="I13" s="10">
-        <f t="shared" si="1"/>
+        <f>NETWORKDAYS(B13, A13)</f>
         <v>1</v>
       </c>
       <c r="J13" s="7">
@@ -3016,7 +3022,7 @@
         <v>32</v>
       </c>
       <c r="I14" s="10">
-        <f t="shared" si="1"/>
+        <f>NETWORKDAYS(B14, A14)</f>
         <v>1</v>
       </c>
       <c r="J14" s="7">
@@ -3080,7 +3086,7 @@
         <v>91</v>
       </c>
       <c r="I15" s="10">
-        <f t="shared" si="1"/>
+        <f>NETWORKDAYS(B15, A15)</f>
         <v>2</v>
       </c>
       <c r="J15" s="7">
@@ -3144,7 +3150,7 @@
         <v>91</v>
       </c>
       <c r="I16" s="10">
-        <f t="shared" si="1"/>
+        <f>NETWORKDAYS(B16, A16)</f>
         <v>10</v>
       </c>
       <c r="J16" s="7">
@@ -3208,7 +3214,7 @@
         <v>34</v>
       </c>
       <c r="I17" s="10">
-        <f t="shared" si="1"/>
+        <f>NETWORKDAYS(B17, A17)</f>
         <v>2</v>
       </c>
       <c r="J17" s="7">
@@ -3272,7 +3278,7 @@
         <v>34</v>
       </c>
       <c r="I18" s="10">
-        <f t="shared" si="1"/>
+        <f>NETWORKDAYS(B18, A18)</f>
         <v>9</v>
       </c>
       <c r="J18" s="7">
@@ -3336,7 +3342,7 @@
         <v>91</v>
       </c>
       <c r="I19" s="10">
-        <f t="shared" si="1"/>
+        <f>NETWORKDAYS(B19, A19)</f>
         <v>1</v>
       </c>
       <c r="J19" s="7">
@@ -3400,7 +3406,7 @@
         <v>32</v>
       </c>
       <c r="I20" s="10">
-        <f t="shared" si="1"/>
+        <f>NETWORKDAYS(B20, A20)</f>
         <v>1</v>
       </c>
       <c r="J20" s="7">
@@ -3464,7 +3470,7 @@
         <v>98</v>
       </c>
       <c r="I21" s="10">
-        <f t="shared" si="1"/>
+        <f>NETWORKDAYS(B21, A21)</f>
         <v>20</v>
       </c>
       <c r="J21" s="7">
@@ -3528,7 +3534,7 @@
         <v>98</v>
       </c>
       <c r="I22" s="10">
-        <f t="shared" si="1"/>
+        <f>NETWORKDAYS(B22, A22)</f>
         <v>3</v>
       </c>
       <c r="J22" s="7">
@@ -3592,7 +3598,7 @@
         <v>96</v>
       </c>
       <c r="I23" s="30">
-        <f t="shared" si="1"/>
+        <f>NETWORKDAYS(B23, A23)</f>
         <v>2</v>
       </c>
       <c r="J23" s="28">
@@ -3656,7 +3662,7 @@
         <v>34</v>
       </c>
       <c r="I24" s="10">
-        <f t="shared" si="1"/>
+        <f>NETWORKDAYS(B24, A24)</f>
         <v>2</v>
       </c>
       <c r="J24" s="7">
@@ -3720,7 +3726,7 @@
         <v>126</v>
       </c>
       <c r="I25" s="10">
-        <f t="shared" si="1"/>
+        <f>NETWORKDAYS(B25, A25)</f>
         <v>1</v>
       </c>
       <c r="J25" s="7">
@@ -3784,7 +3790,7 @@
         <v>130</v>
       </c>
       <c r="I26" s="10">
-        <f t="shared" si="1"/>
+        <f>NETWORKDAYS(B26, A26)</f>
         <v>1</v>
       </c>
       <c r="J26" s="7">
@@ -3848,7 +3854,7 @@
         <v>32</v>
       </c>
       <c r="I27" s="10">
-        <f t="shared" si="1"/>
+        <f>NETWORKDAYS(B27, A27)</f>
         <v>1</v>
       </c>
       <c r="J27" s="7">
@@ -3912,7 +3918,7 @@
         <v>32</v>
       </c>
       <c r="I28" s="10">
-        <f t="shared" si="1"/>
+        <f>NETWORKDAYS(B28, A28)</f>
         <v>1</v>
       </c>
       <c r="J28" s="7">
@@ -3976,7 +3982,7 @@
         <v>32</v>
       </c>
       <c r="I29" s="10">
-        <f t="shared" si="1"/>
+        <f>NETWORKDAYS(B29, A29)</f>
         <v>1</v>
       </c>
       <c r="J29" s="7">
@@ -4040,7 +4046,7 @@
         <v>138</v>
       </c>
       <c r="I30" s="10">
-        <f t="shared" si="1"/>
+        <f>NETWORKDAYS(B30, A30)</f>
         <v>1</v>
       </c>
       <c r="J30" s="7">
@@ -4104,7 +4110,7 @@
         <v>32</v>
       </c>
       <c r="I31" s="10">
-        <f t="shared" si="1"/>
+        <f>NETWORKDAYS(B31, A31)</f>
         <v>1</v>
       </c>
       <c r="J31" s="7">
@@ -4168,7 +4174,7 @@
         <v>130</v>
       </c>
       <c r="I32" s="10">
-        <f t="shared" si="1"/>
+        <f>NETWORKDAYS(B32, A32)</f>
         <v>3</v>
       </c>
       <c r="J32" s="7">
@@ -4232,7 +4238,7 @@
         <v>130</v>
       </c>
       <c r="I33" s="10">
-        <f t="shared" si="1"/>
+        <f>NETWORKDAYS(B33, A33)</f>
         <v>36</v>
       </c>
       <c r="J33" s="7">
@@ -4296,7 +4302,7 @@
         <v>34</v>
       </c>
       <c r="I34" s="10">
-        <f t="shared" si="1"/>
+        <f>NETWORKDAYS(B34, A34)</f>
         <v>1</v>
       </c>
       <c r="J34" s="7">
@@ -4360,7 +4366,7 @@
         <v>130</v>
       </c>
       <c r="I35" s="10">
-        <f t="shared" si="1"/>
+        <f>NETWORKDAYS(B35, A35)</f>
         <v>37</v>
       </c>
       <c r="J35" s="7">
@@ -4424,7 +4430,7 @@
         <v>98</v>
       </c>
       <c r="I36" s="10">
-        <f t="shared" si="1"/>
+        <f>NETWORKDAYS(B36, A36)</f>
         <v>4</v>
       </c>
       <c r="J36" s="7">
@@ -4488,7 +4494,7 @@
         <v>91</v>
       </c>
       <c r="I37" s="10">
-        <f t="shared" si="1"/>
+        <f>NETWORKDAYS(B37, A37)</f>
         <v>3</v>
       </c>
       <c r="J37" s="7">
@@ -4552,7 +4558,7 @@
         <v>91</v>
       </c>
       <c r="I38" s="10">
-        <f t="shared" si="1"/>
+        <f>NETWORKDAYS(B38, A38)</f>
         <v>3</v>
       </c>
       <c r="J38" s="7">
@@ -4616,7 +4622,7 @@
         <v>130</v>
       </c>
       <c r="I39" s="10">
-        <f t="shared" si="1"/>
+        <f>NETWORKDAYS(B39, A39)</f>
         <v>1</v>
       </c>
       <c r="J39" s="7">
@@ -4680,7 +4686,7 @@
         <v>32</v>
       </c>
       <c r="I40" s="10">
-        <f t="shared" si="1"/>
+        <f>NETWORKDAYS(B40, A40)</f>
         <v>1</v>
       </c>
       <c r="J40" s="7">
@@ -4744,7 +4750,7 @@
         <v>98</v>
       </c>
       <c r="I41" s="10">
-        <f t="shared" si="1"/>
+        <f>NETWORKDAYS(B41, A41)</f>
         <v>1</v>
       </c>
       <c r="J41" s="7">
@@ -4808,7 +4814,7 @@
         <v>34</v>
       </c>
       <c r="I42" s="10">
-        <f t="shared" si="1"/>
+        <f>NETWORKDAYS(B42, A42)</f>
         <v>9</v>
       </c>
       <c r="J42" s="7">
@@ -4872,7 +4878,7 @@
         <v>130</v>
       </c>
       <c r="I43" s="10">
-        <f t="shared" si="1"/>
+        <f>NETWORKDAYS(B43, A43)</f>
         <v>1</v>
       </c>
       <c r="J43" s="7">
@@ -4936,7 +4942,7 @@
         <v>34</v>
       </c>
       <c r="I44" s="10">
-        <f t="shared" si="1"/>
+        <f>NETWORKDAYS(B44, A44)</f>
         <v>9</v>
       </c>
       <c r="J44" s="7">
@@ -5000,7 +5006,7 @@
         <v>34</v>
       </c>
       <c r="I45" s="10">
-        <f t="shared" si="1"/>
+        <f>NETWORKDAYS(B45, A45)</f>
         <v>9</v>
       </c>
       <c r="J45" s="7">
@@ -5064,7 +5070,7 @@
         <v>32</v>
       </c>
       <c r="I46" s="10">
-        <f t="shared" si="1"/>
+        <f>NETWORKDAYS(B46, A46)</f>
         <v>1</v>
       </c>
       <c r="J46" s="7">
@@ -5128,7 +5134,7 @@
         <v>32</v>
       </c>
       <c r="I47" s="10">
-        <f t="shared" si="1"/>
+        <f>NETWORKDAYS(B47, A47)</f>
         <v>2</v>
       </c>
       <c r="J47" s="7">
@@ -5192,7 +5198,7 @@
         <v>130</v>
       </c>
       <c r="I48" s="10">
-        <f t="shared" si="1"/>
+        <f>NETWORKDAYS(B48, A48)</f>
         <v>1</v>
       </c>
       <c r="J48" s="7">
@@ -5256,7 +5262,7 @@
         <v>130</v>
       </c>
       <c r="I49" s="10">
-        <f t="shared" si="1"/>
+        <f>NETWORKDAYS(B49, A49)</f>
         <v>1</v>
       </c>
       <c r="J49" s="7">
@@ -5320,7 +5326,7 @@
         <v>130</v>
       </c>
       <c r="I50" s="10">
-        <f t="shared" si="1"/>
+        <f>NETWORKDAYS(B50, A50)</f>
         <v>1</v>
       </c>
       <c r="J50" s="7">
@@ -5384,7 +5390,7 @@
         <v>130</v>
       </c>
       <c r="I51" s="10">
-        <f t="shared" si="1"/>
+        <f>NETWORKDAYS(B51, A51)</f>
         <v>1</v>
       </c>
       <c r="J51" s="7">
@@ -5448,7 +5454,7 @@
         <v>98</v>
       </c>
       <c r="I52" s="10">
-        <f t="shared" si="1"/>
+        <f>NETWORKDAYS(B52, A52)</f>
         <v>1</v>
       </c>
       <c r="J52" s="7">
@@ -5512,7 +5518,7 @@
         <v>98</v>
       </c>
       <c r="I53" s="10">
-        <f t="shared" si="1"/>
+        <f>NETWORKDAYS(B53, A53)</f>
         <v>9</v>
       </c>
       <c r="J53" s="7">
@@ -5576,7 +5582,7 @@
         <v>34</v>
       </c>
       <c r="I54" s="10">
-        <f t="shared" si="1"/>
+        <f>NETWORKDAYS(B54, A54)</f>
         <v>1</v>
       </c>
       <c r="J54" s="7">
@@ -5640,7 +5646,7 @@
         <v>126</v>
       </c>
       <c r="I55" s="10">
-        <f t="shared" si="1"/>
+        <f>NETWORKDAYS(B55, A55)</f>
         <v>6</v>
       </c>
       <c r="J55" s="7">
@@ -5704,7 +5710,7 @@
         <v>130</v>
       </c>
       <c r="I56" s="10">
-        <f t="shared" si="1"/>
+        <f>NETWORKDAYS(B56, A56)</f>
         <v>1</v>
       </c>
       <c r="J56" s="7">
@@ -5768,7 +5774,7 @@
         <v>96</v>
       </c>
       <c r="I57" s="10">
-        <f t="shared" si="1"/>
+        <f>NETWORKDAYS(B57, A57)</f>
         <v>2</v>
       </c>
       <c r="J57" s="7">
@@ -5832,7 +5838,7 @@
         <v>32</v>
       </c>
       <c r="I58" s="10">
-        <f t="shared" si="1"/>
+        <f>NETWORKDAYS(B58, A58)</f>
         <v>1</v>
       </c>
       <c r="J58" s="7">
@@ -5896,7 +5902,7 @@
         <v>32</v>
       </c>
       <c r="I59" s="10">
-        <f t="shared" si="1"/>
+        <f>NETWORKDAYS(B59, A59)</f>
         <v>1</v>
       </c>
       <c r="J59" s="7">
@@ -5960,7 +5966,7 @@
         <v>32</v>
       </c>
       <c r="I60" s="10">
-        <f t="shared" si="1"/>
+        <f>NETWORKDAYS(B60, A60)</f>
         <v>1</v>
       </c>
       <c r="J60" s="7">
@@ -6024,7 +6030,7 @@
         <v>34</v>
       </c>
       <c r="I61" s="10">
-        <f t="shared" si="1"/>
+        <f>NETWORKDAYS(B61, A61)</f>
         <v>10</v>
       </c>
       <c r="J61" s="7">
@@ -6088,7 +6094,7 @@
         <v>130</v>
       </c>
       <c r="I62" s="10">
-        <f t="shared" si="1"/>
+        <f>NETWORKDAYS(B62, A62)</f>
         <v>1</v>
       </c>
       <c r="J62" s="7">
@@ -6152,7 +6158,7 @@
         <v>34</v>
       </c>
       <c r="I63" s="10">
-        <f t="shared" si="1"/>
+        <f>NETWORKDAYS(B63, A63)</f>
         <v>18</v>
       </c>
       <c r="J63" s="7">
@@ -6216,7 +6222,7 @@
         <v>91</v>
       </c>
       <c r="I64" s="10">
-        <f t="shared" si="1"/>
+        <f>NETWORKDAYS(B64, A64)</f>
         <v>4</v>
       </c>
       <c r="J64" s="7">
@@ -6280,7 +6286,7 @@
         <v>98</v>
       </c>
       <c r="I65" s="10">
-        <f t="shared" si="1"/>
+        <f>NETWORKDAYS(B65, A65)</f>
         <v>1</v>
       </c>
       <c r="J65" s="7">
@@ -6344,7 +6350,7 @@
         <v>98</v>
       </c>
       <c r="I66" s="10">
-        <f t="shared" si="1"/>
+        <f>NETWORKDAYS(B66, A66)</f>
         <v>2</v>
       </c>
       <c r="J66" s="7">
@@ -6408,7 +6414,7 @@
         <v>91</v>
       </c>
       <c r="I67" s="10">
-        <f t="shared" si="1"/>
+        <f>NETWORKDAYS(B67, A67)</f>
         <v>3</v>
       </c>
       <c r="J67" s="7">
@@ -6472,7 +6478,7 @@
         <v>32</v>
       </c>
       <c r="I68" s="10">
-        <f t="shared" si="1"/>
+        <f>NETWORKDAYS(B68, A68)</f>
         <v>1</v>
       </c>
       <c r="J68" s="7">
@@ -6536,7 +6542,7 @@
         <v>34</v>
       </c>
       <c r="I69" s="10">
-        <f t="shared" si="1"/>
+        <f>NETWORKDAYS(B69, A69)</f>
         <v>1</v>
       </c>
       <c r="J69" s="7">
@@ -6600,7 +6606,7 @@
         <v>98</v>
       </c>
       <c r="I70" s="10">
-        <f t="shared" si="1"/>
+        <f>NETWORKDAYS(B70, A70)</f>
         <v>4</v>
       </c>
       <c r="J70" s="7">
@@ -6664,7 +6670,7 @@
         <v>98</v>
       </c>
       <c r="I71" s="10">
-        <f t="shared" si="1"/>
+        <f>NETWORKDAYS(B71, A71)</f>
         <v>3</v>
       </c>
       <c r="J71" s="7">
@@ -6728,7 +6734,7 @@
         <v>98</v>
       </c>
       <c r="I72" s="10">
-        <f t="shared" si="1"/>
+        <f>NETWORKDAYS(B72, A72)</f>
         <v>2</v>
       </c>
       <c r="J72" s="7">
@@ -6792,7 +6798,7 @@
         <v>98</v>
       </c>
       <c r="I73" s="10">
-        <f t="shared" si="1"/>
+        <f>NETWORKDAYS(B73, A73)</f>
         <v>8</v>
       </c>
       <c r="J73" s="7">
@@ -6856,7 +6862,7 @@
         <v>98</v>
       </c>
       <c r="I74" s="10">
-        <f t="shared" si="1"/>
+        <f>NETWORKDAYS(B74, A74)</f>
         <v>26</v>
       </c>
       <c r="J74" s="7">
@@ -6920,7 +6926,7 @@
         <v>98</v>
       </c>
       <c r="I75" s="10">
-        <f t="shared" ref="I75:I138" si="2">NETWORKDAYS(B75, A75)</f>
+        <f>NETWORKDAYS(B75, A75)</f>
         <v>6</v>
       </c>
       <c r="J75" s="7">
@@ -6984,7 +6990,7 @@
         <v>91</v>
       </c>
       <c r="I76" s="10">
-        <f t="shared" si="2"/>
+        <f>NETWORKDAYS(B76, A76)</f>
         <v>3</v>
       </c>
       <c r="J76" s="7">
@@ -7048,7 +7054,7 @@
         <v>98</v>
       </c>
       <c r="I77" s="10">
-        <f t="shared" si="2"/>
+        <f>NETWORKDAYS(B77, A77)</f>
         <v>2</v>
       </c>
       <c r="J77" s="7">
@@ -7112,7 +7118,7 @@
         <v>32</v>
       </c>
       <c r="I78" s="10">
-        <f t="shared" si="2"/>
+        <f>NETWORKDAYS(B78, A78)</f>
         <v>1</v>
       </c>
       <c r="J78" s="7">
@@ -7176,7 +7182,7 @@
         <v>32</v>
       </c>
       <c r="I79" s="10">
-        <f t="shared" si="2"/>
+        <f>NETWORKDAYS(B79, A79)</f>
         <v>1</v>
       </c>
       <c r="J79" s="7">
@@ -7240,7 +7246,7 @@
         <v>138</v>
       </c>
       <c r="I80" s="10">
-        <f t="shared" si="2"/>
+        <f>NETWORKDAYS(B80, A80)</f>
         <v>1</v>
       </c>
       <c r="J80" s="7">
@@ -7304,7 +7310,7 @@
         <v>130</v>
       </c>
       <c r="I81" s="10">
-        <f t="shared" si="2"/>
+        <f>NETWORKDAYS(B81, A81)</f>
         <v>1</v>
       </c>
       <c r="J81" s="7">
@@ -7368,7 +7374,7 @@
         <v>98</v>
       </c>
       <c r="I82" s="10">
-        <f t="shared" si="2"/>
+        <f>NETWORKDAYS(B82, A82)</f>
         <v>1</v>
       </c>
       <c r="J82" s="7">
@@ -7432,7 +7438,7 @@
         <v>130</v>
       </c>
       <c r="I83" s="10">
-        <f t="shared" si="2"/>
+        <f>NETWORKDAYS(B83, A83)</f>
         <v>1</v>
       </c>
       <c r="J83" s="7">
@@ -7496,7 +7502,7 @@
         <v>98</v>
       </c>
       <c r="I84" s="10">
-        <f t="shared" si="2"/>
+        <f>NETWORKDAYS(B84, A84)</f>
         <v>2</v>
       </c>
       <c r="J84" s="7">
@@ -7560,7 +7566,7 @@
         <v>98</v>
       </c>
       <c r="I85" s="10">
-        <f t="shared" si="2"/>
+        <f>NETWORKDAYS(B85, A85)</f>
         <v>2</v>
       </c>
       <c r="J85" s="7">
@@ -7624,7 +7630,7 @@
         <v>34</v>
       </c>
       <c r="I86" s="30">
-        <f t="shared" si="2"/>
+        <f>NETWORKDAYS(B86, A86)</f>
         <v>2</v>
       </c>
       <c r="J86" s="28">
@@ -7688,7 +7694,7 @@
         <v>32</v>
       </c>
       <c r="I87" s="10">
-        <f t="shared" si="2"/>
+        <f>NETWORKDAYS(B87, A87)</f>
         <v>1</v>
       </c>
       <c r="J87" s="7">
@@ -7752,7 +7758,7 @@
         <v>32</v>
       </c>
       <c r="I88" s="10">
-        <f t="shared" si="2"/>
+        <f>NETWORKDAYS(B88, A88)</f>
         <v>1</v>
       </c>
       <c r="J88" s="7">
@@ -7816,7 +7822,7 @@
         <v>126</v>
       </c>
       <c r="I89" s="10">
-        <f t="shared" si="2"/>
+        <f>NETWORKDAYS(B89, A89)</f>
         <v>1</v>
       </c>
       <c r="J89" s="7">
@@ -7880,7 +7886,7 @@
         <v>98</v>
       </c>
       <c r="I90" s="10">
-        <f t="shared" si="2"/>
+        <f>NETWORKDAYS(B90, A90)</f>
         <v>1</v>
       </c>
       <c r="J90" s="7">
@@ -7944,7 +7950,7 @@
         <v>32</v>
       </c>
       <c r="I91" s="10">
-        <f t="shared" si="2"/>
+        <f>NETWORKDAYS(B91, A91)</f>
         <v>1</v>
       </c>
       <c r="J91" s="7">
@@ -8008,7 +8014,7 @@
         <v>98</v>
       </c>
       <c r="I92" s="10">
-        <f t="shared" si="2"/>
+        <f>NETWORKDAYS(B92, A92)</f>
         <v>4</v>
       </c>
       <c r="J92" s="7">
@@ -8072,7 +8078,7 @@
         <v>126</v>
       </c>
       <c r="I93" s="10">
-        <f t="shared" si="2"/>
+        <f>NETWORKDAYS(B93, A93)</f>
         <v>3</v>
       </c>
       <c r="J93" s="7">
@@ -8136,7 +8142,7 @@
         <v>126</v>
       </c>
       <c r="I94" s="10">
-        <f t="shared" si="2"/>
+        <f>NETWORKDAYS(B94, A94)</f>
         <v>1</v>
       </c>
       <c r="J94" s="7">
@@ -8200,7 +8206,7 @@
         <v>34</v>
       </c>
       <c r="I95" s="10">
-        <f t="shared" si="2"/>
+        <f>NETWORKDAYS(B95, A95)</f>
         <v>2</v>
       </c>
       <c r="J95" s="7">
@@ -8264,7 +8270,7 @@
         <v>130</v>
       </c>
       <c r="I96" s="10">
-        <f t="shared" si="2"/>
+        <f>NETWORKDAYS(B96, A96)</f>
         <v>1</v>
       </c>
       <c r="J96" s="7">
@@ -8328,7 +8334,7 @@
         <v>138</v>
       </c>
       <c r="I97" s="10">
-        <f t="shared" si="2"/>
+        <f>NETWORKDAYS(B97, A97)</f>
         <v>1</v>
       </c>
       <c r="J97" s="7">
@@ -8392,7 +8398,7 @@
         <v>98</v>
       </c>
       <c r="I98" s="10">
-        <f t="shared" si="2"/>
+        <f>NETWORKDAYS(B98, A98)</f>
         <v>1</v>
       </c>
       <c r="J98" s="7">
@@ -8456,7 +8462,7 @@
         <v>130</v>
       </c>
       <c r="I99" s="10">
-        <f t="shared" si="2"/>
+        <f>NETWORKDAYS(B99, A99)</f>
         <v>1</v>
       </c>
       <c r="J99" s="7">
@@ -8520,7 +8526,7 @@
         <v>130</v>
       </c>
       <c r="I100" s="10">
-        <f t="shared" si="2"/>
+        <f>NETWORKDAYS(B100, A100)</f>
         <v>24</v>
       </c>
       <c r="J100" s="7">
@@ -8584,7 +8590,7 @@
         <v>126</v>
       </c>
       <c r="I101" s="10">
-        <f t="shared" si="2"/>
+        <f>NETWORKDAYS(B101, A101)</f>
         <v>25</v>
       </c>
       <c r="J101" s="7">
@@ -8648,7 +8654,7 @@
         <v>98</v>
       </c>
       <c r="I102" s="10">
-        <f t="shared" si="2"/>
+        <f>NETWORKDAYS(B102, A102)</f>
         <v>1</v>
       </c>
       <c r="J102" s="7">
@@ -8712,7 +8718,7 @@
         <v>91</v>
       </c>
       <c r="I103" s="10">
-        <f t="shared" si="2"/>
+        <f>NETWORKDAYS(B103, A103)</f>
         <v>3</v>
       </c>
       <c r="J103" s="7">
@@ -8776,7 +8782,7 @@
         <v>91</v>
       </c>
       <c r="I104" s="10">
-        <f t="shared" si="2"/>
+        <f>NETWORKDAYS(B104, A104)</f>
         <v>3</v>
       </c>
       <c r="J104" s="7">
@@ -8840,7 +8846,7 @@
         <v>32</v>
       </c>
       <c r="I105" s="10">
-        <f t="shared" si="2"/>
+        <f>NETWORKDAYS(B105, A105)</f>
         <v>1</v>
       </c>
       <c r="J105" s="7">
@@ -8904,7 +8910,7 @@
         <v>32</v>
       </c>
       <c r="I106" s="10">
-        <f t="shared" si="2"/>
+        <f>NETWORKDAYS(B106, A106)</f>
         <v>1</v>
       </c>
       <c r="J106" s="7">
@@ -8968,7 +8974,7 @@
         <v>98</v>
       </c>
       <c r="I107" s="10">
-        <f t="shared" si="2"/>
+        <f>NETWORKDAYS(B107, A107)</f>
         <v>1</v>
       </c>
       <c r="J107" s="7">
@@ -9032,7 +9038,7 @@
         <v>96</v>
       </c>
       <c r="I108" s="10">
-        <f t="shared" si="2"/>
+        <f>NETWORKDAYS(B108, A108)</f>
         <v>6</v>
       </c>
       <c r="J108" s="7">
@@ -9096,7 +9102,7 @@
         <v>91</v>
       </c>
       <c r="I109" s="10">
-        <f t="shared" si="2"/>
+        <f>NETWORKDAYS(B109, A109)</f>
         <v>4</v>
       </c>
       <c r="J109" s="7">
@@ -9160,7 +9166,7 @@
         <v>91</v>
       </c>
       <c r="I110" s="10">
-        <f t="shared" si="2"/>
+        <f>NETWORKDAYS(B110, A110)</f>
         <v>4</v>
       </c>
       <c r="J110" s="7">
@@ -9224,7 +9230,7 @@
         <v>91</v>
       </c>
       <c r="I111" s="10">
-        <f t="shared" si="2"/>
+        <f>NETWORKDAYS(B111, A111)</f>
         <v>4</v>
       </c>
       <c r="J111" s="7">
@@ -9288,7 +9294,7 @@
         <v>126</v>
       </c>
       <c r="I112" s="10">
-        <f t="shared" si="2"/>
+        <f>NETWORKDAYS(B112, A112)</f>
         <v>9</v>
       </c>
       <c r="J112" s="7">
@@ -9352,7 +9358,7 @@
         <v>32</v>
       </c>
       <c r="I113" s="10">
-        <f t="shared" si="2"/>
+        <f>NETWORKDAYS(B113, A113)</f>
         <v>1</v>
       </c>
       <c r="J113" s="7">
@@ -9416,7 +9422,7 @@
         <v>96</v>
       </c>
       <c r="I114" s="10">
-        <f t="shared" si="2"/>
+        <f>NETWORKDAYS(B114, A114)</f>
         <v>1</v>
       </c>
       <c r="J114" s="7">
@@ -9480,7 +9486,7 @@
         <v>91</v>
       </c>
       <c r="I115" s="10">
-        <f t="shared" si="2"/>
+        <f>NETWORKDAYS(B115, A115)</f>
         <v>2</v>
       </c>
       <c r="J115" s="7">
@@ -9544,7 +9550,7 @@
         <v>32</v>
       </c>
       <c r="I116" s="10">
-        <f t="shared" si="2"/>
+        <f>NETWORKDAYS(B116, A116)</f>
         <v>1</v>
       </c>
       <c r="J116" s="7">
@@ -9608,7 +9614,7 @@
         <v>98</v>
       </c>
       <c r="I117" s="10">
-        <f t="shared" si="2"/>
+        <f>NETWORKDAYS(B117, A117)</f>
         <v>1</v>
       </c>
       <c r="J117" s="7">
@@ -9672,7 +9678,7 @@
         <v>91</v>
       </c>
       <c r="I118" s="10">
-        <f t="shared" si="2"/>
+        <f>NETWORKDAYS(B118, A118)</f>
         <v>5</v>
       </c>
       <c r="J118" s="7">
@@ -9736,7 +9742,7 @@
         <v>91</v>
       </c>
       <c r="I119" s="10">
-        <f t="shared" si="2"/>
+        <f>NETWORKDAYS(B119, A119)</f>
         <v>1</v>
       </c>
       <c r="J119" s="7">
@@ -9800,7 +9806,7 @@
         <v>91</v>
       </c>
       <c r="I120" s="10">
-        <f t="shared" si="2"/>
+        <f>NETWORKDAYS(B120, A120)</f>
         <v>1</v>
       </c>
       <c r="J120" s="7">
@@ -9864,7 +9870,7 @@
         <v>98</v>
       </c>
       <c r="I121" s="10">
-        <f t="shared" si="2"/>
+        <f>NETWORKDAYS(B121, A121)</f>
         <v>1</v>
       </c>
       <c r="J121" s="7">
@@ -9928,7 +9934,7 @@
         <v>126</v>
       </c>
       <c r="I122" s="10">
-        <f t="shared" si="2"/>
+        <f>NETWORKDAYS(B122, A122)</f>
         <v>18</v>
       </c>
       <c r="J122" s="7">
@@ -9992,7 +9998,7 @@
         <v>91</v>
       </c>
       <c r="I123" s="10">
-        <f t="shared" si="2"/>
+        <f>NETWORKDAYS(B123, A123)</f>
         <v>1</v>
       </c>
       <c r="J123" s="7">
@@ -10056,7 +10062,7 @@
         <v>32</v>
       </c>
       <c r="I124" s="10">
-        <f t="shared" si="2"/>
+        <f>NETWORKDAYS(B124, A124)</f>
         <v>1</v>
       </c>
       <c r="J124" s="7">
@@ -10120,7 +10126,7 @@
         <v>130</v>
       </c>
       <c r="I125" s="10">
-        <f t="shared" si="2"/>
+        <f>NETWORKDAYS(B125, A125)</f>
         <v>1</v>
       </c>
       <c r="J125" s="7">
@@ -10184,7 +10190,7 @@
         <v>130</v>
       </c>
       <c r="I126" s="10">
-        <f t="shared" si="2"/>
+        <f>NETWORKDAYS(B126, A126)</f>
         <v>1</v>
       </c>
       <c r="J126" s="7">
@@ -10248,7 +10254,7 @@
         <v>98</v>
       </c>
       <c r="I127" s="10">
-        <f t="shared" si="2"/>
+        <f>NETWORKDAYS(B127, A127)</f>
         <v>1</v>
       </c>
       <c r="J127" s="7">
@@ -10312,7 +10318,7 @@
         <v>130</v>
       </c>
       <c r="I128" s="10">
-        <f t="shared" si="2"/>
+        <f>NETWORKDAYS(B128, A128)</f>
         <v>1</v>
       </c>
       <c r="J128" s="7">
@@ -10376,7 +10382,7 @@
         <v>32</v>
       </c>
       <c r="I129" s="10">
-        <f t="shared" si="2"/>
+        <f>NETWORKDAYS(B129, A129)</f>
         <v>1</v>
       </c>
       <c r="J129" s="7">
@@ -10440,7 +10446,7 @@
         <v>32</v>
       </c>
       <c r="I130" s="10">
-        <f t="shared" si="2"/>
+        <f>NETWORKDAYS(B130, A130)</f>
         <v>1</v>
       </c>
       <c r="J130" s="7">
@@ -10504,7 +10510,7 @@
         <v>91</v>
       </c>
       <c r="I131" s="10">
-        <f t="shared" si="2"/>
+        <f>NETWORKDAYS(B131, A131)</f>
         <v>2</v>
       </c>
       <c r="J131" s="7">
@@ -10568,7 +10574,7 @@
         <v>126</v>
       </c>
       <c r="I132" s="10">
-        <f t="shared" si="2"/>
+        <f>NETWORKDAYS(B132, A132)</f>
         <v>28</v>
       </c>
       <c r="J132" s="7">
@@ -10632,7 +10638,7 @@
         <v>98</v>
       </c>
       <c r="I133" s="10">
-        <f t="shared" si="2"/>
+        <f>NETWORKDAYS(B133, A133)</f>
         <v>7</v>
       </c>
       <c r="J133" s="7">
@@ -10696,7 +10702,7 @@
         <v>126</v>
       </c>
       <c r="I134" s="10">
-        <f t="shared" si="2"/>
+        <f>NETWORKDAYS(B134, A134)</f>
         <v>6</v>
       </c>
       <c r="J134" s="7">
@@ -10760,7 +10766,7 @@
         <v>126</v>
       </c>
       <c r="I135" s="10">
-        <f t="shared" si="2"/>
+        <f>NETWORKDAYS(B135, A135)</f>
         <v>7</v>
       </c>
       <c r="J135" s="7">
@@ -10824,7 +10830,7 @@
         <v>32</v>
       </c>
       <c r="I136" s="10">
-        <f t="shared" si="2"/>
+        <f>NETWORKDAYS(B136, A136)</f>
         <v>1</v>
       </c>
       <c r="J136" s="7">
@@ -10888,7 +10894,7 @@
         <v>98</v>
       </c>
       <c r="I137" s="10">
-        <f t="shared" si="2"/>
+        <f>NETWORKDAYS(B137, A137)</f>
         <v>2</v>
       </c>
       <c r="J137" s="7">
@@ -10952,7 +10958,7 @@
         <v>98</v>
       </c>
       <c r="I138" s="10">
-        <f t="shared" si="2"/>
+        <f>NETWORKDAYS(B138, A138)</f>
         <v>7</v>
       </c>
       <c r="J138" s="7">
@@ -11016,7 +11022,7 @@
         <v>98</v>
       </c>
       <c r="I139" s="10">
-        <f t="shared" ref="I139:I202" si="3">NETWORKDAYS(B139, A139)</f>
+        <f>NETWORKDAYS(B139, A139)</f>
         <v>18</v>
       </c>
       <c r="J139" s="7">
@@ -11080,7 +11086,7 @@
         <v>91</v>
       </c>
       <c r="I140" s="10">
-        <f t="shared" si="3"/>
+        <f>NETWORKDAYS(B140, A140)</f>
         <v>6</v>
       </c>
       <c r="J140" s="7">
@@ -11144,7 +11150,7 @@
         <v>130</v>
       </c>
       <c r="I141" s="10">
-        <f t="shared" si="3"/>
+        <f>NETWORKDAYS(B141, A141)</f>
         <v>1</v>
       </c>
       <c r="J141" s="7">
@@ -11208,7 +11214,7 @@
         <v>372</v>
       </c>
       <c r="I142" s="10">
-        <f t="shared" si="3"/>
+        <f>NETWORKDAYS(B142, A142)</f>
         <v>1</v>
       </c>
       <c r="J142" s="7">
@@ -11272,7 +11278,7 @@
         <v>98</v>
       </c>
       <c r="I143" s="10">
-        <f t="shared" si="3"/>
+        <f>NETWORKDAYS(B143, A143)</f>
         <v>1</v>
       </c>
       <c r="J143" s="7">
@@ -11336,7 +11342,7 @@
         <v>34</v>
       </c>
       <c r="I144" s="10">
-        <f t="shared" si="3"/>
+        <f>NETWORKDAYS(B144, A144)</f>
         <v>1</v>
       </c>
       <c r="J144" s="7">
@@ -11400,7 +11406,7 @@
         <v>126</v>
       </c>
       <c r="I145" s="10">
-        <f t="shared" si="3"/>
+        <f>NETWORKDAYS(B145, A145)</f>
         <v>12</v>
       </c>
       <c r="J145" s="7">
@@ -11464,7 +11470,7 @@
         <v>91</v>
       </c>
       <c r="I146" s="10">
-        <f t="shared" si="3"/>
+        <f>NETWORKDAYS(B146, A146)</f>
         <v>4</v>
       </c>
       <c r="J146" s="7">
@@ -11528,7 +11534,7 @@
         <v>98</v>
       </c>
       <c r="I147" s="10">
-        <f t="shared" si="3"/>
+        <f>NETWORKDAYS(B147, A147)</f>
         <v>1</v>
       </c>
       <c r="J147" s="7">
@@ -11592,7 +11598,7 @@
         <v>138</v>
       </c>
       <c r="I148" s="10">
-        <f t="shared" si="3"/>
+        <f>NETWORKDAYS(B148, A148)</f>
         <v>1</v>
       </c>
       <c r="J148" s="7">
@@ -11656,7 +11662,7 @@
         <v>91</v>
       </c>
       <c r="I149" s="10">
-        <f t="shared" si="3"/>
+        <f>NETWORKDAYS(B149, A149)</f>
         <v>9</v>
       </c>
       <c r="J149" s="7">
@@ -11720,7 +11726,7 @@
         <v>130</v>
       </c>
       <c r="I150" s="10">
-        <f t="shared" si="3"/>
+        <f>NETWORKDAYS(B150, A150)</f>
         <v>1</v>
       </c>
       <c r="J150" s="7">
@@ -11784,7 +11790,7 @@
         <v>32</v>
       </c>
       <c r="I151" s="10">
-        <f t="shared" si="3"/>
+        <f>NETWORKDAYS(B151, A151)</f>
         <v>1</v>
       </c>
       <c r="J151" s="7">
@@ -11848,7 +11854,7 @@
         <v>91</v>
       </c>
       <c r="I152" s="10">
-        <f t="shared" si="3"/>
+        <f>NETWORKDAYS(B152, A152)</f>
         <v>1</v>
       </c>
       <c r="J152" s="7">
@@ -11912,7 +11918,7 @@
         <v>32</v>
       </c>
       <c r="I153" s="10">
-        <f t="shared" si="3"/>
+        <f>NETWORKDAYS(B153, A153)</f>
         <v>1</v>
       </c>
       <c r="J153" s="7">
@@ -11976,7 +11982,7 @@
         <v>34</v>
       </c>
       <c r="I154" s="10">
-        <f t="shared" si="3"/>
+        <f>NETWORKDAYS(B154, A154)</f>
         <v>1</v>
       </c>
       <c r="J154" s="7">
@@ -12040,7 +12046,7 @@
         <v>130</v>
       </c>
       <c r="I155" s="10">
-        <f t="shared" si="3"/>
+        <f>NETWORKDAYS(B155, A155)</f>
         <v>1</v>
       </c>
       <c r="J155" s="7">
@@ -12104,7 +12110,7 @@
         <v>98</v>
       </c>
       <c r="I156" s="10">
-        <f t="shared" si="3"/>
+        <f>NETWORKDAYS(B156, A156)</f>
         <v>1</v>
       </c>
       <c r="J156" s="7">
@@ -12168,7 +12174,7 @@
         <v>91</v>
       </c>
       <c r="I157" s="10">
-        <f t="shared" si="3"/>
+        <f>NETWORKDAYS(B157, A157)</f>
         <v>1</v>
       </c>
       <c r="J157" s="7">
@@ -12232,7 +12238,7 @@
         <v>91</v>
       </c>
       <c r="I158" s="10">
-        <f t="shared" si="3"/>
+        <f>NETWORKDAYS(B158, A158)</f>
         <v>1</v>
       </c>
       <c r="J158" s="7">
@@ -12296,7 +12302,7 @@
         <v>32</v>
       </c>
       <c r="I159" s="10">
-        <f t="shared" si="3"/>
+        <f>NETWORKDAYS(B159, A159)</f>
         <v>1</v>
       </c>
       <c r="J159" s="7">
@@ -12360,7 +12366,7 @@
         <v>32</v>
       </c>
       <c r="I160" s="10">
-        <f t="shared" si="3"/>
+        <f>NETWORKDAYS(B160, A160)</f>
         <v>1</v>
       </c>
       <c r="J160" s="7">
@@ -12424,7 +12430,7 @@
         <v>32</v>
       </c>
       <c r="I161" s="10">
-        <f t="shared" si="3"/>
+        <f>NETWORKDAYS(B161, A161)</f>
         <v>1</v>
       </c>
       <c r="J161" s="7">
@@ -12488,7 +12494,7 @@
         <v>32</v>
       </c>
       <c r="I162" s="10">
-        <f t="shared" si="3"/>
+        <f>NETWORKDAYS(B162, A162)</f>
         <v>1</v>
       </c>
       <c r="J162" s="7">
@@ -12552,7 +12558,7 @@
         <v>185</v>
       </c>
       <c r="I163" s="10">
-        <f t="shared" si="3"/>
+        <f>NETWORKDAYS(B163, A163)</f>
         <v>1</v>
       </c>
       <c r="J163" s="7">
@@ -12616,7 +12622,7 @@
         <v>91</v>
       </c>
       <c r="I164" s="10">
-        <f t="shared" si="3"/>
+        <f>NETWORKDAYS(B164, A164)</f>
         <v>17</v>
       </c>
       <c r="J164" s="7">
@@ -12680,7 +12686,7 @@
         <v>98</v>
       </c>
       <c r="I165" s="10">
-        <f t="shared" si="3"/>
+        <f>NETWORKDAYS(B165, A165)</f>
         <v>2</v>
       </c>
       <c r="J165" s="7">
@@ -12744,7 +12750,7 @@
         <v>91</v>
       </c>
       <c r="I166" s="10">
-        <f t="shared" si="3"/>
+        <f>NETWORKDAYS(B166, A166)</f>
         <v>4</v>
       </c>
       <c r="J166" s="7">
@@ -12808,7 +12814,7 @@
         <v>130</v>
       </c>
       <c r="I167" s="10">
-        <f t="shared" si="3"/>
+        <f>NETWORKDAYS(B167, A167)</f>
         <v>5</v>
       </c>
       <c r="J167" s="7">
@@ -12872,7 +12878,7 @@
         <v>32</v>
       </c>
       <c r="I168" s="10">
-        <f t="shared" si="3"/>
+        <f>NETWORKDAYS(B168, A168)</f>
         <v>1</v>
       </c>
       <c r="J168" s="7">
@@ -12936,7 +12942,7 @@
         <v>130</v>
       </c>
       <c r="I169" s="10">
-        <f t="shared" si="3"/>
+        <f>NETWORKDAYS(B169, A169)</f>
         <v>5</v>
       </c>
       <c r="J169" s="7">
@@ -13000,7 +13006,7 @@
         <v>130</v>
       </c>
       <c r="I170" s="10">
-        <f t="shared" si="3"/>
+        <f>NETWORKDAYS(B170, A170)</f>
         <v>1</v>
       </c>
       <c r="J170" s="7">
@@ -13064,7 +13070,7 @@
         <v>126</v>
       </c>
       <c r="I171" s="10">
-        <f t="shared" si="3"/>
+        <f>NETWORKDAYS(B171, A171)</f>
         <v>1</v>
       </c>
       <c r="J171" s="7">
@@ -13128,7 +13134,7 @@
         <v>130</v>
       </c>
       <c r="I172" s="10">
-        <f t="shared" si="3"/>
+        <f>NETWORKDAYS(B172, A172)</f>
         <v>1</v>
       </c>
       <c r="J172" s="7">
@@ -13192,7 +13198,7 @@
         <v>372</v>
       </c>
       <c r="I173" s="13">
-        <f t="shared" si="3"/>
+        <f>NETWORKDAYS(B173, A173)</f>
         <v>1</v>
       </c>
       <c r="J173" s="12">
@@ -13256,7 +13262,7 @@
         <v>32</v>
       </c>
       <c r="I174" s="10">
-        <f t="shared" si="3"/>
+        <f>NETWORKDAYS(B174, A174)</f>
         <v>1</v>
       </c>
       <c r="J174" s="7">
@@ -13320,7 +13326,7 @@
         <v>32</v>
       </c>
       <c r="I175" s="10">
-        <f t="shared" si="3"/>
+        <f>NETWORKDAYS(B175, A175)</f>
         <v>1</v>
       </c>
       <c r="J175" s="7">
@@ -13384,7 +13390,7 @@
         <v>138</v>
       </c>
       <c r="I176" s="10">
-        <f t="shared" si="3"/>
+        <f>NETWORKDAYS(B176, A176)</f>
         <v>1</v>
       </c>
       <c r="J176" s="7">
@@ -13448,7 +13454,7 @@
         <v>32</v>
       </c>
       <c r="I177" s="10">
-        <f t="shared" si="3"/>
+        <f>NETWORKDAYS(B177, A177)</f>
         <v>1</v>
       </c>
       <c r="J177" s="7">
@@ -13512,7 +13518,7 @@
         <v>130</v>
       </c>
       <c r="I178" s="10">
-        <f t="shared" si="3"/>
+        <f>NETWORKDAYS(B178, A178)</f>
         <v>1</v>
       </c>
       <c r="J178" s="7">
@@ -13576,7 +13582,7 @@
         <v>32</v>
       </c>
       <c r="I179" s="10">
-        <f t="shared" si="3"/>
+        <f>NETWORKDAYS(B179, A179)</f>
         <v>1</v>
       </c>
       <c r="J179" s="7">
@@ -13615,66 +13621,66 @@
       </c>
     </row>
     <row r="180" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A180" s="11">
-        <v>45785</v>
-      </c>
-      <c r="B180" s="11">
-        <v>45784</v>
-      </c>
-      <c r="C180" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="D180" s="11" t="s">
+      <c r="A180" s="46">
+        <v>45877</v>
+      </c>
+      <c r="B180" s="46">
+        <v>45877</v>
+      </c>
+      <c r="C180" s="46" t="s">
+        <v>7</v>
+      </c>
+      <c r="D180" s="46" t="s">
         <v>5</v>
       </c>
-      <c r="E180" s="11" t="s">
-        <v>113</v>
-      </c>
-      <c r="F180" s="12">
-        <v>68369</v>
-      </c>
-      <c r="G180" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="H180" s="12" t="s">
-        <v>98</v>
-      </c>
-      <c r="I180" s="13">
-        <f t="shared" si="3"/>
-        <v>2</v>
-      </c>
-      <c r="J180" s="12">
-        <v>65234</v>
-      </c>
-      <c r="K180" s="12">
-        <v>11610</v>
-      </c>
-      <c r="L180" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="M180" s="11">
+      <c r="E180" s="46" t="s">
+        <v>142</v>
+      </c>
+      <c r="F180" s="47" t="s">
+        <v>3</v>
+      </c>
+      <c r="G180" s="47" t="s">
+        <v>3</v>
+      </c>
+      <c r="H180" s="47" t="s">
+        <v>32</v>
+      </c>
+      <c r="I180" s="48">
+        <f>NETWORKDAYS(B180, A180)</f>
+        <v>1</v>
+      </c>
+      <c r="J180" s="47">
+        <v>66627</v>
+      </c>
+      <c r="K180" s="47">
+        <v>11127</v>
+      </c>
+      <c r="L180" s="47" t="s">
+        <v>221</v>
+      </c>
+      <c r="M180" s="46">
         <v>45881</v>
       </c>
-      <c r="N180" s="14">
-        <v>9114.5499999999993</v>
-      </c>
-      <c r="O180" s="12" t="s">
+      <c r="N180" s="49">
+        <v>547.91999999999996</v>
+      </c>
+      <c r="O180" s="47" t="s">
         <v>122</v>
       </c>
-      <c r="P180" s="12">
-        <v>28</v>
-      </c>
-      <c r="Q180" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="R180" s="12">
-        <f>DATEDIF(Tabela1[[#This Row],[Atendimento]],Tabela1[[#This Row],[Previsao de Entrega]],"D")</f>
-        <v>96</v>
-      </c>
-      <c r="S180" s="14">
-        <v>183.5</v>
-      </c>
-      <c r="T180" s="14">
+      <c r="P180" s="47">
+        <v>35</v>
+      </c>
+      <c r="Q180" s="47" t="s">
+        <v>407</v>
+      </c>
+      <c r="R180" s="47">
+        <f>DATEDIF(Tabela1[[#This Row],[Atendimento]],Tabela1[[#This Row],[Previsao de Entrega]],"D")</f>
+        <v>4</v>
+      </c>
+      <c r="S180" s="49">
+        <v>0</v>
+      </c>
+      <c r="T180" s="49">
         <v>0</v>
       </c>
     </row>
@@ -13704,7 +13710,7 @@
         <v>91</v>
       </c>
       <c r="I181" s="10">
-        <f t="shared" si="3"/>
+        <f>NETWORKDAYS(B181, A181)</f>
         <v>1</v>
       </c>
       <c r="J181" s="7">
@@ -13742,67 +13748,67 @@
         <v>0</v>
       </c>
     </row>
-    <row r="182" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A182" s="11">
+    <row r="182" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A182" s="6">
         <v>45846</v>
       </c>
-      <c r="B182" s="11">
+      <c r="B182" s="6">
         <v>45846</v>
       </c>
-      <c r="C182" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="D182" s="11" t="s">
+      <c r="C182" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D182" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="E182" s="11" t="s">
+      <c r="E182" s="6" t="s">
         <v>113</v>
       </c>
-      <c r="F182" s="12">
+      <c r="F182" s="7">
         <v>68456</v>
       </c>
-      <c r="G182" s="12" t="s">
+      <c r="G182" s="7" t="s">
         <v>321</v>
       </c>
-      <c r="H182" s="12" t="s">
+      <c r="H182" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="I182" s="13">
-        <f t="shared" si="3"/>
+      <c r="I182" s="10">
+        <f>NETWORKDAYS(B182, A182)</f>
         <v>1</v>
       </c>
-      <c r="J182" s="12">
+      <c r="J182" s="7">
         <v>66118</v>
       </c>
-      <c r="K182" s="12">
+      <c r="K182" s="7">
         <v>2289</v>
       </c>
-      <c r="L182" s="12" t="s">
+      <c r="L182" s="7" t="s">
         <v>360</v>
       </c>
-      <c r="M182" s="11">
+      <c r="M182" s="6">
         <v>45881</v>
       </c>
-      <c r="N182" s="14">
+      <c r="N182" s="8">
         <v>607.57000000000005</v>
       </c>
-      <c r="O182" s="12" t="s">
+      <c r="O182" s="7" t="s">
         <v>122</v>
       </c>
-      <c r="P182" s="12">
+      <c r="P182" s="7">
         <v>21</v>
       </c>
-      <c r="Q182" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="R182" s="12">
+      <c r="Q182" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="R182" s="7">
         <f>DATEDIF(Tabela1[[#This Row],[Atendimento]],Tabela1[[#This Row],[Previsao de Entrega]],"D")</f>
         <v>35</v>
       </c>
-      <c r="S182" s="14">
-        <v>0</v>
-      </c>
-      <c r="T182" s="14">
+      <c r="S182" s="8">
+        <v>0</v>
+      </c>
+      <c r="T182" s="8">
         <v>0</v>
       </c>
     </row>
@@ -13832,7 +13838,7 @@
         <v>98</v>
       </c>
       <c r="I183" s="10">
-        <f t="shared" si="3"/>
+        <f>NETWORKDAYS(B183, A183)</f>
         <v>1</v>
       </c>
       <c r="J183" s="7">
@@ -13896,7 +13902,7 @@
         <v>98</v>
       </c>
       <c r="I184" s="10">
-        <f t="shared" si="3"/>
+        <f>NETWORKDAYS(B184, A184)</f>
         <v>1</v>
       </c>
       <c r="J184" s="7">
@@ -13960,7 +13966,7 @@
         <v>34</v>
       </c>
       <c r="I185" s="10">
-        <f t="shared" si="3"/>
+        <f>NETWORKDAYS(B185, A185)</f>
         <v>1</v>
       </c>
       <c r="J185" s="7">
@@ -14024,7 +14030,7 @@
         <v>96</v>
       </c>
       <c r="I186" s="10">
-        <f t="shared" si="3"/>
+        <f>NETWORKDAYS(B186, A186)</f>
         <v>1</v>
       </c>
       <c r="J186" s="7">
@@ -14088,7 +14094,7 @@
         <v>32</v>
       </c>
       <c r="I187" s="10">
-        <f t="shared" si="3"/>
+        <f>NETWORKDAYS(B187, A187)</f>
         <v>1</v>
       </c>
       <c r="J187" s="7">
@@ -14127,66 +14133,66 @@
       </c>
     </row>
     <row r="188" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A188" s="46">
-        <v>45877</v>
-      </c>
-      <c r="B188" s="46">
-        <v>45877</v>
-      </c>
-      <c r="C188" s="46" t="s">
-        <v>7</v>
-      </c>
-      <c r="D188" s="46" t="s">
+      <c r="A188" s="11">
+        <v>45868</v>
+      </c>
+      <c r="B188" s="11">
+        <v>45868</v>
+      </c>
+      <c r="C188" s="11" t="s">
+        <v>128</v>
+      </c>
+      <c r="D188" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="E188" s="46" t="s">
-        <v>142</v>
-      </c>
-      <c r="F188" s="47" t="s">
-        <v>3</v>
-      </c>
-      <c r="G188" s="47" t="s">
-        <v>3</v>
-      </c>
-      <c r="H188" s="47" t="s">
-        <v>32</v>
-      </c>
-      <c r="I188" s="48">
-        <f t="shared" si="3"/>
+      <c r="E188" s="11" t="s">
+        <v>394</v>
+      </c>
+      <c r="F188" s="12">
+        <v>68487</v>
+      </c>
+      <c r="G188" s="12" t="s">
+        <v>395</v>
+      </c>
+      <c r="H188" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="I188" s="13">
+        <f>NETWORKDAYS(B188, A188)</f>
         <v>1</v>
       </c>
-      <c r="J188" s="47">
-        <v>66627</v>
-      </c>
-      <c r="K188" s="47">
-        <v>11127</v>
-      </c>
-      <c r="L188" s="47" t="s">
-        <v>221</v>
-      </c>
-      <c r="M188" s="46">
-        <v>45881</v>
-      </c>
-      <c r="N188" s="49">
-        <v>547.91999999999996</v>
-      </c>
-      <c r="O188" s="47" t="s">
-        <v>122</v>
-      </c>
-      <c r="P188" s="47">
-        <v>35</v>
-      </c>
-      <c r="Q188" s="47" t="s">
-        <v>407</v>
-      </c>
-      <c r="R188" s="47">
-        <f>DATEDIF(Tabela1[[#This Row],[Atendimento]],Tabela1[[#This Row],[Previsao de Entrega]],"D")</f>
-        <v>4</v>
-      </c>
-      <c r="S188" s="49">
-        <v>0</v>
-      </c>
-      <c r="T188" s="49">
+      <c r="J188" s="12">
+        <v>66489</v>
+      </c>
+      <c r="K188" s="12">
+        <v>11614</v>
+      </c>
+      <c r="L188" s="12" t="s">
+        <v>396</v>
+      </c>
+      <c r="M188" s="11">
+        <v>45882</v>
+      </c>
+      <c r="N188" s="14">
+        <v>6633</v>
+      </c>
+      <c r="O188" s="12" t="s">
+        <v>121</v>
+      </c>
+      <c r="P188" s="12">
+        <v>1</v>
+      </c>
+      <c r="Q188" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="R188" s="12">
+        <f>DATEDIF(Tabela1[[#This Row],[Atendimento]],Tabela1[[#This Row],[Previsao de Entrega]],"D")</f>
+        <v>14</v>
+      </c>
+      <c r="S188" s="14">
+        <v>0</v>
+      </c>
+      <c r="T188" s="14">
         <v>0</v>
       </c>
     </row>
@@ -14216,7 +14222,7 @@
         <v>34</v>
       </c>
       <c r="I189" s="10">
-        <f t="shared" si="3"/>
+        <f>NETWORKDAYS(B189, A189)</f>
         <v>1</v>
       </c>
       <c r="J189" s="7">
@@ -14280,7 +14286,7 @@
         <v>91</v>
       </c>
       <c r="I190" s="10">
-        <f t="shared" si="3"/>
+        <f>NETWORKDAYS(B190, A190)</f>
         <v>1</v>
       </c>
       <c r="J190" s="7">
@@ -14344,7 +14350,7 @@
         <v>34</v>
       </c>
       <c r="I191" s="10">
-        <f t="shared" si="3"/>
+        <f>NETWORKDAYS(B191, A191)</f>
         <v>1</v>
       </c>
       <c r="J191" s="7">
@@ -14384,63 +14390,63 @@
     </row>
     <row r="192" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A192" s="11">
-        <v>45868</v>
+        <v>45867</v>
       </c>
       <c r="B192" s="11">
-        <v>45868</v>
+        <v>45867</v>
       </c>
       <c r="C192" s="11" t="s">
         <v>128</v>
       </c>
       <c r="D192" s="11" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="E192" s="11" t="s">
-        <v>394</v>
+        <v>113</v>
       </c>
       <c r="F192" s="12">
-        <v>68487</v>
+        <v>68486</v>
       </c>
       <c r="G192" s="12" t="s">
-        <v>395</v>
+        <v>296</v>
       </c>
       <c r="H192" s="12" t="s">
         <v>96</v>
       </c>
       <c r="I192" s="13">
-        <f t="shared" si="3"/>
+        <f>NETWORKDAYS(B192, A192)</f>
         <v>1</v>
       </c>
       <c r="J192" s="12">
-        <v>66489</v>
+        <v>66478</v>
       </c>
       <c r="K192" s="12">
-        <v>11614</v>
+        <v>10460</v>
       </c>
       <c r="L192" s="12" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="M192" s="11">
-        <v>45882</v>
+        <v>45883</v>
       </c>
       <c r="N192" s="14">
-        <v>6633</v>
+        <v>4789.6099999999997</v>
       </c>
       <c r="O192" s="12" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="P192" s="12">
-        <v>1</v>
+        <v>28</v>
       </c>
       <c r="Q192" s="12" t="s">
         <v>24</v>
       </c>
       <c r="R192" s="12">
         <f>DATEDIF(Tabela1[[#This Row],[Atendimento]],Tabela1[[#This Row],[Previsao de Entrega]],"D")</f>
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="S192" s="14">
-        <v>0</v>
+        <v>1080.08</v>
       </c>
       <c r="T192" s="14">
         <v>0</v>
@@ -14472,7 +14478,7 @@
         <v>98</v>
       </c>
       <c r="I193" s="10">
-        <f t="shared" si="3"/>
+        <f>NETWORKDAYS(B193, A193)</f>
         <v>1</v>
       </c>
       <c r="J193" s="7">
@@ -14536,7 +14542,7 @@
         <v>372</v>
       </c>
       <c r="I194" s="10">
-        <f t="shared" si="3"/>
+        <f>NETWORKDAYS(B194, A194)</f>
         <v>1</v>
       </c>
       <c r="J194" s="7">
@@ -14600,7 +14606,7 @@
         <v>32</v>
       </c>
       <c r="I195" s="10">
-        <f t="shared" si="3"/>
+        <f>NETWORKDAYS(B195, A195)</f>
         <v>1</v>
       </c>
       <c r="J195" s="7">
@@ -14664,7 +14670,7 @@
         <v>372</v>
       </c>
       <c r="I196" s="10">
-        <f t="shared" si="3"/>
+        <f>NETWORKDAYS(B196, A196)</f>
         <v>1</v>
       </c>
       <c r="J196" s="7">
@@ -14728,7 +14734,7 @@
         <v>372</v>
       </c>
       <c r="I197" s="10">
-        <f t="shared" si="3"/>
+        <f>NETWORKDAYS(B197, A197)</f>
         <v>1</v>
       </c>
       <c r="J197" s="7">
@@ -14792,7 +14798,7 @@
         <v>372</v>
       </c>
       <c r="I198" s="10">
-        <f t="shared" si="3"/>
+        <f>NETWORKDAYS(B198, A198)</f>
         <v>1</v>
       </c>
       <c r="J198" s="7">
@@ -14856,7 +14862,7 @@
         <v>32</v>
       </c>
       <c r="I199" s="10">
-        <f t="shared" si="3"/>
+        <f>NETWORKDAYS(B199, A199)</f>
         <v>1</v>
       </c>
       <c r="J199" s="7">
@@ -14920,7 +14926,7 @@
         <v>32</v>
       </c>
       <c r="I200" s="10">
-        <f t="shared" si="3"/>
+        <f>NETWORKDAYS(B200, A200)</f>
         <v>1</v>
       </c>
       <c r="J200" s="7">
@@ -14984,7 +14990,7 @@
         <v>126</v>
       </c>
       <c r="I201" s="10">
-        <f t="shared" si="3"/>
+        <f>NETWORKDAYS(B201, A201)</f>
         <v>1</v>
       </c>
       <c r="J201" s="7">
@@ -15048,7 +15054,7 @@
         <v>130</v>
       </c>
       <c r="I202" s="10">
-        <f t="shared" si="3"/>
+        <f>NETWORKDAYS(B202, A202)</f>
         <v>1</v>
       </c>
       <c r="J202" s="7">
@@ -15112,7 +15118,7 @@
         <v>32</v>
       </c>
       <c r="I203" s="10">
-        <f t="shared" ref="I203:I257" si="4">NETWORKDAYS(B203, A203)</f>
+        <f>NETWORKDAYS(B203, A203)</f>
         <v>1</v>
       </c>
       <c r="J203" s="7">
@@ -15176,7 +15182,7 @@
         <v>32</v>
       </c>
       <c r="I204" s="10">
-        <f t="shared" si="4"/>
+        <f>NETWORKDAYS(B204, A204)</f>
         <v>1</v>
       </c>
       <c r="J204" s="7">
@@ -15240,7 +15246,7 @@
         <v>34</v>
       </c>
       <c r="I205" s="10">
-        <f t="shared" si="4"/>
+        <f>NETWORKDAYS(B205, A205)</f>
         <v>1</v>
       </c>
       <c r="J205" s="7">
@@ -15304,7 +15310,7 @@
         <v>126</v>
       </c>
       <c r="I206" s="10">
-        <f t="shared" si="4"/>
+        <f>NETWORKDAYS(B206, A206)</f>
         <v>1</v>
       </c>
       <c r="J206" s="7">
@@ -15368,7 +15374,7 @@
         <v>130</v>
       </c>
       <c r="I207" s="10">
-        <f t="shared" si="4"/>
+        <f>NETWORKDAYS(B207, A207)</f>
         <v>1</v>
       </c>
       <c r="J207" s="7">
@@ -15432,7 +15438,7 @@
         <v>130</v>
       </c>
       <c r="I208" s="10">
-        <f t="shared" si="4"/>
+        <f>NETWORKDAYS(B208, A208)</f>
         <v>1</v>
       </c>
       <c r="J208" s="7">
@@ -15496,7 +15502,7 @@
         <v>130</v>
       </c>
       <c r="I209" s="10">
-        <f t="shared" si="4"/>
+        <f>NETWORKDAYS(B209, A209)</f>
         <v>1</v>
       </c>
       <c r="J209" s="7">
@@ -15560,7 +15566,7 @@
         <v>130</v>
       </c>
       <c r="I210" s="10">
-        <f t="shared" si="4"/>
+        <f>NETWORKDAYS(B210, A210)</f>
         <v>1</v>
       </c>
       <c r="J210" s="7">
@@ -15624,7 +15630,7 @@
         <v>34</v>
       </c>
       <c r="I211" s="10">
-        <f t="shared" si="4"/>
+        <f>NETWORKDAYS(B211, A211)</f>
         <v>1</v>
       </c>
       <c r="J211" s="7">
@@ -15688,7 +15694,7 @@
         <v>32</v>
       </c>
       <c r="I212" s="10">
-        <f t="shared" si="4"/>
+        <f>NETWORKDAYS(B212, A212)</f>
         <v>1</v>
       </c>
       <c r="J212" s="7">
@@ -15752,7 +15758,7 @@
         <v>138</v>
       </c>
       <c r="I213" s="10">
-        <f t="shared" si="4"/>
+        <f>NETWORKDAYS(B213, A213)</f>
         <v>1</v>
       </c>
       <c r="J213" s="7">
@@ -15816,7 +15822,7 @@
         <v>91</v>
       </c>
       <c r="I214" s="10">
-        <f t="shared" si="4"/>
+        <f>NETWORKDAYS(B214, A214)</f>
         <v>1</v>
       </c>
       <c r="J214" s="7">
@@ -15880,7 +15886,7 @@
         <v>98</v>
       </c>
       <c r="I215" s="10">
-        <f t="shared" si="4"/>
+        <f>NETWORKDAYS(B215, A215)</f>
         <v>1</v>
       </c>
       <c r="J215" s="7">
@@ -15944,7 +15950,7 @@
         <v>138</v>
       </c>
       <c r="I216" s="10">
-        <f t="shared" si="4"/>
+        <f>NETWORKDAYS(B216, A216)</f>
         <v>1</v>
       </c>
       <c r="J216" s="7">
@@ -16008,7 +16014,7 @@
         <v>98</v>
       </c>
       <c r="I217" s="10">
-        <f t="shared" si="4"/>
+        <f>NETWORKDAYS(B217, A217)</f>
         <v>1</v>
       </c>
       <c r="J217" s="7">
@@ -16047,66 +16053,66 @@
       </c>
     </row>
     <row r="218" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A218" s="46">
-        <v>45868</v>
-      </c>
-      <c r="B218" s="46">
-        <v>45862</v>
-      </c>
-      <c r="C218" s="46" t="s">
-        <v>7</v>
-      </c>
-      <c r="D218" s="46" t="s">
+      <c r="A218" s="11">
+        <v>45870</v>
+      </c>
+      <c r="B218" s="11">
+        <v>45869</v>
+      </c>
+      <c r="C218" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D218" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="E218" s="46" t="s">
+      <c r="E218" s="11" t="s">
         <v>113</v>
       </c>
-      <c r="F218" s="47">
-        <v>68476</v>
-      </c>
-      <c r="G218" s="47" t="s">
-        <v>227</v>
-      </c>
-      <c r="H218" s="47" t="s">
-        <v>98</v>
-      </c>
-      <c r="I218" s="48">
-        <f t="shared" si="4"/>
-        <v>5</v>
-      </c>
-      <c r="J218" s="47">
-        <v>66491</v>
-      </c>
-      <c r="K218" s="47">
-        <v>11522</v>
-      </c>
-      <c r="L218" s="47" t="s">
-        <v>376</v>
-      </c>
-      <c r="M218" s="46">
-        <v>45888</v>
-      </c>
-      <c r="N218" s="49">
-        <v>1680.4</v>
-      </c>
-      <c r="O218" s="47" t="s">
+      <c r="F218" s="12">
+        <v>68491</v>
+      </c>
+      <c r="G218" s="12" t="s">
+        <v>371</v>
+      </c>
+      <c r="H218" s="12" t="s">
+        <v>372</v>
+      </c>
+      <c r="I218" s="13">
+        <f>NETWORKDAYS(B218, A218)</f>
+        <v>2</v>
+      </c>
+      <c r="J218" s="12">
+        <v>66521</v>
+      </c>
+      <c r="K218" s="12">
+        <v>3061</v>
+      </c>
+      <c r="L218" s="12" t="s">
+        <v>192</v>
+      </c>
+      <c r="M218" s="11">
+        <v>45883</v>
+      </c>
+      <c r="N218" s="14">
+        <v>3000</v>
+      </c>
+      <c r="O218" s="12" t="s">
         <v>122</v>
       </c>
-      <c r="P218" s="47">
-        <v>28</v>
-      </c>
-      <c r="Q218" s="47" t="s">
-        <v>407</v>
-      </c>
-      <c r="R218" s="47">
-        <f>DATEDIF(Tabela1[[#This Row],[Atendimento]],Tabela1[[#This Row],[Previsao de Entrega]],"D")</f>
-        <v>20</v>
-      </c>
-      <c r="S218" s="49">
-        <v>0</v>
-      </c>
-      <c r="T218" s="49">
+      <c r="P218" s="12">
+        <v>15</v>
+      </c>
+      <c r="Q218" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="R218" s="12">
+        <f>DATEDIF(Tabela1[[#This Row],[Atendimento]],Tabela1[[#This Row],[Previsao de Entrega]],"D")</f>
+        <v>13</v>
+      </c>
+      <c r="S218" s="14">
+        <v>50</v>
+      </c>
+      <c r="T218" s="14">
         <v>0</v>
       </c>
     </row>
@@ -16136,7 +16142,7 @@
         <v>130</v>
       </c>
       <c r="I219" s="10">
-        <f t="shared" si="4"/>
+        <f>NETWORKDAYS(B219, A219)</f>
         <v>1</v>
       </c>
       <c r="J219" s="7">
@@ -16200,7 +16206,7 @@
         <v>130</v>
       </c>
       <c r="I220" s="10">
-        <f t="shared" si="4"/>
+        <f>NETWORKDAYS(B220, A220)</f>
         <v>1</v>
       </c>
       <c r="J220" s="7">
@@ -16264,7 +16270,7 @@
         <v>98</v>
       </c>
       <c r="I221" s="10">
-        <f t="shared" si="4"/>
+        <f>NETWORKDAYS(B221, A221)</f>
         <v>1</v>
       </c>
       <c r="J221" s="7">
@@ -16328,7 +16334,7 @@
         <v>91</v>
       </c>
       <c r="I222" s="10">
-        <f t="shared" si="4"/>
+        <f>NETWORKDAYS(B222, A222)</f>
         <v>1</v>
       </c>
       <c r="J222" s="7">
@@ -16392,7 +16398,7 @@
         <v>32</v>
       </c>
       <c r="I223" s="10">
-        <f t="shared" si="4"/>
+        <f>NETWORKDAYS(B223, A223)</f>
         <v>1</v>
       </c>
       <c r="J223" s="7">
@@ -16456,7 +16462,7 @@
         <v>372</v>
       </c>
       <c r="I224" s="10">
-        <f t="shared" si="4"/>
+        <f>NETWORKDAYS(B224, A224)</f>
         <v>2</v>
       </c>
       <c r="J224" s="7">
@@ -16520,7 +16526,7 @@
         <v>32</v>
       </c>
       <c r="I225" s="10">
-        <f t="shared" si="4"/>
+        <f>NETWORKDAYS(B225, A225)</f>
         <v>1</v>
       </c>
       <c r="J225" s="7">
@@ -16559,128 +16565,128 @@
       </c>
     </row>
     <row r="226" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A226" s="41">
-        <v>45826</v>
-      </c>
-      <c r="B226" s="41">
-        <v>45826</v>
-      </c>
-      <c r="C226" s="41" t="s">
-        <v>7</v>
-      </c>
-      <c r="D226" s="41" t="s">
+      <c r="A226" s="11">
+        <v>45870</v>
+      </c>
+      <c r="B226" s="11">
+        <v>45867</v>
+      </c>
+      <c r="C226" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D226" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="E226" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="F226" s="12">
+        <v>68485</v>
+      </c>
+      <c r="G226" s="12" t="s">
+        <v>371</v>
+      </c>
+      <c r="H226" s="12" t="s">
+        <v>372</v>
+      </c>
+      <c r="I226" s="13">
+        <f>NETWORKDAYS(B226, A226)</f>
+        <v>4</v>
+      </c>
+      <c r="J226" s="12">
+        <v>66526</v>
+      </c>
+      <c r="K226" s="12">
+        <v>3061</v>
+      </c>
+      <c r="L226" s="12" t="s">
+        <v>192</v>
+      </c>
+      <c r="M226" s="11">
+        <v>45884</v>
+      </c>
+      <c r="N226" s="14">
+        <v>1150</v>
+      </c>
+      <c r="O226" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="P226" s="12">
         <v>15</v>
       </c>
-      <c r="E226" s="41" t="s">
-        <v>124</v>
-      </c>
-      <c r="F226" s="42" t="s">
-        <v>3</v>
-      </c>
-      <c r="G226" s="42" t="s">
-        <v>125</v>
-      </c>
-      <c r="H226" s="42" t="s">
-        <v>126</v>
-      </c>
-      <c r="I226" s="13">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="J226" s="42">
-        <v>66341</v>
-      </c>
-      <c r="K226" s="42">
-        <v>11758</v>
-      </c>
-      <c r="L226" s="42" t="s">
-        <v>316</v>
-      </c>
-      <c r="M226" s="41">
-        <v>45883</v>
-      </c>
-      <c r="N226" s="43">
-        <v>924.61</v>
-      </c>
-      <c r="O226" s="42" t="s">
-        <v>122</v>
-      </c>
-      <c r="P226" s="42">
-        <v>28</v>
-      </c>
-      <c r="Q226" s="42" t="s">
+      <c r="Q226" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="R226" s="42">
-        <f>DATEDIF(Tabela1[[#This Row],[Atendimento]],Tabela1[[#This Row],[Previsao de Entrega]],"D")</f>
-        <v>57</v>
-      </c>
-      <c r="S226" s="43">
-        <v>0</v>
-      </c>
-      <c r="T226" s="43">
+      <c r="R226" s="12">
+        <f>DATEDIF(Tabela1[[#This Row],[Atendimento]],Tabela1[[#This Row],[Previsao de Entrega]],"D")</f>
+        <v>14</v>
+      </c>
+      <c r="S226" s="14">
+        <v>0</v>
+      </c>
+      <c r="T226" s="14">
         <v>0</v>
       </c>
     </row>
     <row r="227" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A227" s="11">
-        <v>45867</v>
+        <v>45880</v>
       </c>
       <c r="B227" s="11">
-        <v>45867</v>
+        <v>45869</v>
       </c>
       <c r="C227" s="11" t="s">
-        <v>128</v>
+        <v>7</v>
       </c>
       <c r="D227" s="11" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="E227" s="11" t="s">
         <v>113</v>
       </c>
       <c r="F227" s="12">
-        <v>68486</v>
+        <v>68490</v>
       </c>
       <c r="G227" s="12" t="s">
-        <v>296</v>
+        <v>227</v>
       </c>
       <c r="H227" s="12" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="I227" s="13">
-        <f t="shared" si="4"/>
-        <v>1</v>
+        <f>NETWORKDAYS(B227, A227)</f>
+        <v>8</v>
       </c>
       <c r="J227" s="12">
-        <v>66478</v>
+        <v>66638</v>
       </c>
       <c r="K227" s="12">
-        <v>10460</v>
+        <v>8992</v>
       </c>
       <c r="L227" s="12" t="s">
-        <v>393</v>
+        <v>180</v>
       </c>
       <c r="M227" s="11">
-        <v>45883</v>
+        <v>45884</v>
       </c>
       <c r="N227" s="14">
-        <v>4789.6099999999997</v>
+        <v>10750</v>
       </c>
       <c r="O227" s="12" t="s">
         <v>122</v>
       </c>
       <c r="P227" s="12">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="Q227" s="12" t="s">
         <v>24</v>
       </c>
       <c r="R227" s="12">
         <f>DATEDIF(Tabela1[[#This Row],[Atendimento]],Tabela1[[#This Row],[Previsao de Entrega]],"D")</f>
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="S227" s="14">
-        <v>1080.08</v>
+        <v>0</v>
       </c>
       <c r="T227" s="14">
         <v>0</v>
@@ -16688,10 +16694,10 @@
     </row>
     <row r="228" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A228" s="11">
-        <v>45870</v>
+        <v>45785</v>
       </c>
       <c r="B228" s="11">
-        <v>45869</v>
+        <v>45784</v>
       </c>
       <c r="C228" s="11" t="s">
         <v>7</v>
@@ -16703,173 +16709,173 @@
         <v>113</v>
       </c>
       <c r="F228" s="12">
-        <v>68491</v>
+        <v>68369</v>
       </c>
       <c r="G228" s="12" t="s">
-        <v>371</v>
+        <v>39</v>
       </c>
       <c r="H228" s="12" t="s">
-        <v>372</v>
+        <v>98</v>
       </c>
       <c r="I228" s="13">
-        <f t="shared" si="4"/>
+        <f>NETWORKDAYS(B228, A228)</f>
         <v>2</v>
       </c>
       <c r="J228" s="12">
-        <v>66521</v>
+        <v>65234</v>
       </c>
       <c r="K228" s="12">
-        <v>3061</v>
+        <v>11610</v>
       </c>
       <c r="L228" s="12" t="s">
-        <v>192</v>
+        <v>38</v>
       </c>
       <c r="M228" s="11">
-        <v>45883</v>
+        <v>45887</v>
       </c>
       <c r="N228" s="14">
-        <v>3000</v>
+        <v>9114.5499999999993</v>
       </c>
       <c r="O228" s="12" t="s">
         <v>122</v>
       </c>
       <c r="P228" s="12">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="Q228" s="12" t="s">
         <v>24</v>
       </c>
       <c r="R228" s="12">
         <f>DATEDIF(Tabela1[[#This Row],[Atendimento]],Tabela1[[#This Row],[Previsao de Entrega]],"D")</f>
-        <v>13</v>
+        <v>102</v>
       </c>
       <c r="S228" s="14">
-        <v>50</v>
+        <v>183.5</v>
       </c>
       <c r="T228" s="14">
         <v>0</v>
       </c>
     </row>
     <row r="229" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A229" s="11">
-        <v>45870</v>
-      </c>
-      <c r="B229" s="11">
-        <v>45867</v>
-      </c>
-      <c r="C229" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="D229" s="11" t="s">
+      <c r="A229" s="46">
+        <v>45868</v>
+      </c>
+      <c r="B229" s="46">
+        <v>45862</v>
+      </c>
+      <c r="C229" s="46" t="s">
+        <v>7</v>
+      </c>
+      <c r="D229" s="46" t="s">
         <v>5</v>
       </c>
-      <c r="E229" s="11" t="s">
+      <c r="E229" s="46" t="s">
         <v>113</v>
       </c>
-      <c r="F229" s="12">
-        <v>68485</v>
-      </c>
-      <c r="G229" s="12" t="s">
-        <v>371</v>
-      </c>
-      <c r="H229" s="12" t="s">
-        <v>372</v>
-      </c>
-      <c r="I229" s="13">
-        <f t="shared" si="4"/>
-        <v>4</v>
-      </c>
-      <c r="J229" s="12">
-        <v>66526</v>
-      </c>
-      <c r="K229" s="12">
-        <v>3061</v>
-      </c>
-      <c r="L229" s="12" t="s">
-        <v>192</v>
-      </c>
-      <c r="M229" s="11">
-        <v>45884</v>
-      </c>
-      <c r="N229" s="14">
-        <v>1150</v>
-      </c>
-      <c r="O229" s="12" t="s">
+      <c r="F229" s="47">
+        <v>68476</v>
+      </c>
+      <c r="G229" s="47" t="s">
+        <v>227</v>
+      </c>
+      <c r="H229" s="47" t="s">
+        <v>98</v>
+      </c>
+      <c r="I229" s="48">
+        <f>NETWORKDAYS(B229, A229)</f>
+        <v>5</v>
+      </c>
+      <c r="J229" s="47">
+        <v>66491</v>
+      </c>
+      <c r="K229" s="47">
+        <v>11522</v>
+      </c>
+      <c r="L229" s="47" t="s">
+        <v>376</v>
+      </c>
+      <c r="M229" s="46">
+        <v>45888</v>
+      </c>
+      <c r="N229" s="49">
+        <v>1680.4</v>
+      </c>
+      <c r="O229" s="47" t="s">
         <v>122</v>
       </c>
-      <c r="P229" s="12">
-        <v>15</v>
-      </c>
-      <c r="Q229" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="R229" s="12">
-        <f>DATEDIF(Tabela1[[#This Row],[Atendimento]],Tabela1[[#This Row],[Previsao de Entrega]],"D")</f>
-        <v>14</v>
-      </c>
-      <c r="S229" s="14">
-        <v>0</v>
-      </c>
-      <c r="T229" s="14">
+      <c r="P229" s="47">
+        <v>28</v>
+      </c>
+      <c r="Q229" s="47" t="s">
+        <v>407</v>
+      </c>
+      <c r="R229" s="47">
+        <f>DATEDIF(Tabela1[[#This Row],[Atendimento]],Tabela1[[#This Row],[Previsao de Entrega]],"D")</f>
+        <v>20</v>
+      </c>
+      <c r="S229" s="49">
+        <v>0</v>
+      </c>
+      <c r="T229" s="49">
         <v>0</v>
       </c>
     </row>
     <row r="230" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A230" s="11">
+        <v>45881</v>
+      </c>
+      <c r="B230" s="11">
         <v>45880</v>
       </c>
-      <c r="B230" s="11">
-        <v>45869</v>
-      </c>
       <c r="C230" s="11" t="s">
         <v>7</v>
       </c>
       <c r="D230" s="11" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="E230" s="11" t="s">
         <v>113</v>
       </c>
       <c r="F230" s="12">
-        <v>68490</v>
+        <v>68500</v>
       </c>
       <c r="G230" s="12" t="s">
-        <v>227</v>
+        <v>371</v>
       </c>
       <c r="H230" s="12" t="s">
-        <v>98</v>
+        <v>372</v>
       </c>
       <c r="I230" s="13">
-        <f t="shared" si="4"/>
-        <v>8</v>
+        <f>NETWORKDAYS(B230, A230)</f>
+        <v>2</v>
       </c>
       <c r="J230" s="12">
-        <v>66638</v>
-      </c>
-      <c r="K230" s="12">
-        <v>8992</v>
+        <v>66660</v>
+      </c>
+      <c r="K230" s="51">
+        <v>160</v>
       </c>
       <c r="L230" s="12" t="s">
-        <v>180</v>
+        <v>201</v>
       </c>
       <c r="M230" s="11">
-        <v>45884</v>
+        <v>45888</v>
       </c>
       <c r="N230" s="14">
-        <v>10750</v>
+        <v>524.1</v>
       </c>
       <c r="O230" s="12" t="s">
         <v>122</v>
       </c>
       <c r="P230" s="12">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="Q230" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="R230" s="12">
-        <f>DATEDIF(Tabela1[[#This Row],[Atendimento]],Tabela1[[#This Row],[Previsao de Entrega]],"D")</f>
-        <v>4</v>
+      <c r="R230" s="51">
+        <f>DATEDIF(Tabela1[[#This Row],[Atendimento]],Tabela1[[#This Row],[Previsao de Entrega]],"D")</f>
+        <v>7</v>
       </c>
       <c r="S230" s="14">
         <v>0</v>
@@ -16904,7 +16910,7 @@
         <v>372</v>
       </c>
       <c r="I231" s="10">
-        <f t="shared" si="4"/>
+        <f>NETWORKDAYS(B231, A231)</f>
         <v>1</v>
       </c>
       <c r="J231" s="7">
@@ -16968,7 +16974,7 @@
         <v>130</v>
       </c>
       <c r="I232" s="13">
-        <f t="shared" si="4"/>
+        <f>NETWORKDAYS(B232, A232)</f>
         <v>6</v>
       </c>
       <c r="J232" s="12">
@@ -17007,75 +17013,75 @@
       </c>
     </row>
     <row r="233" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A233" s="11">
-        <v>45877</v>
-      </c>
-      <c r="B233" s="11">
-        <v>45877</v>
-      </c>
-      <c r="C233" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="D233" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="E233" s="11" t="s">
-        <v>113</v>
-      </c>
-      <c r="F233" s="12">
-        <v>68458</v>
-      </c>
-      <c r="G233" s="12" t="s">
-        <v>227</v>
-      </c>
-      <c r="H233" s="12" t="s">
-        <v>98</v>
+      <c r="A233" s="41">
+        <v>45826</v>
+      </c>
+      <c r="B233" s="41">
+        <v>45826</v>
+      </c>
+      <c r="C233" s="41" t="s">
+        <v>7</v>
+      </c>
+      <c r="D233" s="41" t="s">
+        <v>15</v>
+      </c>
+      <c r="E233" s="41" t="s">
+        <v>124</v>
+      </c>
+      <c r="F233" s="42" t="s">
+        <v>3</v>
+      </c>
+      <c r="G233" s="42" t="s">
+        <v>125</v>
+      </c>
+      <c r="H233" s="42" t="s">
+        <v>126</v>
       </c>
       <c r="I233" s="13">
-        <f t="shared" si="4"/>
+        <f>NETWORKDAYS(B233, A233)</f>
         <v>1</v>
       </c>
-      <c r="J233" s="12">
-        <v>66605</v>
-      </c>
-      <c r="K233" s="12">
-        <v>561</v>
-      </c>
-      <c r="L233" s="12" t="s">
-        <v>324</v>
-      </c>
-      <c r="M233" s="11">
+      <c r="J233" s="42">
+        <v>66341</v>
+      </c>
+      <c r="K233" s="42">
+        <v>11758</v>
+      </c>
+      <c r="L233" s="42" t="s">
+        <v>316</v>
+      </c>
+      <c r="M233" s="41">
         <v>45891</v>
       </c>
-      <c r="N233" s="14">
-        <v>758.53</v>
-      </c>
-      <c r="O233" s="12" t="s">
+      <c r="N233" s="43">
+        <v>924.61</v>
+      </c>
+      <c r="O233" s="42" t="s">
         <v>122</v>
       </c>
-      <c r="P233" s="12">
+      <c r="P233" s="42">
         <v>28</v>
       </c>
-      <c r="Q233" s="12" t="s">
+      <c r="Q233" s="42" t="s">
         <v>24</v>
       </c>
-      <c r="R233" s="12">
-        <f>DATEDIF(Tabela1[[#This Row],[Atendimento]],Tabela1[[#This Row],[Previsao de Entrega]],"D")</f>
-        <v>14</v>
-      </c>
-      <c r="S233" s="14">
-        <v>0</v>
-      </c>
-      <c r="T233" s="14">
+      <c r="R233" s="42">
+        <f>DATEDIF(Tabela1[[#This Row],[Atendimento]],Tabela1[[#This Row],[Previsao de Entrega]],"D")</f>
+        <v>65</v>
+      </c>
+      <c r="S233" s="43">
+        <v>0</v>
+      </c>
+      <c r="T233" s="43">
         <v>0</v>
       </c>
     </row>
     <row r="234" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A234" s="11">
-        <v>45880</v>
+        <v>45877</v>
       </c>
       <c r="B234" s="11">
-        <v>45868</v>
+        <v>45877</v>
       </c>
       <c r="C234" s="11" t="s">
         <v>7</v>
@@ -17086,39 +17092,39 @@
       <c r="E234" s="11" t="s">
         <v>113</v>
       </c>
-      <c r="F234" s="12" t="s">
-        <v>3</v>
+      <c r="F234" s="12">
+        <v>68458</v>
       </c>
       <c r="G234" s="12" t="s">
-        <v>3</v>
+        <v>227</v>
       </c>
       <c r="H234" s="12" t="s">
-        <v>32</v>
+        <v>98</v>
       </c>
       <c r="I234" s="13">
-        <f t="shared" si="4"/>
-        <v>9</v>
+        <f>NETWORKDAYS(B234, A234)</f>
+        <v>1</v>
       </c>
       <c r="J234" s="12">
-        <v>66629</v>
+        <v>66605</v>
       </c>
       <c r="K234" s="12">
-        <v>11121</v>
+        <v>561</v>
       </c>
       <c r="L234" s="12" t="s">
-        <v>143</v>
+        <v>324</v>
       </c>
       <c r="M234" s="11">
-        <v>45894</v>
+        <v>45891</v>
       </c>
       <c r="N234" s="14">
-        <v>1242.04</v>
+        <v>758.53</v>
       </c>
       <c r="O234" s="12" t="s">
         <v>122</v>
       </c>
       <c r="P234" s="12">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="Q234" s="12" t="s">
         <v>24</v>
@@ -17128,7 +17134,7 @@
         <v>14</v>
       </c>
       <c r="S234" s="14">
-        <v>108</v>
+        <v>0</v>
       </c>
       <c r="T234" s="14">
         <v>0</v>
@@ -17136,7 +17142,7 @@
     </row>
     <row r="235" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A235" s="11">
-        <v>45868</v>
+        <v>45880</v>
       </c>
       <c r="B235" s="11">
         <v>45868</v>
@@ -17145,120 +17151,120 @@
         <v>7</v>
       </c>
       <c r="D235" s="11" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="E235" s="11" t="s">
-        <v>124</v>
+        <v>113</v>
       </c>
       <c r="F235" s="12" t="s">
         <v>3</v>
       </c>
       <c r="G235" s="12" t="s">
-        <v>125</v>
+        <v>3</v>
       </c>
       <c r="H235" s="12" t="s">
-        <v>126</v>
+        <v>32</v>
       </c>
       <c r="I235" s="13">
-        <f t="shared" si="4"/>
-        <v>1</v>
+        <f>NETWORKDAYS(B235, A235)</f>
+        <v>9</v>
       </c>
       <c r="J235" s="12">
-        <v>66504</v>
+        <v>66629</v>
       </c>
       <c r="K235" s="12">
-        <v>3034</v>
+        <v>11121</v>
       </c>
       <c r="L235" s="12" t="s">
-        <v>349</v>
+        <v>143</v>
       </c>
       <c r="M235" s="11">
-        <v>45897</v>
+        <v>45894</v>
       </c>
       <c r="N235" s="14">
-        <v>2220</v>
+        <v>1242.04</v>
       </c>
       <c r="O235" s="12" t="s">
         <v>122</v>
       </c>
       <c r="P235" s="12">
-        <v>90</v>
+        <v>30</v>
       </c>
       <c r="Q235" s="12" t="s">
         <v>24</v>
       </c>
       <c r="R235" s="12">
         <f>DATEDIF(Tabela1[[#This Row],[Atendimento]],Tabela1[[#This Row],[Previsao de Entrega]],"D")</f>
-        <v>29</v>
+        <v>14</v>
       </c>
       <c r="S235" s="14">
-        <v>80</v>
+        <v>108</v>
       </c>
       <c r="T235" s="14">
         <v>0</v>
       </c>
     </row>
     <row r="236" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A236" s="11">
-        <v>45869</v>
-      </c>
-      <c r="B236" s="11">
-        <v>45869</v>
-      </c>
-      <c r="C236" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="D236" s="11" t="s">
+      <c r="A236" s="46">
+        <v>45881</v>
+      </c>
+      <c r="B236" s="46">
+        <v>45881</v>
+      </c>
+      <c r="C236" s="46" t="s">
+        <v>7</v>
+      </c>
+      <c r="D236" s="46" t="s">
         <v>15</v>
       </c>
-      <c r="E236" s="11" t="s">
+      <c r="E236" s="46" t="s">
         <v>124</v>
       </c>
-      <c r="F236" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="G236" s="12" t="s">
-        <v>125</v>
-      </c>
-      <c r="H236" s="12" t="s">
-        <v>126</v>
-      </c>
-      <c r="I236" s="13">
-        <f t="shared" si="4"/>
+      <c r="F236" s="47">
+        <v>68501</v>
+      </c>
+      <c r="G236" s="47" t="s">
+        <v>90</v>
+      </c>
+      <c r="H236" s="47" t="s">
+        <v>91</v>
+      </c>
+      <c r="I236" s="48">
+        <f>NETWORKDAYS(B236, A236)</f>
         <v>1</v>
       </c>
-      <c r="J236" s="12">
-        <v>66427</v>
-      </c>
-      <c r="K236" s="12">
-        <v>1277</v>
-      </c>
-      <c r="L236" s="12" t="s">
-        <v>398</v>
-      </c>
-      <c r="M236" s="11">
-        <v>45897</v>
-      </c>
-      <c r="N236" s="14">
-        <v>2715.75</v>
-      </c>
-      <c r="O236" s="12" t="s">
+      <c r="J236" s="47">
+        <v>66662</v>
+      </c>
+      <c r="K236" s="50">
+        <v>3040</v>
+      </c>
+      <c r="L236" s="47" t="s">
+        <v>214</v>
+      </c>
+      <c r="M236" s="46">
+        <v>45896</v>
+      </c>
+      <c r="N236" s="49">
+        <v>1000</v>
+      </c>
+      <c r="O236" s="47" t="s">
         <v>122</v>
       </c>
-      <c r="P236" s="12">
+      <c r="P236" s="47">
         <v>30</v>
       </c>
-      <c r="Q236" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="R236" s="12">
-        <f>DATEDIF(Tabela1[[#This Row],[Atendimento]],Tabela1[[#This Row],[Previsao de Entrega]],"D")</f>
-        <v>28</v>
-      </c>
-      <c r="S236" s="14">
-        <v>950</v>
-      </c>
-      <c r="T236" s="14">
+      <c r="Q236" s="47" t="s">
+        <v>407</v>
+      </c>
+      <c r="R236" s="50">
+        <f>DATEDIF(Tabela1[[#This Row],[Atendimento]],Tabela1[[#This Row],[Previsao de Entrega]],"D")</f>
+        <v>15</v>
+      </c>
+      <c r="S236" s="49">
+        <v>0</v>
+      </c>
+      <c r="T236" s="49">
         <v>0</v>
       </c>
     </row>
@@ -17288,7 +17294,7 @@
         <v>34</v>
       </c>
       <c r="I237" s="10">
-        <f t="shared" si="4"/>
+        <f>NETWORKDAYS(B237, A237)</f>
         <v>1</v>
       </c>
       <c r="J237" s="7">
@@ -17352,7 +17358,7 @@
         <v>130</v>
       </c>
       <c r="I238" s="10">
-        <f t="shared" si="4"/>
+        <f>NETWORKDAYS(B238, A238)</f>
         <v>1</v>
       </c>
       <c r="J238" s="7">
@@ -17416,7 +17422,7 @@
         <v>130</v>
       </c>
       <c r="I239" s="10">
-        <f t="shared" si="4"/>
+        <f>NETWORKDAYS(B239, A239)</f>
         <v>1</v>
       </c>
       <c r="J239" s="7">
@@ -17480,7 +17486,7 @@
         <v>130</v>
       </c>
       <c r="I240" s="10">
-        <f t="shared" si="4"/>
+        <f>NETWORKDAYS(B240, A240)</f>
         <v>1</v>
       </c>
       <c r="J240" s="7">
@@ -17544,7 +17550,7 @@
         <v>32</v>
       </c>
       <c r="I241" s="10">
-        <f t="shared" si="4"/>
+        <f>NETWORKDAYS(B241, A241)</f>
         <v>1</v>
       </c>
       <c r="J241" s="7">
@@ -17608,7 +17614,7 @@
         <v>126</v>
       </c>
       <c r="I242" s="10">
-        <f t="shared" si="4"/>
+        <f>NETWORKDAYS(B242, A242)</f>
         <v>1</v>
       </c>
       <c r="J242" s="7">
@@ -17672,7 +17678,7 @@
         <v>138</v>
       </c>
       <c r="I243" s="10">
-        <f t="shared" si="4"/>
+        <f>NETWORKDAYS(B243, A243)</f>
         <v>1</v>
       </c>
       <c r="J243" s="7">
@@ -17712,13 +17718,13 @@
     </row>
     <row r="244" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A244" s="11">
-        <v>45875</v>
+        <v>45868</v>
       </c>
       <c r="B244" s="11">
-        <v>45873</v>
+        <v>45868</v>
       </c>
       <c r="C244" s="11" t="s">
-        <v>128</v>
+        <v>7</v>
       </c>
       <c r="D244" s="11" t="s">
         <v>15</v>
@@ -17726,35 +17732,35 @@
       <c r="E244" s="11" t="s">
         <v>124</v>
       </c>
-      <c r="F244" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="G244" s="11" t="s">
+      <c r="F244" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="G244" s="12" t="s">
         <v>125</v>
       </c>
-      <c r="H244" s="11" t="s">
+      <c r="H244" s="12" t="s">
         <v>126</v>
       </c>
       <c r="I244" s="13">
-        <f t="shared" si="4"/>
-        <v>3</v>
+        <f>NETWORKDAYS(B244, A244)</f>
+        <v>1</v>
       </c>
       <c r="J244" s="12">
-        <v>66430</v>
+        <v>66504</v>
       </c>
       <c r="K244" s="12">
-        <v>333</v>
+        <v>3034</v>
       </c>
       <c r="L244" s="12" t="s">
-        <v>400</v>
+        <v>349</v>
       </c>
       <c r="M244" s="11">
-        <v>45901</v>
-      </c>
-      <c r="N244" s="45">
-        <v>1483685.03</v>
-      </c>
-      <c r="O244" s="11" t="s">
+        <v>45897</v>
+      </c>
+      <c r="N244" s="14">
+        <v>2220</v>
+      </c>
+      <c r="O244" s="12" t="s">
         <v>122</v>
       </c>
       <c r="P244" s="12">
@@ -17765,13 +17771,13 @@
       </c>
       <c r="R244" s="12">
         <f>DATEDIF(Tabela1[[#This Row],[Atendimento]],Tabela1[[#This Row],[Previsao de Entrega]],"D")</f>
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="S244" s="14">
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="T244" s="14">
-        <v>59008.35</v>
+        <v>0</v>
       </c>
     </row>
     <row r="245" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
@@ -17800,7 +17806,7 @@
         <v>32</v>
       </c>
       <c r="I245" s="10">
-        <f t="shared" si="4"/>
+        <f>NETWORKDAYS(B245, A245)</f>
         <v>1</v>
       </c>
       <c r="J245" s="7">
@@ -17840,10 +17846,10 @@
     </row>
     <row r="246" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A246" s="11">
-        <v>45856</v>
+        <v>45869</v>
       </c>
       <c r="B246" s="11">
-        <v>45856</v>
+        <v>45869</v>
       </c>
       <c r="C246" s="11" t="s">
         <v>7</v>
@@ -17854,8 +17860,8 @@
       <c r="E246" s="11" t="s">
         <v>124</v>
       </c>
-      <c r="F246" s="12">
-        <v>68466</v>
+      <c r="F246" s="12" t="s">
+        <v>3</v>
       </c>
       <c r="G246" s="12" t="s">
         <v>125</v>
@@ -17864,39 +17870,39 @@
         <v>126</v>
       </c>
       <c r="I246" s="13">
-        <f t="shared" si="4"/>
+        <f>NETWORKDAYS(B246, A246)</f>
         <v>1</v>
       </c>
       <c r="J246" s="12">
-        <v>66337</v>
+        <v>66427</v>
       </c>
       <c r="K246" s="12">
-        <v>11736</v>
+        <v>1277</v>
       </c>
       <c r="L246" s="12" t="s">
-        <v>127</v>
+        <v>398</v>
       </c>
       <c r="M246" s="11">
-        <v>45902</v>
+        <v>45897</v>
       </c>
       <c r="N246" s="14">
-        <v>16134.54</v>
+        <v>2715.75</v>
       </c>
       <c r="O246" s="12" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="P246" s="12">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="Q246" s="12" t="s">
         <v>24</v>
       </c>
       <c r="R246" s="12">
         <f>DATEDIF(Tabela1[[#This Row],[Atendimento]],Tabela1[[#This Row],[Previsao de Entrega]],"D")</f>
-        <v>46</v>
+        <v>28</v>
       </c>
       <c r="S246" s="14">
-        <v>25720</v>
+        <v>950</v>
       </c>
       <c r="T246" s="14">
         <v>0</v>
@@ -17928,7 +17934,7 @@
         <v>32</v>
       </c>
       <c r="I247" s="10">
-        <f t="shared" si="4"/>
+        <f>NETWORKDAYS(B247, A247)</f>
         <v>1</v>
       </c>
       <c r="J247" s="7">
@@ -17992,7 +17998,7 @@
         <v>98</v>
       </c>
       <c r="I248" s="10">
-        <f t="shared" si="4"/>
+        <f>NETWORKDAYS(B248, A248)</f>
         <v>1</v>
       </c>
       <c r="J248" s="7">
@@ -18056,7 +18062,7 @@
         <v>98</v>
       </c>
       <c r="I249" s="10">
-        <f t="shared" si="4"/>
+        <f>NETWORKDAYS(B249, A249)</f>
         <v>1</v>
       </c>
       <c r="J249" s="7">
@@ -18096,127 +18102,127 @@
     </row>
     <row r="250" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A250" s="11">
-        <v>45840</v>
+        <v>45875</v>
       </c>
       <c r="B250" s="11">
-        <v>45840</v>
+        <v>45873</v>
       </c>
       <c r="C250" s="11" t="s">
-        <v>7</v>
+        <v>128</v>
       </c>
       <c r="D250" s="11" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="E250" s="11" t="s">
-        <v>113</v>
-      </c>
-      <c r="F250" s="12">
-        <v>68452</v>
-      </c>
-      <c r="G250" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="H250" s="12" t="s">
-        <v>34</v>
+        <v>124</v>
+      </c>
+      <c r="F250" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="G250" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="H250" s="11" t="s">
+        <v>126</v>
       </c>
       <c r="I250" s="13">
-        <f t="shared" si="4"/>
-        <v>1</v>
+        <f>NETWORKDAYS(B250, A250)</f>
+        <v>3</v>
       </c>
       <c r="J250" s="12">
-        <v>66037</v>
+        <v>66430</v>
       </c>
       <c r="K250" s="12">
-        <v>11775</v>
+        <v>333</v>
       </c>
       <c r="L250" s="12" t="s">
-        <v>353</v>
+        <v>400</v>
       </c>
       <c r="M250" s="11">
-        <v>45905</v>
-      </c>
-      <c r="N250" s="14">
-        <v>1750</v>
-      </c>
-      <c r="O250" s="12" t="s">
+        <v>45901</v>
+      </c>
+      <c r="N250" s="45">
+        <v>1483685.03</v>
+      </c>
+      <c r="O250" s="11" t="s">
         <v>122</v>
       </c>
       <c r="P250" s="12">
-        <v>30</v>
+        <v>90</v>
       </c>
       <c r="Q250" s="12" t="s">
         <v>24</v>
       </c>
       <c r="R250" s="12">
         <f>DATEDIF(Tabela1[[#This Row],[Atendimento]],Tabela1[[#This Row],[Previsao de Entrega]],"D")</f>
-        <v>65</v>
+        <v>26</v>
       </c>
       <c r="S250" s="14">
         <v>0</v>
       </c>
       <c r="T250" s="14">
-        <v>0</v>
+        <v>59008.35</v>
       </c>
     </row>
     <row r="251" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A251" s="11">
-        <v>45848</v>
+        <v>45856</v>
       </c>
       <c r="B251" s="11">
-        <v>45848</v>
+        <v>45856</v>
       </c>
       <c r="C251" s="11" t="s">
         <v>7</v>
       </c>
       <c r="D251" s="11" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="E251" s="11" t="s">
-        <v>113</v>
+        <v>124</v>
       </c>
       <c r="F251" s="12">
-        <v>68457</v>
+        <v>68466</v>
       </c>
       <c r="G251" s="12" t="s">
-        <v>33</v>
+        <v>125</v>
       </c>
       <c r="H251" s="12" t="s">
-        <v>34</v>
+        <v>126</v>
       </c>
       <c r="I251" s="13">
-        <f t="shared" si="4"/>
+        <f>NETWORKDAYS(B251, A251)</f>
         <v>1</v>
       </c>
       <c r="J251" s="12">
-        <v>66126</v>
+        <v>66337</v>
       </c>
       <c r="K251" s="12">
-        <v>2931</v>
+        <v>11736</v>
       </c>
       <c r="L251" s="12" t="s">
-        <v>366</v>
+        <v>127</v>
       </c>
       <c r="M251" s="11">
-        <v>45905</v>
+        <v>45902</v>
       </c>
       <c r="N251" s="14">
-        <v>3500</v>
+        <v>16134.54</v>
       </c>
       <c r="O251" s="12" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="P251" s="12">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="Q251" s="12" t="s">
         <v>24</v>
       </c>
       <c r="R251" s="12">
         <f>DATEDIF(Tabela1[[#This Row],[Atendimento]],Tabela1[[#This Row],[Previsao de Entrega]],"D")</f>
-        <v>57</v>
+        <v>46</v>
       </c>
       <c r="S251" s="14">
-        <v>320</v>
+        <v>25720</v>
       </c>
       <c r="T251" s="14">
         <v>0</v>
@@ -18224,63 +18230,63 @@
     </row>
     <row r="252" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A252" s="11">
-        <v>45874</v>
+        <v>45840</v>
       </c>
       <c r="B252" s="11">
-        <v>45853</v>
+        <v>45840</v>
       </c>
       <c r="C252" s="11" t="s">
         <v>7</v>
       </c>
       <c r="D252" s="11" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="E252" s="11" t="s">
-        <v>124</v>
+        <v>113</v>
       </c>
       <c r="F252" s="12">
-        <v>68465</v>
+        <v>68452</v>
       </c>
       <c r="G252" s="12" t="s">
-        <v>125</v>
+        <v>33</v>
       </c>
       <c r="H252" s="12" t="s">
-        <v>126</v>
+        <v>34</v>
       </c>
       <c r="I252" s="13">
-        <f t="shared" si="4"/>
-        <v>16</v>
+        <f>NETWORKDAYS(B252, A252)</f>
+        <v>1</v>
       </c>
       <c r="J252" s="12">
-        <v>66555</v>
+        <v>66037</v>
       </c>
       <c r="K252" s="12">
-        <v>11791</v>
+        <v>11775</v>
       </c>
       <c r="L252" s="12" t="s">
-        <v>403</v>
+        <v>353</v>
       </c>
       <c r="M252" s="11">
-        <v>45906</v>
+        <v>45905</v>
       </c>
       <c r="N252" s="14">
-        <v>1075.55</v>
+        <v>1750</v>
       </c>
       <c r="O252" s="12" t="s">
         <v>122</v>
       </c>
       <c r="P252" s="12">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="Q252" s="12" t="s">
         <v>24</v>
       </c>
       <c r="R252" s="12">
         <f>DATEDIF(Tabela1[[#This Row],[Atendimento]],Tabela1[[#This Row],[Previsao de Entrega]],"D")</f>
-        <v>32</v>
+        <v>65</v>
       </c>
       <c r="S252" s="14">
-        <v>1215.25</v>
+        <v>0</v>
       </c>
       <c r="T252" s="14">
         <v>0</v>
@@ -18312,7 +18318,7 @@
         <v>32</v>
       </c>
       <c r="I253" s="10">
-        <f t="shared" si="4"/>
+        <f>NETWORKDAYS(B253, A253)</f>
         <v>1</v>
       </c>
       <c r="J253" s="7">
@@ -18376,7 +18382,7 @@
         <v>32</v>
       </c>
       <c r="I254" s="10">
-        <f t="shared" si="4"/>
+        <f>NETWORKDAYS(B254, A254)</f>
         <v>1</v>
       </c>
       <c r="J254" s="7">
@@ -18416,10 +18422,10 @@
     </row>
     <row r="255" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A255" s="11">
-        <v>45877</v>
+        <v>45848</v>
       </c>
       <c r="B255" s="11">
-        <v>45873</v>
+        <v>45848</v>
       </c>
       <c r="C255" s="11" t="s">
         <v>7</v>
@@ -18431,32 +18437,32 @@
         <v>113</v>
       </c>
       <c r="F255" s="12">
-        <v>68493</v>
+        <v>68457</v>
       </c>
       <c r="G255" s="12" t="s">
-        <v>321</v>
+        <v>33</v>
       </c>
       <c r="H255" s="12" t="s">
-        <v>91</v>
+        <v>34</v>
       </c>
       <c r="I255" s="13">
-        <f t="shared" si="4"/>
-        <v>5</v>
+        <f>NETWORKDAYS(B255, A255)</f>
+        <v>1</v>
       </c>
       <c r="J255" s="12">
-        <v>66607</v>
+        <v>66126</v>
       </c>
       <c r="K255" s="12">
-        <v>1586</v>
+        <v>2931</v>
       </c>
       <c r="L255" s="12" t="s">
-        <v>408</v>
+        <v>366</v>
       </c>
       <c r="M255" s="11">
-        <v>45907</v>
+        <v>45905</v>
       </c>
       <c r="N255" s="14">
-        <v>680</v>
+        <v>3500</v>
       </c>
       <c r="O255" s="12" t="s">
         <v>122</v>
@@ -18469,10 +18475,10 @@
       </c>
       <c r="R255" s="12">
         <f>DATEDIF(Tabela1[[#This Row],[Atendimento]],Tabela1[[#This Row],[Previsao de Entrega]],"D")</f>
-        <v>30</v>
+        <v>57</v>
       </c>
       <c r="S255" s="14">
-        <v>0</v>
+        <v>320</v>
       </c>
       <c r="T255" s="14">
         <v>0</v>
@@ -18480,10 +18486,10 @@
     </row>
     <row r="256" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A256" s="11">
-        <v>45867</v>
+        <v>45874</v>
       </c>
       <c r="B256" s="11">
-        <v>45866</v>
+        <v>45853</v>
       </c>
       <c r="C256" s="11" t="s">
         <v>7</v>
@@ -18495,7 +18501,7 @@
         <v>124</v>
       </c>
       <c r="F256" s="12">
-        <v>68483</v>
+        <v>68465</v>
       </c>
       <c r="G256" s="12" t="s">
         <v>125</v>
@@ -18504,39 +18510,39 @@
         <v>126</v>
       </c>
       <c r="I256" s="13">
-        <f t="shared" si="4"/>
-        <v>2</v>
+        <f>NETWORKDAYS(B256, A256)</f>
+        <v>16</v>
       </c>
       <c r="J256" s="12">
-        <v>66467</v>
+        <v>66555</v>
       </c>
       <c r="K256" s="12">
-        <v>11164</v>
+        <v>11791</v>
       </c>
       <c r="L256" s="12" t="s">
-        <v>298</v>
+        <v>403</v>
       </c>
       <c r="M256" s="11">
-        <v>45908</v>
+        <v>45906</v>
       </c>
       <c r="N256" s="14">
-        <v>2623.03</v>
+        <v>1075.55</v>
       </c>
       <c r="O256" s="12" t="s">
         <v>122</v>
       </c>
       <c r="P256" s="12">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="Q256" s="12" t="s">
         <v>24</v>
       </c>
       <c r="R256" s="12">
         <f>DATEDIF(Tabela1[[#This Row],[Atendimento]],Tabela1[[#This Row],[Previsao de Entrega]],"D")</f>
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="S256" s="14">
-        <v>52</v>
+        <v>1215.25</v>
       </c>
       <c r="T256" s="14">
         <v>0</v>
@@ -18544,65 +18550,193 @@
     </row>
     <row r="257" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A257" s="11">
-        <v>45870</v>
+        <v>45877</v>
       </c>
       <c r="B257" s="11">
-        <v>45870</v>
+        <v>45873</v>
       </c>
       <c r="C257" s="11" t="s">
-        <v>128</v>
+        <v>7</v>
       </c>
       <c r="D257" s="11" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="E257" s="11" t="s">
-        <v>124</v>
-      </c>
-      <c r="F257" s="12" t="s">
-        <v>3</v>
+        <v>113</v>
+      </c>
+      <c r="F257" s="12">
+        <v>68493</v>
       </c>
       <c r="G257" s="12" t="s">
-        <v>125</v>
+        <v>321</v>
       </c>
       <c r="H257" s="12" t="s">
-        <v>126</v>
+        <v>91</v>
       </c>
       <c r="I257" s="13">
-        <f t="shared" si="4"/>
-        <v>1</v>
+        <f>NETWORKDAYS(B257, A257)</f>
+        <v>5</v>
       </c>
       <c r="J257" s="12">
-        <v>66430</v>
+        <v>66607</v>
       </c>
       <c r="K257" s="12">
-        <v>333</v>
+        <v>1586</v>
       </c>
       <c r="L257" s="12" t="s">
-        <v>400</v>
+        <v>408</v>
       </c>
       <c r="M257" s="11">
-        <v>46113</v>
+        <v>45907</v>
       </c>
       <c r="N257" s="14">
-        <v>281569.34000000003</v>
+        <v>680</v>
       </c>
       <c r="O257" s="12" t="s">
         <v>122</v>
       </c>
       <c r="P257" s="12">
-        <v>120</v>
+        <v>30</v>
       </c>
       <c r="Q257" s="12" t="s">
         <v>24</v>
       </c>
       <c r="R257" s="12">
         <f>DATEDIF(Tabela1[[#This Row],[Atendimento]],Tabela1[[#This Row],[Previsao de Entrega]],"D")</f>
+        <v>30</v>
+      </c>
+      <c r="S257" s="14">
+        <v>0</v>
+      </c>
+      <c r="T257" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="258" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A258" s="11">
+        <v>45867</v>
+      </c>
+      <c r="B258" s="11">
+        <v>45866</v>
+      </c>
+      <c r="C258" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D258" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="E258" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="F258" s="12">
+        <v>68483</v>
+      </c>
+      <c r="G258" s="12" t="s">
+        <v>125</v>
+      </c>
+      <c r="H258" s="12" t="s">
+        <v>126</v>
+      </c>
+      <c r="I258" s="13">
+        <f>NETWORKDAYS(B258, A258)</f>
+        <v>2</v>
+      </c>
+      <c r="J258" s="12">
+        <v>66467</v>
+      </c>
+      <c r="K258" s="12">
+        <v>11164</v>
+      </c>
+      <c r="L258" s="12" t="s">
+        <v>298</v>
+      </c>
+      <c r="M258" s="11">
+        <v>45908</v>
+      </c>
+      <c r="N258" s="14">
+        <v>2623.03</v>
+      </c>
+      <c r="O258" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="P258" s="12">
+        <v>28</v>
+      </c>
+      <c r="Q258" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="R258" s="12">
+        <f>DATEDIF(Tabela1[[#This Row],[Atendimento]],Tabela1[[#This Row],[Previsao de Entrega]],"D")</f>
+        <v>41</v>
+      </c>
+      <c r="S258" s="14">
+        <v>52</v>
+      </c>
+      <c r="T258" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="259" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A259" s="11">
+        <v>45870</v>
+      </c>
+      <c r="B259" s="11">
+        <v>45870</v>
+      </c>
+      <c r="C259" s="11" t="s">
+        <v>128</v>
+      </c>
+      <c r="D259" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="E259" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="F259" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="G259" s="12" t="s">
+        <v>125</v>
+      </c>
+      <c r="H259" s="12" t="s">
+        <v>126</v>
+      </c>
+      <c r="I259" s="13">
+        <f>NETWORKDAYS(B259, A259)</f>
+        <v>1</v>
+      </c>
+      <c r="J259" s="12">
+        <v>66430</v>
+      </c>
+      <c r="K259" s="12">
+        <v>333</v>
+      </c>
+      <c r="L259" s="12" t="s">
+        <v>400</v>
+      </c>
+      <c r="M259" s="11">
+        <v>46113</v>
+      </c>
+      <c r="N259" s="14">
+        <v>281569.34000000003</v>
+      </c>
+      <c r="O259" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="P259" s="12">
+        <v>120</v>
+      </c>
+      <c r="Q259" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="R259" s="12">
+        <f>DATEDIF(Tabela1[[#This Row],[Atendimento]],Tabela1[[#This Row],[Previsao de Entrega]],"D")</f>
         <v>243</v>
       </c>
-      <c r="S257" s="14">
-        <v>0</v>
-      </c>
-      <c r="T257" s="14">
+      <c r="S259" s="14">
+        <v>0</v>
+      </c>
+      <c r="T259" s="14">
         <v>0</v>
       </c>
     </row>
@@ -20631,12 +20765,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -20766,15 +20897,26 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F1DB20CA-6C9E-462A-9B1E-209C1B3156BD}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{258E5A34-0198-4570-927D-9873053383F0}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="b7545978-8353-4157-ab02-92f5c69a97d9"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -20798,17 +20940,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{258E5A34-0198-4570-927D-9873053383F0}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F1DB20CA-6C9E-462A-9B1E-209C1B3156BD}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="b7545978-8353-4157-ab02-92f5c69a97d9"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Atualização de Base - 13/08
</commit_message>
<xml_diff>
--- a/Atendimento.xlsx
+++ b/Atendimento.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\PUBLICO\Compras\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24F456F7-9CE7-4B18-B33F-8262E1E652F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F253B68B-F7EB-40B5-B748-62BFDAD2826A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -76,7 +76,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2590" uniqueCount="411">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2658" uniqueCount="413">
   <si>
     <t>SC</t>
   </si>
@@ -1309,6 +1309,12 @@
   </si>
   <si>
     <t>C T MOL PINTURAS LTDA – ME</t>
+  </si>
+  <si>
+    <t>PALACIO DAS FERRAMENTAS E PARAFUSOS LTDA</t>
+  </si>
+  <si>
+    <t>PULIRE INDUSTRIA E COMERCIO DE MATERIAIS DE LIMPEZA EIRELI</t>
   </si>
 </sst>
 </file>
@@ -1375,7 +1381,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1409,6 +1415,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1452,7 +1464,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1573,10 +1585,16 @@
     <xf numFmtId="44" fontId="0" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1760,8 +1778,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0C573FEE-B8A0-4FE7-911C-81B026DE4530}" name="Tabela1" displayName="Tabela1" ref="A1:T259" totalsRowShown="0" headerRowDxfId="36" dataDxfId="35">
-  <autoFilter ref="A1:T259" xr:uid="{0C573FEE-B8A0-4FE7-911C-81B026DE4530}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0C573FEE-B8A0-4FE7-911C-81B026DE4530}" name="Tabela1" displayName="Tabela1" ref="A1:T267" totalsRowShown="0" headerRowDxfId="36" dataDxfId="35">
+  <autoFilter ref="A1:T267" xr:uid="{0C573FEE-B8A0-4FE7-911C-81B026DE4530}">
     <filterColumn colId="16">
       <filters>
         <filter val="AGUARDANDO APROVAÇÃO"/>
@@ -1859,8 +1877,8 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{BB230BD9-36EF-4D37-BEB8-0438680DF5A9}" name="Tabela6" displayName="Tabela6" ref="A1:E41" totalsRowShown="0">
-  <autoFilter ref="A1:E41" xr:uid="{BB230BD9-36EF-4D37-BEB8-0438680DF5A9}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{BB230BD9-36EF-4D37-BEB8-0438680DF5A9}" name="Tabela6" displayName="Tabela6" ref="A1:E42" totalsRowShown="0">
+  <autoFilter ref="A1:E42" xr:uid="{BB230BD9-36EF-4D37-BEB8-0438680DF5A9}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{40ADAE7E-AD00-4188-9DB3-F04A606A9D2B}" name="data"/>
     <tableColumn id="2" xr3:uid="{D9B738D8-98DD-4AD6-8BCF-D51CBE71FF94}" name="solicitante"/>
@@ -2135,10 +2153,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T259"/>
+  <dimension ref="A1:T267"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A180" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K262" sqref="K262"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L233" sqref="L233"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2830,7 +2848,7 @@
         <v>364</v>
       </c>
       <c r="I11" s="13">
-        <f>NETWORKDAYS(B11, A11)</f>
+        <f t="shared" ref="I11:I74" si="1">NETWORKDAYS(B11, A11)</f>
         <v>1</v>
       </c>
       <c r="J11" s="12">
@@ -2894,7 +2912,7 @@
         <v>32</v>
       </c>
       <c r="I12" s="10">
-        <f>NETWORKDAYS(B12, A12)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="J12" s="7">
@@ -2958,7 +2976,7 @@
         <v>138</v>
       </c>
       <c r="I13" s="10">
-        <f>NETWORKDAYS(B13, A13)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="J13" s="7">
@@ -3022,7 +3040,7 @@
         <v>32</v>
       </c>
       <c r="I14" s="10">
-        <f>NETWORKDAYS(B14, A14)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="J14" s="7">
@@ -3086,7 +3104,7 @@
         <v>91</v>
       </c>
       <c r="I15" s="10">
-        <f>NETWORKDAYS(B15, A15)</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="J15" s="7">
@@ -3150,7 +3168,7 @@
         <v>91</v>
       </c>
       <c r="I16" s="10">
-        <f>NETWORKDAYS(B16, A16)</f>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="J16" s="7">
@@ -3214,7 +3232,7 @@
         <v>34</v>
       </c>
       <c r="I17" s="10">
-        <f>NETWORKDAYS(B17, A17)</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="J17" s="7">
@@ -3278,7 +3296,7 @@
         <v>34</v>
       </c>
       <c r="I18" s="10">
-        <f>NETWORKDAYS(B18, A18)</f>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="J18" s="7">
@@ -3342,7 +3360,7 @@
         <v>91</v>
       </c>
       <c r="I19" s="10">
-        <f>NETWORKDAYS(B19, A19)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="J19" s="7">
@@ -3406,7 +3424,7 @@
         <v>32</v>
       </c>
       <c r="I20" s="10">
-        <f>NETWORKDAYS(B20, A20)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="J20" s="7">
@@ -3470,7 +3488,7 @@
         <v>98</v>
       </c>
       <c r="I21" s="10">
-        <f>NETWORKDAYS(B21, A21)</f>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="J21" s="7">
@@ -3534,7 +3552,7 @@
         <v>98</v>
       </c>
       <c r="I22" s="10">
-        <f>NETWORKDAYS(B22, A22)</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="J22" s="7">
@@ -3598,7 +3616,7 @@
         <v>96</v>
       </c>
       <c r="I23" s="30">
-        <f>NETWORKDAYS(B23, A23)</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="J23" s="28">
@@ -3662,7 +3680,7 @@
         <v>34</v>
       </c>
       <c r="I24" s="10">
-        <f>NETWORKDAYS(B24, A24)</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="J24" s="7">
@@ -3726,7 +3744,7 @@
         <v>126</v>
       </c>
       <c r="I25" s="10">
-        <f>NETWORKDAYS(B25, A25)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="J25" s="7">
@@ -3790,7 +3808,7 @@
         <v>130</v>
       </c>
       <c r="I26" s="10">
-        <f>NETWORKDAYS(B26, A26)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="J26" s="7">
@@ -3854,7 +3872,7 @@
         <v>32</v>
       </c>
       <c r="I27" s="10">
-        <f>NETWORKDAYS(B27, A27)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="J27" s="7">
@@ -3918,7 +3936,7 @@
         <v>32</v>
       </c>
       <c r="I28" s="10">
-        <f>NETWORKDAYS(B28, A28)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="J28" s="7">
@@ -3982,7 +4000,7 @@
         <v>32</v>
       </c>
       <c r="I29" s="10">
-        <f>NETWORKDAYS(B29, A29)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="J29" s="7">
@@ -4046,7 +4064,7 @@
         <v>138</v>
       </c>
       <c r="I30" s="10">
-        <f>NETWORKDAYS(B30, A30)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="J30" s="7">
@@ -4110,7 +4128,7 @@
         <v>32</v>
       </c>
       <c r="I31" s="10">
-        <f>NETWORKDAYS(B31, A31)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="J31" s="7">
@@ -4174,7 +4192,7 @@
         <v>130</v>
       </c>
       <c r="I32" s="10">
-        <f>NETWORKDAYS(B32, A32)</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="J32" s="7">
@@ -4238,7 +4256,7 @@
         <v>130</v>
       </c>
       <c r="I33" s="10">
-        <f>NETWORKDAYS(B33, A33)</f>
+        <f t="shared" si="1"/>
         <v>36</v>
       </c>
       <c r="J33" s="7">
@@ -4302,7 +4320,7 @@
         <v>34</v>
       </c>
       <c r="I34" s="10">
-        <f>NETWORKDAYS(B34, A34)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="J34" s="7">
@@ -4366,7 +4384,7 @@
         <v>130</v>
       </c>
       <c r="I35" s="10">
-        <f>NETWORKDAYS(B35, A35)</f>
+        <f t="shared" si="1"/>
         <v>37</v>
       </c>
       <c r="J35" s="7">
@@ -4430,7 +4448,7 @@
         <v>98</v>
       </c>
       <c r="I36" s="10">
-        <f>NETWORKDAYS(B36, A36)</f>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="J36" s="7">
@@ -4494,7 +4512,7 @@
         <v>91</v>
       </c>
       <c r="I37" s="10">
-        <f>NETWORKDAYS(B37, A37)</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="J37" s="7">
@@ -4558,7 +4576,7 @@
         <v>91</v>
       </c>
       <c r="I38" s="10">
-        <f>NETWORKDAYS(B38, A38)</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="J38" s="7">
@@ -4622,7 +4640,7 @@
         <v>130</v>
       </c>
       <c r="I39" s="10">
-        <f>NETWORKDAYS(B39, A39)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="J39" s="7">
@@ -4686,7 +4704,7 @@
         <v>32</v>
       </c>
       <c r="I40" s="10">
-        <f>NETWORKDAYS(B40, A40)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="J40" s="7">
@@ -4750,7 +4768,7 @@
         <v>98</v>
       </c>
       <c r="I41" s="10">
-        <f>NETWORKDAYS(B41, A41)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="J41" s="7">
@@ -4814,7 +4832,7 @@
         <v>34</v>
       </c>
       <c r="I42" s="10">
-        <f>NETWORKDAYS(B42, A42)</f>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="J42" s="7">
@@ -4878,7 +4896,7 @@
         <v>130</v>
       </c>
       <c r="I43" s="10">
-        <f>NETWORKDAYS(B43, A43)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="J43" s="7">
@@ -4942,7 +4960,7 @@
         <v>34</v>
       </c>
       <c r="I44" s="10">
-        <f>NETWORKDAYS(B44, A44)</f>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="J44" s="7">
@@ -5006,7 +5024,7 @@
         <v>34</v>
       </c>
       <c r="I45" s="10">
-        <f>NETWORKDAYS(B45, A45)</f>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="J45" s="7">
@@ -5070,7 +5088,7 @@
         <v>32</v>
       </c>
       <c r="I46" s="10">
-        <f>NETWORKDAYS(B46, A46)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="J46" s="7">
@@ -5134,7 +5152,7 @@
         <v>32</v>
       </c>
       <c r="I47" s="10">
-        <f>NETWORKDAYS(B47, A47)</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="J47" s="7">
@@ -5198,7 +5216,7 @@
         <v>130</v>
       </c>
       <c r="I48" s="10">
-        <f>NETWORKDAYS(B48, A48)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="J48" s="7">
@@ -5262,7 +5280,7 @@
         <v>130</v>
       </c>
       <c r="I49" s="10">
-        <f>NETWORKDAYS(B49, A49)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="J49" s="7">
@@ -5326,7 +5344,7 @@
         <v>130</v>
       </c>
       <c r="I50" s="10">
-        <f>NETWORKDAYS(B50, A50)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="J50" s="7">
@@ -5390,7 +5408,7 @@
         <v>130</v>
       </c>
       <c r="I51" s="10">
-        <f>NETWORKDAYS(B51, A51)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="J51" s="7">
@@ -5454,7 +5472,7 @@
         <v>98</v>
       </c>
       <c r="I52" s="10">
-        <f>NETWORKDAYS(B52, A52)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="J52" s="7">
@@ -5518,7 +5536,7 @@
         <v>98</v>
       </c>
       <c r="I53" s="10">
-        <f>NETWORKDAYS(B53, A53)</f>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="J53" s="7">
@@ -5582,7 +5600,7 @@
         <v>34</v>
       </c>
       <c r="I54" s="10">
-        <f>NETWORKDAYS(B54, A54)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="J54" s="7">
@@ -5646,7 +5664,7 @@
         <v>126</v>
       </c>
       <c r="I55" s="10">
-        <f>NETWORKDAYS(B55, A55)</f>
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="J55" s="7">
@@ -5710,7 +5728,7 @@
         <v>130</v>
       </c>
       <c r="I56" s="10">
-        <f>NETWORKDAYS(B56, A56)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="J56" s="7">
@@ -5774,7 +5792,7 @@
         <v>96</v>
       </c>
       <c r="I57" s="10">
-        <f>NETWORKDAYS(B57, A57)</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="J57" s="7">
@@ -5838,7 +5856,7 @@
         <v>32</v>
       </c>
       <c r="I58" s="10">
-        <f>NETWORKDAYS(B58, A58)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="J58" s="7">
@@ -5902,7 +5920,7 @@
         <v>32</v>
       </c>
       <c r="I59" s="10">
-        <f>NETWORKDAYS(B59, A59)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="J59" s="7">
@@ -5966,7 +5984,7 @@
         <v>32</v>
       </c>
       <c r="I60" s="10">
-        <f>NETWORKDAYS(B60, A60)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="J60" s="7">
@@ -6030,7 +6048,7 @@
         <v>34</v>
       </c>
       <c r="I61" s="10">
-        <f>NETWORKDAYS(B61, A61)</f>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="J61" s="7">
@@ -6094,7 +6112,7 @@
         <v>130</v>
       </c>
       <c r="I62" s="10">
-        <f>NETWORKDAYS(B62, A62)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="J62" s="7">
@@ -6158,7 +6176,7 @@
         <v>34</v>
       </c>
       <c r="I63" s="10">
-        <f>NETWORKDAYS(B63, A63)</f>
+        <f t="shared" si="1"/>
         <v>18</v>
       </c>
       <c r="J63" s="7">
@@ -6222,7 +6240,7 @@
         <v>91</v>
       </c>
       <c r="I64" s="10">
-        <f>NETWORKDAYS(B64, A64)</f>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="J64" s="7">
@@ -6286,7 +6304,7 @@
         <v>98</v>
       </c>
       <c r="I65" s="10">
-        <f>NETWORKDAYS(B65, A65)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="J65" s="7">
@@ -6350,7 +6368,7 @@
         <v>98</v>
       </c>
       <c r="I66" s="10">
-        <f>NETWORKDAYS(B66, A66)</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="J66" s="7">
@@ -6414,7 +6432,7 @@
         <v>91</v>
       </c>
       <c r="I67" s="10">
-        <f>NETWORKDAYS(B67, A67)</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="J67" s="7">
@@ -6478,7 +6496,7 @@
         <v>32</v>
       </c>
       <c r="I68" s="10">
-        <f>NETWORKDAYS(B68, A68)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="J68" s="7">
@@ -6542,7 +6560,7 @@
         <v>34</v>
       </c>
       <c r="I69" s="10">
-        <f>NETWORKDAYS(B69, A69)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="J69" s="7">
@@ -6606,7 +6624,7 @@
         <v>98</v>
       </c>
       <c r="I70" s="10">
-        <f>NETWORKDAYS(B70, A70)</f>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="J70" s="7">
@@ -6670,7 +6688,7 @@
         <v>98</v>
       </c>
       <c r="I71" s="10">
-        <f>NETWORKDAYS(B71, A71)</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="J71" s="7">
@@ -6734,7 +6752,7 @@
         <v>98</v>
       </c>
       <c r="I72" s="10">
-        <f>NETWORKDAYS(B72, A72)</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="J72" s="7">
@@ -6798,7 +6816,7 @@
         <v>98</v>
       </c>
       <c r="I73" s="10">
-        <f>NETWORKDAYS(B73, A73)</f>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="J73" s="7">
@@ -6862,7 +6880,7 @@
         <v>98</v>
       </c>
       <c r="I74" s="10">
-        <f>NETWORKDAYS(B74, A74)</f>
+        <f t="shared" si="1"/>
         <v>26</v>
       </c>
       <c r="J74" s="7">
@@ -6926,7 +6944,7 @@
         <v>98</v>
       </c>
       <c r="I75" s="10">
-        <f>NETWORKDAYS(B75, A75)</f>
+        <f t="shared" ref="I75:I138" si="2">NETWORKDAYS(B75, A75)</f>
         <v>6</v>
       </c>
       <c r="J75" s="7">
@@ -6990,7 +7008,7 @@
         <v>91</v>
       </c>
       <c r="I76" s="10">
-        <f>NETWORKDAYS(B76, A76)</f>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="J76" s="7">
@@ -7054,7 +7072,7 @@
         <v>98</v>
       </c>
       <c r="I77" s="10">
-        <f>NETWORKDAYS(B77, A77)</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="J77" s="7">
@@ -7118,7 +7136,7 @@
         <v>32</v>
       </c>
       <c r="I78" s="10">
-        <f>NETWORKDAYS(B78, A78)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="J78" s="7">
@@ -7182,7 +7200,7 @@
         <v>32</v>
       </c>
       <c r="I79" s="10">
-        <f>NETWORKDAYS(B79, A79)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="J79" s="7">
@@ -7246,7 +7264,7 @@
         <v>138</v>
       </c>
       <c r="I80" s="10">
-        <f>NETWORKDAYS(B80, A80)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="J80" s="7">
@@ -7310,7 +7328,7 @@
         <v>130</v>
       </c>
       <c r="I81" s="10">
-        <f>NETWORKDAYS(B81, A81)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="J81" s="7">
@@ -7374,7 +7392,7 @@
         <v>98</v>
       </c>
       <c r="I82" s="10">
-        <f>NETWORKDAYS(B82, A82)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="J82" s="7">
@@ -7438,7 +7456,7 @@
         <v>130</v>
       </c>
       <c r="I83" s="10">
-        <f>NETWORKDAYS(B83, A83)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="J83" s="7">
@@ -7502,7 +7520,7 @@
         <v>98</v>
       </c>
       <c r="I84" s="10">
-        <f>NETWORKDAYS(B84, A84)</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="J84" s="7">
@@ -7566,7 +7584,7 @@
         <v>98</v>
       </c>
       <c r="I85" s="10">
-        <f>NETWORKDAYS(B85, A85)</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="J85" s="7">
@@ -7630,7 +7648,7 @@
         <v>34</v>
       </c>
       <c r="I86" s="30">
-        <f>NETWORKDAYS(B86, A86)</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="J86" s="28">
@@ -7694,7 +7712,7 @@
         <v>32</v>
       </c>
       <c r="I87" s="10">
-        <f>NETWORKDAYS(B87, A87)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="J87" s="7">
@@ -7758,7 +7776,7 @@
         <v>32</v>
       </c>
       <c r="I88" s="10">
-        <f>NETWORKDAYS(B88, A88)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="J88" s="7">
@@ -7822,7 +7840,7 @@
         <v>126</v>
       </c>
       <c r="I89" s="10">
-        <f>NETWORKDAYS(B89, A89)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="J89" s="7">
@@ -7886,7 +7904,7 @@
         <v>98</v>
       </c>
       <c r="I90" s="10">
-        <f>NETWORKDAYS(B90, A90)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="J90" s="7">
@@ -7950,7 +7968,7 @@
         <v>32</v>
       </c>
       <c r="I91" s="10">
-        <f>NETWORKDAYS(B91, A91)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="J91" s="7">
@@ -8014,7 +8032,7 @@
         <v>98</v>
       </c>
       <c r="I92" s="10">
-        <f>NETWORKDAYS(B92, A92)</f>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="J92" s="7">
@@ -8078,7 +8096,7 @@
         <v>126</v>
       </c>
       <c r="I93" s="10">
-        <f>NETWORKDAYS(B93, A93)</f>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="J93" s="7">
@@ -8142,7 +8160,7 @@
         <v>126</v>
       </c>
       <c r="I94" s="10">
-        <f>NETWORKDAYS(B94, A94)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="J94" s="7">
@@ -8206,7 +8224,7 @@
         <v>34</v>
       </c>
       <c r="I95" s="10">
-        <f>NETWORKDAYS(B95, A95)</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="J95" s="7">
@@ -8270,7 +8288,7 @@
         <v>130</v>
       </c>
       <c r="I96" s="10">
-        <f>NETWORKDAYS(B96, A96)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="J96" s="7">
@@ -8334,7 +8352,7 @@
         <v>138</v>
       </c>
       <c r="I97" s="10">
-        <f>NETWORKDAYS(B97, A97)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="J97" s="7">
@@ -8398,7 +8416,7 @@
         <v>98</v>
       </c>
       <c r="I98" s="10">
-        <f>NETWORKDAYS(B98, A98)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="J98" s="7">
@@ -8462,7 +8480,7 @@
         <v>130</v>
       </c>
       <c r="I99" s="10">
-        <f>NETWORKDAYS(B99, A99)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="J99" s="7">
@@ -8526,7 +8544,7 @@
         <v>130</v>
       </c>
       <c r="I100" s="10">
-        <f>NETWORKDAYS(B100, A100)</f>
+        <f t="shared" si="2"/>
         <v>24</v>
       </c>
       <c r="J100" s="7">
@@ -8590,7 +8608,7 @@
         <v>126</v>
       </c>
       <c r="I101" s="10">
-        <f>NETWORKDAYS(B101, A101)</f>
+        <f t="shared" si="2"/>
         <v>25</v>
       </c>
       <c r="J101" s="7">
@@ -8654,7 +8672,7 @@
         <v>98</v>
       </c>
       <c r="I102" s="10">
-        <f>NETWORKDAYS(B102, A102)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="J102" s="7">
@@ -8718,7 +8736,7 @@
         <v>91</v>
       </c>
       <c r="I103" s="10">
-        <f>NETWORKDAYS(B103, A103)</f>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="J103" s="7">
@@ -8782,7 +8800,7 @@
         <v>91</v>
       </c>
       <c r="I104" s="10">
-        <f>NETWORKDAYS(B104, A104)</f>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="J104" s="7">
@@ -8846,7 +8864,7 @@
         <v>32</v>
       </c>
       <c r="I105" s="10">
-        <f>NETWORKDAYS(B105, A105)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="J105" s="7">
@@ -8910,7 +8928,7 @@
         <v>32</v>
       </c>
       <c r="I106" s="10">
-        <f>NETWORKDAYS(B106, A106)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="J106" s="7">
@@ -8974,7 +8992,7 @@
         <v>98</v>
       </c>
       <c r="I107" s="10">
-        <f>NETWORKDAYS(B107, A107)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="J107" s="7">
@@ -9038,7 +9056,7 @@
         <v>96</v>
       </c>
       <c r="I108" s="10">
-        <f>NETWORKDAYS(B108, A108)</f>
+        <f t="shared" si="2"/>
         <v>6</v>
       </c>
       <c r="J108" s="7">
@@ -9102,7 +9120,7 @@
         <v>91</v>
       </c>
       <c r="I109" s="10">
-        <f>NETWORKDAYS(B109, A109)</f>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="J109" s="7">
@@ -9166,7 +9184,7 @@
         <v>91</v>
       </c>
       <c r="I110" s="10">
-        <f>NETWORKDAYS(B110, A110)</f>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="J110" s="7">
@@ -9230,7 +9248,7 @@
         <v>91</v>
       </c>
       <c r="I111" s="10">
-        <f>NETWORKDAYS(B111, A111)</f>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="J111" s="7">
@@ -9294,7 +9312,7 @@
         <v>126</v>
       </c>
       <c r="I112" s="10">
-        <f>NETWORKDAYS(B112, A112)</f>
+        <f t="shared" si="2"/>
         <v>9</v>
       </c>
       <c r="J112" s="7">
@@ -9358,7 +9376,7 @@
         <v>32</v>
       </c>
       <c r="I113" s="10">
-        <f>NETWORKDAYS(B113, A113)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="J113" s="7">
@@ -9422,7 +9440,7 @@
         <v>96</v>
       </c>
       <c r="I114" s="10">
-        <f>NETWORKDAYS(B114, A114)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="J114" s="7">
@@ -9486,7 +9504,7 @@
         <v>91</v>
       </c>
       <c r="I115" s="10">
-        <f>NETWORKDAYS(B115, A115)</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="J115" s="7">
@@ -9550,7 +9568,7 @@
         <v>32</v>
       </c>
       <c r="I116" s="10">
-        <f>NETWORKDAYS(B116, A116)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="J116" s="7">
@@ -9614,7 +9632,7 @@
         <v>98</v>
       </c>
       <c r="I117" s="10">
-        <f>NETWORKDAYS(B117, A117)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="J117" s="7">
@@ -9678,7 +9696,7 @@
         <v>91</v>
       </c>
       <c r="I118" s="10">
-        <f>NETWORKDAYS(B118, A118)</f>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="J118" s="7">
@@ -9742,7 +9760,7 @@
         <v>91</v>
       </c>
       <c r="I119" s="10">
-        <f>NETWORKDAYS(B119, A119)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="J119" s="7">
@@ -9806,7 +9824,7 @@
         <v>91</v>
       </c>
       <c r="I120" s="10">
-        <f>NETWORKDAYS(B120, A120)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="J120" s="7">
@@ -9870,7 +9888,7 @@
         <v>98</v>
       </c>
       <c r="I121" s="10">
-        <f>NETWORKDAYS(B121, A121)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="J121" s="7">
@@ -9934,7 +9952,7 @@
         <v>126</v>
       </c>
       <c r="I122" s="10">
-        <f>NETWORKDAYS(B122, A122)</f>
+        <f t="shared" si="2"/>
         <v>18</v>
       </c>
       <c r="J122" s="7">
@@ -9998,7 +10016,7 @@
         <v>91</v>
       </c>
       <c r="I123" s="10">
-        <f>NETWORKDAYS(B123, A123)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="J123" s="7">
@@ -10062,7 +10080,7 @@
         <v>32</v>
       </c>
       <c r="I124" s="10">
-        <f>NETWORKDAYS(B124, A124)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="J124" s="7">
@@ -10126,7 +10144,7 @@
         <v>130</v>
       </c>
       <c r="I125" s="10">
-        <f>NETWORKDAYS(B125, A125)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="J125" s="7">
@@ -10190,7 +10208,7 @@
         <v>130</v>
       </c>
       <c r="I126" s="10">
-        <f>NETWORKDAYS(B126, A126)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="J126" s="7">
@@ -10254,7 +10272,7 @@
         <v>98</v>
       </c>
       <c r="I127" s="10">
-        <f>NETWORKDAYS(B127, A127)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="J127" s="7">
@@ -10318,7 +10336,7 @@
         <v>130</v>
       </c>
       <c r="I128" s="10">
-        <f>NETWORKDAYS(B128, A128)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="J128" s="7">
@@ -10382,7 +10400,7 @@
         <v>32</v>
       </c>
       <c r="I129" s="10">
-        <f>NETWORKDAYS(B129, A129)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="J129" s="7">
@@ -10446,7 +10464,7 @@
         <v>32</v>
       </c>
       <c r="I130" s="10">
-        <f>NETWORKDAYS(B130, A130)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="J130" s="7">
@@ -10510,7 +10528,7 @@
         <v>91</v>
       </c>
       <c r="I131" s="10">
-        <f>NETWORKDAYS(B131, A131)</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="J131" s="7">
@@ -10574,7 +10592,7 @@
         <v>126</v>
       </c>
       <c r="I132" s="10">
-        <f>NETWORKDAYS(B132, A132)</f>
+        <f t="shared" si="2"/>
         <v>28</v>
       </c>
       <c r="J132" s="7">
@@ -10638,7 +10656,7 @@
         <v>98</v>
       </c>
       <c r="I133" s="10">
-        <f>NETWORKDAYS(B133, A133)</f>
+        <f t="shared" si="2"/>
         <v>7</v>
       </c>
       <c r="J133" s="7">
@@ -10702,7 +10720,7 @@
         <v>126</v>
       </c>
       <c r="I134" s="10">
-        <f>NETWORKDAYS(B134, A134)</f>
+        <f t="shared" si="2"/>
         <v>6</v>
       </c>
       <c r="J134" s="7">
@@ -10766,7 +10784,7 @@
         <v>126</v>
       </c>
       <c r="I135" s="10">
-        <f>NETWORKDAYS(B135, A135)</f>
+        <f t="shared" si="2"/>
         <v>7</v>
       </c>
       <c r="J135" s="7">
@@ -10830,7 +10848,7 @@
         <v>32</v>
       </c>
       <c r="I136" s="10">
-        <f>NETWORKDAYS(B136, A136)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="J136" s="7">
@@ -10894,7 +10912,7 @@
         <v>98</v>
       </c>
       <c r="I137" s="10">
-        <f>NETWORKDAYS(B137, A137)</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="J137" s="7">
@@ -10958,7 +10976,7 @@
         <v>98</v>
       </c>
       <c r="I138" s="10">
-        <f>NETWORKDAYS(B138, A138)</f>
+        <f t="shared" si="2"/>
         <v>7</v>
       </c>
       <c r="J138" s="7">
@@ -11022,7 +11040,7 @@
         <v>98</v>
       </c>
       <c r="I139" s="10">
-        <f>NETWORKDAYS(B139, A139)</f>
+        <f t="shared" ref="I139:I202" si="3">NETWORKDAYS(B139, A139)</f>
         <v>18</v>
       </c>
       <c r="J139" s="7">
@@ -11086,7 +11104,7 @@
         <v>91</v>
       </c>
       <c r="I140" s="10">
-        <f>NETWORKDAYS(B140, A140)</f>
+        <f t="shared" si="3"/>
         <v>6</v>
       </c>
       <c r="J140" s="7">
@@ -11150,7 +11168,7 @@
         <v>130</v>
       </c>
       <c r="I141" s="10">
-        <f>NETWORKDAYS(B141, A141)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="J141" s="7">
@@ -11214,7 +11232,7 @@
         <v>372</v>
       </c>
       <c r="I142" s="10">
-        <f>NETWORKDAYS(B142, A142)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="J142" s="7">
@@ -11278,7 +11296,7 @@
         <v>98</v>
       </c>
       <c r="I143" s="10">
-        <f>NETWORKDAYS(B143, A143)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="J143" s="7">
@@ -11342,7 +11360,7 @@
         <v>34</v>
       </c>
       <c r="I144" s="10">
-        <f>NETWORKDAYS(B144, A144)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="J144" s="7">
@@ -11406,7 +11424,7 @@
         <v>126</v>
       </c>
       <c r="I145" s="10">
-        <f>NETWORKDAYS(B145, A145)</f>
+        <f t="shared" si="3"/>
         <v>12</v>
       </c>
       <c r="J145" s="7">
@@ -11470,7 +11488,7 @@
         <v>91</v>
       </c>
       <c r="I146" s="10">
-        <f>NETWORKDAYS(B146, A146)</f>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="J146" s="7">
@@ -11534,7 +11552,7 @@
         <v>98</v>
       </c>
       <c r="I147" s="10">
-        <f>NETWORKDAYS(B147, A147)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="J147" s="7">
@@ -11598,7 +11616,7 @@
         <v>138</v>
       </c>
       <c r="I148" s="10">
-        <f>NETWORKDAYS(B148, A148)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="J148" s="7">
@@ -11662,7 +11680,7 @@
         <v>91</v>
       </c>
       <c r="I149" s="10">
-        <f>NETWORKDAYS(B149, A149)</f>
+        <f t="shared" si="3"/>
         <v>9</v>
       </c>
       <c r="J149" s="7">
@@ -11726,7 +11744,7 @@
         <v>130</v>
       </c>
       <c r="I150" s="10">
-        <f>NETWORKDAYS(B150, A150)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="J150" s="7">
@@ -11790,7 +11808,7 @@
         <v>32</v>
       </c>
       <c r="I151" s="10">
-        <f>NETWORKDAYS(B151, A151)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="J151" s="7">
@@ -11854,7 +11872,7 @@
         <v>91</v>
       </c>
       <c r="I152" s="10">
-        <f>NETWORKDAYS(B152, A152)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="J152" s="7">
@@ -11918,7 +11936,7 @@
         <v>32</v>
       </c>
       <c r="I153" s="10">
-        <f>NETWORKDAYS(B153, A153)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="J153" s="7">
@@ -11982,7 +12000,7 @@
         <v>34</v>
       </c>
       <c r="I154" s="10">
-        <f>NETWORKDAYS(B154, A154)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="J154" s="7">
@@ -12046,7 +12064,7 @@
         <v>130</v>
       </c>
       <c r="I155" s="10">
-        <f>NETWORKDAYS(B155, A155)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="J155" s="7">
@@ -12110,7 +12128,7 @@
         <v>98</v>
       </c>
       <c r="I156" s="10">
-        <f>NETWORKDAYS(B156, A156)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="J156" s="7">
@@ -12174,7 +12192,7 @@
         <v>91</v>
       </c>
       <c r="I157" s="10">
-        <f>NETWORKDAYS(B157, A157)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="J157" s="7">
@@ -12238,7 +12256,7 @@
         <v>91</v>
       </c>
       <c r="I158" s="10">
-        <f>NETWORKDAYS(B158, A158)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="J158" s="7">
@@ -12302,7 +12320,7 @@
         <v>32</v>
       </c>
       <c r="I159" s="10">
-        <f>NETWORKDAYS(B159, A159)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="J159" s="7">
@@ -12366,7 +12384,7 @@
         <v>32</v>
       </c>
       <c r="I160" s="10">
-        <f>NETWORKDAYS(B160, A160)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="J160" s="7">
@@ -12430,7 +12448,7 @@
         <v>32</v>
       </c>
       <c r="I161" s="10">
-        <f>NETWORKDAYS(B161, A161)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="J161" s="7">
@@ -12494,7 +12512,7 @@
         <v>32</v>
       </c>
       <c r="I162" s="10">
-        <f>NETWORKDAYS(B162, A162)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="J162" s="7">
@@ -12558,7 +12576,7 @@
         <v>185</v>
       </c>
       <c r="I163" s="10">
-        <f>NETWORKDAYS(B163, A163)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="J163" s="7">
@@ -12622,7 +12640,7 @@
         <v>91</v>
       </c>
       <c r="I164" s="10">
-        <f>NETWORKDAYS(B164, A164)</f>
+        <f t="shared" si="3"/>
         <v>17</v>
       </c>
       <c r="J164" s="7">
@@ -12686,7 +12704,7 @@
         <v>98</v>
       </c>
       <c r="I165" s="10">
-        <f>NETWORKDAYS(B165, A165)</f>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="J165" s="7">
@@ -12750,7 +12768,7 @@
         <v>91</v>
       </c>
       <c r="I166" s="10">
-        <f>NETWORKDAYS(B166, A166)</f>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="J166" s="7">
@@ -12814,7 +12832,7 @@
         <v>130</v>
       </c>
       <c r="I167" s="10">
-        <f>NETWORKDAYS(B167, A167)</f>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
       <c r="J167" s="7">
@@ -12878,7 +12896,7 @@
         <v>32</v>
       </c>
       <c r="I168" s="10">
-        <f>NETWORKDAYS(B168, A168)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="J168" s="7">
@@ -12942,7 +12960,7 @@
         <v>130</v>
       </c>
       <c r="I169" s="10">
-        <f>NETWORKDAYS(B169, A169)</f>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
       <c r="J169" s="7">
@@ -13006,7 +13024,7 @@
         <v>130</v>
       </c>
       <c r="I170" s="10">
-        <f>NETWORKDAYS(B170, A170)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="J170" s="7">
@@ -13070,7 +13088,7 @@
         <v>126</v>
       </c>
       <c r="I171" s="10">
-        <f>NETWORKDAYS(B171, A171)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="J171" s="7">
@@ -13134,7 +13152,7 @@
         <v>130</v>
       </c>
       <c r="I172" s="10">
-        <f>NETWORKDAYS(B172, A172)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="J172" s="7">
@@ -13198,7 +13216,7 @@
         <v>372</v>
       </c>
       <c r="I173" s="13">
-        <f>NETWORKDAYS(B173, A173)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="J173" s="12">
@@ -13262,7 +13280,7 @@
         <v>32</v>
       </c>
       <c r="I174" s="10">
-        <f>NETWORKDAYS(B174, A174)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="J174" s="7">
@@ -13326,7 +13344,7 @@
         <v>32</v>
       </c>
       <c r="I175" s="10">
-        <f>NETWORKDAYS(B175, A175)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="J175" s="7">
@@ -13390,7 +13408,7 @@
         <v>138</v>
       </c>
       <c r="I176" s="10">
-        <f>NETWORKDAYS(B176, A176)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="J176" s="7">
@@ -13454,7 +13472,7 @@
         <v>32</v>
       </c>
       <c r="I177" s="10">
-        <f>NETWORKDAYS(B177, A177)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="J177" s="7">
@@ -13518,7 +13536,7 @@
         <v>130</v>
       </c>
       <c r="I178" s="10">
-        <f>NETWORKDAYS(B178, A178)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="J178" s="7">
@@ -13582,7 +13600,7 @@
         <v>32</v>
       </c>
       <c r="I179" s="10">
-        <f>NETWORKDAYS(B179, A179)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="J179" s="7">
@@ -13620,67 +13638,67 @@
         <v>0</v>
       </c>
     </row>
-    <row r="180" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A180" s="46">
+    <row r="180" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A180" s="6">
         <v>45877</v>
       </c>
-      <c r="B180" s="46">
+      <c r="B180" s="6">
         <v>45877</v>
       </c>
-      <c r="C180" s="46" t="s">
-        <v>7</v>
-      </c>
-      <c r="D180" s="46" t="s">
+      <c r="C180" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D180" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E180" s="46" t="s">
+      <c r="E180" s="6" t="s">
         <v>142</v>
       </c>
-      <c r="F180" s="47" t="s">
-        <v>3</v>
-      </c>
-      <c r="G180" s="47" t="s">
-        <v>3</v>
-      </c>
-      <c r="H180" s="47" t="s">
+      <c r="F180" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="G180" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="H180" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="I180" s="48">
-        <f>NETWORKDAYS(B180, A180)</f>
+      <c r="I180" s="10">
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="J180" s="47">
+      <c r="J180" s="7">
         <v>66627</v>
       </c>
-      <c r="K180" s="47">
+      <c r="K180" s="7">
         <v>11127</v>
       </c>
-      <c r="L180" s="47" t="s">
+      <c r="L180" s="7" t="s">
         <v>221</v>
       </c>
-      <c r="M180" s="46">
+      <c r="M180" s="6">
         <v>45881</v>
       </c>
-      <c r="N180" s="49">
+      <c r="N180" s="8">
         <v>547.91999999999996</v>
       </c>
-      <c r="O180" s="47" t="s">
+      <c r="O180" s="7" t="s">
         <v>122</v>
       </c>
-      <c r="P180" s="47">
+      <c r="P180" s="7">
         <v>35</v>
       </c>
-      <c r="Q180" s="47" t="s">
-        <v>407</v>
-      </c>
-      <c r="R180" s="47">
+      <c r="Q180" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="R180" s="7">
         <f>DATEDIF(Tabela1[[#This Row],[Atendimento]],Tabela1[[#This Row],[Previsao de Entrega]],"D")</f>
         <v>4</v>
       </c>
-      <c r="S180" s="49">
-        <v>0</v>
-      </c>
-      <c r="T180" s="49">
+      <c r="S180" s="8">
+        <v>0</v>
+      </c>
+      <c r="T180" s="8">
         <v>0</v>
       </c>
     </row>
@@ -13710,7 +13728,7 @@
         <v>91</v>
       </c>
       <c r="I181" s="10">
-        <f>NETWORKDAYS(B181, A181)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="J181" s="7">
@@ -13774,7 +13792,7 @@
         <v>91</v>
       </c>
       <c r="I182" s="10">
-        <f>NETWORKDAYS(B182, A182)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="J182" s="7">
@@ -13838,7 +13856,7 @@
         <v>98</v>
       </c>
       <c r="I183" s="10">
-        <f>NETWORKDAYS(B183, A183)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="J183" s="7">
@@ -13902,7 +13920,7 @@
         <v>98</v>
       </c>
       <c r="I184" s="10">
-        <f>NETWORKDAYS(B184, A184)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="J184" s="7">
@@ -13966,11 +13984,11 @@
         <v>34</v>
       </c>
       <c r="I185" s="10">
-        <f>NETWORKDAYS(B185, A185)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="J185" s="7">
-        <v>65769</v>
+        <v>65768</v>
       </c>
       <c r="K185" s="7">
         <v>175</v>
@@ -14030,7 +14048,7 @@
         <v>96</v>
       </c>
       <c r="I186" s="10">
-        <f>NETWORKDAYS(B186, A186)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="J186" s="7">
@@ -14094,7 +14112,7 @@
         <v>32</v>
       </c>
       <c r="I187" s="10">
-        <f>NETWORKDAYS(B187, A187)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="J187" s="7">
@@ -14132,67 +14150,67 @@
         <v>0</v>
       </c>
     </row>
-    <row r="188" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A188" s="11">
+    <row r="188" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A188" s="6">
         <v>45868</v>
       </c>
-      <c r="B188" s="11">
+      <c r="B188" s="6">
         <v>45868</v>
       </c>
-      <c r="C188" s="11" t="s">
+      <c r="C188" s="6" t="s">
         <v>128</v>
       </c>
-      <c r="D188" s="11" t="s">
+      <c r="D188" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E188" s="11" t="s">
+      <c r="E188" s="6" t="s">
         <v>394</v>
       </c>
-      <c r="F188" s="12">
+      <c r="F188" s="7">
         <v>68487</v>
       </c>
-      <c r="G188" s="12" t="s">
+      <c r="G188" s="7" t="s">
         <v>395</v>
       </c>
-      <c r="H188" s="12" t="s">
+      <c r="H188" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="I188" s="13">
-        <f>NETWORKDAYS(B188, A188)</f>
+      <c r="I188" s="10">
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="J188" s="12">
+      <c r="J188" s="7">
         <v>66489</v>
       </c>
-      <c r="K188" s="12">
+      <c r="K188" s="7">
         <v>11614</v>
       </c>
-      <c r="L188" s="12" t="s">
+      <c r="L188" s="7" t="s">
         <v>396</v>
       </c>
-      <c r="M188" s="11">
+      <c r="M188" s="6">
         <v>45882</v>
       </c>
-      <c r="N188" s="14">
+      <c r="N188" s="8">
         <v>6633</v>
       </c>
-      <c r="O188" s="12" t="s">
+      <c r="O188" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="P188" s="12">
+      <c r="P188" s="7">
         <v>1</v>
       </c>
-      <c r="Q188" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="R188" s="12">
+      <c r="Q188" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="R188" s="7">
         <f>DATEDIF(Tabela1[[#This Row],[Atendimento]],Tabela1[[#This Row],[Previsao de Entrega]],"D")</f>
         <v>14</v>
       </c>
-      <c r="S188" s="14">
-        <v>0</v>
-      </c>
-      <c r="T188" s="14">
+      <c r="S188" s="8">
+        <v>0</v>
+      </c>
+      <c r="T188" s="8">
         <v>0</v>
       </c>
     </row>
@@ -14222,7 +14240,7 @@
         <v>34</v>
       </c>
       <c r="I189" s="10">
-        <f>NETWORKDAYS(B189, A189)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="J189" s="7">
@@ -14286,7 +14304,7 @@
         <v>91</v>
       </c>
       <c r="I190" s="10">
-        <f>NETWORKDAYS(B190, A190)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="J190" s="7">
@@ -14350,7 +14368,7 @@
         <v>34</v>
       </c>
       <c r="I191" s="10">
-        <f>NETWORKDAYS(B191, A191)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="J191" s="7">
@@ -14414,7 +14432,7 @@
         <v>96</v>
       </c>
       <c r="I192" s="13">
-        <f>NETWORKDAYS(B192, A192)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="J192" s="12">
@@ -14478,7 +14496,7 @@
         <v>98</v>
       </c>
       <c r="I193" s="10">
-        <f>NETWORKDAYS(B193, A193)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="J193" s="7">
@@ -14542,7 +14560,7 @@
         <v>372</v>
       </c>
       <c r="I194" s="10">
-        <f>NETWORKDAYS(B194, A194)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="J194" s="7">
@@ -14606,7 +14624,7 @@
         <v>32</v>
       </c>
       <c r="I195" s="10">
-        <f>NETWORKDAYS(B195, A195)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="J195" s="7">
@@ -14670,7 +14688,7 @@
         <v>372</v>
       </c>
       <c r="I196" s="10">
-        <f>NETWORKDAYS(B196, A196)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="J196" s="7">
@@ -14734,7 +14752,7 @@
         <v>372</v>
       </c>
       <c r="I197" s="10">
-        <f>NETWORKDAYS(B197, A197)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="J197" s="7">
@@ -14798,7 +14816,7 @@
         <v>372</v>
       </c>
       <c r="I198" s="10">
-        <f>NETWORKDAYS(B198, A198)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="J198" s="7">
@@ -14862,7 +14880,7 @@
         <v>32</v>
       </c>
       <c r="I199" s="10">
-        <f>NETWORKDAYS(B199, A199)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="J199" s="7">
@@ -14926,7 +14944,7 @@
         <v>32</v>
       </c>
       <c r="I200" s="10">
-        <f>NETWORKDAYS(B200, A200)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="J200" s="7">
@@ -14990,7 +15008,7 @@
         <v>126</v>
       </c>
       <c r="I201" s="10">
-        <f>NETWORKDAYS(B201, A201)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="J201" s="7">
@@ -15054,7 +15072,7 @@
         <v>130</v>
       </c>
       <c r="I202" s="10">
-        <f>NETWORKDAYS(B202, A202)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="J202" s="7">
@@ -15118,7 +15136,7 @@
         <v>32</v>
       </c>
       <c r="I203" s="10">
-        <f>NETWORKDAYS(B203, A203)</f>
+        <f t="shared" ref="I203:I259" si="4">NETWORKDAYS(B203, A203)</f>
         <v>1</v>
       </c>
       <c r="J203" s="7">
@@ -15182,7 +15200,7 @@
         <v>32</v>
       </c>
       <c r="I204" s="10">
-        <f>NETWORKDAYS(B204, A204)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="J204" s="7">
@@ -15246,7 +15264,7 @@
         <v>34</v>
       </c>
       <c r="I205" s="10">
-        <f>NETWORKDAYS(B205, A205)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="J205" s="7">
@@ -15310,7 +15328,7 @@
         <v>126</v>
       </c>
       <c r="I206" s="10">
-        <f>NETWORKDAYS(B206, A206)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="J206" s="7">
@@ -15374,7 +15392,7 @@
         <v>130</v>
       </c>
       <c r="I207" s="10">
-        <f>NETWORKDAYS(B207, A207)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="J207" s="7">
@@ -15438,7 +15456,7 @@
         <v>130</v>
       </c>
       <c r="I208" s="10">
-        <f>NETWORKDAYS(B208, A208)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="J208" s="7">
@@ -15502,7 +15520,7 @@
         <v>130</v>
       </c>
       <c r="I209" s="10">
-        <f>NETWORKDAYS(B209, A209)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="J209" s="7">
@@ -15566,7 +15584,7 @@
         <v>130</v>
       </c>
       <c r="I210" s="10">
-        <f>NETWORKDAYS(B210, A210)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="J210" s="7">
@@ -15630,7 +15648,7 @@
         <v>34</v>
       </c>
       <c r="I211" s="10">
-        <f>NETWORKDAYS(B211, A211)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="J211" s="7">
@@ -15694,7 +15712,7 @@
         <v>32</v>
       </c>
       <c r="I212" s="10">
-        <f>NETWORKDAYS(B212, A212)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="J212" s="7">
@@ -15758,7 +15776,7 @@
         <v>138</v>
       </c>
       <c r="I213" s="10">
-        <f>NETWORKDAYS(B213, A213)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="J213" s="7">
@@ -15822,7 +15840,7 @@
         <v>91</v>
       </c>
       <c r="I214" s="10">
-        <f>NETWORKDAYS(B214, A214)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="J214" s="7">
@@ -15886,7 +15904,7 @@
         <v>98</v>
       </c>
       <c r="I215" s="10">
-        <f>NETWORKDAYS(B215, A215)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="J215" s="7">
@@ -15950,7 +15968,7 @@
         <v>138</v>
       </c>
       <c r="I216" s="10">
-        <f>NETWORKDAYS(B216, A216)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="J216" s="7">
@@ -16014,7 +16032,7 @@
         <v>98</v>
       </c>
       <c r="I217" s="10">
-        <f>NETWORKDAYS(B217, A217)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="J217" s="7">
@@ -16078,7 +16096,7 @@
         <v>372</v>
       </c>
       <c r="I218" s="13">
-        <f>NETWORKDAYS(B218, A218)</f>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="J218" s="12">
@@ -16142,7 +16160,7 @@
         <v>130</v>
       </c>
       <c r="I219" s="10">
-        <f>NETWORKDAYS(B219, A219)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="J219" s="7">
@@ -16206,7 +16224,7 @@
         <v>130</v>
       </c>
       <c r="I220" s="10">
-        <f>NETWORKDAYS(B220, A220)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="J220" s="7">
@@ -16270,7 +16288,7 @@
         <v>98</v>
       </c>
       <c r="I221" s="10">
-        <f>NETWORKDAYS(B221, A221)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="J221" s="7">
@@ -16334,7 +16352,7 @@
         <v>91</v>
       </c>
       <c r="I222" s="10">
-        <f>NETWORKDAYS(B222, A222)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="J222" s="7">
@@ -16398,7 +16416,7 @@
         <v>32</v>
       </c>
       <c r="I223" s="10">
-        <f>NETWORKDAYS(B223, A223)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="J223" s="7">
@@ -16462,7 +16480,7 @@
         <v>372</v>
       </c>
       <c r="I224" s="10">
-        <f>NETWORKDAYS(B224, A224)</f>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="J224" s="7">
@@ -16526,7 +16544,7 @@
         <v>32</v>
       </c>
       <c r="I225" s="10">
-        <f>NETWORKDAYS(B225, A225)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="J225" s="7">
@@ -16590,7 +16608,7 @@
         <v>372</v>
       </c>
       <c r="I226" s="13">
-        <f>NETWORKDAYS(B226, A226)</f>
+        <f t="shared" si="4"/>
         <v>4</v>
       </c>
       <c r="J226" s="12">
@@ -16654,7 +16672,7 @@
         <v>98</v>
       </c>
       <c r="I227" s="13">
-        <f>NETWORKDAYS(B227, A227)</f>
+        <f t="shared" si="4"/>
         <v>8</v>
       </c>
       <c r="J227" s="12">
@@ -16718,7 +16736,7 @@
         <v>98</v>
       </c>
       <c r="I228" s="13">
-        <f>NETWORKDAYS(B228, A228)</f>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="J228" s="12">
@@ -16757,66 +16775,66 @@
       </c>
     </row>
     <row r="229" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A229" s="46">
+      <c r="A229" s="11">
         <v>45868</v>
       </c>
-      <c r="B229" s="46">
+      <c r="B229" s="11">
         <v>45862</v>
       </c>
-      <c r="C229" s="46" t="s">
-        <v>7</v>
-      </c>
-      <c r="D229" s="46" t="s">
+      <c r="C229" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D229" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="E229" s="46" t="s">
+      <c r="E229" s="11" t="s">
         <v>113</v>
       </c>
-      <c r="F229" s="47">
+      <c r="F229" s="12">
         <v>68476</v>
       </c>
-      <c r="G229" s="47" t="s">
+      <c r="G229" s="12" t="s">
         <v>227</v>
       </c>
-      <c r="H229" s="47" t="s">
+      <c r="H229" s="12" t="s">
         <v>98</v>
       </c>
-      <c r="I229" s="48">
-        <f>NETWORKDAYS(B229, A229)</f>
+      <c r="I229" s="13">
+        <f t="shared" si="4"/>
         <v>5</v>
       </c>
-      <c r="J229" s="47">
+      <c r="J229" s="12">
         <v>66491</v>
       </c>
-      <c r="K229" s="47">
+      <c r="K229" s="12">
         <v>11522</v>
       </c>
-      <c r="L229" s="47" t="s">
+      <c r="L229" s="12" t="s">
         <v>376</v>
       </c>
-      <c r="M229" s="46">
+      <c r="M229" s="11">
         <v>45888</v>
       </c>
-      <c r="N229" s="49">
+      <c r="N229" s="14">
         <v>1680.4</v>
       </c>
-      <c r="O229" s="47" t="s">
+      <c r="O229" s="12" t="s">
         <v>122</v>
       </c>
-      <c r="P229" s="47">
+      <c r="P229" s="12">
         <v>28</v>
       </c>
-      <c r="Q229" s="47" t="s">
-        <v>407</v>
-      </c>
-      <c r="R229" s="47">
+      <c r="Q229" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="R229" s="12">
         <f>DATEDIF(Tabela1[[#This Row],[Atendimento]],Tabela1[[#This Row],[Previsao de Entrega]],"D")</f>
         <v>20</v>
       </c>
-      <c r="S229" s="49">
-        <v>0</v>
-      </c>
-      <c r="T229" s="49">
+      <c r="S229" s="14">
+        <v>0</v>
+      </c>
+      <c r="T229" s="14">
         <v>0</v>
       </c>
     </row>
@@ -16846,13 +16864,13 @@
         <v>372</v>
       </c>
       <c r="I230" s="13">
-        <f>NETWORKDAYS(B230, A230)</f>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="J230" s="12">
         <v>66660</v>
       </c>
-      <c r="K230" s="51">
+      <c r="K230" s="12">
         <v>160</v>
       </c>
       <c r="L230" s="12" t="s">
@@ -16873,7 +16891,7 @@
       <c r="Q230" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="R230" s="51">
+      <c r="R230" s="12">
         <f>DATEDIF(Tabela1[[#This Row],[Atendimento]],Tabela1[[#This Row],[Previsao de Entrega]],"D")</f>
         <v>7</v>
       </c>
@@ -16910,7 +16928,7 @@
         <v>372</v>
       </c>
       <c r="I231" s="10">
-        <f>NETWORKDAYS(B231, A231)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="J231" s="7">
@@ -16974,7 +16992,7 @@
         <v>130</v>
       </c>
       <c r="I232" s="13">
-        <f>NETWORKDAYS(B232, A232)</f>
+        <f t="shared" si="4"/>
         <v>6</v>
       </c>
       <c r="J232" s="12">
@@ -17038,7 +17056,7 @@
         <v>126</v>
       </c>
       <c r="I233" s="13">
-        <f>NETWORKDAYS(B233, A233)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="J233" s="42">
@@ -17102,7 +17120,7 @@
         <v>98</v>
       </c>
       <c r="I234" s="13">
-        <f>NETWORKDAYS(B234, A234)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="J234" s="12">
@@ -17166,7 +17184,7 @@
         <v>32</v>
       </c>
       <c r="I235" s="13">
-        <f>NETWORKDAYS(B235, A235)</f>
+        <f t="shared" si="4"/>
         <v>9</v>
       </c>
       <c r="J235" s="12">
@@ -17205,66 +17223,66 @@
       </c>
     </row>
     <row r="236" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A236" s="46">
+      <c r="A236" s="11">
         <v>45881</v>
       </c>
-      <c r="B236" s="46">
+      <c r="B236" s="11">
         <v>45881</v>
       </c>
-      <c r="C236" s="46" t="s">
-        <v>7</v>
-      </c>
-      <c r="D236" s="46" t="s">
+      <c r="C236" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D236" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="E236" s="46" t="s">
+      <c r="E236" s="11" t="s">
         <v>124</v>
       </c>
-      <c r="F236" s="47">
+      <c r="F236" s="12">
         <v>68501</v>
       </c>
-      <c r="G236" s="47" t="s">
+      <c r="G236" s="12" t="s">
         <v>90</v>
       </c>
-      <c r="H236" s="47" t="s">
+      <c r="H236" s="12" t="s">
         <v>91</v>
       </c>
-      <c r="I236" s="48">
-        <f>NETWORKDAYS(B236, A236)</f>
+      <c r="I236" s="13">
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="J236" s="47">
+      <c r="J236" s="12">
         <v>66662</v>
       </c>
-      <c r="K236" s="50">
+      <c r="K236" s="12">
         <v>3040</v>
       </c>
-      <c r="L236" s="47" t="s">
+      <c r="L236" s="12" t="s">
         <v>214</v>
       </c>
-      <c r="M236" s="46">
+      <c r="M236" s="11">
         <v>45896</v>
       </c>
-      <c r="N236" s="49">
+      <c r="N236" s="14">
         <v>1000</v>
       </c>
-      <c r="O236" s="47" t="s">
+      <c r="O236" s="12" t="s">
         <v>122</v>
       </c>
-      <c r="P236" s="47">
+      <c r="P236" s="12">
         <v>30</v>
       </c>
-      <c r="Q236" s="47" t="s">
-        <v>407</v>
-      </c>
-      <c r="R236" s="50">
+      <c r="Q236" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="R236" s="12">
         <f>DATEDIF(Tabela1[[#This Row],[Atendimento]],Tabela1[[#This Row],[Previsao de Entrega]],"D")</f>
         <v>15</v>
       </c>
-      <c r="S236" s="49">
-        <v>0</v>
-      </c>
-      <c r="T236" s="49">
+      <c r="S236" s="14">
+        <v>0</v>
+      </c>
+      <c r="T236" s="14">
         <v>0</v>
       </c>
     </row>
@@ -17294,7 +17312,7 @@
         <v>34</v>
       </c>
       <c r="I237" s="10">
-        <f>NETWORKDAYS(B237, A237)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="J237" s="7">
@@ -17358,7 +17376,7 @@
         <v>130</v>
       </c>
       <c r="I238" s="10">
-        <f>NETWORKDAYS(B238, A238)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="J238" s="7">
@@ -17422,7 +17440,7 @@
         <v>130</v>
       </c>
       <c r="I239" s="10">
-        <f>NETWORKDAYS(B239, A239)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="J239" s="7">
@@ -17486,7 +17504,7 @@
         <v>130</v>
       </c>
       <c r="I240" s="10">
-        <f>NETWORKDAYS(B240, A240)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="J240" s="7">
@@ -17550,7 +17568,7 @@
         <v>32</v>
       </c>
       <c r="I241" s="10">
-        <f>NETWORKDAYS(B241, A241)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="J241" s="7">
@@ -17614,7 +17632,7 @@
         <v>126</v>
       </c>
       <c r="I242" s="10">
-        <f>NETWORKDAYS(B242, A242)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="J242" s="7">
@@ -17678,7 +17696,7 @@
         <v>138</v>
       </c>
       <c r="I243" s="10">
-        <f>NETWORKDAYS(B243, A243)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="J243" s="7">
@@ -17742,7 +17760,7 @@
         <v>126</v>
       </c>
       <c r="I244" s="13">
-        <f>NETWORKDAYS(B244, A244)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="J244" s="12">
@@ -17806,7 +17824,7 @@
         <v>32</v>
       </c>
       <c r="I245" s="10">
-        <f>NETWORKDAYS(B245, A245)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="J245" s="7">
@@ -17870,7 +17888,7 @@
         <v>126</v>
       </c>
       <c r="I246" s="13">
-        <f>NETWORKDAYS(B246, A246)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="J246" s="12">
@@ -17934,7 +17952,7 @@
         <v>32</v>
       </c>
       <c r="I247" s="10">
-        <f>NETWORKDAYS(B247, A247)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="J247" s="7">
@@ -17998,7 +18016,7 @@
         <v>98</v>
       </c>
       <c r="I248" s="10">
-        <f>NETWORKDAYS(B248, A248)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="J248" s="7">
@@ -18062,7 +18080,7 @@
         <v>98</v>
       </c>
       <c r="I249" s="10">
-        <f>NETWORKDAYS(B249, A249)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="J249" s="7">
@@ -18126,7 +18144,7 @@
         <v>126</v>
       </c>
       <c r="I250" s="13">
-        <f>NETWORKDAYS(B250, A250)</f>
+        <f t="shared" si="4"/>
         <v>3</v>
       </c>
       <c r="J250" s="12">
@@ -18190,7 +18208,7 @@
         <v>126</v>
       </c>
       <c r="I251" s="13">
-        <f>NETWORKDAYS(B251, A251)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="J251" s="12">
@@ -18254,7 +18272,7 @@
         <v>34</v>
       </c>
       <c r="I252" s="13">
-        <f>NETWORKDAYS(B252, A252)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="J252" s="12">
@@ -18318,7 +18336,7 @@
         <v>32</v>
       </c>
       <c r="I253" s="10">
-        <f>NETWORKDAYS(B253, A253)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="J253" s="7">
@@ -18382,7 +18400,7 @@
         <v>32</v>
       </c>
       <c r="I254" s="10">
-        <f>NETWORKDAYS(B254, A254)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="J254" s="7">
@@ -18446,7 +18464,7 @@
         <v>34</v>
       </c>
       <c r="I255" s="13">
-        <f>NETWORKDAYS(B255, A255)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="J255" s="12">
@@ -18510,7 +18528,7 @@
         <v>126</v>
       </c>
       <c r="I256" s="13">
-        <f>NETWORKDAYS(B256, A256)</f>
+        <f t="shared" si="4"/>
         <v>16</v>
       </c>
       <c r="J256" s="12">
@@ -18574,7 +18592,7 @@
         <v>91</v>
       </c>
       <c r="I257" s="13">
-        <f>NETWORKDAYS(B257, A257)</f>
+        <f t="shared" si="4"/>
         <v>5</v>
       </c>
       <c r="J257" s="12">
@@ -18638,7 +18656,7 @@
         <v>126</v>
       </c>
       <c r="I258" s="13">
-        <f>NETWORKDAYS(B258, A258)</f>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="J258" s="12">
@@ -18702,7 +18720,7 @@
         <v>126</v>
       </c>
       <c r="I259" s="13">
-        <f>NETWORKDAYS(B259, A259)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="J259" s="12">
@@ -18738,6 +18756,518 @@
       </c>
       <c r="T259" s="14">
         <v>0</v>
+      </c>
+    </row>
+    <row r="260" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A260" s="11">
+        <v>45882</v>
+      </c>
+      <c r="B260" s="11">
+        <v>45881</v>
+      </c>
+      <c r="C260" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D260" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="E260" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="F260" s="12">
+        <v>68503</v>
+      </c>
+      <c r="G260" s="12" t="s">
+        <v>227</v>
+      </c>
+      <c r="H260" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="I260" s="13">
+        <f>NETWORKDAYS(B260, A260)</f>
+        <v>2</v>
+      </c>
+      <c r="J260" s="12">
+        <v>66669</v>
+      </c>
+      <c r="K260" s="52">
+        <v>3509</v>
+      </c>
+      <c r="L260" s="12" t="s">
+        <v>333</v>
+      </c>
+      <c r="M260" s="11">
+        <v>45894</v>
+      </c>
+      <c r="N260" s="14">
+        <v>1920</v>
+      </c>
+      <c r="O260" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="P260" s="12">
+        <v>7</v>
+      </c>
+      <c r="Q260" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="R260" s="52">
+        <f>DATEDIF(Tabela1[[#This Row],[Atendimento]],Tabela1[[#This Row],[Previsao de Entrega]],"D")</f>
+        <v>12</v>
+      </c>
+      <c r="S260" s="14">
+        <v>0</v>
+      </c>
+      <c r="T260" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="261" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A261" s="46">
+        <v>45882</v>
+      </c>
+      <c r="B261" s="46">
+        <v>45880</v>
+      </c>
+      <c r="C261" s="46" t="s">
+        <v>7</v>
+      </c>
+      <c r="D261" s="46" t="s">
+        <v>15</v>
+      </c>
+      <c r="E261" s="46" t="s">
+        <v>113</v>
+      </c>
+      <c r="F261" s="47">
+        <v>68498</v>
+      </c>
+      <c r="G261" s="47" t="s">
+        <v>321</v>
+      </c>
+      <c r="H261" s="47" t="s">
+        <v>91</v>
+      </c>
+      <c r="I261" s="48">
+        <f>NETWORKDAYS(B261, A261)</f>
+        <v>3</v>
+      </c>
+      <c r="J261" s="53">
+        <v>66670</v>
+      </c>
+      <c r="K261" s="51">
+        <v>11796</v>
+      </c>
+      <c r="L261" s="47" t="s">
+        <v>411</v>
+      </c>
+      <c r="M261" s="46">
+        <v>45890</v>
+      </c>
+      <c r="N261" s="49">
+        <v>42.23</v>
+      </c>
+      <c r="O261" s="47" t="s">
+        <v>121</v>
+      </c>
+      <c r="P261" s="47">
+        <v>0</v>
+      </c>
+      <c r="Q261" s="47" t="s">
+        <v>407</v>
+      </c>
+      <c r="R261" s="51">
+        <f>DATEDIF(Tabela1[[#This Row],[Atendimento]],Tabela1[[#This Row],[Previsao de Entrega]],"D")</f>
+        <v>8</v>
+      </c>
+      <c r="S261" s="49">
+        <v>0</v>
+      </c>
+      <c r="T261" s="49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="262" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A262" s="11">
+        <v>45882</v>
+      </c>
+      <c r="B262" s="11">
+        <v>45880</v>
+      </c>
+      <c r="C262" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D262" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="E262" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="F262" s="12">
+        <v>68499</v>
+      </c>
+      <c r="G262" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="H262" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="I262" s="13">
+        <f>NETWORKDAYS(B262, A262)</f>
+        <v>3</v>
+      </c>
+      <c r="J262" s="12">
+        <v>66671</v>
+      </c>
+      <c r="K262" s="52">
+        <v>1277</v>
+      </c>
+      <c r="L262" s="12" t="s">
+        <v>398</v>
+      </c>
+      <c r="M262" s="11">
+        <v>45884</v>
+      </c>
+      <c r="N262" s="14">
+        <v>207.68</v>
+      </c>
+      <c r="O262" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="P262" s="12">
+        <v>35</v>
+      </c>
+      <c r="Q262" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="R262" s="52">
+        <f>DATEDIF(Tabela1[[#This Row],[Atendimento]],Tabela1[[#This Row],[Previsao de Entrega]],"D")</f>
+        <v>2</v>
+      </c>
+      <c r="S262" s="14">
+        <v>0</v>
+      </c>
+      <c r="T262" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="263" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A263" s="11">
+        <v>45882</v>
+      </c>
+      <c r="B263" s="11">
+        <v>45881</v>
+      </c>
+      <c r="C263" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D263" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="E263" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="F263" s="12">
+        <v>68502</v>
+      </c>
+      <c r="G263" s="12" t="s">
+        <v>321</v>
+      </c>
+      <c r="H263" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="I263" s="13">
+        <f>NETWORKDAYS(B263, A263)</f>
+        <v>2</v>
+      </c>
+      <c r="J263" s="12">
+        <v>66672</v>
+      </c>
+      <c r="K263" s="52">
+        <v>10594</v>
+      </c>
+      <c r="L263" s="12" t="s">
+        <v>412</v>
+      </c>
+      <c r="M263" s="11">
+        <v>45891</v>
+      </c>
+      <c r="N263" s="14">
+        <v>1159.8</v>
+      </c>
+      <c r="O263" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="P263" s="12">
+        <v>28</v>
+      </c>
+      <c r="Q263" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="R263" s="52">
+        <f>DATEDIF(Tabela1[[#This Row],[Atendimento]],Tabela1[[#This Row],[Previsao de Entrega]],"D")</f>
+        <v>9</v>
+      </c>
+      <c r="S263" s="14">
+        <v>0</v>
+      </c>
+      <c r="T263" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="264" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A264" s="11">
+        <v>45882</v>
+      </c>
+      <c r="B264" s="11">
+        <v>45881</v>
+      </c>
+      <c r="C264" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D264" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="E264" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="F264" s="12">
+        <v>68502</v>
+      </c>
+      <c r="G264" s="12" t="s">
+        <v>321</v>
+      </c>
+      <c r="H264" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="I264" s="13">
+        <f>NETWORKDAYS(B264, A264)</f>
+        <v>2</v>
+      </c>
+      <c r="J264" s="12">
+        <v>66673</v>
+      </c>
+      <c r="K264" s="52">
+        <v>11682</v>
+      </c>
+      <c r="L264" s="12" t="s">
+        <v>179</v>
+      </c>
+      <c r="M264" s="11">
+        <v>45891</v>
+      </c>
+      <c r="N264" s="14">
+        <v>1173.95</v>
+      </c>
+      <c r="O264" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="P264" s="12">
+        <v>28</v>
+      </c>
+      <c r="Q264" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="R264" s="52">
+        <f>DATEDIF(Tabela1[[#This Row],[Atendimento]],Tabela1[[#This Row],[Previsao de Entrega]],"D")</f>
+        <v>9</v>
+      </c>
+      <c r="S264" s="14">
+        <v>0</v>
+      </c>
+      <c r="T264" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="265" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A265" s="11">
+        <v>45882</v>
+      </c>
+      <c r="B265" s="11">
+        <v>45881</v>
+      </c>
+      <c r="C265" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D265" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="E265" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="F265" s="12">
+        <v>68502</v>
+      </c>
+      <c r="G265" s="12" t="s">
+        <v>321</v>
+      </c>
+      <c r="H265" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="I265" s="13">
+        <f>NETWORKDAYS(B265, A265)</f>
+        <v>2</v>
+      </c>
+      <c r="J265" s="12">
+        <v>66675</v>
+      </c>
+      <c r="K265" s="52">
+        <v>11783</v>
+      </c>
+      <c r="L265" s="12" t="s">
+        <v>373</v>
+      </c>
+      <c r="M265" s="11">
+        <v>45891</v>
+      </c>
+      <c r="N265" s="14">
+        <v>227.88</v>
+      </c>
+      <c r="O265" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="P265" s="12">
+        <v>28</v>
+      </c>
+      <c r="Q265" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="R265" s="52">
+        <f>DATEDIF(Tabela1[[#This Row],[Atendimento]],Tabela1[[#This Row],[Previsao de Entrega]],"D")</f>
+        <v>9</v>
+      </c>
+      <c r="S265" s="14">
+        <v>0</v>
+      </c>
+      <c r="T265" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="266" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A266" s="11">
+        <v>45882</v>
+      </c>
+      <c r="B266" s="11">
+        <v>45882</v>
+      </c>
+      <c r="C266" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D266" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="E266" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="F266" s="12">
+        <v>68507</v>
+      </c>
+      <c r="G266" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="H266" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="I266" s="13">
+        <f>NETWORKDAYS(B266, A266)</f>
+        <v>1</v>
+      </c>
+      <c r="J266" s="12">
+        <v>66681</v>
+      </c>
+      <c r="K266" s="52">
+        <v>10627</v>
+      </c>
+      <c r="L266" s="12" t="s">
+        <v>362</v>
+      </c>
+      <c r="M266" s="11">
+        <v>45890</v>
+      </c>
+      <c r="N266" s="14">
+        <v>850</v>
+      </c>
+      <c r="O266" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="P266" s="12">
+        <v>28</v>
+      </c>
+      <c r="Q266" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="R266" s="52">
+        <f>DATEDIF(Tabela1[[#This Row],[Atendimento]],Tabela1[[#This Row],[Previsao de Entrega]],"D")</f>
+        <v>8</v>
+      </c>
+      <c r="S266" s="14">
+        <v>0</v>
+      </c>
+      <c r="T266" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="267" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A267" s="6">
+        <v>45882</v>
+      </c>
+      <c r="B267" s="6">
+        <v>45882</v>
+      </c>
+      <c r="C267" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D267" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E267" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="F267" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="G267" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="H267" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="I267" s="10">
+        <f>NETWORKDAYS(B267, A267)</f>
+        <v>1</v>
+      </c>
+      <c r="J267" s="7">
+        <v>65768</v>
+      </c>
+      <c r="K267" s="50">
+        <v>175</v>
+      </c>
+      <c r="L267" s="7" t="s">
+        <v>188</v>
+      </c>
+      <c r="M267" s="6">
+        <v>45882</v>
+      </c>
+      <c r="N267" s="8">
+        <v>3685</v>
+      </c>
+      <c r="O267" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="P267" s="7">
+        <v>30</v>
+      </c>
+      <c r="Q267" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="R267" s="50">
+        <f>DATEDIF(Tabela1[[#This Row],[Atendimento]],Tabela1[[#This Row],[Previsao de Entrega]],"D")</f>
+        <v>0</v>
+      </c>
+      <c r="S267" s="8">
+        <v>0</v>
+      </c>
+      <c r="T267" s="8">
+        <v>191</v>
       </c>
     </row>
   </sheetData>
@@ -19013,7 +19543,7 @@
       </c>
       <c r="E2" s="24">
         <f t="shared" ref="E2:E6" ca="1" si="0">TODAY()</f>
-        <v>45881</v>
+        <v>45882</v>
       </c>
       <c r="F2" s="22" t="str">
         <f ca="1">IF(Tabela4[[#This Row],[Hoje]] &lt;= Tabela4[[#This Row],[Validade]],
@@ -19021,7 +19551,7 @@
       "Negociar",
       "Faltam " &amp; DATEDIF(Tabela4[[#This Row],[Hoje]],Tabela4[[#This Row],[Validade]],"D") &amp; " dias para vencer"),
    "Venceu há " &amp; DATEDIF(Tabela4[[#This Row],[Validade]],Tabela4[[#This Row],[Hoje]],"D") &amp; " dias")</f>
-        <v>Faltam 585 dias para vencer</v>
+        <v>Faltam 584 dias para vencer</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.35">
@@ -19039,7 +19569,7 @@
       </c>
       <c r="E3" s="26">
         <f t="shared" ca="1" si="0"/>
-        <v>45881</v>
+        <v>45882</v>
       </c>
       <c r="F3" s="21" t="str">
         <f ca="1">IF(Tabela4[[#This Row],[Hoje]] &lt;= Tabela4[[#This Row],[Validade]],
@@ -19047,7 +19577,7 @@
       "Negociar",
       "Faltam " &amp; DATEDIF(Tabela4[[#This Row],[Hoje]],Tabela4[[#This Row],[Validade]],"D") &amp; " dias para vencer"),
    "Venceu há " &amp; DATEDIF(Tabela4[[#This Row],[Validade]],Tabela4[[#This Row],[Hoje]],"D") &amp; " dias")</f>
-        <v>Venceu há 315 dias</v>
+        <v>Venceu há 316 dias</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.35">
@@ -19065,7 +19595,7 @@
       </c>
       <c r="E4" s="32">
         <f t="shared" ca="1" si="0"/>
-        <v>45881</v>
+        <v>45882</v>
       </c>
       <c r="F4" s="33" t="str">
         <f ca="1">IF(Tabela4[[#This Row],[Hoje]] &lt;= Tabela4[[#This Row],[Validade]],
@@ -19073,7 +19603,7 @@
       "Negociar",
       "Faltam " &amp; DATEDIF(Tabela4[[#This Row],[Hoje]],Tabela4[[#This Row],[Validade]],"D") &amp; " dias para vencer"),
    "Venceu há " &amp; DATEDIF(Tabela4[[#This Row],[Validade]],Tabela4[[#This Row],[Hoje]],"D") &amp; " dias")</f>
-        <v>Venceu há 23 dias</v>
+        <v>Venceu há 24 dias</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.35">
@@ -19091,7 +19621,7 @@
       </c>
       <c r="E5" s="17">
         <f t="shared" ca="1" si="0"/>
-        <v>45881</v>
+        <v>45882</v>
       </c>
       <c r="F5" s="3" t="str">
         <f ca="1">IF(Tabela4[[#This Row],[Hoje]] &lt;= Tabela4[[#This Row],[Validade]],
@@ -19117,7 +19647,7 @@
       </c>
       <c r="E6" s="17">
         <f t="shared" ca="1" si="0"/>
-        <v>45881</v>
+        <v>45882</v>
       </c>
       <c r="F6" s="3" t="str">
         <f ca="1">IF(Tabela4[[#This Row],[Hoje]] &lt;= Tabela4[[#This Row],[Validade]],
@@ -19143,7 +19673,7 @@
       </c>
       <c r="E7" s="26">
         <f t="shared" ref="E7:E9" ca="1" si="1">TODAY()</f>
-        <v>45881</v>
+        <v>45882</v>
       </c>
       <c r="F7" s="21" t="str">
         <f ca="1">IF(Tabela4[[#This Row],[Hoje]] &lt;= Tabela4[[#This Row],[Validade]],
@@ -19151,7 +19681,7 @@
       "Negociar",
       "Faltam " &amp; DATEDIF(Tabela4[[#This Row],[Hoje]],Tabela4[[#This Row],[Validade]],"D") &amp; " dias para vencer"),
    "Venceu há " &amp; DATEDIF(Tabela4[[#This Row],[Validade]],Tabela4[[#This Row],[Hoje]],"D") &amp; " dias")</f>
-        <v>Venceu há 147 dias</v>
+        <v>Venceu há 148 dias</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.35">
@@ -19169,7 +19699,7 @@
       </c>
       <c r="E8" s="26">
         <f t="shared" ca="1" si="1"/>
-        <v>45881</v>
+        <v>45882</v>
       </c>
       <c r="F8" s="21" t="str">
         <f ca="1">IF(Tabela4[[#This Row],[Hoje]] &lt;= Tabela4[[#This Row],[Validade]],
@@ -19177,7 +19707,7 @@
       "Negociar",
       "Faltam " &amp; DATEDIF(Tabela4[[#This Row],[Hoje]],Tabela4[[#This Row],[Validade]],"D") &amp; " dias para vencer"),
    "Venceu há " &amp; DATEDIF(Tabela4[[#This Row],[Validade]],Tabela4[[#This Row],[Hoje]],"D") &amp; " dias")</f>
-        <v>Venceu há 890 dias</v>
+        <v>Venceu há 891 dias</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.35">
@@ -19195,7 +19725,7 @@
       </c>
       <c r="E9" s="24">
         <f t="shared" ca="1" si="1"/>
-        <v>45881</v>
+        <v>45882</v>
       </c>
       <c r="F9" s="22" t="str">
         <f ca="1">IF(Tabela4[[#This Row],[Hoje]] &lt;= Tabela4[[#This Row],[Validade]],
@@ -19203,7 +19733,7 @@
       "Negociar",
       "Faltam " &amp; DATEDIF(Tabela4[[#This Row],[Hoje]],Tabela4[[#This Row],[Validade]],"D") &amp; " dias para vencer"),
    "Venceu há " &amp; DATEDIF(Tabela4[[#This Row],[Validade]],Tabela4[[#This Row],[Hoje]],"D") &amp; " dias")</f>
-        <v>Faltam 401 dias para vencer</v>
+        <v>Faltam 400 dias para vencer</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.35">
@@ -19221,7 +19751,7 @@
       </c>
       <c r="E10" s="24">
         <f ca="1">TODAY()</f>
-        <v>45881</v>
+        <v>45882</v>
       </c>
       <c r="F10" s="22" t="str">
         <f ca="1">IF(Tabela4[[#This Row],[Hoje]] &lt;= Tabela4[[#This Row],[Validade]],
@@ -19229,7 +19759,7 @@
       "Negociar",
       "Faltam " &amp; DATEDIF(Tabela4[[#This Row],[Hoje]],Tabela4[[#This Row],[Validade]],"D") &amp; " dias para vencer"),
    "Venceu há " &amp; DATEDIF(Tabela4[[#This Row],[Validade]],Tabela4[[#This Row],[Hoje]],"D") &amp; " dias")</f>
-        <v>Faltam 322 dias para vencer</v>
+        <v>Faltam 321 dias para vencer</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.35">
@@ -19247,7 +19777,7 @@
       </c>
       <c r="E11" s="24">
         <f ca="1">TODAY()</f>
-        <v>45881</v>
+        <v>45882</v>
       </c>
       <c r="F11" s="22" t="str">
         <f ca="1">IF(Tabela4[[#This Row],[Hoje]] &lt;= Tabela4[[#This Row],[Validade]],
@@ -19255,7 +19785,7 @@
       "Negociar",
       "Faltam " &amp; DATEDIF(Tabela4[[#This Row],[Hoje]],Tabela4[[#This Row],[Validade]],"D") &amp; " dias para vencer"),
    "Venceu há " &amp; DATEDIF(Tabela4[[#This Row],[Validade]],Tabela4[[#This Row],[Hoje]],"D") &amp; " dias")</f>
-        <v>Faltam 111 dias para vencer</v>
+        <v>Faltam 110 dias para vencer</v>
       </c>
     </row>
   </sheetData>
@@ -19995,10 +20525,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CC6577E-1BBE-47C5-96B8-0E0691F59A60}">
-  <dimension ref="A1:E41"/>
+  <dimension ref="A1:E42"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+      <selection activeCell="E44" sqref="E44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -20705,6 +21235,23 @@
       </c>
       <c r="E41" t="s">
         <v>410</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A42" s="17">
+        <v>45882</v>
+      </c>
+      <c r="B42" t="s">
+        <v>286</v>
+      </c>
+      <c r="C42" t="s">
+        <v>287</v>
+      </c>
+      <c r="D42">
+        <v>11796</v>
+      </c>
+      <c r="E42" t="s">
+        <v>411</v>
       </c>
     </row>
   </sheetData>
@@ -20765,9 +21312,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -20897,26 +21447,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{258E5A34-0198-4570-927D-9873053383F0}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F1DB20CA-6C9E-462A-9B1E-209C1B3156BD}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="b7545978-8353-4157-ab02-92f5c69a97d9"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -20940,9 +21479,17 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F1DB20CA-6C9E-462A-9B1E-209C1B3156BD}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{258E5A34-0198-4570-927D-9873053383F0}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="b7545978-8353-4157-ab02-92f5c69a97d9"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Atualização de Base = 15/08
</commit_message>
<xml_diff>
--- a/Atendimento.xlsx
+++ b/Atendimento.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\PUBLICO\Compras\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\splfps01\data$\GROUP\PUBLICO\Compras\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F253B68B-F7EB-40B5-B748-62BFDAD2826A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A07F3F46-CE99-4938-A209-24B41561AA8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -76,7 +76,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2658" uniqueCount="413">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2729" uniqueCount="420">
   <si>
     <t>SC</t>
   </si>
@@ -1254,67 +1254,88 @@
     <t>Previsao de Entrega</t>
   </si>
   <si>
+    <t>PERTEC PERFIL TÉCNICO</t>
+  </si>
+  <si>
+    <t>indiretos</t>
+  </si>
+  <si>
+    <t>Thais Spena</t>
+  </si>
+  <si>
+    <t>TRAYES PRODUÇÕES E CENOGRAFIA</t>
+  </si>
+  <si>
+    <t>ELTRON COMERCIAL DE FERRAMENTAS LTDA</t>
+  </si>
+  <si>
+    <t>DALLANESE COM.E MANUF.DE PARAFUSOS LTDA</t>
+  </si>
+  <si>
+    <t>YESCODE AUTOMACAO LTDA - ME</t>
+  </si>
+  <si>
+    <t>CADSERVICE PRODUTOS ELETRONICOS LTDA</t>
+  </si>
+  <si>
+    <t>CARBOROIL COMERCIO DE DERIVADOS DE PETROLEO LTDA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">INDUSTRIA E COMERCIO DE MOLAS CASA VERDE LTDA </t>
+  </si>
+  <si>
+    <t>INDUSTRIA E COMERCIO DE MOLAS CASA VERDE LTDA</t>
+  </si>
+  <si>
+    <t>Geovana</t>
+  </si>
+  <si>
+    <t>LOCALIZA RENT A CAR AS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HOTELARIA ACCOR BRASIL SA </t>
+  </si>
+  <si>
+    <t>METALEX FERRAMENTARIA INDUSTRIA E COMERCIO LTDA</t>
+  </si>
+  <si>
+    <t>Gabriela</t>
+  </si>
+  <si>
+    <t>C T MOL PINTURAS LTDA – ME</t>
+  </si>
+  <si>
+    <t>PALACIO DAS FERRAMENTAS E PARAFUSOS LTDA</t>
+  </si>
+  <si>
+    <t>PULIRE INDUSTRIA E COMERCIO DE MATERIAIS DE LIMPEZA EIRELI</t>
+  </si>
+  <si>
+    <t>AGUARDANDO PAGAMENTO</t>
+  </si>
+  <si>
+    <t>Thais</t>
+  </si>
+  <si>
+    <t>FOTON TEM CONSULTORIA E PRODUCAO LTDA</t>
+  </si>
+  <si>
+    <t>AGUARDANDO APROVAÇÃO</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>logistica</t>
+  </si>
+  <si>
+    <t>TRANSLIGUE TRANSPORTES E SERVICOS LTDA</t>
+  </si>
+  <si>
+    <t>GARCIQUIMICA COM.PRODS.QUIMICOS LTDA</t>
+  </si>
+  <si>
     <t>Razao Social</t>
-  </si>
-  <si>
-    <t>PERTEC PERFIL TÉCNICO</t>
-  </si>
-  <si>
-    <t>indiretos</t>
-  </si>
-  <si>
-    <t>Thais Spena</t>
-  </si>
-  <si>
-    <t>TRAYES PRODUÇÕES E CENOGRAFIA</t>
-  </si>
-  <si>
-    <t>ELTRON COMERCIAL DE FERRAMENTAS LTDA</t>
-  </si>
-  <si>
-    <t>DALLANESE COM.E MANUF.DE PARAFUSOS LTDA</t>
-  </si>
-  <si>
-    <t>YESCODE AUTOMACAO LTDA - ME</t>
-  </si>
-  <si>
-    <t>CADSERVICE PRODUTOS ELETRONICOS LTDA</t>
-  </si>
-  <si>
-    <t>CARBOROIL COMERCIO DE DERIVADOS DE PETROLEO LTDA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">INDUSTRIA E COMERCIO DE MOLAS CASA VERDE LTDA </t>
-  </si>
-  <si>
-    <t>INDUSTRIA E COMERCIO DE MOLAS CASA VERDE LTDA</t>
-  </si>
-  <si>
-    <t>Geovana</t>
-  </si>
-  <si>
-    <t>LOCALIZA RENT A CAR AS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HOTELARIA ACCOR BRASIL SA </t>
-  </si>
-  <si>
-    <t>AGUARDANDO APROVAÇÃO</t>
-  </si>
-  <si>
-    <t>METALEX FERRAMENTARIA INDUSTRIA E COMERCIO LTDA</t>
-  </si>
-  <si>
-    <t>Gabriela</t>
-  </si>
-  <si>
-    <t>C T MOL PINTURAS LTDA – ME</t>
-  </si>
-  <si>
-    <t>PALACIO DAS FERRAMENTAS E PARAFUSOS LTDA</t>
-  </si>
-  <si>
-    <t>PULIRE INDUSTRIA E COMERCIO DE MATERIAIS DE LIMPEZA EIRELI</t>
   </si>
 </sst>
 </file>
@@ -1381,7 +1402,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1415,12 +1436,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1464,7 +1479,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1573,6 +1588,18 @@
     <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="14" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1585,16 +1612,7 @@
     <xf numFmtId="44" fontId="0" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1778,17 +1796,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0C573FEE-B8A0-4FE7-911C-81B026DE4530}" name="Tabela1" displayName="Tabela1" ref="A1:T267" totalsRowShown="0" headerRowDxfId="36" dataDxfId="35">
-  <autoFilter ref="A1:T267" xr:uid="{0C573FEE-B8A0-4FE7-911C-81B026DE4530}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0C573FEE-B8A0-4FE7-911C-81B026DE4530}" name="Tabela1" displayName="Tabela1" ref="A1:T275" totalsRowShown="0" headerRowDxfId="36" dataDxfId="35">
+  <autoFilter ref="A1:T275" xr:uid="{0C573FEE-B8A0-4FE7-911C-81B026DE4530}">
     <filterColumn colId="16">
       <filters>
         <filter val="AGUARDANDO APROVAÇÃO"/>
         <filter val="AGUARDANDO ENTREGA"/>
+        <filter val="AGUARDANDO PAGAMENTO"/>
       </filters>
     </filterColumn>
   </autoFilter>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A11:T259">
-    <sortCondition ref="M1:M259"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A11:T271">
+    <sortCondition ref="M1:M271"/>
   </sortState>
   <tableColumns count="20">
     <tableColumn id="1" xr3:uid="{FD977268-8F92-4E92-82D7-959136F54294}" name="Atendimento" dataDxfId="34"/>
@@ -1858,13 +1877,7 @@
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{78239A7E-FC7B-49B4-8A55-E7BC213AA07B}" name="Tabela3" displayName="Tabela3" ref="A1:E24" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
-  <autoFilter ref="A1:E24" xr:uid="{78239A7E-FC7B-49B4-8A55-E7BC213AA07B}">
-    <filterColumn colId="1">
-      <filters>
-        <filter val="MRO - Ferramentas"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:E24" xr:uid="{78239A7E-FC7B-49B4-8A55-E7BC213AA07B}"/>
   <tableColumns count="5">
     <tableColumn id="2" xr3:uid="{D8511443-CF4D-4DC9-8296-BF1A944D3CAC}" name="Fornecedor" dataDxfId="5"/>
     <tableColumn id="7" xr3:uid="{D2B0299B-E81C-4AF4-BF9F-2F26C1F2794A}" name="Segmento" dataDxfId="4"/>
@@ -1877,8 +1890,8 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{BB230BD9-36EF-4D37-BEB8-0438680DF5A9}" name="Tabela6" displayName="Tabela6" ref="A1:E42" totalsRowShown="0">
-  <autoFilter ref="A1:E42" xr:uid="{BB230BD9-36EF-4D37-BEB8-0438680DF5A9}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{BB230BD9-36EF-4D37-BEB8-0438680DF5A9}" name="Tabela6" displayName="Tabela6" ref="A1:E44" totalsRowShown="0">
+  <autoFilter ref="A1:E44" xr:uid="{BB230BD9-36EF-4D37-BEB8-0438680DF5A9}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{40ADAE7E-AD00-4188-9DB3-F04A606A9D2B}" name="data"/>
     <tableColumn id="2" xr3:uid="{D9B738D8-98DD-4AD6-8BCF-D51CBE71FF94}" name="solicitante"/>
@@ -2153,33 +2166,33 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T267"/>
+  <dimension ref="A1:T281"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L233" sqref="L233"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I229" sqref="I229"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="16.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.7265625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="12.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.90625" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17.81640625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.7265625" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="7.453125" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="19.7265625" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="20.1796875" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="27.81640625" style="9" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="19.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.6328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.08984375" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="76.7265625" style="1" customWidth="1"/>
-    <col min="13" max="13" width="22.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="22.36328125" style="1" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="15.26953125" style="2" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="15.81640625" style="1" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="26.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="25.1796875" style="1" customWidth="1"/>
+    <col min="17" max="17" width="25.36328125" style="1" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="26.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12.6328125" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="19.453125" style="1" bestFit="1" customWidth="1"/>
     <col min="21" max="16384" width="16.81640625" style="1"/>
   </cols>
@@ -2219,7 +2232,7 @@
         <v>106</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>392</v>
+        <v>419</v>
       </c>
       <c r="M1" s="1" t="s">
         <v>391</v>
@@ -14164,13 +14177,13 @@
         <v>5</v>
       </c>
       <c r="E188" s="6" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="F188" s="7">
         <v>68487</v>
       </c>
       <c r="G188" s="7" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="H188" s="7" t="s">
         <v>96</v>
@@ -14186,7 +14199,7 @@
         <v>11614</v>
       </c>
       <c r="L188" s="7" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="M188" s="6">
         <v>45882</v>
@@ -14406,67 +14419,67 @@
         <v>0</v>
       </c>
     </row>
-    <row r="192" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A192" s="11">
+    <row r="192" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A192" s="6">
         <v>45867</v>
       </c>
-      <c r="B192" s="11">
+      <c r="B192" s="6">
         <v>45867</v>
       </c>
-      <c r="C192" s="11" t="s">
+      <c r="C192" s="6" t="s">
         <v>128</v>
       </c>
-      <c r="D192" s="11" t="s">
+      <c r="D192" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="E192" s="11" t="s">
+      <c r="E192" s="6" t="s">
         <v>113</v>
       </c>
-      <c r="F192" s="12">
+      <c r="F192" s="7">
         <v>68486</v>
       </c>
-      <c r="G192" s="12" t="s">
+      <c r="G192" s="7" t="s">
         <v>296</v>
       </c>
-      <c r="H192" s="12" t="s">
+      <c r="H192" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="I192" s="13">
+      <c r="I192" s="10">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="J192" s="12">
+      <c r="J192" s="7">
         <v>66478</v>
       </c>
-      <c r="K192" s="12">
+      <c r="K192" s="7">
         <v>10460</v>
       </c>
-      <c r="L192" s="12" t="s">
-        <v>393</v>
-      </c>
-      <c r="M192" s="11">
+      <c r="L192" s="7" t="s">
+        <v>392</v>
+      </c>
+      <c r="M192" s="6">
         <v>45883</v>
       </c>
-      <c r="N192" s="14">
+      <c r="N192" s="8">
         <v>4789.6099999999997</v>
       </c>
-      <c r="O192" s="12" t="s">
+      <c r="O192" s="7" t="s">
         <v>122</v>
       </c>
-      <c r="P192" s="12">
+      <c r="P192" s="7">
         <v>28</v>
       </c>
-      <c r="Q192" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="R192" s="12">
+      <c r="Q192" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="R192" s="7">
         <f>DATEDIF(Tabela1[[#This Row],[Atendimento]],Tabela1[[#This Row],[Previsao de Entrega]],"D")</f>
         <v>16</v>
       </c>
-      <c r="S192" s="14">
+      <c r="S192" s="8">
         <v>1080.08</v>
       </c>
-      <c r="T192" s="14">
+      <c r="T192" s="8">
         <v>0</v>
       </c>
     </row>
@@ -15136,7 +15149,7 @@
         <v>32</v>
       </c>
       <c r="I203" s="10">
-        <f t="shared" ref="I203:I259" si="4">NETWORKDAYS(B203, A203)</f>
+        <f t="shared" ref="I203:I266" si="4">NETWORKDAYS(B203, A203)</f>
         <v>1</v>
       </c>
       <c r="J203" s="7">
@@ -15338,7 +15351,7 @@
         <v>9</v>
       </c>
       <c r="L206" s="7" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="M206" s="6">
         <v>45880</v>
@@ -16710,177 +16723,177 @@
         <v>0</v>
       </c>
     </row>
-    <row r="228" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A228" s="11">
+    <row r="228" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A228" s="6">
+        <v>45882</v>
+      </c>
+      <c r="B228" s="6">
+        <v>45880</v>
+      </c>
+      <c r="C228" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D228" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E228" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="F228" s="7">
+        <v>68499</v>
+      </c>
+      <c r="G228" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="H228" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="I228" s="10">
+        <f t="shared" si="4"/>
+        <v>3</v>
+      </c>
+      <c r="J228" s="7">
+        <v>66671</v>
+      </c>
+      <c r="K228" s="7">
+        <v>1277</v>
+      </c>
+      <c r="L228" s="7" t="s">
+        <v>397</v>
+      </c>
+      <c r="M228" s="6">
+        <v>45884</v>
+      </c>
+      <c r="N228" s="8">
+        <v>207.68</v>
+      </c>
+      <c r="O228" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="P228" s="7">
+        <v>35</v>
+      </c>
+      <c r="Q228" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="R228" s="7">
+        <f>DATEDIF(Tabela1[[#This Row],[Atendimento]],Tabela1[[#This Row],[Previsao de Entrega]],"D")</f>
+        <v>2</v>
+      </c>
+      <c r="S228" s="8">
+        <v>0</v>
+      </c>
+      <c r="T228" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="229" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A229" s="11">
         <v>45785</v>
       </c>
-      <c r="B228" s="11">
+      <c r="B229" s="11">
         <v>45784</v>
       </c>
-      <c r="C228" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="D228" s="11" t="s">
+      <c r="C229" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D229" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="E228" s="11" t="s">
+      <c r="E229" s="11" t="s">
         <v>113</v>
       </c>
-      <c r="F228" s="12">
+      <c r="F229" s="12">
         <v>68369</v>
       </c>
-      <c r="G228" s="12" t="s">
+      <c r="G229" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="H228" s="12" t="s">
+      <c r="H229" s="12" t="s">
         <v>98</v>
       </c>
-      <c r="I228" s="13">
+      <c r="I229" s="13">
         <f t="shared" si="4"/>
         <v>2</v>
       </c>
-      <c r="J228" s="12">
+      <c r="J229" s="12">
         <v>65234</v>
       </c>
-      <c r="K228" s="12">
+      <c r="K229" s="12">
         <v>11610</v>
       </c>
-      <c r="L228" s="12" t="s">
+      <c r="L229" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="M228" s="11">
+      <c r="M229" s="11">
         <v>45887</v>
       </c>
-      <c r="N228" s="14">
+      <c r="N229" s="14">
         <v>9114.5499999999993</v>
       </c>
-      <c r="O228" s="12" t="s">
+      <c r="O229" s="12" t="s">
         <v>122</v>
       </c>
-      <c r="P228" s="12">
+      <c r="P229" s="12">
         <v>28</v>
       </c>
-      <c r="Q228" s="12" t="s">
+      <c r="Q229" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="R228" s="12">
+      <c r="R229" s="12">
         <f>DATEDIF(Tabela1[[#This Row],[Atendimento]],Tabela1[[#This Row],[Previsao de Entrega]],"D")</f>
         <v>102</v>
       </c>
-      <c r="S228" s="14">
+      <c r="S229" s="14">
         <v>183.5</v>
       </c>
-      <c r="T228" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="229" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A229" s="11">
+      <c r="T229" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="230" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A230" s="11">
         <v>45868</v>
       </c>
-      <c r="B229" s="11">
+      <c r="B230" s="11">
         <v>45862</v>
       </c>
-      <c r="C229" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="D229" s="11" t="s">
+      <c r="C230" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D230" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="E229" s="11" t="s">
+      <c r="E230" s="11" t="s">
         <v>113</v>
       </c>
-      <c r="F229" s="12">
+      <c r="F230" s="12">
         <v>68476</v>
       </c>
-      <c r="G229" s="12" t="s">
+      <c r="G230" s="12" t="s">
         <v>227</v>
       </c>
-      <c r="H229" s="12" t="s">
+      <c r="H230" s="12" t="s">
         <v>98</v>
       </c>
-      <c r="I229" s="13">
+      <c r="I230" s="13">
         <f t="shared" si="4"/>
         <v>5</v>
       </c>
-      <c r="J229" s="12">
+      <c r="J230" s="12">
         <v>66491</v>
       </c>
-      <c r="K229" s="12">
+      <c r="K230" s="12">
         <v>11522</v>
       </c>
-      <c r="L229" s="12" t="s">
+      <c r="L230" s="12" t="s">
         <v>376</v>
-      </c>
-      <c r="M229" s="11">
-        <v>45888</v>
-      </c>
-      <c r="N229" s="14">
-        <v>1680.4</v>
-      </c>
-      <c r="O229" s="12" t="s">
-        <v>122</v>
-      </c>
-      <c r="P229" s="12">
-        <v>28</v>
-      </c>
-      <c r="Q229" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="R229" s="12">
-        <f>DATEDIF(Tabela1[[#This Row],[Atendimento]],Tabela1[[#This Row],[Previsao de Entrega]],"D")</f>
-        <v>20</v>
-      </c>
-      <c r="S229" s="14">
-        <v>0</v>
-      </c>
-      <c r="T229" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="230" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A230" s="11">
-        <v>45881</v>
-      </c>
-      <c r="B230" s="11">
-        <v>45880</v>
-      </c>
-      <c r="C230" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="D230" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="E230" s="11" t="s">
-        <v>113</v>
-      </c>
-      <c r="F230" s="12">
-        <v>68500</v>
-      </c>
-      <c r="G230" s="12" t="s">
-        <v>371</v>
-      </c>
-      <c r="H230" s="12" t="s">
-        <v>372</v>
-      </c>
-      <c r="I230" s="13">
-        <f t="shared" si="4"/>
-        <v>2</v>
-      </c>
-      <c r="J230" s="12">
-        <v>66660</v>
-      </c>
-      <c r="K230" s="12">
-        <v>160</v>
-      </c>
-      <c r="L230" s="12" t="s">
-        <v>201</v>
       </c>
       <c r="M230" s="11">
         <v>45888</v>
       </c>
       <c r="N230" s="14">
-        <v>524.1</v>
+        <v>1680.4</v>
       </c>
       <c r="O230" s="12" t="s">
         <v>122</v>
@@ -16893,7 +16906,7 @@
       </c>
       <c r="R230" s="12">
         <f>DATEDIF(Tabela1[[#This Row],[Atendimento]],Tabela1[[#This Row],[Previsao de Entrega]],"D")</f>
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="S230" s="14">
         <v>0</v>
@@ -16938,7 +16951,7 @@
         <v>10556</v>
       </c>
       <c r="L231" s="7" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="M231" s="6">
         <v>45877</v>
@@ -16968,10 +16981,10 @@
     </row>
     <row r="232" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A232" s="11">
-        <v>45870</v>
+        <v>45881</v>
       </c>
       <c r="B232" s="11">
-        <v>45863</v>
+        <v>45880</v>
       </c>
       <c r="C232" s="11" t="s">
         <v>7</v>
@@ -16983,45 +16996,45 @@
         <v>113</v>
       </c>
       <c r="F232" s="12">
-        <v>68482</v>
+        <v>68500</v>
       </c>
       <c r="G232" s="12" t="s">
-        <v>129</v>
+        <v>371</v>
       </c>
       <c r="H232" s="12" t="s">
-        <v>130</v>
+        <v>372</v>
       </c>
       <c r="I232" s="13">
         <f t="shared" si="4"/>
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="J232" s="12">
-        <v>66522</v>
+        <v>66660</v>
       </c>
       <c r="K232" s="12">
-        <v>679</v>
+        <v>160</v>
       </c>
       <c r="L232" s="12" t="s">
-        <v>346</v>
+        <v>201</v>
       </c>
       <c r="M232" s="11">
-        <v>45889</v>
+        <v>45888</v>
       </c>
       <c r="N232" s="14">
-        <v>6048.2</v>
+        <v>524.1</v>
       </c>
       <c r="O232" s="12" t="s">
         <v>122</v>
       </c>
       <c r="P232" s="12">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="Q232" s="12" t="s">
         <v>24</v>
       </c>
       <c r="R232" s="12">
         <f>DATEDIF(Tabela1[[#This Row],[Atendimento]],Tabela1[[#This Row],[Previsao de Entrega]],"D")</f>
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="S232" s="14">
         <v>0</v>
@@ -17031,258 +17044,258 @@
       </c>
     </row>
     <row r="233" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A233" s="41">
-        <v>45826</v>
-      </c>
-      <c r="B233" s="41">
-        <v>45826</v>
-      </c>
-      <c r="C233" s="41" t="s">
-        <v>7</v>
-      </c>
-      <c r="D233" s="41" t="s">
+      <c r="A233" s="11">
+        <v>45870</v>
+      </c>
+      <c r="B233" s="11">
+        <v>45863</v>
+      </c>
+      <c r="C233" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D233" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="E233" s="41" t="s">
-        <v>124</v>
-      </c>
-      <c r="F233" s="42" t="s">
-        <v>3</v>
-      </c>
-      <c r="G233" s="42" t="s">
-        <v>125</v>
-      </c>
-      <c r="H233" s="42" t="s">
-        <v>126</v>
+      <c r="E233" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="F233" s="12">
+        <v>68482</v>
+      </c>
+      <c r="G233" s="12" t="s">
+        <v>129</v>
+      </c>
+      <c r="H233" s="12" t="s">
+        <v>130</v>
       </c>
       <c r="I233" s="13">
         <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="J233" s="42">
-        <v>66341</v>
-      </c>
-      <c r="K233" s="42">
-        <v>11758</v>
-      </c>
-      <c r="L233" s="42" t="s">
-        <v>316</v>
-      </c>
-      <c r="M233" s="41">
-        <v>45891</v>
-      </c>
-      <c r="N233" s="43">
-        <v>924.61</v>
-      </c>
-      <c r="O233" s="42" t="s">
+        <v>6</v>
+      </c>
+      <c r="J233" s="12">
+        <v>66522</v>
+      </c>
+      <c r="K233" s="12">
+        <v>679</v>
+      </c>
+      <c r="L233" s="12" t="s">
+        <v>346</v>
+      </c>
+      <c r="M233" s="11">
+        <v>45889</v>
+      </c>
+      <c r="N233" s="14">
+        <v>6048.2</v>
+      </c>
+      <c r="O233" s="12" t="s">
         <v>122</v>
       </c>
-      <c r="P233" s="42">
-        <v>28</v>
-      </c>
-      <c r="Q233" s="42" t="s">
+      <c r="P233" s="12">
+        <v>30</v>
+      </c>
+      <c r="Q233" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="R233" s="42">
-        <f>DATEDIF(Tabela1[[#This Row],[Atendimento]],Tabela1[[#This Row],[Previsao de Entrega]],"D")</f>
-        <v>65</v>
-      </c>
-      <c r="S233" s="43">
-        <v>0</v>
-      </c>
-      <c r="T233" s="43">
+      <c r="R233" s="12">
+        <f>DATEDIF(Tabela1[[#This Row],[Atendimento]],Tabela1[[#This Row],[Previsao de Entrega]],"D")</f>
+        <v>19</v>
+      </c>
+      <c r="S233" s="14">
+        <v>0</v>
+      </c>
+      <c r="T233" s="14">
         <v>0</v>
       </c>
     </row>
     <row r="234" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A234" s="11">
-        <v>45877</v>
-      </c>
-      <c r="B234" s="11">
-        <v>45877</v>
-      </c>
-      <c r="C234" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="D234" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="E234" s="11" t="s">
+      <c r="A234" s="46">
+        <v>45882</v>
+      </c>
+      <c r="B234" s="46">
+        <v>45880</v>
+      </c>
+      <c r="C234" s="46" t="s">
+        <v>7</v>
+      </c>
+      <c r="D234" s="46" t="s">
+        <v>15</v>
+      </c>
+      <c r="E234" s="46" t="s">
         <v>113</v>
       </c>
-      <c r="F234" s="12">
-        <v>68458</v>
-      </c>
-      <c r="G234" s="12" t="s">
-        <v>227</v>
-      </c>
-      <c r="H234" s="12" t="s">
-        <v>98</v>
-      </c>
-      <c r="I234" s="13">
+      <c r="F234" s="47">
+        <v>68498</v>
+      </c>
+      <c r="G234" s="47" t="s">
+        <v>321</v>
+      </c>
+      <c r="H234" s="47" t="s">
+        <v>91</v>
+      </c>
+      <c r="I234" s="48">
+        <f t="shared" si="4"/>
+        <v>3</v>
+      </c>
+      <c r="J234" s="47">
+        <v>66670</v>
+      </c>
+      <c r="K234" s="47">
+        <v>11796</v>
+      </c>
+      <c r="L234" s="47" t="s">
+        <v>409</v>
+      </c>
+      <c r="M234" s="46">
+        <v>45890</v>
+      </c>
+      <c r="N234" s="49">
+        <v>42.23</v>
+      </c>
+      <c r="O234" s="47" t="s">
+        <v>121</v>
+      </c>
+      <c r="P234" s="47">
+        <v>0</v>
+      </c>
+      <c r="Q234" s="47" t="s">
+        <v>411</v>
+      </c>
+      <c r="R234" s="47">
+        <f>DATEDIF(Tabela1[[#This Row],[Atendimento]],Tabela1[[#This Row],[Previsao de Entrega]],"D")</f>
+        <v>8</v>
+      </c>
+      <c r="S234" s="49">
+        <v>0</v>
+      </c>
+      <c r="T234" s="49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="235" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A235" s="11">
+        <v>45882</v>
+      </c>
+      <c r="B235" s="11">
+        <v>45882</v>
+      </c>
+      <c r="C235" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D235" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="E235" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="F235" s="12">
+        <v>68507</v>
+      </c>
+      <c r="G235" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="H235" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="I235" s="13">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="J234" s="12">
-        <v>66605</v>
-      </c>
-      <c r="K234" s="12">
-        <v>561</v>
-      </c>
-      <c r="L234" s="12" t="s">
-        <v>324</v>
-      </c>
-      <c r="M234" s="11">
-        <v>45891</v>
-      </c>
-      <c r="N234" s="14">
-        <v>758.53</v>
-      </c>
-      <c r="O234" s="12" t="s">
-        <v>122</v>
-      </c>
-      <c r="P234" s="12">
-        <v>28</v>
-      </c>
-      <c r="Q234" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="R234" s="12">
-        <f>DATEDIF(Tabela1[[#This Row],[Atendimento]],Tabela1[[#This Row],[Previsao de Entrega]],"D")</f>
-        <v>14</v>
-      </c>
-      <c r="S234" s="14">
-        <v>0</v>
-      </c>
-      <c r="T234" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="235" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A235" s="11">
-        <v>45880</v>
-      </c>
-      <c r="B235" s="11">
-        <v>45868</v>
-      </c>
-      <c r="C235" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="D235" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="E235" s="11" t="s">
-        <v>113</v>
-      </c>
-      <c r="F235" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="G235" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="H235" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="I235" s="13">
-        <f t="shared" si="4"/>
-        <v>9</v>
-      </c>
       <c r="J235" s="12">
-        <v>66629</v>
+        <v>66681</v>
       </c>
       <c r="K235" s="12">
-        <v>11121</v>
+        <v>10627</v>
       </c>
       <c r="L235" s="12" t="s">
-        <v>143</v>
+        <v>362</v>
       </c>
       <c r="M235" s="11">
-        <v>45894</v>
+        <v>45890</v>
       </c>
       <c r="N235" s="14">
-        <v>1242.04</v>
+        <v>850</v>
       </c>
       <c r="O235" s="12" t="s">
         <v>122</v>
       </c>
       <c r="P235" s="12">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="Q235" s="12" t="s">
         <v>24</v>
       </c>
       <c r="R235" s="12">
         <f>DATEDIF(Tabela1[[#This Row],[Atendimento]],Tabela1[[#This Row],[Previsao de Entrega]],"D")</f>
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="S235" s="14">
-        <v>108</v>
+        <v>0</v>
       </c>
       <c r="T235" s="14">
         <v>0</v>
       </c>
     </row>
     <row r="236" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A236" s="11">
-        <v>45881</v>
-      </c>
-      <c r="B236" s="11">
-        <v>45881</v>
-      </c>
-      <c r="C236" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="D236" s="11" t="s">
+      <c r="A236" s="41">
+        <v>45826</v>
+      </c>
+      <c r="B236" s="41">
+        <v>45826</v>
+      </c>
+      <c r="C236" s="41" t="s">
+        <v>7</v>
+      </c>
+      <c r="D236" s="41" t="s">
         <v>15</v>
       </c>
-      <c r="E236" s="11" t="s">
+      <c r="E236" s="41" t="s">
         <v>124</v>
       </c>
-      <c r="F236" s="12">
-        <v>68501</v>
-      </c>
-      <c r="G236" s="12" t="s">
-        <v>90</v>
-      </c>
-      <c r="H236" s="12" t="s">
-        <v>91</v>
+      <c r="F236" s="42" t="s">
+        <v>3</v>
+      </c>
+      <c r="G236" s="42" t="s">
+        <v>125</v>
+      </c>
+      <c r="H236" s="42" t="s">
+        <v>126</v>
       </c>
       <c r="I236" s="13">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="J236" s="12">
-        <v>66662</v>
-      </c>
-      <c r="K236" s="12">
-        <v>3040</v>
-      </c>
-      <c r="L236" s="12" t="s">
-        <v>214</v>
-      </c>
-      <c r="M236" s="11">
-        <v>45896</v>
-      </c>
-      <c r="N236" s="14">
-        <v>1000</v>
-      </c>
-      <c r="O236" s="12" t="s">
+      <c r="J236" s="42">
+        <v>66341</v>
+      </c>
+      <c r="K236" s="42">
+        <v>11758</v>
+      </c>
+      <c r="L236" s="42" t="s">
+        <v>316</v>
+      </c>
+      <c r="M236" s="41">
+        <v>45891</v>
+      </c>
+      <c r="N236" s="43">
+        <v>924.61</v>
+      </c>
+      <c r="O236" s="42" t="s">
         <v>122</v>
       </c>
-      <c r="P236" s="12">
-        <v>30</v>
-      </c>
-      <c r="Q236" s="12" t="s">
+      <c r="P236" s="42">
+        <v>28</v>
+      </c>
+      <c r="Q236" s="42" t="s">
         <v>24</v>
       </c>
-      <c r="R236" s="12">
-        <f>DATEDIF(Tabela1[[#This Row],[Atendimento]],Tabela1[[#This Row],[Previsao de Entrega]],"D")</f>
-        <v>15</v>
-      </c>
-      <c r="S236" s="14">
-        <v>0</v>
-      </c>
-      <c r="T236" s="14">
+      <c r="R236" s="42">
+        <f>DATEDIF(Tabela1[[#This Row],[Atendimento]],Tabela1[[#This Row],[Previsao de Entrega]],"D")</f>
+        <v>65</v>
+      </c>
+      <c r="S236" s="43">
+        <v>0</v>
+      </c>
+      <c r="T236" s="43">
         <v>0</v>
       </c>
     </row>
@@ -17322,7 +17335,7 @@
         <v>11790</v>
       </c>
       <c r="L237" s="7" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="M237" s="6">
         <v>45873</v>
@@ -17386,7 +17399,7 @@
         <v>2856</v>
       </c>
       <c r="L238" s="7" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="M238" s="6">
         <v>45875</v>
@@ -17498,7 +17511,7 @@
         <v>3</v>
       </c>
       <c r="G240" s="7" t="s">
-        <v>129</v>
+        <v>3</v>
       </c>
       <c r="H240" s="7" t="s">
         <v>130</v>
@@ -17736,63 +17749,63 @@
     </row>
     <row r="244" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A244" s="11">
-        <v>45868</v>
+        <v>45877</v>
       </c>
       <c r="B244" s="11">
-        <v>45868</v>
+        <v>45877</v>
       </c>
       <c r="C244" s="11" t="s">
         <v>7</v>
       </c>
       <c r="D244" s="11" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="E244" s="11" t="s">
-        <v>124</v>
-      </c>
-      <c r="F244" s="12" t="s">
-        <v>3</v>
+        <v>113</v>
+      </c>
+      <c r="F244" s="12">
+        <v>68458</v>
       </c>
       <c r="G244" s="12" t="s">
-        <v>125</v>
+        <v>227</v>
       </c>
       <c r="H244" s="12" t="s">
-        <v>126</v>
+        <v>98</v>
       </c>
       <c r="I244" s="13">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="J244" s="12">
-        <v>66504</v>
+        <v>66605</v>
       </c>
       <c r="K244" s="12">
-        <v>3034</v>
+        <v>561</v>
       </c>
       <c r="L244" s="12" t="s">
-        <v>349</v>
+        <v>324</v>
       </c>
       <c r="M244" s="11">
-        <v>45897</v>
+        <v>45891</v>
       </c>
       <c r="N244" s="14">
-        <v>2220</v>
+        <v>758.53</v>
       </c>
       <c r="O244" s="12" t="s">
         <v>122</v>
       </c>
       <c r="P244" s="12">
-        <v>90</v>
+        <v>28</v>
       </c>
       <c r="Q244" s="12" t="s">
         <v>24</v>
       </c>
       <c r="R244" s="12">
         <f>DATEDIF(Tabela1[[#This Row],[Atendimento]],Tabela1[[#This Row],[Previsao de Entrega]],"D")</f>
-        <v>29</v>
+        <v>14</v>
       </c>
       <c r="S244" s="14">
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="T244" s="14">
         <v>0</v>
@@ -17864,10 +17877,10 @@
     </row>
     <row r="246" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A246" s="11">
-        <v>45869</v>
+        <v>45882</v>
       </c>
       <c r="B246" s="11">
-        <v>45869</v>
+        <v>45881</v>
       </c>
       <c r="C246" s="11" t="s">
         <v>7</v>
@@ -17876,51 +17889,51 @@
         <v>15</v>
       </c>
       <c r="E246" s="11" t="s">
-        <v>124</v>
-      </c>
-      <c r="F246" s="12" t="s">
-        <v>3</v>
+        <v>113</v>
+      </c>
+      <c r="F246" s="12">
+        <v>68502</v>
       </c>
       <c r="G246" s="12" t="s">
-        <v>125</v>
+        <v>321</v>
       </c>
       <c r="H246" s="12" t="s">
-        <v>126</v>
+        <v>91</v>
       </c>
       <c r="I246" s="13">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J246" s="12">
-        <v>66427</v>
+        <v>66672</v>
       </c>
       <c r="K246" s="12">
-        <v>1277</v>
+        <v>10594</v>
       </c>
       <c r="L246" s="12" t="s">
-        <v>398</v>
+        <v>410</v>
       </c>
       <c r="M246" s="11">
-        <v>45897</v>
+        <v>45891</v>
       </c>
       <c r="N246" s="14">
-        <v>2715.75</v>
+        <v>2446.5500000000002</v>
       </c>
       <c r="O246" s="12" t="s">
         <v>122</v>
       </c>
       <c r="P246" s="12">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="Q246" s="12" t="s">
         <v>24</v>
       </c>
       <c r="R246" s="12">
         <f>DATEDIF(Tabela1[[#This Row],[Atendimento]],Tabela1[[#This Row],[Previsao de Entrega]],"D")</f>
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="S246" s="14">
-        <v>950</v>
+        <v>0</v>
       </c>
       <c r="T246" s="14">
         <v>0</v>
@@ -18120,127 +18133,127 @@
     </row>
     <row r="250" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A250" s="11">
-        <v>45875</v>
+        <v>45882</v>
       </c>
       <c r="B250" s="11">
-        <v>45873</v>
+        <v>45881</v>
       </c>
       <c r="C250" s="11" t="s">
-        <v>128</v>
+        <v>7</v>
       </c>
       <c r="D250" s="11" t="s">
         <v>15</v>
       </c>
       <c r="E250" s="11" t="s">
-        <v>124</v>
-      </c>
-      <c r="F250" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="G250" s="11" t="s">
-        <v>125</v>
-      </c>
-      <c r="H250" s="11" t="s">
-        <v>126</v>
+        <v>113</v>
+      </c>
+      <c r="F250" s="12">
+        <v>68502</v>
+      </c>
+      <c r="G250" s="12" t="s">
+        <v>321</v>
+      </c>
+      <c r="H250" s="12" t="s">
+        <v>91</v>
       </c>
       <c r="I250" s="13">
         <f t="shared" si="4"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J250" s="12">
-        <v>66430</v>
+        <v>66675</v>
       </c>
       <c r="K250" s="12">
-        <v>333</v>
+        <v>11783</v>
       </c>
       <c r="L250" s="12" t="s">
-        <v>400</v>
+        <v>373</v>
       </c>
       <c r="M250" s="11">
-        <v>45901</v>
-      </c>
-      <c r="N250" s="45">
-        <v>1483685.03</v>
-      </c>
-      <c r="O250" s="11" t="s">
+        <v>45891</v>
+      </c>
+      <c r="N250" s="14">
+        <v>227.88</v>
+      </c>
+      <c r="O250" s="12" t="s">
         <v>122</v>
       </c>
       <c r="P250" s="12">
-        <v>90</v>
+        <v>28</v>
       </c>
       <c r="Q250" s="12" t="s">
         <v>24</v>
       </c>
       <c r="R250" s="12">
         <f>DATEDIF(Tabela1[[#This Row],[Atendimento]],Tabela1[[#This Row],[Previsao de Entrega]],"D")</f>
-        <v>26</v>
+        <v>9</v>
       </c>
       <c r="S250" s="14">
         <v>0</v>
       </c>
       <c r="T250" s="14">
-        <v>59008.35</v>
+        <v>0</v>
       </c>
     </row>
     <row r="251" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A251" s="11">
-        <v>45856</v>
+        <v>45883</v>
       </c>
       <c r="B251" s="11">
-        <v>45856</v>
+        <v>45882</v>
       </c>
       <c r="C251" s="11" t="s">
         <v>7</v>
       </c>
       <c r="D251" s="11" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="E251" s="11" t="s">
         <v>124</v>
       </c>
       <c r="F251" s="12">
-        <v>68466</v>
+        <v>68504</v>
       </c>
       <c r="G251" s="12" t="s">
-        <v>125</v>
+        <v>227</v>
       </c>
       <c r="H251" s="12" t="s">
-        <v>126</v>
+        <v>98</v>
       </c>
       <c r="I251" s="13">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J251" s="12">
-        <v>66337</v>
+        <v>66691</v>
       </c>
       <c r="K251" s="12">
-        <v>11736</v>
+        <v>3509</v>
       </c>
       <c r="L251" s="12" t="s">
-        <v>127</v>
+        <v>333</v>
       </c>
       <c r="M251" s="11">
-        <v>45902</v>
+        <v>45891</v>
       </c>
       <c r="N251" s="14">
-        <v>16134.54</v>
+        <v>1920</v>
       </c>
       <c r="O251" s="12" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="P251" s="12">
-        <v>28</v>
+        <v>7</v>
       </c>
       <c r="Q251" s="12" t="s">
         <v>24</v>
       </c>
       <c r="R251" s="12">
         <f>DATEDIF(Tabela1[[#This Row],[Atendimento]],Tabela1[[#This Row],[Previsao de Entrega]],"D")</f>
-        <v>46</v>
+        <v>8</v>
       </c>
       <c r="S251" s="14">
-        <v>25720</v>
+        <v>0</v>
       </c>
       <c r="T251" s="14">
         <v>0</v>
@@ -18248,10 +18261,10 @@
     </row>
     <row r="252" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A252" s="11">
-        <v>45840</v>
+        <v>45883</v>
       </c>
       <c r="B252" s="11">
-        <v>45840</v>
+        <v>45882</v>
       </c>
       <c r="C252" s="11" t="s">
         <v>7</v>
@@ -18260,48 +18273,48 @@
         <v>5</v>
       </c>
       <c r="E252" s="11" t="s">
-        <v>113</v>
+        <v>124</v>
       </c>
       <c r="F252" s="12">
-        <v>68452</v>
+        <v>68506</v>
       </c>
       <c r="G252" s="12" t="s">
-        <v>33</v>
+        <v>227</v>
       </c>
       <c r="H252" s="12" t="s">
-        <v>34</v>
+        <v>98</v>
       </c>
       <c r="I252" s="13">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J252" s="12">
-        <v>66037</v>
+        <v>66692</v>
       </c>
       <c r="K252" s="12">
-        <v>11775</v>
+        <v>3509</v>
       </c>
       <c r="L252" s="12" t="s">
-        <v>353</v>
+        <v>333</v>
       </c>
       <c r="M252" s="11">
-        <v>45905</v>
+        <v>45891</v>
       </c>
       <c r="N252" s="14">
-        <v>1750</v>
+        <v>1920</v>
       </c>
       <c r="O252" s="12" t="s">
         <v>122</v>
       </c>
       <c r="P252" s="12">
-        <v>30</v>
+        <v>7</v>
       </c>
       <c r="Q252" s="12" t="s">
         <v>24</v>
       </c>
       <c r="R252" s="12">
         <f>DATEDIF(Tabela1[[#This Row],[Atendimento]],Tabela1[[#This Row],[Previsao de Entrega]],"D")</f>
-        <v>65</v>
+        <v>8</v>
       </c>
       <c r="S252" s="14">
         <v>0</v>
@@ -18440,63 +18453,63 @@
     </row>
     <row r="255" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A255" s="11">
-        <v>45848</v>
+        <v>45883</v>
       </c>
       <c r="B255" s="11">
-        <v>45848</v>
+        <v>45874</v>
       </c>
       <c r="C255" s="11" t="s">
         <v>7</v>
       </c>
       <c r="D255" s="11" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="E255" s="11" t="s">
         <v>113</v>
       </c>
       <c r="F255" s="12">
-        <v>68457</v>
+        <v>68495</v>
       </c>
       <c r="G255" s="12" t="s">
-        <v>33</v>
+        <v>136</v>
       </c>
       <c r="H255" s="12" t="s">
-        <v>34</v>
+        <v>126</v>
       </c>
       <c r="I255" s="13">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="J255" s="12">
-        <v>66126</v>
+        <v>66694</v>
       </c>
       <c r="K255" s="12">
-        <v>2931</v>
+        <v>2289</v>
       </c>
       <c r="L255" s="12" t="s">
-        <v>366</v>
+        <v>360</v>
       </c>
       <c r="M255" s="11">
-        <v>45905</v>
+        <v>45891</v>
       </c>
       <c r="N255" s="14">
-        <v>3500</v>
+        <v>682.1</v>
       </c>
       <c r="O255" s="12" t="s">
         <v>122</v>
       </c>
       <c r="P255" s="12">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="Q255" s="12" t="s">
         <v>24</v>
       </c>
       <c r="R255" s="12">
         <f>DATEDIF(Tabela1[[#This Row],[Atendimento]],Tabela1[[#This Row],[Previsao de Entrega]],"D")</f>
-        <v>57</v>
+        <v>8</v>
       </c>
       <c r="S255" s="14">
-        <v>320</v>
+        <v>0</v>
       </c>
       <c r="T255" s="14">
         <v>0</v>
@@ -18504,10 +18517,10 @@
     </row>
     <row r="256" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A256" s="11">
-        <v>45874</v>
+        <v>45883</v>
       </c>
       <c r="B256" s="11">
-        <v>45853</v>
+        <v>45880</v>
       </c>
       <c r="C256" s="11" t="s">
         <v>7</v>
@@ -18516,51 +18529,51 @@
         <v>15</v>
       </c>
       <c r="E256" s="11" t="s">
-        <v>124</v>
+        <v>113</v>
       </c>
       <c r="F256" s="12">
-        <v>68465</v>
+        <v>68500</v>
       </c>
       <c r="G256" s="12" t="s">
-        <v>125</v>
+        <v>371</v>
       </c>
       <c r="H256" s="12" t="s">
-        <v>126</v>
+        <v>372</v>
       </c>
       <c r="I256" s="13">
         <f t="shared" si="4"/>
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="J256" s="12">
-        <v>66555</v>
+        <v>66708</v>
       </c>
       <c r="K256" s="12">
-        <v>11791</v>
+        <v>4656</v>
       </c>
       <c r="L256" s="12" t="s">
-        <v>403</v>
+        <v>70</v>
       </c>
       <c r="M256" s="11">
-        <v>45906</v>
+        <v>45891</v>
       </c>
       <c r="N256" s="14">
-        <v>1075.55</v>
+        <v>2207.7399999999998</v>
       </c>
       <c r="O256" s="12" t="s">
         <v>122</v>
       </c>
       <c r="P256" s="12">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="Q256" s="12" t="s">
         <v>24</v>
       </c>
       <c r="R256" s="12">
         <f>DATEDIF(Tabela1[[#This Row],[Atendimento]],Tabela1[[#This Row],[Previsao de Entrega]],"D")</f>
-        <v>32</v>
+        <v>8</v>
       </c>
       <c r="S256" s="14">
-        <v>1215.25</v>
+        <v>0</v>
       </c>
       <c r="T256" s="14">
         <v>0</v>
@@ -18568,10 +18581,10 @@
     </row>
     <row r="257" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A257" s="11">
-        <v>45877</v>
+        <v>45880</v>
       </c>
       <c r="B257" s="11">
-        <v>45873</v>
+        <v>45868</v>
       </c>
       <c r="C257" s="11" t="s">
         <v>7</v>
@@ -18582,33 +18595,33 @@
       <c r="E257" s="11" t="s">
         <v>113</v>
       </c>
-      <c r="F257" s="12">
-        <v>68493</v>
+      <c r="F257" s="12" t="s">
+        <v>3</v>
       </c>
       <c r="G257" s="12" t="s">
-        <v>321</v>
+        <v>3</v>
       </c>
       <c r="H257" s="12" t="s">
-        <v>91</v>
+        <v>32</v>
       </c>
       <c r="I257" s="13">
         <f t="shared" si="4"/>
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="J257" s="12">
-        <v>66607</v>
+        <v>66629</v>
       </c>
       <c r="K257" s="12">
-        <v>1586</v>
+        <v>11121</v>
       </c>
       <c r="L257" s="12" t="s">
-        <v>408</v>
+        <v>143</v>
       </c>
       <c r="M257" s="11">
-        <v>45907</v>
+        <v>45894</v>
       </c>
       <c r="N257" s="14">
-        <v>680</v>
+        <v>1242.04</v>
       </c>
       <c r="O257" s="12" t="s">
         <v>122</v>
@@ -18621,10 +18634,10 @@
       </c>
       <c r="R257" s="12">
         <f>DATEDIF(Tabela1[[#This Row],[Atendimento]],Tabela1[[#This Row],[Previsao de Entrega]],"D")</f>
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="S257" s="14">
-        <v>0</v>
+        <v>108</v>
       </c>
       <c r="T257" s="14">
         <v>0</v>
@@ -18632,63 +18645,63 @@
     </row>
     <row r="258" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A258" s="11">
-        <v>45867</v>
+        <v>45882</v>
       </c>
       <c r="B258" s="11">
-        <v>45866</v>
+        <v>45881</v>
       </c>
       <c r="C258" s="11" t="s">
         <v>7</v>
       </c>
       <c r="D258" s="11" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="E258" s="11" t="s">
         <v>124</v>
       </c>
       <c r="F258" s="12">
-        <v>68483</v>
+        <v>68503</v>
       </c>
       <c r="G258" s="12" t="s">
-        <v>125</v>
+        <v>227</v>
       </c>
       <c r="H258" s="12" t="s">
-        <v>126</v>
+        <v>98</v>
       </c>
       <c r="I258" s="13">
         <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="J258" s="12">
-        <v>66467</v>
+        <v>66669</v>
       </c>
       <c r="K258" s="12">
-        <v>11164</v>
+        <v>3509</v>
       </c>
       <c r="L258" s="12" t="s">
-        <v>298</v>
+        <v>333</v>
       </c>
       <c r="M258" s="11">
-        <v>45908</v>
+        <v>45894</v>
       </c>
       <c r="N258" s="14">
-        <v>2623.03</v>
+        <v>1920</v>
       </c>
       <c r="O258" s="12" t="s">
         <v>122</v>
       </c>
       <c r="P258" s="12">
-        <v>28</v>
+        <v>7</v>
       </c>
       <c r="Q258" s="12" t="s">
         <v>24</v>
       </c>
       <c r="R258" s="12">
         <f>DATEDIF(Tabela1[[#This Row],[Atendimento]],Tabela1[[#This Row],[Previsao de Entrega]],"D")</f>
-        <v>41</v>
+        <v>12</v>
       </c>
       <c r="S258" s="14">
-        <v>52</v>
+        <v>0</v>
       </c>
       <c r="T258" s="14">
         <v>0</v>
@@ -18696,13 +18709,13 @@
     </row>
     <row r="259" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A259" s="11">
-        <v>45870</v>
+        <v>45881</v>
       </c>
       <c r="B259" s="11">
-        <v>45870</v>
+        <v>45881</v>
       </c>
       <c r="C259" s="11" t="s">
-        <v>128</v>
+        <v>7</v>
       </c>
       <c r="D259" s="11" t="s">
         <v>15</v>
@@ -18710,46 +18723,46 @@
       <c r="E259" s="11" t="s">
         <v>124</v>
       </c>
-      <c r="F259" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="G259" s="12" t="s">
-        <v>125</v>
+      <c r="F259" s="12">
+        <v>68501</v>
+      </c>
+      <c r="G259" s="12">
+        <v>2289</v>
       </c>
       <c r="H259" s="12" t="s">
-        <v>126</v>
+        <v>91</v>
       </c>
       <c r="I259" s="13">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="J259" s="12">
-        <v>66430</v>
+        <v>66662</v>
       </c>
       <c r="K259" s="12">
-        <v>333</v>
+        <v>3040</v>
       </c>
       <c r="L259" s="12" t="s">
-        <v>400</v>
+        <v>214</v>
       </c>
       <c r="M259" s="11">
-        <v>46113</v>
+        <v>45896</v>
       </c>
       <c r="N259" s="14">
-        <v>281569.34000000003</v>
+        <v>1000</v>
       </c>
       <c r="O259" s="12" t="s">
         <v>122</v>
       </c>
       <c r="P259" s="12">
-        <v>120</v>
+        <v>30</v>
       </c>
       <c r="Q259" s="12" t="s">
         <v>24</v>
       </c>
       <c r="R259" s="12">
         <f>DATEDIF(Tabela1[[#This Row],[Atendimento]],Tabela1[[#This Row],[Previsao de Entrega]],"D")</f>
-        <v>243</v>
+        <v>15</v>
       </c>
       <c r="S259" s="14">
         <v>0</v>
@@ -18760,141 +18773,141 @@
     </row>
     <row r="260" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A260" s="11">
-        <v>45882</v>
+        <v>45868</v>
       </c>
       <c r="B260" s="11">
-        <v>45881</v>
+        <v>45868</v>
       </c>
       <c r="C260" s="11" t="s">
         <v>7</v>
       </c>
       <c r="D260" s="11" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="E260" s="11" t="s">
         <v>124</v>
       </c>
-      <c r="F260" s="12">
-        <v>68503</v>
+      <c r="F260" s="12" t="s">
+        <v>3</v>
       </c>
       <c r="G260" s="12" t="s">
-        <v>227</v>
+        <v>125</v>
       </c>
       <c r="H260" s="12" t="s">
-        <v>98</v>
+        <v>126</v>
       </c>
       <c r="I260" s="13">
-        <f>NETWORKDAYS(B260, A260)</f>
-        <v>2</v>
+        <f t="shared" si="4"/>
+        <v>1</v>
       </c>
       <c r="J260" s="12">
-        <v>66669</v>
-      </c>
-      <c r="K260" s="52">
-        <v>3509</v>
+        <v>66504</v>
+      </c>
+      <c r="K260" s="12">
+        <v>3034</v>
       </c>
       <c r="L260" s="12" t="s">
-        <v>333</v>
+        <v>349</v>
       </c>
       <c r="M260" s="11">
-        <v>45894</v>
+        <v>45897</v>
       </c>
       <c r="N260" s="14">
-        <v>1920</v>
+        <v>2220</v>
       </c>
       <c r="O260" s="12" t="s">
         <v>122</v>
       </c>
       <c r="P260" s="12">
-        <v>7</v>
+        <v>90</v>
       </c>
       <c r="Q260" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="R260" s="52">
-        <f>DATEDIF(Tabela1[[#This Row],[Atendimento]],Tabela1[[#This Row],[Previsao de Entrega]],"D")</f>
-        <v>12</v>
+      <c r="R260" s="12">
+        <f>DATEDIF(Tabela1[[#This Row],[Atendimento]],Tabela1[[#This Row],[Previsao de Entrega]],"D")</f>
+        <v>29</v>
       </c>
       <c r="S260" s="14">
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="T260" s="14">
         <v>0</v>
       </c>
     </row>
     <row r="261" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A261" s="46">
-        <v>45882</v>
-      </c>
-      <c r="B261" s="46">
-        <v>45880</v>
-      </c>
-      <c r="C261" s="46" t="s">
-        <v>7</v>
-      </c>
-      <c r="D261" s="46" t="s">
+      <c r="A261" s="11">
+        <v>45869</v>
+      </c>
+      <c r="B261" s="11">
+        <v>45869</v>
+      </c>
+      <c r="C261" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D261" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="E261" s="46" t="s">
-        <v>113</v>
-      </c>
-      <c r="F261" s="47">
-        <v>68498</v>
-      </c>
-      <c r="G261" s="47" t="s">
-        <v>321</v>
-      </c>
-      <c r="H261" s="47" t="s">
-        <v>91</v>
-      </c>
-      <c r="I261" s="48">
-        <f>NETWORKDAYS(B261, A261)</f>
-        <v>3</v>
-      </c>
-      <c r="J261" s="53">
-        <v>66670</v>
-      </c>
-      <c r="K261" s="51">
-        <v>11796</v>
-      </c>
-      <c r="L261" s="47" t="s">
-        <v>411</v>
-      </c>
-      <c r="M261" s="46">
-        <v>45890</v>
-      </c>
-      <c r="N261" s="49">
-        <v>42.23</v>
-      </c>
-      <c r="O261" s="47" t="s">
-        <v>121</v>
-      </c>
-      <c r="P261" s="47">
-        <v>0</v>
-      </c>
-      <c r="Q261" s="47" t="s">
-        <v>407</v>
-      </c>
-      <c r="R261" s="51">
-        <f>DATEDIF(Tabela1[[#This Row],[Atendimento]],Tabela1[[#This Row],[Previsao de Entrega]],"D")</f>
-        <v>8</v>
-      </c>
-      <c r="S261" s="49">
-        <v>0</v>
-      </c>
-      <c r="T261" s="49">
+      <c r="E261" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="F261" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="G261" s="12" t="s">
+        <v>125</v>
+      </c>
+      <c r="H261" s="12" t="s">
+        <v>126</v>
+      </c>
+      <c r="I261" s="13">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="J261" s="12">
+        <v>66427</v>
+      </c>
+      <c r="K261" s="12">
+        <v>1277</v>
+      </c>
+      <c r="L261" s="12" t="s">
+        <v>397</v>
+      </c>
+      <c r="M261" s="11">
+        <v>45897</v>
+      </c>
+      <c r="N261" s="14">
+        <v>2715.75</v>
+      </c>
+      <c r="O261" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="P261" s="12">
+        <v>30</v>
+      </c>
+      <c r="Q261" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="R261" s="12">
+        <f>DATEDIF(Tabela1[[#This Row],[Atendimento]],Tabela1[[#This Row],[Previsao de Entrega]],"D")</f>
+        <v>28</v>
+      </c>
+      <c r="S261" s="14">
+        <v>950</v>
+      </c>
+      <c r="T261" s="14">
         <v>0</v>
       </c>
     </row>
     <row r="262" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A262" s="11">
-        <v>45882</v>
+        <v>45875</v>
       </c>
       <c r="B262" s="11">
-        <v>45880</v>
+        <v>45873</v>
       </c>
       <c r="C262" s="11" t="s">
-        <v>7</v>
+        <v>128</v>
       </c>
       <c r="D262" s="11" t="s">
         <v>15</v>
@@ -18902,60 +18915,60 @@
       <c r="E262" s="11" t="s">
         <v>124</v>
       </c>
-      <c r="F262" s="12">
-        <v>68499</v>
-      </c>
-      <c r="G262" s="12" t="s">
+      <c r="F262" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="G262" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="H262" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="I262" s="13">
+        <f t="shared" si="4"/>
+        <v>3</v>
+      </c>
+      <c r="J262" s="12">
+        <v>66430</v>
+      </c>
+      <c r="K262" s="12">
+        <v>333</v>
+      </c>
+      <c r="L262" s="12" t="s">
+        <v>399</v>
+      </c>
+      <c r="M262" s="11">
+        <v>45901</v>
+      </c>
+      <c r="N262" s="45">
+        <v>1483685.03</v>
+      </c>
+      <c r="O262" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="P262" s="12">
         <v>90</v>
-      </c>
-      <c r="H262" s="12" t="s">
-        <v>91</v>
-      </c>
-      <c r="I262" s="13">
-        <f>NETWORKDAYS(B262, A262)</f>
-        <v>3</v>
-      </c>
-      <c r="J262" s="12">
-        <v>66671</v>
-      </c>
-      <c r="K262" s="52">
-        <v>1277</v>
-      </c>
-      <c r="L262" s="12" t="s">
-        <v>398</v>
-      </c>
-      <c r="M262" s="11">
-        <v>45884</v>
-      </c>
-      <c r="N262" s="14">
-        <v>207.68</v>
-      </c>
-      <c r="O262" s="12" t="s">
-        <v>122</v>
-      </c>
-      <c r="P262" s="12">
-        <v>35</v>
       </c>
       <c r="Q262" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="R262" s="52">
-        <f>DATEDIF(Tabela1[[#This Row],[Atendimento]],Tabela1[[#This Row],[Previsao de Entrega]],"D")</f>
-        <v>2</v>
+      <c r="R262" s="12">
+        <f>DATEDIF(Tabela1[[#This Row],[Atendimento]],Tabela1[[#This Row],[Previsao de Entrega]],"D")</f>
+        <v>26</v>
       </c>
       <c r="S262" s="14">
         <v>0</v>
       </c>
       <c r="T262" s="14">
-        <v>0</v>
+        <v>59008.35</v>
       </c>
     </row>
     <row r="263" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A263" s="11">
-        <v>45882</v>
+        <v>45856</v>
       </c>
       <c r="B263" s="11">
-        <v>45881</v>
+        <v>45856</v>
       </c>
       <c r="C263" s="11" t="s">
         <v>7</v>
@@ -18964,38 +18977,38 @@
         <v>15</v>
       </c>
       <c r="E263" s="11" t="s">
-        <v>113</v>
+        <v>124</v>
       </c>
       <c r="F263" s="12">
-        <v>68502</v>
+        <v>68466</v>
       </c>
       <c r="G263" s="12" t="s">
-        <v>321</v>
+        <v>125</v>
       </c>
       <c r="H263" s="12" t="s">
-        <v>91</v>
+        <v>126</v>
       </c>
       <c r="I263" s="13">
-        <f>NETWORKDAYS(B263, A263)</f>
-        <v>2</v>
+        <f t="shared" si="4"/>
+        <v>1</v>
       </c>
       <c r="J263" s="12">
-        <v>66672</v>
-      </c>
-      <c r="K263" s="52">
-        <v>10594</v>
+        <v>66337</v>
+      </c>
+      <c r="K263" s="12">
+        <v>11736</v>
       </c>
       <c r="L263" s="12" t="s">
-        <v>412</v>
+        <v>127</v>
       </c>
       <c r="M263" s="11">
-        <v>45891</v>
+        <v>45902</v>
       </c>
       <c r="N263" s="14">
-        <v>1159.8</v>
+        <v>16134.54</v>
       </c>
       <c r="O263" s="12" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="P263" s="12">
         <v>28</v>
@@ -19003,271 +19016,788 @@
       <c r="Q263" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="R263" s="52">
-        <f>DATEDIF(Tabela1[[#This Row],[Atendimento]],Tabela1[[#This Row],[Previsao de Entrega]],"D")</f>
-        <v>9</v>
+      <c r="R263" s="12">
+        <f>DATEDIF(Tabela1[[#This Row],[Atendimento]],Tabela1[[#This Row],[Previsao de Entrega]],"D")</f>
+        <v>46</v>
       </c>
       <c r="S263" s="14">
-        <v>0</v>
+        <v>25720</v>
       </c>
       <c r="T263" s="14">
         <v>0</v>
       </c>
     </row>
     <row r="264" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A264" s="11">
-        <v>45882</v>
-      </c>
-      <c r="B264" s="11">
-        <v>45881</v>
-      </c>
-      <c r="C264" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="D264" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="E264" s="11" t="s">
+      <c r="A264" s="50">
+        <v>45840</v>
+      </c>
+      <c r="B264" s="50">
+        <v>45840</v>
+      </c>
+      <c r="C264" s="50" t="s">
+        <v>7</v>
+      </c>
+      <c r="D264" s="50" t="s">
+        <v>5</v>
+      </c>
+      <c r="E264" s="50" t="s">
         <v>113</v>
       </c>
-      <c r="F264" s="12">
-        <v>68502</v>
-      </c>
-      <c r="G264" s="12" t="s">
-        <v>321</v>
-      </c>
-      <c r="H264" s="12" t="s">
-        <v>91</v>
-      </c>
-      <c r="I264" s="13">
-        <f>NETWORKDAYS(B264, A264)</f>
-        <v>2</v>
-      </c>
-      <c r="J264" s="12">
-        <v>66673</v>
-      </c>
-      <c r="K264" s="52">
-        <v>11682</v>
-      </c>
-      <c r="L264" s="12" t="s">
-        <v>179</v>
-      </c>
-      <c r="M264" s="11">
-        <v>45891</v>
-      </c>
-      <c r="N264" s="14">
-        <v>1173.95</v>
-      </c>
-      <c r="O264" s="12" t="s">
+      <c r="F264" s="51">
+        <v>68452</v>
+      </c>
+      <c r="G264" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="H264" s="51" t="s">
+        <v>34</v>
+      </c>
+      <c r="I264" s="52">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="J264" s="51">
+        <v>66037</v>
+      </c>
+      <c r="K264" s="51">
+        <v>11775</v>
+      </c>
+      <c r="L264" s="51" t="s">
+        <v>353</v>
+      </c>
+      <c r="M264" s="50">
+        <v>45905</v>
+      </c>
+      <c r="N264" s="53">
+        <v>1750</v>
+      </c>
+      <c r="O264" s="51" t="s">
         <v>122</v>
       </c>
-      <c r="P264" s="12">
-        <v>28</v>
-      </c>
-      <c r="Q264" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="R264" s="52">
-        <f>DATEDIF(Tabela1[[#This Row],[Atendimento]],Tabela1[[#This Row],[Previsao de Entrega]],"D")</f>
-        <v>9</v>
-      </c>
-      <c r="S264" s="14">
-        <v>0</v>
-      </c>
-      <c r="T264" s="14">
+      <c r="P264" s="51">
+        <v>30</v>
+      </c>
+      <c r="Q264" s="51" t="s">
+        <v>414</v>
+      </c>
+      <c r="R264" s="51">
+        <f>DATEDIF(Tabela1[[#This Row],[Atendimento]],Tabela1[[#This Row],[Previsao de Entrega]],"D")</f>
+        <v>65</v>
+      </c>
+      <c r="S264" s="53">
+        <v>0</v>
+      </c>
+      <c r="T264" s="53">
         <v>0</v>
       </c>
     </row>
     <row r="265" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A265" s="11">
-        <v>45882</v>
+        <v>45848</v>
       </c>
       <c r="B265" s="11">
-        <v>45881</v>
+        <v>45848</v>
       </c>
       <c r="C265" s="11" t="s">
         <v>7</v>
       </c>
       <c r="D265" s="11" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="E265" s="11" t="s">
         <v>113</v>
       </c>
       <c r="F265" s="12">
-        <v>68502</v>
+        <v>68457</v>
       </c>
       <c r="G265" s="12" t="s">
-        <v>321</v>
+        <v>33</v>
       </c>
       <c r="H265" s="12" t="s">
-        <v>91</v>
+        <v>34</v>
       </c>
       <c r="I265" s="13">
-        <f>NETWORKDAYS(B265, A265)</f>
-        <v>2</v>
+        <f t="shared" si="4"/>
+        <v>1</v>
       </c>
       <c r="J265" s="12">
-        <v>66675</v>
-      </c>
-      <c r="K265" s="52">
-        <v>11783</v>
+        <v>66126</v>
+      </c>
+      <c r="K265" s="12">
+        <v>2931</v>
       </c>
       <c r="L265" s="12" t="s">
-        <v>373</v>
+        <v>366</v>
       </c>
       <c r="M265" s="11">
-        <v>45891</v>
+        <v>45905</v>
       </c>
       <c r="N265" s="14">
-        <v>227.88</v>
+        <v>3500</v>
       </c>
       <c r="O265" s="12" t="s">
         <v>122</v>
       </c>
       <c r="P265" s="12">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="Q265" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="R265" s="52">
-        <f>DATEDIF(Tabela1[[#This Row],[Atendimento]],Tabela1[[#This Row],[Previsao de Entrega]],"D")</f>
+      <c r="R265" s="12">
+        <f>DATEDIF(Tabela1[[#This Row],[Atendimento]],Tabela1[[#This Row],[Previsao de Entrega]],"D")</f>
+        <v>57</v>
+      </c>
+      <c r="S265" s="14">
+        <v>320</v>
+      </c>
+      <c r="T265" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="266" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A266" s="6">
+        <v>45882</v>
+      </c>
+      <c r="B266" s="6">
+        <v>45882</v>
+      </c>
+      <c r="C266" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D266" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E266" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="F266" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="G266" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="H266" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="I266" s="10">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="J266" s="7">
+        <v>65768</v>
+      </c>
+      <c r="K266" s="7">
+        <v>175</v>
+      </c>
+      <c r="L266" s="7" t="s">
+        <v>188</v>
+      </c>
+      <c r="M266" s="6">
+        <v>45882</v>
+      </c>
+      <c r="N266" s="8">
+        <v>3685</v>
+      </c>
+      <c r="O266" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="P266" s="7">
+        <v>30</v>
+      </c>
+      <c r="Q266" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="R266" s="7">
+        <f>DATEDIF(Tabela1[[#This Row],[Atendimento]],Tabela1[[#This Row],[Previsao de Entrega]],"D")</f>
+        <v>0</v>
+      </c>
+      <c r="S266" s="8">
+        <v>0</v>
+      </c>
+      <c r="T266" s="8">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="267" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A267" s="11">
+        <v>45874</v>
+      </c>
+      <c r="B267" s="11">
+        <v>45853</v>
+      </c>
+      <c r="C267" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D267" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="E267" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="F267" s="12">
+        <v>68465</v>
+      </c>
+      <c r="G267" s="12" t="s">
+        <v>125</v>
+      </c>
+      <c r="H267" s="12" t="s">
+        <v>126</v>
+      </c>
+      <c r="I267" s="13">
+        <f t="shared" ref="I267:I273" si="5">NETWORKDAYS(B267, A267)</f>
+        <v>16</v>
+      </c>
+      <c r="J267" s="12">
+        <v>66555</v>
+      </c>
+      <c r="K267" s="12">
+        <v>11791</v>
+      </c>
+      <c r="L267" s="12" t="s">
+        <v>402</v>
+      </c>
+      <c r="M267" s="11">
+        <v>45906</v>
+      </c>
+      <c r="N267" s="14">
+        <v>1075.55</v>
+      </c>
+      <c r="O267" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="P267" s="12">
+        <v>20</v>
+      </c>
+      <c r="Q267" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="R267" s="12">
+        <f>DATEDIF(Tabela1[[#This Row],[Atendimento]],Tabela1[[#This Row],[Previsao de Entrega]],"D")</f>
+        <v>32</v>
+      </c>
+      <c r="S267" s="14">
+        <v>1215.25</v>
+      </c>
+      <c r="T267" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="268" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A268" s="11">
+        <v>45877</v>
+      </c>
+      <c r="B268" s="11">
+        <v>45873</v>
+      </c>
+      <c r="C268" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D268" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="E268" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="F268" s="12">
+        <v>68493</v>
+      </c>
+      <c r="G268" s="12" t="s">
+        <v>321</v>
+      </c>
+      <c r="H268" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="I268" s="13">
+        <f t="shared" si="5"/>
+        <v>5</v>
+      </c>
+      <c r="J268" s="12">
+        <v>66607</v>
+      </c>
+      <c r="K268" s="12">
+        <v>1586</v>
+      </c>
+      <c r="L268" s="12" t="s">
+        <v>406</v>
+      </c>
+      <c r="M268" s="11">
+        <v>45907</v>
+      </c>
+      <c r="N268" s="14">
+        <v>680</v>
+      </c>
+      <c r="O268" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="P268" s="12">
+        <v>30</v>
+      </c>
+      <c r="Q268" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="R268" s="12">
+        <f>DATEDIF(Tabela1[[#This Row],[Atendimento]],Tabela1[[#This Row],[Previsao de Entrega]],"D")</f>
+        <v>30</v>
+      </c>
+      <c r="S268" s="14">
+        <v>0</v>
+      </c>
+      <c r="T268" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="269" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A269" s="11">
+        <v>45867</v>
+      </c>
+      <c r="B269" s="11">
+        <v>45866</v>
+      </c>
+      <c r="C269" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D269" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="E269" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="F269" s="12">
+        <v>68483</v>
+      </c>
+      <c r="G269" s="12" t="s">
+        <v>125</v>
+      </c>
+      <c r="H269" s="12" t="s">
+        <v>126</v>
+      </c>
+      <c r="I269" s="13">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="J269" s="12">
+        <v>66467</v>
+      </c>
+      <c r="K269" s="12">
+        <v>11164</v>
+      </c>
+      <c r="L269" s="12" t="s">
+        <v>298</v>
+      </c>
+      <c r="M269" s="11">
+        <v>45908</v>
+      </c>
+      <c r="N269" s="14">
+        <v>2623.03</v>
+      </c>
+      <c r="O269" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="P269" s="12">
+        <v>28</v>
+      </c>
+      <c r="Q269" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="R269" s="12">
+        <f>DATEDIF(Tabela1[[#This Row],[Atendimento]],Tabela1[[#This Row],[Previsao de Entrega]],"D")</f>
+        <v>41</v>
+      </c>
+      <c r="S269" s="14">
+        <v>52</v>
+      </c>
+      <c r="T269" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="270" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A270" s="6">
+        <v>45883</v>
+      </c>
+      <c r="B270" s="6">
+        <v>45883</v>
+      </c>
+      <c r="C270" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D270" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E270" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="F270" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="G270" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="H270" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="I270" s="10">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="J270" s="7">
+        <v>66706</v>
+      </c>
+      <c r="K270" s="7">
+        <v>10581</v>
+      </c>
+      <c r="L270" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="M270" s="6">
+        <v>45883</v>
+      </c>
+      <c r="N270" s="8">
+        <v>9854.93</v>
+      </c>
+      <c r="O270" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="P270" s="7">
+        <v>14</v>
+      </c>
+      <c r="Q270" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="R270" s="7">
+        <f>DATEDIF(Tabela1[[#This Row],[Atendimento]],Tabela1[[#This Row],[Previsao de Entrega]],"D")</f>
+        <v>0</v>
+      </c>
+      <c r="S270" s="8">
+        <v>0</v>
+      </c>
+      <c r="T270" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="271" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A271" s="11">
+        <v>45870</v>
+      </c>
+      <c r="B271" s="11">
+        <v>45870</v>
+      </c>
+      <c r="C271" s="11" t="s">
+        <v>128</v>
+      </c>
+      <c r="D271" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="E271" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="F271" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="G271" s="12" t="s">
+        <v>125</v>
+      </c>
+      <c r="H271" s="12" t="s">
+        <v>126</v>
+      </c>
+      <c r="I271" s="13">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="J271" s="12">
+        <v>66430</v>
+      </c>
+      <c r="K271" s="12">
+        <v>333</v>
+      </c>
+      <c r="L271" s="12" t="s">
+        <v>399</v>
+      </c>
+      <c r="M271" s="11">
+        <v>46113</v>
+      </c>
+      <c r="N271" s="14">
+        <v>281569.34000000003</v>
+      </c>
+      <c r="O271" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="P271" s="12">
+        <v>120</v>
+      </c>
+      <c r="Q271" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="R271" s="12">
+        <f>DATEDIF(Tabela1[[#This Row],[Atendimento]],Tabela1[[#This Row],[Previsao de Entrega]],"D")</f>
+        <v>243</v>
+      </c>
+      <c r="S271" s="14">
+        <v>0</v>
+      </c>
+      <c r="T271" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="272" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A272" s="11">
+        <v>45884</v>
+      </c>
+      <c r="B272" s="11">
+        <v>45883</v>
+      </c>
+      <c r="C272" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D272" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="E272" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="F272" s="12">
+        <v>68509</v>
+      </c>
+      <c r="G272" s="12" t="s">
+        <v>321</v>
+      </c>
+      <c r="H272" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="I272" s="13">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="J272" s="12">
+        <v>66713</v>
+      </c>
+      <c r="K272" s="12">
+        <v>3636</v>
+      </c>
+      <c r="L272" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="M272" s="11">
+        <v>45890</v>
+      </c>
+      <c r="N272" s="14">
+        <v>425.09</v>
+      </c>
+      <c r="O272" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="P272" s="12">
+        <v>28</v>
+      </c>
+      <c r="Q272" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="R272" s="12">
+        <f>DATEDIF(Tabela1[[#This Row],[Atendimento]],Tabela1[[#This Row],[Previsao de Entrega]],"D")</f>
+        <v>6</v>
+      </c>
+      <c r="S272" s="14">
+        <v>0</v>
+      </c>
+      <c r="T272" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="273" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A273" s="11">
+        <v>45884</v>
+      </c>
+      <c r="B273" s="11">
+        <v>45874</v>
+      </c>
+      <c r="C273" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D273" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="E273" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="F273" s="12">
+        <v>68496</v>
+      </c>
+      <c r="G273" s="12" t="s">
+        <v>136</v>
+      </c>
+      <c r="H273" s="12" t="s">
+        <v>126</v>
+      </c>
+      <c r="I273" s="13">
+        <f t="shared" si="5"/>
         <v>9</v>
       </c>
-      <c r="S265" s="14">
-        <v>0</v>
-      </c>
-      <c r="T265" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="266" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A266" s="11">
-        <v>45882</v>
-      </c>
-      <c r="B266" s="11">
-        <v>45882</v>
-      </c>
-      <c r="C266" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="D266" s="11" t="s">
+      <c r="J273" s="12">
+        <v>66714</v>
+      </c>
+      <c r="K273" s="12">
+        <v>881</v>
+      </c>
+      <c r="L273" s="12" t="s">
+        <v>418</v>
+      </c>
+      <c r="M273" s="11">
+        <v>45891</v>
+      </c>
+      <c r="N273" s="14">
+        <v>4736.25</v>
+      </c>
+      <c r="O273" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="P273" s="12">
+        <v>35</v>
+      </c>
+      <c r="Q273" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="R273" s="12">
+        <f>DATEDIF(Tabela1[[#This Row],[Atendimento]],Tabela1[[#This Row],[Previsao de Entrega]],"D")</f>
+        <v>7</v>
+      </c>
+      <c r="S273" s="14">
+        <v>0</v>
+      </c>
+      <c r="T273" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="274" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A274" s="11">
+        <v>45884</v>
+      </c>
+      <c r="B274" s="11">
+        <v>45874</v>
+      </c>
+      <c r="C274" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D274" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="E266" s="11" t="s">
+      <c r="E274" s="11" t="s">
         <v>113</v>
       </c>
-      <c r="F266" s="12">
-        <v>68507</v>
-      </c>
-      <c r="G266" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="H266" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="I266" s="13">
-        <f>NETWORKDAYS(B266, A266)</f>
+      <c r="F274" s="12">
+        <v>68496</v>
+      </c>
+      <c r="G274" s="12" t="s">
+        <v>136</v>
+      </c>
+      <c r="H274" s="12" t="s">
+        <v>126</v>
+      </c>
+      <c r="I274" s="13">
+        <f>NETWORKDAYS(B274, A274)</f>
+        <v>9</v>
+      </c>
+      <c r="J274" s="12">
+        <v>66718</v>
+      </c>
+      <c r="K274" s="12">
+        <v>3011</v>
+      </c>
+      <c r="L274" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="M274" s="11">
+        <v>45890</v>
+      </c>
+      <c r="N274" s="14">
+        <v>223.6</v>
+      </c>
+      <c r="O274" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="P274" s="12">
+        <v>28</v>
+      </c>
+      <c r="Q274" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="R274" s="12">
+        <f>DATEDIF(Tabela1[[#This Row],[Atendimento]],Tabela1[[#This Row],[Previsao de Entrega]],"D")</f>
+        <v>6</v>
+      </c>
+      <c r="S274" s="14">
+        <v>0</v>
+      </c>
+      <c r="T274" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="275" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A275" s="50">
+        <v>45884</v>
+      </c>
+      <c r="B275" s="50">
+        <v>45884</v>
+      </c>
+      <c r="C275" s="50" t="s">
+        <v>7</v>
+      </c>
+      <c r="D275" s="50" t="s">
+        <v>15</v>
+      </c>
+      <c r="E275" s="50" t="s">
+        <v>113</v>
+      </c>
+      <c r="F275" s="51">
+        <v>68511</v>
+      </c>
+      <c r="G275" s="51" t="s">
+        <v>296</v>
+      </c>
+      <c r="H275" s="51" t="s">
+        <v>96</v>
+      </c>
+      <c r="I275" s="52">
+        <f>NETWORKDAYS(B275, A275)</f>
         <v>1</v>
       </c>
-      <c r="J266" s="12">
-        <v>66681</v>
-      </c>
-      <c r="K266" s="52">
-        <v>10627</v>
-      </c>
-      <c r="L266" s="12" t="s">
-        <v>362</v>
-      </c>
-      <c r="M266" s="11">
+      <c r="J275" s="51">
+        <v>66720</v>
+      </c>
+      <c r="K275" s="51">
+        <v>74</v>
+      </c>
+      <c r="L275" s="51" t="s">
+        <v>97</v>
+      </c>
+      <c r="M275" s="50">
         <v>45890</v>
       </c>
-      <c r="N266" s="14">
-        <v>850</v>
-      </c>
-      <c r="O266" s="12" t="s">
+      <c r="N275" s="53">
+        <v>299.72000000000003</v>
+      </c>
+      <c r="O275" s="51" t="s">
         <v>122</v>
       </c>
-      <c r="P266" s="12">
+      <c r="P275" s="51">
         <v>28</v>
       </c>
-      <c r="Q266" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="R266" s="52">
-        <f>DATEDIF(Tabela1[[#This Row],[Atendimento]],Tabela1[[#This Row],[Previsao de Entrega]],"D")</f>
-        <v>8</v>
-      </c>
-      <c r="S266" s="14">
-        <v>0</v>
-      </c>
-      <c r="T266" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="267" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A267" s="6">
-        <v>45882</v>
-      </c>
-      <c r="B267" s="6">
-        <v>45882</v>
-      </c>
-      <c r="C267" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="D267" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="E267" s="6" t="s">
-        <v>142</v>
-      </c>
-      <c r="F267" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="G267" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="H267" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="I267" s="10">
-        <f>NETWORKDAYS(B267, A267)</f>
-        <v>1</v>
-      </c>
-      <c r="J267" s="7">
-        <v>65768</v>
-      </c>
-      <c r="K267" s="50">
-        <v>175</v>
-      </c>
-      <c r="L267" s="7" t="s">
-        <v>188</v>
-      </c>
-      <c r="M267" s="6">
-        <v>45882</v>
-      </c>
-      <c r="N267" s="8">
-        <v>3685</v>
-      </c>
-      <c r="O267" s="7" t="s">
-        <v>122</v>
-      </c>
-      <c r="P267" s="7">
-        <v>30</v>
-      </c>
-      <c r="Q267" s="7" t="s">
-        <v>116</v>
-      </c>
-      <c r="R267" s="50">
-        <f>DATEDIF(Tabela1[[#This Row],[Atendimento]],Tabela1[[#This Row],[Previsao de Entrega]],"D")</f>
-        <v>0</v>
-      </c>
-      <c r="S267" s="8">
-        <v>0</v>
-      </c>
-      <c r="T267" s="8">
-        <v>191</v>
+      <c r="Q275" s="51" t="s">
+        <v>414</v>
+      </c>
+      <c r="R275" s="51">
+        <f>DATEDIF(Tabela1[[#This Row],[Atendimento]],Tabela1[[#This Row],[Previsao de Entrega]],"D")</f>
+        <v>6</v>
+      </c>
+      <c r="S275" s="53">
+        <v>0</v>
+      </c>
+      <c r="T275" s="53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="281" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="J281" s="54" t="s">
+        <v>415</v>
       </c>
     </row>
   </sheetData>
@@ -19285,7 +19815,7 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -19543,7 +20073,7 @@
       </c>
       <c r="E2" s="24">
         <f t="shared" ref="E2:E6" ca="1" si="0">TODAY()</f>
-        <v>45882</v>
+        <v>45884</v>
       </c>
       <c r="F2" s="22" t="str">
         <f ca="1">IF(Tabela4[[#This Row],[Hoje]] &lt;= Tabela4[[#This Row],[Validade]],
@@ -19551,7 +20081,7 @@
       "Negociar",
       "Faltam " &amp; DATEDIF(Tabela4[[#This Row],[Hoje]],Tabela4[[#This Row],[Validade]],"D") &amp; " dias para vencer"),
    "Venceu há " &amp; DATEDIF(Tabela4[[#This Row],[Validade]],Tabela4[[#This Row],[Hoje]],"D") &amp; " dias")</f>
-        <v>Faltam 584 dias para vencer</v>
+        <v>Faltam 582 dias para vencer</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.35">
@@ -19569,7 +20099,7 @@
       </c>
       <c r="E3" s="26">
         <f t="shared" ca="1" si="0"/>
-        <v>45882</v>
+        <v>45884</v>
       </c>
       <c r="F3" s="21" t="str">
         <f ca="1">IF(Tabela4[[#This Row],[Hoje]] &lt;= Tabela4[[#This Row],[Validade]],
@@ -19577,7 +20107,7 @@
       "Negociar",
       "Faltam " &amp; DATEDIF(Tabela4[[#This Row],[Hoje]],Tabela4[[#This Row],[Validade]],"D") &amp; " dias para vencer"),
    "Venceu há " &amp; DATEDIF(Tabela4[[#This Row],[Validade]],Tabela4[[#This Row],[Hoje]],"D") &amp; " dias")</f>
-        <v>Venceu há 316 dias</v>
+        <v>Venceu há 318 dias</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.35">
@@ -19595,7 +20125,7 @@
       </c>
       <c r="E4" s="32">
         <f t="shared" ca="1" si="0"/>
-        <v>45882</v>
+        <v>45884</v>
       </c>
       <c r="F4" s="33" t="str">
         <f ca="1">IF(Tabela4[[#This Row],[Hoje]] &lt;= Tabela4[[#This Row],[Validade]],
@@ -19603,7 +20133,7 @@
       "Negociar",
       "Faltam " &amp; DATEDIF(Tabela4[[#This Row],[Hoje]],Tabela4[[#This Row],[Validade]],"D") &amp; " dias para vencer"),
    "Venceu há " &amp; DATEDIF(Tabela4[[#This Row],[Validade]],Tabela4[[#This Row],[Hoje]],"D") &amp; " dias")</f>
-        <v>Venceu há 24 dias</v>
+        <v>Venceu há 26 dias</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.35">
@@ -19621,7 +20151,7 @@
       </c>
       <c r="E5" s="17">
         <f t="shared" ca="1" si="0"/>
-        <v>45882</v>
+        <v>45884</v>
       </c>
       <c r="F5" s="3" t="str">
         <f ca="1">IF(Tabela4[[#This Row],[Hoje]] &lt;= Tabela4[[#This Row],[Validade]],
@@ -19647,7 +20177,7 @@
       </c>
       <c r="E6" s="17">
         <f t="shared" ca="1" si="0"/>
-        <v>45882</v>
+        <v>45884</v>
       </c>
       <c r="F6" s="3" t="str">
         <f ca="1">IF(Tabela4[[#This Row],[Hoje]] &lt;= Tabela4[[#This Row],[Validade]],
@@ -19673,7 +20203,7 @@
       </c>
       <c r="E7" s="26">
         <f t="shared" ref="E7:E9" ca="1" si="1">TODAY()</f>
-        <v>45882</v>
+        <v>45884</v>
       </c>
       <c r="F7" s="21" t="str">
         <f ca="1">IF(Tabela4[[#This Row],[Hoje]] &lt;= Tabela4[[#This Row],[Validade]],
@@ -19681,7 +20211,7 @@
       "Negociar",
       "Faltam " &amp; DATEDIF(Tabela4[[#This Row],[Hoje]],Tabela4[[#This Row],[Validade]],"D") &amp; " dias para vencer"),
    "Venceu há " &amp; DATEDIF(Tabela4[[#This Row],[Validade]],Tabela4[[#This Row],[Hoje]],"D") &amp; " dias")</f>
-        <v>Venceu há 148 dias</v>
+        <v>Venceu há 150 dias</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.35">
@@ -19699,7 +20229,7 @@
       </c>
       <c r="E8" s="26">
         <f t="shared" ca="1" si="1"/>
-        <v>45882</v>
+        <v>45884</v>
       </c>
       <c r="F8" s="21" t="str">
         <f ca="1">IF(Tabela4[[#This Row],[Hoje]] &lt;= Tabela4[[#This Row],[Validade]],
@@ -19707,7 +20237,7 @@
       "Negociar",
       "Faltam " &amp; DATEDIF(Tabela4[[#This Row],[Hoje]],Tabela4[[#This Row],[Validade]],"D") &amp; " dias para vencer"),
    "Venceu há " &amp; DATEDIF(Tabela4[[#This Row],[Validade]],Tabela4[[#This Row],[Hoje]],"D") &amp; " dias")</f>
-        <v>Venceu há 891 dias</v>
+        <v>Venceu há 893 dias</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.35">
@@ -19725,7 +20255,7 @@
       </c>
       <c r="E9" s="24">
         <f t="shared" ca="1" si="1"/>
-        <v>45882</v>
+        <v>45884</v>
       </c>
       <c r="F9" s="22" t="str">
         <f ca="1">IF(Tabela4[[#This Row],[Hoje]] &lt;= Tabela4[[#This Row],[Validade]],
@@ -19733,7 +20263,7 @@
       "Negociar",
       "Faltam " &amp; DATEDIF(Tabela4[[#This Row],[Hoje]],Tabela4[[#This Row],[Validade]],"D") &amp; " dias para vencer"),
    "Venceu há " &amp; DATEDIF(Tabela4[[#This Row],[Validade]],Tabela4[[#This Row],[Hoje]],"D") &amp; " dias")</f>
-        <v>Faltam 400 dias para vencer</v>
+        <v>Faltam 398 dias para vencer</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.35">
@@ -19751,7 +20281,7 @@
       </c>
       <c r="E10" s="24">
         <f ca="1">TODAY()</f>
-        <v>45882</v>
+        <v>45884</v>
       </c>
       <c r="F10" s="22" t="str">
         <f ca="1">IF(Tabela4[[#This Row],[Hoje]] &lt;= Tabela4[[#This Row],[Validade]],
@@ -19759,7 +20289,7 @@
       "Negociar",
       "Faltam " &amp; DATEDIF(Tabela4[[#This Row],[Hoje]],Tabela4[[#This Row],[Validade]],"D") &amp; " dias para vencer"),
    "Venceu há " &amp; DATEDIF(Tabela4[[#This Row],[Validade]],Tabela4[[#This Row],[Hoje]],"D") &amp; " dias")</f>
-        <v>Faltam 321 dias para vencer</v>
+        <v>Faltam 319 dias para vencer</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.35">
@@ -19777,7 +20307,7 @@
       </c>
       <c r="E11" s="24">
         <f ca="1">TODAY()</f>
-        <v>45882</v>
+        <v>45884</v>
       </c>
       <c r="F11" s="22" t="str">
         <f ca="1">IF(Tabela4[[#This Row],[Hoje]] &lt;= Tabela4[[#This Row],[Validade]],
@@ -19785,7 +20315,7 @@
       "Negociar",
       "Faltam " &amp; DATEDIF(Tabela4[[#This Row],[Hoje]],Tabela4[[#This Row],[Validade]],"D") &amp; " dias para vencer"),
    "Venceu há " &amp; DATEDIF(Tabela4[[#This Row],[Validade]],Tabela4[[#This Row],[Hoje]],"D") &amp; " dias")</f>
-        <v>Faltam 110 dias para vencer</v>
+        <v>Faltam 108 dias para vencer</v>
       </c>
     </row>
   </sheetData>
@@ -19807,7 +20337,7 @@
   <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B48" sqref="B48"/>
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -19854,7 +20384,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="3" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
@@ -19888,7 +20418,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="5" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>28</v>
       </c>
@@ -19905,7 +20435,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>72</v>
       </c>
@@ -19922,7 +20452,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="7" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
         <v>70</v>
       </c>
@@ -19939,7 +20469,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="8" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
         <v>80</v>
       </c>
@@ -19956,7 +20486,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="9" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
         <v>84</v>
       </c>
@@ -19973,7 +20503,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="10" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
         <v>93</v>
       </c>
@@ -19990,7 +20520,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="11" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
         <v>131</v>
       </c>
@@ -20007,7 +20537,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="12" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
         <v>153</v>
       </c>
@@ -20024,7 +20554,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="13" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
         <v>162</v>
       </c>
@@ -20041,7 +20571,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="14" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
         <v>163</v>
       </c>
@@ -20058,7 +20588,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="15" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
         <v>172</v>
       </c>
@@ -20075,7 +20605,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="16" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
         <v>135</v>
       </c>
@@ -20092,7 +20622,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="17" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" s="3" t="s">
         <v>197</v>
       </c>
@@ -20109,7 +20639,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="18" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" s="3" t="s">
         <v>217</v>
       </c>
@@ -20126,7 +20656,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="19" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" s="3" t="s">
         <v>234</v>
       </c>
@@ -20143,7 +20673,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="20" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" s="3" t="s">
         <v>254</v>
       </c>
@@ -20160,7 +20690,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="21" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" s="3" t="s">
         <v>258</v>
       </c>
@@ -20194,7 +20724,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="23" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" s="3" t="s">
         <v>306</v>
       </c>
@@ -20211,7 +20741,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="24" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" s="3" t="s">
         <v>315</v>
       </c>
@@ -20525,10 +21055,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CC6577E-1BBE-47C5-96B8-0E0691F59A60}">
-  <dimension ref="A1:E42"/>
+  <dimension ref="A1:E44"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="E44" sqref="E44"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="E49" sqref="E49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -21166,7 +21696,7 @@
         <v>11790</v>
       </c>
       <c r="E37" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.35">
@@ -21183,7 +21713,7 @@
         <v>11791</v>
       </c>
       <c r="E38" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.35">
@@ -21191,7 +21721,7 @@
         <v>45875</v>
       </c>
       <c r="B39" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="C39" t="s">
         <v>185</v>
@@ -21200,7 +21730,7 @@
         <v>11792</v>
       </c>
       <c r="E39" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.35">
@@ -21217,7 +21747,7 @@
         <v>11793</v>
       </c>
       <c r="E40" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.35">
@@ -21225,7 +21755,7 @@
         <v>45880</v>
       </c>
       <c r="B41" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="C41" t="s">
         <v>287</v>
@@ -21234,7 +21764,7 @@
         <v>11795</v>
       </c>
       <c r="E41" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.35">
@@ -21251,7 +21781,41 @@
         <v>11796</v>
       </c>
       <c r="E42" t="s">
-        <v>411</v>
+        <v>409</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A43" s="17">
+        <v>45883</v>
+      </c>
+      <c r="B43" t="s">
+        <v>412</v>
+      </c>
+      <c r="C43" t="s">
+        <v>96</v>
+      </c>
+      <c r="D43">
+        <v>11797</v>
+      </c>
+      <c r="E43" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A44" s="17">
+        <v>45883</v>
+      </c>
+      <c r="B44" t="s">
+        <v>384</v>
+      </c>
+      <c r="C44" t="s">
+        <v>416</v>
+      </c>
+      <c r="D44">
+        <v>11798</v>
+      </c>
+      <c r="E44" t="s">
+        <v>417</v>
       </c>
     </row>
   </sheetData>

</xml_diff>